<commit_message>
ci: rename models.md properly
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E0F44F-DAA4-514D-9630-7228BE02FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B738CAD8-5999-494D-8763-717E003574EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm" sheetId="2" r:id="rId2"/>
-    <sheet name="Models" sheetId="3" r:id="rId3"/>
+    <sheet name="Model" sheetId="3" r:id="rId3"/>
     <sheet name="Data" sheetId="5" r:id="rId4"/>
     <sheet name="MA Pair" sheetId="6" r:id="rId5"/>
     <sheet name="DMA Tuple" sheetId="4" r:id="rId6"/>
@@ -711,9 +711,6 @@
     <t>an abstract definition of which microservice shall run on which host, to indicate which Microservices may need to run on the same host</t>
   </si>
   <si>
-    <t xml:space="preserve"> Metadata for Models v0.9</t>
-  </si>
-  <si>
     <t>example Value</t>
   </si>
   <si>
@@ -1864,6 +1861,9 @@
   </si>
   <si>
     <t>{microserviceA: [microserviceA, microserviceB], microserviceB:[], microserviceC:[]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Metadata for Model v0.9</t>
   </si>
 </sst>
 </file>
@@ -2454,30 +2454,30 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2924,16 +2924,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3155,7 +3155,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>41</v>
@@ -3172,13 +3172,13 @@
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>534</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="F14" s="19" t="s">
         <v>535</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>536</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>13</v>
@@ -3188,17 +3188,17 @@
     <row r="15" spans="1:8" ht="54" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>548</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>549</v>
-      </c>
       <c r="F15" s="19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>47</v>
@@ -3208,17 +3208,17 @@
     <row r="16" spans="1:8" ht="54" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>541</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>542</v>
-      </c>
       <c r="F16" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>47</v>
@@ -3228,17 +3228,17 @@
     <row r="17" spans="1:8" ht="54" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>47</v>
@@ -3261,7 +3261,7 @@
       <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="112"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
@@ -3281,7 +3281,7 @@
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="112"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="9" t="s">
         <v>48</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A22" s="112"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="9" t="s">
         <v>50</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A23" s="112"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="9" t="s">
         <v>52</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A24" s="112"/>
+      <c r="A24" s="111"/>
       <c r="B24" s="9" t="s">
         <v>54</v>
       </c>
@@ -3361,7 +3361,7 @@
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A25" s="112"/>
+      <c r="A25" s="111"/>
       <c r="B25" s="9" t="s">
         <v>57</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="72" x14ac:dyDescent="0.2">
-      <c r="A26" s="112"/>
+      <c r="A26" s="111"/>
       <c r="B26" s="9" t="s">
         <v>61</v>
       </c>
@@ -3401,7 +3401,7 @@
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A27" s="112"/>
+      <c r="A27" s="111"/>
       <c r="B27" s="9" t="s">
         <v>65</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A28" s="112"/>
+      <c r="A28" s="111"/>
       <c r="B28" s="9" t="s">
         <v>67</v>
       </c>
@@ -3441,7 +3441,7 @@
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="112"/>
+      <c r="A29" s="111"/>
       <c r="B29" s="9" t="s">
         <v>69</v>
       </c>
@@ -3461,7 +3461,7 @@
       <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A30" s="112"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="9" t="s">
         <v>71</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="112"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="9" t="s">
         <v>73</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="113"/>
+      <c r="A33" s="116"/>
       <c r="B33" s="27" t="s">
         <v>77</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="113"/>
+      <c r="A34" s="116"/>
       <c r="B34" s="27" t="s">
         <v>80</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="113"/>
+      <c r="A35" s="116"/>
       <c r="B35" s="27" t="s">
         <v>83</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="113"/>
+      <c r="A36" s="116"/>
       <c r="B36" s="27" t="s">
         <v>86</v>
       </c>
@@ -3605,7 +3605,7 @@
       <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="72" x14ac:dyDescent="0.2">
-      <c r="A38" s="112"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="9" t="s">
         <v>90</v>
       </c>
@@ -3625,8 +3625,8 @@
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="112"/>
-      <c r="B39" s="114" t="s">
+      <c r="A39" s="111"/>
+      <c r="B39" s="112" t="s">
         <v>94</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -3647,8 +3647,8 @@
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A40" s="112"/>
-      <c r="B40" s="114"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="9" t="s">
         <v>98</v>
       </c>
@@ -3667,8 +3667,8 @@
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A41" s="112"/>
-      <c r="B41" s="114"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="9" t="s">
         <v>102</v>
       </c>
@@ -3687,8 +3687,8 @@
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A42" s="112"/>
-      <c r="B42" s="114"/>
+      <c r="A42" s="111"/>
+      <c r="B42" s="112"/>
       <c r="C42" s="9" t="s">
         <v>106</v>
       </c>
@@ -3707,8 +3707,8 @@
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="72" x14ac:dyDescent="0.2">
-      <c r="A43" s="112"/>
-      <c r="B43" s="114"/>
+      <c r="A43" s="111"/>
+      <c r="B43" s="112"/>
       <c r="C43" s="9" t="s">
         <v>110</v>
       </c>
@@ -3727,8 +3727,8 @@
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="112"/>
-      <c r="B44" s="114"/>
+      <c r="A44" s="111"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="9" t="s">
         <v>114</v>
       </c>
@@ -3747,8 +3747,8 @@
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="112"/>
-      <c r="B45" s="114"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="9" t="s">
         <v>118</v>
       </c>
@@ -3767,8 +3767,8 @@
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A46" s="112"/>
-      <c r="B46" s="114"/>
+      <c r="A46" s="111"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="9" t="s">
         <v>122</v>
       </c>
@@ -3787,8 +3787,8 @@
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A47" s="112"/>
-      <c r="B47" s="114"/>
+      <c r="A47" s="111"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="9" t="s">
         <v>126</v>
       </c>
@@ -3807,8 +3807,8 @@
       <c r="H47" s="12"/>
     </row>
     <row r="48" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A48" s="112"/>
-      <c r="B48" s="114"/>
+      <c r="A48" s="111"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="9" t="s">
         <v>130</v>
       </c>
@@ -3827,8 +3827,8 @@
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="112"/>
-      <c r="B49" s="114"/>
+      <c r="A49" s="111"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="9" t="s">
         <v>134</v>
       </c>
@@ -3847,8 +3847,8 @@
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A50" s="112"/>
-      <c r="B50" s="114"/>
+      <c r="A50" s="111"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="9" t="s">
         <v>138</v>
       </c>
@@ -3879,7 +3879,7 @@
       <c r="H51" s="26"/>
     </row>
     <row r="52" spans="1:8" ht="72" x14ac:dyDescent="0.2">
-      <c r="A52" s="115"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="32" t="s">
         <v>143</v>
       </c>
@@ -3899,8 +3899,8 @@
       <c r="H52" s="26"/>
     </row>
     <row r="53" spans="1:8" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116" t="s">
+      <c r="A53" s="113"/>
+      <c r="B53" s="114" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="35" t="s">
@@ -3921,8 +3921,8 @@
       <c r="H53" s="26"/>
     </row>
     <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A54" s="115"/>
-      <c r="B54" s="116"/>
+      <c r="A54" s="113"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="32" t="s">
         <v>98</v>
       </c>
@@ -3941,8 +3941,8 @@
       <c r="H54" s="26"/>
     </row>
     <row r="55" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A55" s="115"/>
-      <c r="B55" s="116"/>
+      <c r="A55" s="113"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="32" t="s">
         <v>102</v>
       </c>
@@ -3961,8 +3961,8 @@
       <c r="H55" s="26"/>
     </row>
     <row r="56" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116"/>
+      <c r="A56" s="113"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="32" t="s">
         <v>106</v>
       </c>
@@ -3981,8 +3981,8 @@
       <c r="H56" s="26"/>
     </row>
     <row r="57" spans="1:8" ht="72" x14ac:dyDescent="0.2">
-      <c r="A57" s="115"/>
-      <c r="B57" s="116"/>
+      <c r="A57" s="113"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="32" t="s">
         <v>110</v>
       </c>
@@ -4001,8 +4001,8 @@
       <c r="H57" s="26"/>
     </row>
     <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="115"/>
-      <c r="B58" s="116"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="32" t="s">
         <v>114</v>
       </c>
@@ -4021,8 +4021,8 @@
       <c r="H58" s="26"/>
     </row>
     <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="115"/>
-      <c r="B59" s="116"/>
+      <c r="A59" s="113"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="32" t="s">
         <v>118</v>
       </c>
@@ -4041,8 +4041,8 @@
       <c r="H59" s="26"/>
     </row>
     <row r="60" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A60" s="115"/>
-      <c r="B60" s="116"/>
+      <c r="A60" s="113"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="32" t="s">
         <v>122</v>
       </c>
@@ -4061,8 +4061,8 @@
       <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A61" s="115"/>
-      <c r="B61" s="116"/>
+      <c r="A61" s="113"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="32" t="s">
         <v>126</v>
       </c>
@@ -4081,8 +4081,8 @@
       <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A62" s="115"/>
-      <c r="B62" s="116"/>
+      <c r="A62" s="113"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="32" t="s">
         <v>130</v>
       </c>
@@ -4101,8 +4101,8 @@
       <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="115"/>
-      <c r="B63" s="116"/>
+      <c r="A63" s="113"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="32" t="s">
         <v>134</v>
       </c>
@@ -4121,8 +4121,8 @@
       <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A64" s="115"/>
-      <c r="B64" s="116"/>
+      <c r="A64" s="113"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="32" t="s">
         <v>138</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="H65" s="17"/>
     </row>
     <row r="66" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A66" s="117"/>
+      <c r="A66" s="115"/>
       <c r="B66" s="36" t="s">
         <v>151</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="H66" s="17"/>
     </row>
     <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A67" s="117"/>
+      <c r="A67" s="115"/>
       <c r="B67" s="36" t="s">
         <v>155</v>
       </c>
@@ -4205,7 +4205,7 @@
       <c r="H68" s="26"/>
     </row>
     <row r="69" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A69" s="113"/>
+      <c r="A69" s="116"/>
       <c r="B69" s="27" t="s">
         <v>160</v>
       </c>
@@ -4223,8 +4223,8 @@
       <c r="H69" s="22"/>
     </row>
     <row r="70" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="113"/>
-      <c r="B70" s="118" t="s">
+      <c r="A70" s="116"/>
+      <c r="B70" s="117" t="s">
         <v>163</v>
       </c>
       <c r="C70" s="27" t="s">
@@ -4245,8 +4245,8 @@
       <c r="H70" s="22"/>
     </row>
     <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A71" s="113"/>
-      <c r="B71" s="118"/>
+      <c r="A71" s="116"/>
+      <c r="B71" s="117"/>
       <c r="C71" s="27" t="s">
         <v>34</v>
       </c>
@@ -4265,8 +4265,8 @@
       <c r="H71" s="22"/>
     </row>
     <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A72" s="113"/>
-      <c r="B72" s="118"/>
+      <c r="A72" s="116"/>
+      <c r="B72" s="117"/>
       <c r="C72" s="27" t="s">
         <v>13</v>
       </c>
@@ -4285,8 +4285,8 @@
       <c r="H72" s="22"/>
     </row>
     <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A73" s="113"/>
-      <c r="B73" s="118"/>
+      <c r="A73" s="116"/>
+      <c r="B73" s="117"/>
       <c r="C73" s="27" t="s">
         <v>172</v>
       </c>
@@ -4305,8 +4305,8 @@
       <c r="H73" s="22"/>
     </row>
     <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A74" s="113"/>
-      <c r="B74" s="118"/>
+      <c r="A74" s="116"/>
+      <c r="B74" s="117"/>
       <c r="C74" s="27" t="s">
         <v>27</v>
       </c>
@@ -4337,7 +4337,7 @@
       <c r="H75" s="17"/>
     </row>
     <row r="76" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A76" s="112"/>
+      <c r="A76" s="111"/>
       <c r="B76" s="9" t="s">
         <v>178</v>
       </c>
@@ -4355,8 +4355,8 @@
       <c r="H76" s="12"/>
     </row>
     <row r="77" spans="1:8" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="112"/>
-      <c r="B77" s="114" t="s">
+      <c r="A77" s="111"/>
+      <c r="B77" s="112" t="s">
         <v>181</v>
       </c>
       <c r="C77" s="9" t="s">
@@ -4377,8 +4377,8 @@
       <c r="H77" s="12"/>
     </row>
     <row r="78" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A78" s="112"/>
-      <c r="B78" s="114"/>
+      <c r="A78" s="111"/>
+      <c r="B78" s="112"/>
       <c r="C78" s="9" t="s">
         <v>184</v>
       </c>
@@ -4397,8 +4397,8 @@
       <c r="H78" s="12"/>
     </row>
     <row r="79" spans="1:8" ht="54" x14ac:dyDescent="0.2">
-      <c r="A79" s="112"/>
-      <c r="B79" s="114"/>
+      <c r="A79" s="111"/>
+      <c r="B79" s="112"/>
       <c r="C79" s="9" t="s">
         <v>187</v>
       </c>
@@ -4417,8 +4417,8 @@
       <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A80" s="112"/>
-      <c r="B80" s="114"/>
+      <c r="A80" s="111"/>
+      <c r="B80" s="112"/>
       <c r="C80" s="9" t="s">
         <v>190</v>
       </c>
@@ -4437,8 +4437,8 @@
       <c r="H80" s="12"/>
     </row>
     <row r="81" spans="1:8" ht="108" x14ac:dyDescent="0.2">
-      <c r="A81" s="112"/>
-      <c r="B81" s="114"/>
+      <c r="A81" s="111"/>
+      <c r="B81" s="112"/>
       <c r="C81" s="9" t="s">
         <v>27</v>
       </c>
@@ -4530,6 +4530,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A20:A31"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A38:A50"/>
+    <mergeCell ref="B39:B50"/>
     <mergeCell ref="A76:A81"/>
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="A52:A64"/>
@@ -4537,11 +4542,6 @@
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="A69:A74"/>
     <mergeCell ref="B70:B74"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A20:A31"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A38:A50"/>
-    <mergeCell ref="B39:B50"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4557,7 +4557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4819,14 +4819,14 @@
     <row r="14" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="122"/>
       <c r="B14" s="19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>213</v>
@@ -4839,14 +4839,14 @@
     <row r="15" spans="1:8" ht="54" x14ac:dyDescent="0.2">
       <c r="A15" s="61"/>
       <c r="B15" s="19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>212</v>
@@ -4872,8 +4872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4890,16 +4890,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="111" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="A1" s="118" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:1024" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="63" t="s">
@@ -4915,7 +4915,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="65" t="s">
         <v>196</v>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="3" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H3" s="68"/>
       <c r="I3" s="69"/>
@@ -4974,15 +4974,15 @@
     <row r="4" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="124"/>
       <c r="B4" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="71"/>
@@ -4990,15 +4990,15 @@
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="124"/>
       <c r="B5" s="71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="71"/>
@@ -5006,15 +5006,15 @@
     <row r="6" spans="1:1024" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="124"/>
       <c r="B6" s="71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="71"/>
@@ -5022,15 +5022,15 @@
     <row r="7" spans="1:1024" ht="40" x14ac:dyDescent="0.2">
       <c r="A7" s="124"/>
       <c r="B7" s="71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="71"/>
@@ -5038,15 +5038,15 @@
     <row r="8" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="124"/>
       <c r="B8" s="71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="71"/>
@@ -5054,15 +5054,15 @@
     <row r="9" spans="1:1024" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="124"/>
       <c r="B9" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="71"/>
@@ -5070,15 +5070,15 @@
     <row r="10" spans="1:1024" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="124"/>
       <c r="B10" s="71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="71"/>
@@ -5103,11 +5103,11 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="71"/>
@@ -5115,15 +5115,15 @@
     <row r="12" spans="1:1024" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="124"/>
       <c r="B12" s="71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="71"/>
@@ -5131,33 +5131,33 @@
     <row r="13" spans="1:1024" ht="108" x14ac:dyDescent="0.2">
       <c r="A13" s="124"/>
       <c r="B13" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="71" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>243</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:1024" ht="54" x14ac:dyDescent="0.2">
       <c r="A14" s="124"/>
       <c r="B14" s="71" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C14" s="110"/>
       <c r="D14" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="110"/>
       <c r="F14" s="71" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G14" s="110" t="s">
         <v>47</v>
@@ -5167,22 +5167,22 @@
     <row r="15" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="124"/>
       <c r="B15" s="71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="71"/>
     </row>
     <row r="16" spans="1:1024" s="69" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="69" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H16" s="75"/>
       <c r="AMJ16" s="62"/>
@@ -5190,15 +5190,15 @@
     <row r="17" spans="1:1024" ht="127" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="125"/>
       <c r="B17" s="77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="77"/>
@@ -5206,13 +5206,13 @@
     <row r="18" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="125"/>
       <c r="B18" s="77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="77"/>
       <c r="E18" s="27"/>
       <c r="F18" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="77"/>
@@ -5220,22 +5220,22 @@
     <row r="19" spans="1:1024" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="125"/>
       <c r="B19" s="77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="77"/>
     </row>
     <row r="20" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H20" s="68"/>
       <c r="I20" s="69"/>
@@ -5280,15 +5280,15 @@
     <row r="21" spans="1:1024" s="74" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="70"/>
       <c r="B21" s="71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="71" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="71"/>
@@ -5326,11 +5326,11 @@
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="77"/>
@@ -5342,11 +5342,11 @@
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="77" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="77"/>
@@ -5358,18 +5358,18 @@
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="77" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="77"/>
     </row>
     <row r="26" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H26" s="68"/>
       <c r="I26" s="69"/>
@@ -5395,15 +5395,15 @@
     <row r="27" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="126"/>
       <c r="B27" s="71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>47</v>
@@ -5413,15 +5413,15 @@
     <row r="28" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="126"/>
       <c r="B28" s="71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="71" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>47</v>
@@ -5435,11 +5435,11 @@
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>47</v>
@@ -5453,11 +5453,11 @@
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>47</v>
@@ -5471,11 +5471,11 @@
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>47</v>
@@ -5509,11 +5509,11 @@
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="71" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>47</v>
@@ -5527,11 +5527,11 @@
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="71" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>47</v>
@@ -5545,11 +5545,11 @@
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>47</v>
@@ -5563,11 +5563,11 @@
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>47</v>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="36" spans="1:1024" s="69" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="123" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B36" s="123"/>
       <c r="C36" s="123"/>
@@ -5594,11 +5594,11 @@
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="77" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="77"/>
@@ -5643,7 +5643,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -5667,7 +5667,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="65" t="s">
         <v>196</v>
@@ -5681,7 +5681,7 @@
     </row>
     <row r="3" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H3" s="68"/>
       <c r="I3" s="69"/>
@@ -5701,106 +5701,106 @@
     <row r="4" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="124"/>
       <c r="B4" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="71" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="F4" s="71" t="s">
-        <v>331</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H4" s="93"/>
     </row>
     <row r="5" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="124"/>
       <c r="B5" s="71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="71" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F5" s="71" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H5" s="93"/>
     </row>
     <row r="6" spans="1:1024" ht="54" x14ac:dyDescent="0.2">
       <c r="A6" s="124"/>
       <c r="B6" s="71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="71" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F6" s="71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H6" s="93"/>
     </row>
     <row r="7" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="124"/>
       <c r="B7" s="71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="71" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="71" t="s">
         <v>338</v>
       </c>
-      <c r="F7" s="71" t="s">
-        <v>339</v>
-      </c>
       <c r="G7" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H7" s="93"/>
     </row>
     <row r="8" spans="1:1024" ht="72" x14ac:dyDescent="0.2">
       <c r="A8" s="124"/>
       <c r="B8" s="71" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="71" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="F8" s="71" t="s">
         <v>341</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="G8" s="9" t="s">
         <v>342</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>343</v>
       </c>
       <c r="H8" s="93"/>
     </row>
     <row r="9" spans="1:1024" s="69" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="123" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B9" s="123"/>
       <c r="C9" s="123"/>
@@ -5814,17 +5814,17 @@
     <row r="10" spans="1:1024" ht="54" x14ac:dyDescent="0.2">
       <c r="A10" s="125"/>
       <c r="B10" s="77" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E10" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="F10" s="77" t="s">
         <v>346</v>
-      </c>
-      <c r="F10" s="77" t="s">
-        <v>347</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>13</v>
@@ -5834,57 +5834,57 @@
     <row r="11" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="125"/>
       <c r="B11" s="77" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="F11" s="77" t="s">
         <v>349</v>
       </c>
-      <c r="F11" s="77" t="s">
-        <v>350</v>
-      </c>
       <c r="G11" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H11" s="94"/>
     </row>
     <row r="12" spans="1:1024" ht="72" x14ac:dyDescent="0.2">
       <c r="A12" s="125"/>
       <c r="B12" s="77" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="77" t="s">
+        <v>351</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="F12" s="77" t="s">
-        <v>354</v>
-      </c>
       <c r="G12" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H12" s="94"/>
     </row>
     <row r="13" spans="1:1024" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="125"/>
       <c r="B13" s="77" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="77" t="s">
         <v>356</v>
-      </c>
-      <c r="F13" s="77" t="s">
-        <v>357</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>13</v>
@@ -5894,44 +5894,44 @@
     <row r="14" spans="1:1024" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="125"/>
       <c r="B14" s="77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="F14" s="77" t="s">
         <v>359</v>
       </c>
-      <c r="F14" s="77" t="s">
-        <v>360</v>
-      </c>
       <c r="G14" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H14" s="94"/>
     </row>
     <row r="15" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="125"/>
       <c r="B15" s="77" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="77" t="s">
+        <v>361</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="F15" s="77" t="s">
         <v>363</v>
-      </c>
-      <c r="F15" s="77" t="s">
-        <v>364</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="94"/>
     </row>
     <row r="16" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H16" s="95"/>
       <c r="I16" s="69"/>
@@ -5947,26 +5947,26 @@
     <row r="17" spans="1:1024" ht="54" x14ac:dyDescent="0.2">
       <c r="A17" s="78"/>
       <c r="B17" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="71" t="s">
         <v>368</v>
       </c>
-      <c r="F17" s="71" t="s">
-        <v>369</v>
-      </c>
       <c r="G17" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H17" s="93"/>
     </row>
     <row r="18" spans="1:1024" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="123" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B18" s="123"/>
       <c r="C18" s="123"/>
@@ -5983,13 +5983,13 @@
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E19" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="F19" s="77" t="s">
         <v>371</v>
-      </c>
-      <c r="F19" s="77" t="s">
-        <v>372</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>13</v>
@@ -6003,13 +6003,13 @@
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E20" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="F20" s="77" t="s">
         <v>373</v>
-      </c>
-      <c r="F20" s="77" t="s">
-        <v>374</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>13</v>
@@ -6023,22 +6023,22 @@
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="77" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E21" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="F21" s="77" t="s">
         <v>375</v>
       </c>
-      <c r="F21" s="77" t="s">
+      <c r="G21" s="27" t="s">
         <v>376</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>377</v>
       </c>
       <c r="H21" s="94"/>
     </row>
     <row r="22" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H22" s="95"/>
       <c r="I22" s="69"/>
@@ -6057,36 +6057,36 @@
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="F23" s="71" t="s">
         <v>379</v>
       </c>
-      <c r="F23" s="71" t="s">
+      <c r="G23" s="9" t="s">
         <v>380</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>381</v>
       </c>
       <c r="H23" s="93"/>
     </row>
     <row r="24" spans="1:1024" ht="146.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="126"/>
       <c r="B24" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E24" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="F24" s="71" t="s">
         <v>383</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="G24" s="9" t="s">
         <v>384</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>385</v>
       </c>
       <c r="H24" s="93"/>
     </row>
@@ -6097,22 +6097,22 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="71" t="s">
+        <v>385</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="71" t="s">
         <v>387</v>
       </c>
-      <c r="F25" s="71" t="s">
+      <c r="G25" s="9" t="s">
         <v>388</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>389</v>
       </c>
       <c r="H25" s="93"/>
     </row>
     <row r="26" spans="1:1024" s="69" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="69" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H26" s="96"/>
       <c r="AMJ26" s="62"/>
@@ -6120,24 +6120,24 @@
     <row r="27" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="76"/>
       <c r="B27" s="77" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="77" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="77" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H27" s="94"/>
     </row>
     <row r="28" spans="1:1024" s="67" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="67" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H28" s="95"/>
       <c r="I28" s="69"/>
@@ -6156,16 +6156,16 @@
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E29" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="F29" s="71" t="s">
         <v>395</v>
       </c>
-      <c r="F29" s="71" t="s">
-        <v>396</v>
-      </c>
       <c r="G29" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H29" s="93"/>
     </row>
@@ -6176,16 +6176,16 @@
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F30" s="71" t="s">
         <v>397</v>
       </c>
-      <c r="F30" s="71" t="s">
-        <v>398</v>
-      </c>
       <c r="G30" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H30" s="93"/>
     </row>
@@ -6196,16 +6196,16 @@
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E31" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="F31" s="71" t="s">
         <v>399</v>
       </c>
-      <c r="F31" s="71" t="s">
-        <v>400</v>
-      </c>
       <c r="G31" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H31" s="93"/>
     </row>
@@ -6216,16 +6216,16 @@
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="F32" s="71" t="s">
         <v>401</v>
       </c>
-      <c r="F32" s="71" t="s">
-        <v>402</v>
-      </c>
       <c r="G32" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H32" s="93"/>
     </row>
@@ -6236,22 +6236,22 @@
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E33" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F33" s="71" t="s">
         <v>403</v>
       </c>
-      <c r="F33" s="71" t="s">
-        <v>404</v>
-      </c>
       <c r="G33" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H33" s="93"/>
     </row>
     <row r="34" spans="1:1024" s="69" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="123" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B34" s="123"/>
       <c r="C34" s="123"/>
@@ -6269,34 +6269,34 @@
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E35" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="F35" s="77" t="s">
         <v>406</v>
       </c>
-      <c r="F35" s="77" t="s">
-        <v>407</v>
-      </c>
       <c r="G35" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H35" s="94"/>
     </row>
     <row r="36" spans="1:1024" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="125"/>
       <c r="B36" s="77" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="77" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H36" s="94"/>
     </row>
@@ -6345,7 +6345,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="46.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -6369,7 +6369,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>196</v>
@@ -6402,47 +6402,47 @@
     <row r="4" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="128"/>
       <c r="B4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E4" s="90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="128"/>
       <c r="B5" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="90" t="s">
         <v>284</v>
       </c>
-      <c r="E5" s="90" t="s">
+      <c r="F5" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>286</v>
-      </c>
       <c r="G5" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="128"/>
       <c r="B6" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="11" t="s">
@@ -6452,7 +6452,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="9"/>
@@ -6460,77 +6460,77 @@
     <row r="7" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="128"/>
       <c r="B7" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="90" t="s">
+        <v>289</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>291</v>
-      </c>
       <c r="G7" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="128"/>
       <c r="B8" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E8" s="90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G8" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="128"/>
       <c r="B9" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="90" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="128"/>
       <c r="B10" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E10" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>416</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>417</v>
       </c>
       <c r="G10" s="84"/>
       <c r="H10" s="9"/>
@@ -6538,17 +6538,17 @@
     <row r="11" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="128"/>
       <c r="B11" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -6556,17 +6556,17 @@
     <row r="12" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="128"/>
       <c r="B12" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="90" t="s">
+        <v>419</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>420</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>421</v>
       </c>
       <c r="G12" s="84"/>
       <c r="H12" s="9"/>
@@ -6574,17 +6574,17 @@
     <row r="13" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="128"/>
       <c r="B13" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E13" s="90" t="s">
+        <v>309</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>310</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>311</v>
       </c>
       <c r="G13" s="84"/>
       <c r="H13" s="9"/>
@@ -6592,17 +6592,17 @@
     <row r="14" spans="1:1024" ht="72" x14ac:dyDescent="0.2">
       <c r="A14" s="128"/>
       <c r="B14" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>424</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>425</v>
       </c>
       <c r="G14" s="84"/>
       <c r="H14" s="9"/>
@@ -6610,17 +6610,17 @@
     <row r="15" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="128"/>
       <c r="B15" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>427</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>428</v>
       </c>
       <c r="G15" s="84"/>
       <c r="H15" s="9"/>
@@ -6628,17 +6628,17 @@
     <row r="16" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="128"/>
       <c r="B16" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>431</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>432</v>
       </c>
       <c r="G16" s="84"/>
       <c r="H16" s="9"/>
@@ -6646,7 +6646,7 @@
     <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="128"/>
       <c r="B17" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
@@ -6656,7 +6656,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G17" s="84"/>
       <c r="H17" s="84"/>
@@ -6664,17 +6664,17 @@
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="128"/>
       <c r="B18" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G18" s="84"/>
       <c r="H18" s="84"/>
@@ -6717,16 +6717,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="111" t="s">
-        <v>278</v>
-      </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="A1" s="118" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6742,7 +6742,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="80" t="s">
         <v>196</v>
@@ -6767,20 +6767,20 @@
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="129"/>
       <c r="B4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="71" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" s="83" t="s">
         <v>279</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="F4" s="71" t="s">
         <v>280</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="G4" s="84" t="s">
         <v>281</v>
-      </c>
-      <c r="G4" s="84" t="s">
-        <v>282</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="24"/>
@@ -6796,20 +6796,20 @@
     <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="129"/>
       <c r="B5" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="71" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="83" t="s">
         <v>284</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="F5" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>286</v>
-      </c>
       <c r="G5" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="24"/>
@@ -6825,17 +6825,17 @@
     <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="129"/>
       <c r="B6" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="71" t="s">
         <v>168</v>
       </c>
       <c r="E6" s="83" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>287</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>288</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="11"/>
@@ -6852,20 +6852,20 @@
     <row r="7" spans="1:17" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="129"/>
       <c r="B7" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E7" s="83" t="s">
+        <v>289</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>291</v>
-      </c>
       <c r="G7" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="24"/>
@@ -6881,20 +6881,20 @@
     <row r="8" spans="1:17" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="129"/>
       <c r="B8" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E8" s="83" t="s">
+        <v>292</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>294</v>
-      </c>
       <c r="G8" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="24"/>
@@ -6910,20 +6910,20 @@
     <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="129"/>
       <c r="B9" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="71" t="s">
+        <v>295</v>
+      </c>
+      <c r="E9" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="E9" s="86" t="s">
+      <c r="F9" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>298</v>
-      </c>
       <c r="G9" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H9" s="87"/>
       <c r="I9" s="24"/>
@@ -6939,17 +6939,17 @@
     <row r="10" spans="1:17" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="129"/>
       <c r="B10" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="71" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" s="83" t="s">
         <v>299</v>
       </c>
-      <c r="E10" s="83" t="s">
+      <c r="F10" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="11"/>
@@ -6966,17 +6966,17 @@
     <row r="11" spans="1:17" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="129"/>
       <c r="B11" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E11" s="83" t="s">
+        <v>302</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>303</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="11"/>
@@ -6993,17 +6993,17 @@
     <row r="12" spans="1:17" s="89" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="129"/>
       <c r="B12" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E12" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>307</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="11"/>
@@ -7020,17 +7020,17 @@
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="129"/>
       <c r="B13" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="71" t="s">
+        <v>308</v>
+      </c>
+      <c r="E13" s="83" t="s">
         <v>309</v>
       </c>
-      <c r="E13" s="83" t="s">
+      <c r="F13" s="9" t="s">
         <v>310</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="11"/>
@@ -7047,17 +7047,17 @@
     <row r="14" spans="1:17" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="129"/>
       <c r="B14" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E14" s="83" t="s">
+        <v>312</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>314</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="11"/>
@@ -7074,17 +7074,17 @@
     <row r="15" spans="1:17" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="129"/>
       <c r="B15" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E15" s="83" t="s">
+        <v>315</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>316</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>317</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="11"/>
@@ -7101,17 +7101,17 @@
     <row r="16" spans="1:17" ht="72" x14ac:dyDescent="0.2">
       <c r="A16" s="129"/>
       <c r="B16" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="71" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E16" s="83" t="s">
+        <v>318</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="11"/>
@@ -7128,17 +7128,17 @@
     <row r="17" spans="1:17" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="129"/>
       <c r="B17" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="E17" s="90" t="s">
         <v>322</v>
       </c>
-      <c r="E17" s="90" t="s">
+      <c r="F17" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>324</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -7155,17 +7155,17 @@
     <row r="18" spans="1:17" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="129"/>
       <c r="B18" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>326</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>327</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -7215,7 +7215,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="44.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -7233,7 +7233,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -7245,7 +7245,7 @@
         <v>196</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>8</v>
@@ -7276,14 +7276,14 @@
       </c>
       <c r="C4" s="71"/>
       <c r="D4" s="71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E4" s="71"/>
       <c r="F4" s="71" t="s">
+        <v>437</v>
+      </c>
+      <c r="G4" s="71" t="s">
         <v>438</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>439</v>
       </c>
       <c r="H4" s="71"/>
     </row>
@@ -7298,10 +7298,10 @@
       </c>
       <c r="E5" s="71"/>
       <c r="F5" s="71" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G5" s="71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H5" s="71"/>
     </row>
@@ -7316,10 +7316,10 @@
       </c>
       <c r="E6" s="71"/>
       <c r="F6" s="71" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G6" s="71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H6" s="71"/>
     </row>
@@ -7334,16 +7334,16 @@
       </c>
       <c r="E7" s="71"/>
       <c r="F7" s="71" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G7" s="71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H7" s="71"/>
     </row>
     <row r="8" spans="1:20" s="105" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="105" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H8" s="106"/>
     </row>
@@ -7354,30 +7354,30 @@
       </c>
       <c r="C9" s="77"/>
       <c r="D9" s="77" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E9" s="77"/>
       <c r="F9" s="77" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G9" s="107" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H9" s="77"/>
     </row>
     <row r="10" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="131"/>
       <c r="B10" s="77" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C10" s="77"/>
       <c r="D10" s="77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E10" s="77"/>
       <c r="F10" s="77"/>
       <c r="G10" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H10" s="77"/>
     </row>
@@ -7385,17 +7385,17 @@
       <c r="A11" s="131"/>
       <c r="B11" s="77"/>
       <c r="C11" s="77" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E11" s="77"/>
       <c r="F11" s="77" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G11" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H11" s="77"/>
     </row>
@@ -7403,17 +7403,17 @@
       <c r="A12" s="131"/>
       <c r="B12" s="77"/>
       <c r="C12" s="77" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="77"/>
       <c r="F12" s="77" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G12" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H12" s="77"/>
     </row>
@@ -7421,17 +7421,17 @@
       <c r="A13" s="131"/>
       <c r="B13" s="77"/>
       <c r="C13" s="77" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D13" s="77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E13" s="77"/>
       <c r="F13" s="77" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G13" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H13" s="77"/>
     </row>
@@ -7439,17 +7439,17 @@
       <c r="A14" s="131"/>
       <c r="B14" s="77"/>
       <c r="C14" s="77" t="s">
+        <v>453</v>
+      </c>
+      <c r="D14" s="77" t="s">
         <v>454</v>
-      </c>
-      <c r="D14" s="77" t="s">
-        <v>455</v>
       </c>
       <c r="E14" s="77"/>
       <c r="F14" s="77" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G14" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H14" s="77"/>
     </row>
@@ -7457,33 +7457,33 @@
       <c r="A15" s="131"/>
       <c r="B15" s="77"/>
       <c r="C15" s="77" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E15" s="77"/>
       <c r="F15" s="77" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G15" s="77" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H15" s="77"/>
     </row>
     <row r="16" spans="1:20" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="131"/>
       <c r="B16" s="77" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C16" s="77"/>
       <c r="D16" s="77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E16" s="77"/>
       <c r="F16" s="77"/>
       <c r="G16" s="77" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H16" s="77"/>
     </row>
@@ -7491,23 +7491,23 @@
       <c r="A17" s="131"/>
       <c r="B17" s="77"/>
       <c r="C17" s="77" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D17" s="77" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E17" s="77"/>
       <c r="F17" s="77" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G17" s="77" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H17" s="77"/>
     </row>
     <row r="18" spans="1:19" s="103" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="103" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H18" s="104"/>
       <c r="I18" s="105"/>
@@ -7525,16 +7525,16 @@
     <row r="19" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="132"/>
       <c r="B19" s="71" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C19" s="71"/>
       <c r="D19" s="71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E19" s="71"/>
       <c r="F19" s="71"/>
       <c r="G19" s="71" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H19" s="71"/>
     </row>
@@ -7542,14 +7542,14 @@
       <c r="A20" s="132"/>
       <c r="B20" s="71"/>
       <c r="C20" s="71" t="s">
+        <v>464</v>
+      </c>
+      <c r="D20" s="71" t="s">
         <v>465</v>
-      </c>
-      <c r="D20" s="71" t="s">
-        <v>466</v>
       </c>
       <c r="E20" s="71"/>
       <c r="F20" s="71" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G20" s="71"/>
       <c r="H20" s="71"/>
@@ -7558,14 +7558,14 @@
       <c r="A21" s="132"/>
       <c r="B21" s="71"/>
       <c r="C21" s="71" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D21" s="71" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E21" s="71"/>
       <c r="F21" s="71" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G21" s="71"/>
       <c r="H21" s="71"/>
@@ -7574,14 +7574,14 @@
       <c r="A22" s="132"/>
       <c r="B22" s="71"/>
       <c r="C22" s="71" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D22" s="71" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E22" s="71"/>
       <c r="F22" s="71" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G22" s="71"/>
       <c r="H22" s="71"/>
@@ -7625,7 +7625,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B1" s="127"/>
       <c r="C1" s="127"/>
@@ -7649,7 +7649,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="65" t="s">
         <v>196</v>
@@ -7663,7 +7663,7 @@
     </row>
     <row r="3" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="108" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -7676,15 +7676,15 @@
     <row r="4" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="126"/>
       <c r="B4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="71"/>
       <c r="D4" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="71" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="71"/>
@@ -7692,15 +7692,15 @@
     <row r="5" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="126"/>
       <c r="B5" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="71" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="71"/>
@@ -7708,7 +7708,7 @@
     <row r="6" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="126"/>
       <c r="B6" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="71"/>
       <c r="D6" s="9" t="s">
@@ -7716,7 +7716,7 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="71" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -7724,15 +7724,15 @@
     <row r="7" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="126"/>
       <c r="B7" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C7" s="71"/>
       <c r="D7" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="71" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="71"/>
@@ -7740,15 +7740,15 @@
     <row r="8" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="126"/>
       <c r="B8" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="71" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="71"/>
@@ -7756,15 +7756,15 @@
     <row r="9" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="126"/>
       <c r="B9" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C9" s="71"/>
       <c r="D9" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="71" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="71"/>
@@ -7772,15 +7772,15 @@
     <row r="10" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="126"/>
       <c r="B10" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="71" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="71"/>
@@ -7788,15 +7788,15 @@
     <row r="11" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="126"/>
       <c r="B11" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C11" s="71"/>
       <c r="D11" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="71" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="71"/>
@@ -7804,37 +7804,37 @@
     <row r="12" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="126"/>
       <c r="B12" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="71" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:1024" s="109" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="109" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AMJ13" s="62"/>
     </row>
     <row r="14" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="125"/>
       <c r="B14" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -7842,15 +7842,15 @@
     <row r="15" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="125"/>
       <c r="B15" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -7858,7 +7858,7 @@
     <row r="16" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A16" s="125"/>
       <c r="B16" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
@@ -7866,7 +7866,7 @@
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
@@ -7874,15 +7874,15 @@
     <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="125"/>
       <c r="B17" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
@@ -7890,15 +7890,15 @@
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="125"/>
       <c r="B18" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
@@ -7910,11 +7910,11 @@
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
@@ -7922,15 +7922,15 @@
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="125"/>
       <c r="B20" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
@@ -7938,15 +7938,15 @@
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="125"/>
       <c r="B21" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E21" s="27"/>
       <c r="F21" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
@@ -7954,15 +7954,15 @@
     <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A22" s="125"/>
       <c r="B22" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
@@ -7970,7 +7970,7 @@
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="125"/>
       <c r="B23" s="27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27" t="s">
@@ -7978,7 +7978,7 @@
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -7986,7 +7986,7 @@
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="125"/>
       <c r="B24" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27" t="s">
@@ -7994,14 +7994,14 @@
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="108" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B25" s="78"/>
       <c r="C25" s="78"/>
@@ -8014,15 +8014,15 @@
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="126"/>
       <c r="B26" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -8030,15 +8030,15 @@
     <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="126"/>
       <c r="B27" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -8046,7 +8046,7 @@
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="126"/>
       <c r="B28" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9" t="s">
@@ -8054,7 +8054,7 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -8062,15 +8062,15 @@
     <row r="29" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="126"/>
       <c r="B29" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -8078,15 +8078,15 @@
     <row r="30" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="126"/>
       <c r="B30" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -8094,15 +8094,15 @@
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="126"/>
       <c r="B31" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -8110,15 +8110,15 @@
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="126"/>
       <c r="B32" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -8126,15 +8126,15 @@
     <row r="33" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="126"/>
       <c r="B33" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -8146,11 +8146,11 @@
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -8158,15 +8158,15 @@
     <row r="35" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="126"/>
       <c r="B35" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -8174,37 +8174,37 @@
     <row r="36" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="126"/>
       <c r="B36" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:1024" s="109" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="109" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AMJ37" s="62"/>
     </row>
     <row r="38" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="125"/>
       <c r="B38" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
@@ -8212,15 +8212,15 @@
     <row r="39" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="125"/>
       <c r="B39" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
@@ -8228,7 +8228,7 @@
     <row r="40" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="125"/>
       <c r="B40" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="27" t="s">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -8244,15 +8244,15 @@
     <row r="41" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A41" s="125"/>
       <c r="B41" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
@@ -8260,15 +8260,15 @@
     <row r="42" spans="1:1024" ht="36" x14ac:dyDescent="0.2">
       <c r="A42" s="125"/>
       <c r="B42" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -8276,15 +8276,15 @@
     <row r="43" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="125"/>
       <c r="B43" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
@@ -8292,15 +8292,15 @@
     <row r="44" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="125"/>
       <c r="B44" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
@@ -8308,15 +8308,15 @@
     <row r="45" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="125"/>
       <c r="B45" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="27" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
@@ -8324,15 +8324,15 @@
     <row r="46" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="125"/>
       <c r="B46" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
@@ -8344,11 +8344,11 @@
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
@@ -8356,15 +8356,15 @@
     <row r="48" spans="1:1024" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="125"/>
       <c r="B48" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>

</xml_diff>

<commit_message>
refactor: rename header to 'comment'
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D26D19-9A06-4A45-A0CE-D38021DEB90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322FC021-DC11-4148-A54C-06C6F5DE9075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -3104,60 +3104,20 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3182,6 +3142,46 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4066,7 +4066,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A105" sqref="A105:XFD105"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4083,16 +4083,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4111,7 +4111,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>6</v>
@@ -4121,7 +4121,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="230" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4133,7 +4133,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="241"/>
+      <c r="A4" s="231"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="241"/>
+      <c r="A5" s="231"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="241"/>
+      <c r="A6" s="231"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4193,7 +4193,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="241"/>
+      <c r="A7" s="231"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="241"/>
+      <c r="A8" s="231"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="241"/>
+      <c r="A9" s="231"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4253,7 +4253,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="241"/>
+      <c r="A10" s="231"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4273,7 +4273,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="242"/>
+      <c r="A11" s="232"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="243" t="s">
+      <c r="A12" s="233" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="217"/>
@@ -4305,7 +4305,7 @@
       <c r="H12" s="220"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="244"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="244"/>
+      <c r="A14" s="234"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4345,7 +4345,7 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="244"/>
+      <c r="A15" s="234"/>
       <c r="B15" s="55" t="s">
         <v>482</v>
       </c>
@@ -5381,7 +5381,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="244"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="55" t="s">
         <v>475</v>
       </c>
@@ -6417,7 +6417,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="245"/>
+      <c r="A17" s="235"/>
       <c r="B17" s="221" t="s">
         <v>476</v>
       </c>
@@ -7705,7 +7705,7 @@
       <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="232" t="s">
+      <c r="A31" s="238" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="62"/>
@@ -7717,7 +7717,7 @@
       <c r="H31" s="64"/>
     </row>
     <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="233"/>
+      <c r="A32" s="239"/>
       <c r="B32" s="65" t="s">
         <v>73</v>
       </c>
@@ -7737,7 +7737,7 @@
       <c r="H32" s="68"/>
     </row>
     <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="233"/>
+      <c r="A33" s="239"/>
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -7757,7 +7757,7 @@
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="233"/>
+      <c r="A34" s="239"/>
       <c r="B34" s="69" t="s">
         <v>79</v>
       </c>
@@ -7777,7 +7777,7 @@
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="234"/>
+      <c r="A35" s="240"/>
       <c r="B35" s="73" t="s">
         <v>82</v>
       </c>
@@ -7797,7 +7797,7 @@
       <c r="H35" s="76"/>
     </row>
     <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="235" t="s">
+      <c r="A36" s="241" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="59"/>
@@ -8846,7 +8846,7 @@
     </row>
     <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="236"/>
-      <c r="B38" s="226" t="s">
+      <c r="B38" s="228" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -9884,7 +9884,7 @@
     </row>
     <row r="39" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="236"/>
-      <c r="B39" s="226"/>
+      <c r="B39" s="228"/>
       <c r="C39" s="47" t="s">
         <v>94</v>
       </c>
@@ -10920,7 +10920,7 @@
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="236"/>
-      <c r="B40" s="226"/>
+      <c r="B40" s="228"/>
       <c r="C40" s="47" t="s">
         <v>98</v>
       </c>
@@ -11956,7 +11956,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="236"/>
-      <c r="B41" s="226"/>
+      <c r="B41" s="228"/>
       <c r="C41" s="47" t="s">
         <v>102</v>
       </c>
@@ -12992,7 +12992,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="236"/>
-      <c r="B42" s="226"/>
+      <c r="B42" s="228"/>
       <c r="C42" s="47" t="s">
         <v>106</v>
       </c>
@@ -14028,7 +14028,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="236"/>
-      <c r="B43" s="226"/>
+      <c r="B43" s="228"/>
       <c r="C43" s="47" t="s">
         <v>110</v>
       </c>
@@ -15064,7 +15064,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="236"/>
-      <c r="B44" s="226"/>
+      <c r="B44" s="228"/>
       <c r="C44" s="47" t="s">
         <v>114</v>
       </c>
@@ -16100,7 +16100,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="236"/>
-      <c r="B45" s="226"/>
+      <c r="B45" s="228"/>
       <c r="C45" s="47" t="s">
         <v>118</v>
       </c>
@@ -17136,7 +17136,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="236"/>
-      <c r="B46" s="226"/>
+      <c r="B46" s="228"/>
       <c r="C46" s="47" t="s">
         <v>122</v>
       </c>
@@ -18172,7 +18172,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="236"/>
-      <c r="B47" s="226"/>
+      <c r="B47" s="228"/>
       <c r="C47" s="47" t="s">
         <v>126</v>
       </c>
@@ -19208,7 +19208,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="236"/>
-      <c r="B48" s="226"/>
+      <c r="B48" s="228"/>
       <c r="C48" s="47" t="s">
         <v>130</v>
       </c>
@@ -20244,7 +20244,7 @@
     </row>
     <row r="49" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="237"/>
-      <c r="B49" s="227"/>
+      <c r="B49" s="229"/>
       <c r="C49" s="51" t="s">
         <v>134</v>
       </c>
@@ -21279,7 +21279,7 @@
       <c r="AMJ49" s="15"/>
     </row>
     <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="232" t="s">
+      <c r="A50" s="238" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="77"/>
@@ -21291,7 +21291,7 @@
       <c r="H50" s="79"/>
     </row>
     <row r="51" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="233"/>
+      <c r="A51" s="239"/>
       <c r="B51" s="80" t="s">
         <v>138</v>
       </c>
@@ -21311,8 +21311,8 @@
       <c r="H51" s="83"/>
     </row>
     <row r="52" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="233"/>
-      <c r="B52" s="228" t="s">
+      <c r="A52" s="239"/>
+      <c r="B52" s="242" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
@@ -21333,8 +21333,8 @@
       <c r="H52" s="83"/>
     </row>
     <row r="53" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="233"/>
-      <c r="B53" s="228"/>
+      <c r="A53" s="239"/>
+      <c r="B53" s="242"/>
       <c r="C53" s="80" t="s">
         <v>94</v>
       </c>
@@ -21353,8 +21353,8 @@
       <c r="H53" s="83"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="233"/>
-      <c r="B54" s="228"/>
+      <c r="A54" s="239"/>
+      <c r="B54" s="242"/>
       <c r="C54" s="80" t="s">
         <v>98</v>
       </c>
@@ -21373,8 +21373,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A55" s="233"/>
-      <c r="B55" s="228"/>
+      <c r="A55" s="239"/>
+      <c r="B55" s="242"/>
       <c r="C55" s="80" t="s">
         <v>102</v>
       </c>
@@ -21393,8 +21393,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="233"/>
-      <c r="B56" s="228"/>
+      <c r="A56" s="239"/>
+      <c r="B56" s="242"/>
       <c r="C56" s="80" t="s">
         <v>106</v>
       </c>
@@ -21413,8 +21413,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="233"/>
-      <c r="B57" s="228"/>
+      <c r="A57" s="239"/>
+      <c r="B57" s="242"/>
       <c r="C57" s="80" t="s">
         <v>110</v>
       </c>
@@ -21433,8 +21433,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="233"/>
-      <c r="B58" s="228"/>
+      <c r="A58" s="239"/>
+      <c r="B58" s="242"/>
       <c r="C58" s="80" t="s">
         <v>114</v>
       </c>
@@ -21453,8 +21453,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A59" s="233"/>
-      <c r="B59" s="228"/>
+      <c r="A59" s="239"/>
+      <c r="B59" s="242"/>
       <c r="C59" s="80" t="s">
         <v>118</v>
       </c>
@@ -21473,8 +21473,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="233"/>
-      <c r="B60" s="228"/>
+      <c r="A60" s="239"/>
+      <c r="B60" s="242"/>
       <c r="C60" s="80" t="s">
         <v>122</v>
       </c>
@@ -21493,8 +21493,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="233"/>
-      <c r="B61" s="228"/>
+      <c r="A61" s="239"/>
+      <c r="B61" s="242"/>
       <c r="C61" s="80" t="s">
         <v>126</v>
       </c>
@@ -21513,8 +21513,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="233"/>
-      <c r="B62" s="228"/>
+      <c r="A62" s="239"/>
+      <c r="B62" s="242"/>
       <c r="C62" s="80" t="s">
         <v>130</v>
       </c>
@@ -21533,8 +21533,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="234"/>
-      <c r="B63" s="229"/>
+      <c r="A63" s="240"/>
+      <c r="B63" s="243"/>
       <c r="C63" s="85" t="s">
         <v>134</v>
       </c>
@@ -21553,7 +21553,7 @@
       <c r="H63" s="87"/>
     </row>
     <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="235" t="s">
+      <c r="A64" s="241" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="59"/>
@@ -24653,7 +24653,7 @@
       <c r="AMJ66" s="13"/>
     </row>
     <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="232" t="s">
+      <c r="A67" s="238" t="s">
         <v>154</v>
       </c>
       <c r="B67" s="29"/>
@@ -24665,7 +24665,7 @@
       <c r="H67" s="64"/>
     </row>
     <row r="68" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="233"/>
+      <c r="A68" s="239"/>
       <c r="B68" s="69" t="s">
         <v>155</v>
       </c>
@@ -24683,8 +24683,8 @@
       <c r="H68" s="72"/>
     </row>
     <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="233"/>
-      <c r="B69" s="230" t="s">
+      <c r="A69" s="239"/>
+      <c r="B69" s="244" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="69" t="s">
@@ -24705,8 +24705,8 @@
       <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="233"/>
-      <c r="B70" s="230"/>
+      <c r="A70" s="239"/>
+      <c r="B70" s="244"/>
       <c r="C70" s="69" t="s">
         <v>30</v>
       </c>
@@ -24725,8 +24725,8 @@
       <c r="H70" s="72"/>
     </row>
     <row r="71" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="233"/>
-      <c r="B71" s="230"/>
+      <c r="A71" s="239"/>
+      <c r="B71" s="244"/>
       <c r="C71" s="69" t="s">
         <v>12</v>
       </c>
@@ -24745,8 +24745,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="233"/>
-      <c r="B72" s="230"/>
+      <c r="A72" s="239"/>
+      <c r="B72" s="244"/>
       <c r="C72" s="69" t="s">
         <v>167</v>
       </c>
@@ -24765,8 +24765,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="234"/>
-      <c r="B73" s="231"/>
+      <c r="A73" s="240"/>
+      <c r="B73" s="245"/>
       <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
@@ -24785,7 +24785,7 @@
       <c r="H73" s="76"/>
     </row>
     <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="235" t="s">
+      <c r="A74" s="241" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="31"/>
@@ -26848,7 +26848,7 @@
     </row>
     <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="236"/>
-      <c r="B76" s="226" t="s">
+      <c r="B76" s="228" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="47" t="s">
@@ -27886,7 +27886,7 @@
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="236"/>
-      <c r="B77" s="226"/>
+      <c r="B77" s="228"/>
       <c r="C77" s="47" t="s">
         <v>179</v>
       </c>
@@ -28922,7 +28922,7 @@
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="236"/>
-      <c r="B78" s="226"/>
+      <c r="B78" s="228"/>
       <c r="C78" s="47" t="s">
         <v>182</v>
       </c>
@@ -29958,7 +29958,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="236"/>
-      <c r="B79" s="226"/>
+      <c r="B79" s="228"/>
       <c r="C79" s="47" t="s">
         <v>185</v>
       </c>
@@ -30994,7 +30994,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="237"/>
-      <c r="B80" s="227"/>
+      <c r="B80" s="229"/>
       <c r="C80" s="51" t="s">
         <v>25</v>
       </c>
@@ -32103,6 +32103,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="B52:B63"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="A50:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A74:A80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A3:A11"/>
@@ -32110,13 +32117,6 @@
     <mergeCell ref="A18:A30"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A36:A49"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B52:B63"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="A50:A63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A74:A80"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32156,16 +32156,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32194,7 +32194,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="230" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -32206,7 +32206,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="241"/>
+      <c r="A4" s="231"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -32226,7 +32226,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="241"/>
+      <c r="A5" s="231"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -32246,7 +32246,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="241"/>
+      <c r="A6" s="231"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -32266,7 +32266,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="241"/>
+      <c r="A7" s="231"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -32286,7 +32286,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="241"/>
+      <c r="A8" s="231"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -32306,7 +32306,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="241"/>
+      <c r="A9" s="231"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -32326,7 +32326,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="241"/>
+      <c r="A10" s="231"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -32346,7 +32346,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="242"/>
+      <c r="A11" s="232"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -32456,16 +32456,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>519</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32494,7 +32494,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="230" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -32544,7 +32544,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="241"/>
+      <c r="A4" s="231"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -32562,7 +32562,7 @@
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="241"/>
+      <c r="A5" s="231"/>
       <c r="B5" s="105" t="s">
         <v>210</v>
       </c>
@@ -32578,7 +32578,7 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="241"/>
+      <c r="A6" s="231"/>
       <c r="B6" s="105" t="s">
         <v>213</v>
       </c>
@@ -32594,7 +32594,7 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="241"/>
+      <c r="A7" s="231"/>
       <c r="B7" s="105" t="s">
         <v>216</v>
       </c>
@@ -32610,7 +32610,7 @@
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="241"/>
+      <c r="A8" s="231"/>
       <c r="B8" s="105" t="s">
         <v>218</v>
       </c>
@@ -32626,7 +32626,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="241"/>
+      <c r="A9" s="231"/>
       <c r="B9" s="105" t="s">
         <v>220</v>
       </c>
@@ -32642,7 +32642,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="241"/>
+      <c r="A10" s="231"/>
       <c r="B10" s="105" t="s">
         <v>223</v>
       </c>
@@ -32671,7 +32671,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="241"/>
+      <c r="A11" s="231"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -32687,7 +32687,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="241"/>
+      <c r="A12" s="231"/>
       <c r="B12" s="105" t="s">
         <v>227</v>
       </c>
@@ -32703,7 +32703,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="241"/>
+      <c r="A13" s="231"/>
       <c r="B13" s="105" t="s">
         <v>230</v>
       </c>
@@ -32721,7 +32721,7 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="241"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="105" t="s">
         <v>485</v>
       </c>
@@ -32739,7 +32739,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="242"/>
+      <c r="A15" s="232"/>
       <c r="B15" s="108" t="s">
         <v>234</v>
       </c>
@@ -32755,7 +32755,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="232" t="s">
+      <c r="A16" s="238" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -32768,7 +32768,7 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:1024" ht="127" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="233"/>
+      <c r="A17" s="239"/>
       <c r="B17" s="113" t="s">
         <v>237</v>
       </c>
@@ -32784,7 +32784,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="233"/>
+      <c r="A18" s="239"/>
       <c r="B18" s="113" t="s">
         <v>240</v>
       </c>
@@ -32798,7 +32798,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="234"/>
+      <c r="A19" s="240"/>
       <c r="B19" s="116" t="s">
         <v>242</v>
       </c>
@@ -32814,7 +32814,7 @@
       <c r="H19" s="118"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="235" t="s">
+      <c r="A20" s="241" t="s">
         <v>245</v>
       </c>
       <c r="B20" s="119"/>
@@ -32899,7 +32899,7 @@
       <c r="AMJ21" s="5"/>
     </row>
     <row r="22" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="232" t="s">
+      <c r="A22" s="238" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="111"/>
@@ -32912,7 +32912,7 @@
       <c r="AMJ22" s="5"/>
     </row>
     <row r="23" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="233"/>
+      <c r="A23" s="239"/>
       <c r="B23" s="113" t="s">
         <v>73</v>
       </c>
@@ -32928,7 +32928,7 @@
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="233"/>
+      <c r="A24" s="239"/>
       <c r="B24" s="113" t="s">
         <v>76</v>
       </c>
@@ -32944,7 +32944,7 @@
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="234"/>
+      <c r="A25" s="240"/>
       <c r="B25" s="116" t="s">
         <v>79</v>
       </c>
@@ -32960,7 +32960,7 @@
       <c r="H25" s="118"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="241" t="s">
         <v>252</v>
       </c>
       <c r="B26" s="121"/>
@@ -33173,7 +33173,7 @@
       <c r="H35" s="110"/>
     </row>
     <row r="36" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="238" t="s">
         <v>532</v>
       </c>
       <c r="B36" s="123"/>
@@ -33186,7 +33186,7 @@
       <c r="AMJ36" s="5"/>
     </row>
     <row r="37" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="234"/>
+      <c r="A37" s="240"/>
       <c r="B37" s="116" t="s">
         <v>5</v>
       </c>
@@ -33248,16 +33248,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -43130,16 +43130,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>521</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -43168,7 +43168,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="241" t="s">
         <v>536</v>
       </c>
       <c r="B3" s="18"/>
@@ -43518,16 +43518,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -44024,16 +44024,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -44062,7 +44062,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="241" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="154"/>
@@ -44158,7 +44158,7 @@
       <c r="H7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="232" t="s">
+      <c r="A8" s="238" t="s">
         <v>303</v>
       </c>
       <c r="B8" s="162"/>
@@ -44170,7 +44170,7 @@
       <c r="H8" s="163"/>
     </row>
     <row r="9" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="233"/>
+      <c r="A9" s="239"/>
       <c r="B9" s="164" t="s">
         <v>30</v>
       </c>
@@ -44188,7 +44188,7 @@
       <c r="H9" s="165"/>
     </row>
     <row r="10" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="233"/>
+      <c r="A10" s="239"/>
       <c r="B10" s="164" t="s">
         <v>393</v>
       </c>
@@ -44202,7 +44202,7 @@
       <c r="H10" s="165"/>
     </row>
     <row r="11" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="233"/>
+      <c r="A11" s="239"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
         <v>395</v>
@@ -44218,7 +44218,7 @@
       <c r="H11" s="165"/>
     </row>
     <row r="12" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="233"/>
+      <c r="A12" s="239"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
         <v>396</v>
@@ -44234,7 +44234,7 @@
       <c r="H12" s="165"/>
     </row>
     <row r="13" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="233"/>
+      <c r="A13" s="239"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
         <v>397</v>
@@ -44250,7 +44250,7 @@
       <c r="H13" s="165"/>
     </row>
     <row r="14" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="233"/>
+      <c r="A14" s="239"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
         <v>398</v>
@@ -44266,7 +44266,7 @@
       <c r="H14" s="165"/>
     </row>
     <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="233"/>
+      <c r="A15" s="239"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
         <v>400</v>
@@ -44282,7 +44282,7 @@
       <c r="H15" s="165"/>
     </row>
     <row r="16" spans="1:20" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="233"/>
+      <c r="A16" s="239"/>
       <c r="B16" s="164" t="s">
         <v>402</v>
       </c>
@@ -44296,7 +44296,7 @@
       <c r="H16" s="165"/>
     </row>
     <row r="17" spans="1:19" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="234"/>
+      <c r="A17" s="240"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
         <v>400</v>
@@ -44312,7 +44312,7 @@
       <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:19" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="235" t="s">
+      <c r="A18" s="241" t="s">
         <v>404</v>
       </c>
       <c r="B18" s="168"/>
@@ -44441,16 +44441,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="226" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -45495,7 +45495,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="241" t="s">
         <v>413</v>
       </c>
       <c r="B3" s="172"/>
@@ -54795,7 +54795,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="232" t="s">
+      <c r="A13" s="238" t="s">
         <v>428</v>
       </c>
       <c r="B13" s="175"/>
@@ -54808,7 +54808,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="233"/>
+      <c r="A14" s="239"/>
       <c r="B14" s="69" t="s">
         <v>207</v>
       </c>
@@ -54824,7 +54824,7 @@
       <c r="H14" s="177"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="233"/>
+      <c r="A15" s="239"/>
       <c r="B15" s="69" t="s">
         <v>268</v>
       </c>
@@ -54840,7 +54840,7 @@
       <c r="H15" s="177"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="233"/>
+      <c r="A16" s="239"/>
       <c r="B16" s="69" t="s">
         <v>213</v>
       </c>
@@ -54856,7 +54856,7 @@
       <c r="H16" s="177"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="233"/>
+      <c r="A17" s="239"/>
       <c r="B17" s="69" t="s">
         <v>274</v>
       </c>
@@ -54872,7 +54872,7 @@
       <c r="H17" s="177"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="233"/>
+      <c r="A18" s="239"/>
       <c r="B18" s="69" t="s">
         <v>210</v>
       </c>
@@ -54888,7 +54888,7 @@
       <c r="H18" s="177"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="233"/>
+      <c r="A19" s="239"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -54904,7 +54904,7 @@
       <c r="H19" s="177"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="233"/>
+      <c r="A20" s="239"/>
       <c r="B20" s="69" t="s">
         <v>434</v>
       </c>
@@ -54920,7 +54920,7 @@
       <c r="H20" s="177"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="233"/>
+      <c r="A21" s="239"/>
       <c r="B21" s="69" t="s">
         <v>334</v>
       </c>
@@ -54936,7 +54936,7 @@
       <c r="H21" s="177"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="233"/>
+      <c r="A22" s="239"/>
       <c r="B22" s="69" t="s">
         <v>437</v>
       </c>
@@ -54952,7 +54952,7 @@
       <c r="H22" s="177"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="233"/>
+      <c r="A23" s="239"/>
       <c r="B23" s="69" t="s">
         <v>439</v>
       </c>
@@ -54968,7 +54968,7 @@
       <c r="H23" s="177"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="234"/>
+      <c r="A24" s="240"/>
       <c r="B24" s="73" t="s">
         <v>441</v>
       </c>
@@ -54984,7 +54984,7 @@
       <c r="H24" s="178"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="235" t="s">
+      <c r="A25" s="241" t="s">
         <v>370</v>
       </c>
       <c r="B25" s="179"/>
@@ -55172,7 +55172,7 @@
       <c r="H36" s="181"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="232" t="s">
+      <c r="A37" s="238" t="s">
         <v>290</v>
       </c>
       <c r="B37" s="175"/>
@@ -55185,7 +55185,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="233"/>
+      <c r="A38" s="239"/>
       <c r="B38" s="69" t="s">
         <v>207</v>
       </c>
@@ -55201,7 +55201,7 @@
       <c r="H38" s="177"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="233"/>
+      <c r="A39" s="239"/>
       <c r="B39" s="69" t="s">
         <v>268</v>
       </c>
@@ -55217,7 +55217,7 @@
       <c r="H39" s="177"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="233"/>
+      <c r="A40" s="239"/>
       <c r="B40" s="69" t="s">
         <v>213</v>
       </c>
@@ -55233,7 +55233,7 @@
       <c r="H40" s="177"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="233"/>
+      <c r="A41" s="239"/>
       <c r="B41" s="69" t="s">
         <v>274</v>
       </c>
@@ -55249,7 +55249,7 @@
       <c r="H41" s="177"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="233"/>
+      <c r="A42" s="239"/>
       <c r="B42" s="69" t="s">
         <v>460</v>
       </c>
@@ -55265,7 +55265,7 @@
       <c r="H42" s="177"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="233"/>
+      <c r="A43" s="239"/>
       <c r="B43" s="69" t="s">
         <v>370</v>
       </c>
@@ -55281,7 +55281,7 @@
       <c r="H43" s="177"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="233"/>
+      <c r="A44" s="239"/>
       <c r="B44" s="69" t="s">
         <v>210</v>
       </c>
@@ -55297,7 +55297,7 @@
       <c r="H44" s="177"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="233"/>
+      <c r="A45" s="239"/>
       <c r="B45" s="69" t="s">
         <v>424</v>
       </c>
@@ -55313,7 +55313,7 @@
       <c r="H45" s="177"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="233"/>
+      <c r="A46" s="239"/>
       <c r="B46" s="69" t="s">
         <v>465</v>
       </c>
@@ -55329,7 +55329,7 @@
       <c r="H46" s="177"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="233"/>
+      <c r="A47" s="239"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -55345,7 +55345,7 @@
       <c r="H47" s="177"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="234"/>
+      <c r="A48" s="240"/>
       <c r="B48" s="73" t="s">
         <v>437</v>
       </c>

</xml_diff>

<commit_message>
fix: add examples in deployment
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322FC021-DC11-4148-A54C-06C6F5DE9075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9726931A-D7FF-1846-A5EC-8E737B771F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="541">
   <si>
     <t>Concept</t>
   </si>
@@ -1741,6 +1741,15 @@
   <si>
     <t>a mapping specifying which microservice should run on which host. By default each microservice is assigned a respective host, but this behaviour is not always ideal (eg. when two or more Microservices may need to run on the same host)</t>
   </si>
+  <si>
+    <t>Configuration data for a CloudBroker instance</t>
+  </si>
+  <si>
+    <t>Connection data for a bring-your-own edge</t>
+  </si>
+  <si>
+    <t>Mapping Microservices to Data assets, as available in the DMA Tuple</t>
+  </si>
 </sst>
 </file>
 
@@ -3104,20 +3113,60 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3142,46 +3191,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4061,7 +4070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -4083,16 +4092,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4121,7 +4130,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4133,7 +4142,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4153,7 +4162,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4173,7 +4182,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4193,7 +4202,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4213,7 +4222,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4233,7 +4242,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4253,7 +4262,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4273,7 +4282,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="232"/>
+      <c r="A11" s="242"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4293,7 +4302,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="233" t="s">
+      <c r="A12" s="243" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="217"/>
@@ -4305,7 +4314,7 @@
       <c r="H12" s="220"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="234"/>
+      <c r="A13" s="244"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4325,7 +4334,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="234"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4345,7 +4354,7 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="234"/>
+      <c r="A15" s="244"/>
       <c r="B15" s="55" t="s">
         <v>482</v>
       </c>
@@ -5381,7 +5390,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="234"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="55" t="s">
         <v>475</v>
       </c>
@@ -6417,7 +6426,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="235"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="221" t="s">
         <v>476</v>
       </c>
@@ -7705,7 +7714,7 @@
       <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="238" t="s">
+      <c r="A31" s="232" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="62"/>
@@ -7717,7 +7726,7 @@
       <c r="H31" s="64"/>
     </row>
     <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="239"/>
+      <c r="A32" s="233"/>
       <c r="B32" s="65" t="s">
         <v>73</v>
       </c>
@@ -7737,7 +7746,7 @@
       <c r="H32" s="68"/>
     </row>
     <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="239"/>
+      <c r="A33" s="233"/>
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -7757,7 +7766,7 @@
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="239"/>
+      <c r="A34" s="233"/>
       <c r="B34" s="69" t="s">
         <v>79</v>
       </c>
@@ -7777,7 +7786,7 @@
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="240"/>
+      <c r="A35" s="234"/>
       <c r="B35" s="73" t="s">
         <v>82</v>
       </c>
@@ -7797,7 +7806,7 @@
       <c r="H35" s="76"/>
     </row>
     <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="241" t="s">
+      <c r="A36" s="235" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="59"/>
@@ -8846,7 +8855,7 @@
     </row>
     <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="236"/>
-      <c r="B38" s="228" t="s">
+      <c r="B38" s="226" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -9884,7 +9893,7 @@
     </row>
     <row r="39" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="236"/>
-      <c r="B39" s="228"/>
+      <c r="B39" s="226"/>
       <c r="C39" s="47" t="s">
         <v>94</v>
       </c>
@@ -10920,7 +10929,7 @@
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="236"/>
-      <c r="B40" s="228"/>
+      <c r="B40" s="226"/>
       <c r="C40" s="47" t="s">
         <v>98</v>
       </c>
@@ -11956,7 +11965,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="236"/>
-      <c r="B41" s="228"/>
+      <c r="B41" s="226"/>
       <c r="C41" s="47" t="s">
         <v>102</v>
       </c>
@@ -12992,7 +13001,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="236"/>
-      <c r="B42" s="228"/>
+      <c r="B42" s="226"/>
       <c r="C42" s="47" t="s">
         <v>106</v>
       </c>
@@ -14028,7 +14037,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="236"/>
-      <c r="B43" s="228"/>
+      <c r="B43" s="226"/>
       <c r="C43" s="47" t="s">
         <v>110</v>
       </c>
@@ -15064,7 +15073,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="236"/>
-      <c r="B44" s="228"/>
+      <c r="B44" s="226"/>
       <c r="C44" s="47" t="s">
         <v>114</v>
       </c>
@@ -16100,7 +16109,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="236"/>
-      <c r="B45" s="228"/>
+      <c r="B45" s="226"/>
       <c r="C45" s="47" t="s">
         <v>118</v>
       </c>
@@ -17136,7 +17145,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="236"/>
-      <c r="B46" s="228"/>
+      <c r="B46" s="226"/>
       <c r="C46" s="47" t="s">
         <v>122</v>
       </c>
@@ -18172,7 +18181,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="236"/>
-      <c r="B47" s="228"/>
+      <c r="B47" s="226"/>
       <c r="C47" s="47" t="s">
         <v>126</v>
       </c>
@@ -19208,7 +19217,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="236"/>
-      <c r="B48" s="228"/>
+      <c r="B48" s="226"/>
       <c r="C48" s="47" t="s">
         <v>130</v>
       </c>
@@ -20244,7 +20253,7 @@
     </row>
     <row r="49" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="237"/>
-      <c r="B49" s="229"/>
+      <c r="B49" s="227"/>
       <c r="C49" s="51" t="s">
         <v>134</v>
       </c>
@@ -21279,7 +21288,7 @@
       <c r="AMJ49" s="15"/>
     </row>
     <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="238" t="s">
+      <c r="A50" s="232" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="77"/>
@@ -21291,7 +21300,7 @@
       <c r="H50" s="79"/>
     </row>
     <row r="51" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="239"/>
+      <c r="A51" s="233"/>
       <c r="B51" s="80" t="s">
         <v>138</v>
       </c>
@@ -21311,8 +21320,8 @@
       <c r="H51" s="83"/>
     </row>
     <row r="52" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="239"/>
-      <c r="B52" s="242" t="s">
+      <c r="A52" s="233"/>
+      <c r="B52" s="228" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
@@ -21333,8 +21342,8 @@
       <c r="H52" s="83"/>
     </row>
     <row r="53" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="239"/>
-      <c r="B53" s="242"/>
+      <c r="A53" s="233"/>
+      <c r="B53" s="228"/>
       <c r="C53" s="80" t="s">
         <v>94</v>
       </c>
@@ -21353,8 +21362,8 @@
       <c r="H53" s="83"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="239"/>
-      <c r="B54" s="242"/>
+      <c r="A54" s="233"/>
+      <c r="B54" s="228"/>
       <c r="C54" s="80" t="s">
         <v>98</v>
       </c>
@@ -21373,8 +21382,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A55" s="239"/>
-      <c r="B55" s="242"/>
+      <c r="A55" s="233"/>
+      <c r="B55" s="228"/>
       <c r="C55" s="80" t="s">
         <v>102</v>
       </c>
@@ -21393,8 +21402,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="239"/>
-      <c r="B56" s="242"/>
+      <c r="A56" s="233"/>
+      <c r="B56" s="228"/>
       <c r="C56" s="80" t="s">
         <v>106</v>
       </c>
@@ -21413,8 +21422,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="239"/>
-      <c r="B57" s="242"/>
+      <c r="A57" s="233"/>
+      <c r="B57" s="228"/>
       <c r="C57" s="80" t="s">
         <v>110</v>
       </c>
@@ -21433,8 +21442,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="239"/>
-      <c r="B58" s="242"/>
+      <c r="A58" s="233"/>
+      <c r="B58" s="228"/>
       <c r="C58" s="80" t="s">
         <v>114</v>
       </c>
@@ -21453,8 +21462,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A59" s="239"/>
-      <c r="B59" s="242"/>
+      <c r="A59" s="233"/>
+      <c r="B59" s="228"/>
       <c r="C59" s="80" t="s">
         <v>118</v>
       </c>
@@ -21473,8 +21482,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="239"/>
-      <c r="B60" s="242"/>
+      <c r="A60" s="233"/>
+      <c r="B60" s="228"/>
       <c r="C60" s="80" t="s">
         <v>122</v>
       </c>
@@ -21493,8 +21502,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="239"/>
-      <c r="B61" s="242"/>
+      <c r="A61" s="233"/>
+      <c r="B61" s="228"/>
       <c r="C61" s="80" t="s">
         <v>126</v>
       </c>
@@ -21513,8 +21522,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="239"/>
-      <c r="B62" s="242"/>
+      <c r="A62" s="233"/>
+      <c r="B62" s="228"/>
       <c r="C62" s="80" t="s">
         <v>130</v>
       </c>
@@ -21533,8 +21542,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="240"/>
-      <c r="B63" s="243"/>
+      <c r="A63" s="234"/>
+      <c r="B63" s="229"/>
       <c r="C63" s="85" t="s">
         <v>134</v>
       </c>
@@ -21553,7 +21562,7 @@
       <c r="H63" s="87"/>
     </row>
     <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="241" t="s">
+      <c r="A64" s="235" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="59"/>
@@ -24653,7 +24662,7 @@
       <c r="AMJ66" s="13"/>
     </row>
     <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="238" t="s">
+      <c r="A67" s="232" t="s">
         <v>154</v>
       </c>
       <c r="B67" s="29"/>
@@ -24665,7 +24674,7 @@
       <c r="H67" s="64"/>
     </row>
     <row r="68" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="239"/>
+      <c r="A68" s="233"/>
       <c r="B68" s="69" t="s">
         <v>155</v>
       </c>
@@ -24683,8 +24692,8 @@
       <c r="H68" s="72"/>
     </row>
     <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="239"/>
-      <c r="B69" s="244" t="s">
+      <c r="A69" s="233"/>
+      <c r="B69" s="230" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="69" t="s">
@@ -24705,8 +24714,8 @@
       <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="239"/>
-      <c r="B70" s="244"/>
+      <c r="A70" s="233"/>
+      <c r="B70" s="230"/>
       <c r="C70" s="69" t="s">
         <v>30</v>
       </c>
@@ -24725,8 +24734,8 @@
       <c r="H70" s="72"/>
     </row>
     <row r="71" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="239"/>
-      <c r="B71" s="244"/>
+      <c r="A71" s="233"/>
+      <c r="B71" s="230"/>
       <c r="C71" s="69" t="s">
         <v>12</v>
       </c>
@@ -24745,8 +24754,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="239"/>
-      <c r="B72" s="244"/>
+      <c r="A72" s="233"/>
+      <c r="B72" s="230"/>
       <c r="C72" s="69" t="s">
         <v>167</v>
       </c>
@@ -24765,8 +24774,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="240"/>
-      <c r="B73" s="245"/>
+      <c r="A73" s="234"/>
+      <c r="B73" s="231"/>
       <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
@@ -24785,7 +24794,7 @@
       <c r="H73" s="76"/>
     </row>
     <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="241" t="s">
+      <c r="A74" s="235" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="31"/>
@@ -26848,7 +26857,7 @@
     </row>
     <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="236"/>
-      <c r="B76" s="228" t="s">
+      <c r="B76" s="226" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="47" t="s">
@@ -27886,7 +27895,7 @@
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="236"/>
-      <c r="B77" s="228"/>
+      <c r="B77" s="226"/>
       <c r="C77" s="47" t="s">
         <v>179</v>
       </c>
@@ -28922,7 +28931,7 @@
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="236"/>
-      <c r="B78" s="228"/>
+      <c r="B78" s="226"/>
       <c r="C78" s="47" t="s">
         <v>182</v>
       </c>
@@ -29958,7 +29967,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="236"/>
-      <c r="B79" s="228"/>
+      <c r="B79" s="226"/>
       <c r="C79" s="47" t="s">
         <v>185</v>
       </c>
@@ -30994,7 +31003,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="237"/>
-      <c r="B80" s="229"/>
+      <c r="B80" s="227"/>
       <c r="C80" s="51" t="s">
         <v>25</v>
       </c>
@@ -32103,6 +32112,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A49"/>
     <mergeCell ref="B76:B80"/>
     <mergeCell ref="B52:B63"/>
     <mergeCell ref="B69:B73"/>
@@ -32110,13 +32126,6 @@
     <mergeCell ref="A64:A66"/>
     <mergeCell ref="A67:A73"/>
     <mergeCell ref="A74:A80"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A49"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32156,16 +32165,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32194,7 +32203,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -32206,7 +32215,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -32226,7 +32235,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -32246,7 +32255,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -32266,7 +32275,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -32286,7 +32295,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -32306,7 +32315,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -32326,7 +32335,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -32346,7 +32355,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="232"/>
+      <c r="A11" s="242"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -32456,16 +32465,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>519</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32494,7 +32503,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -32544,7 +32553,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -32562,7 +32571,7 @@
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="105" t="s">
         <v>210</v>
       </c>
@@ -32578,7 +32587,7 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="105" t="s">
         <v>213</v>
       </c>
@@ -32594,7 +32603,7 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="105" t="s">
         <v>216</v>
       </c>
@@ -32610,7 +32619,7 @@
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="105" t="s">
         <v>218</v>
       </c>
@@ -32626,7 +32635,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="105" t="s">
         <v>220</v>
       </c>
@@ -32642,7 +32651,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="105" t="s">
         <v>223</v>
       </c>
@@ -32671,7 +32680,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="231"/>
+      <c r="A11" s="241"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -32687,7 +32696,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="231"/>
+      <c r="A12" s="241"/>
       <c r="B12" s="105" t="s">
         <v>227</v>
       </c>
@@ -32703,7 +32712,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="231"/>
+      <c r="A13" s="241"/>
       <c r="B13" s="105" t="s">
         <v>230</v>
       </c>
@@ -32721,7 +32730,7 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="231"/>
+      <c r="A14" s="241"/>
       <c r="B14" s="105" t="s">
         <v>485</v>
       </c>
@@ -32739,7 +32748,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="232"/>
+      <c r="A15" s="242"/>
       <c r="B15" s="108" t="s">
         <v>234</v>
       </c>
@@ -32755,7 +32764,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="238" t="s">
+      <c r="A16" s="232" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -32768,7 +32777,7 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:1024" ht="127" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="239"/>
+      <c r="A17" s="233"/>
       <c r="B17" s="113" t="s">
         <v>237</v>
       </c>
@@ -32784,7 +32793,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="239"/>
+      <c r="A18" s="233"/>
       <c r="B18" s="113" t="s">
         <v>240</v>
       </c>
@@ -32798,7 +32807,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="240"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="116" t="s">
         <v>242</v>
       </c>
@@ -32814,7 +32823,7 @@
       <c r="H19" s="118"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="241" t="s">
+      <c r="A20" s="235" t="s">
         <v>245</v>
       </c>
       <c r="B20" s="119"/>
@@ -32899,7 +32908,7 @@
       <c r="AMJ21" s="5"/>
     </row>
     <row r="22" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="238" t="s">
+      <c r="A22" s="232" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="111"/>
@@ -32912,7 +32921,7 @@
       <c r="AMJ22" s="5"/>
     </row>
     <row r="23" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="239"/>
+      <c r="A23" s="233"/>
       <c r="B23" s="113" t="s">
         <v>73</v>
       </c>
@@ -32928,7 +32937,7 @@
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="239"/>
+      <c r="A24" s="233"/>
       <c r="B24" s="113" t="s">
         <v>76</v>
       </c>
@@ -32944,7 +32953,7 @@
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="240"/>
+      <c r="A25" s="234"/>
       <c r="B25" s="116" t="s">
         <v>79</v>
       </c>
@@ -32960,7 +32969,7 @@
       <c r="H25" s="118"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="241" t="s">
+      <c r="A26" s="235" t="s">
         <v>252</v>
       </c>
       <c r="B26" s="121"/>
@@ -33173,7 +33182,7 @@
       <c r="H35" s="110"/>
     </row>
     <row r="36" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="238" t="s">
+      <c r="A36" s="232" t="s">
         <v>532</v>
       </c>
       <c r="B36" s="123"/>
@@ -33186,7 +33195,7 @@
       <c r="AMJ36" s="5"/>
     </row>
     <row r="37" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="240"/>
+      <c r="A37" s="234"/>
       <c r="B37" s="116" t="s">
         <v>5</v>
       </c>
@@ -33248,16 +33257,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -43130,16 +43139,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>521</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -43168,7 +43177,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="235" t="s">
         <v>536</v>
       </c>
       <c r="B3" s="18"/>
@@ -43518,16 +43527,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>522</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -44001,12 +44010,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -44024,16 +44033,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -44062,7 +44071,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="235" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="154"/>
@@ -44158,7 +44167,7 @@
       <c r="H7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="238" t="s">
+      <c r="A8" s="232" t="s">
         <v>303</v>
       </c>
       <c r="B8" s="162"/>
@@ -44170,7 +44179,7 @@
       <c r="H8" s="163"/>
     </row>
     <row r="9" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="239"/>
+      <c r="A9" s="233"/>
       <c r="B9" s="164" t="s">
         <v>30</v>
       </c>
@@ -44188,7 +44197,7 @@
       <c r="H9" s="165"/>
     </row>
     <row r="10" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="239"/>
+      <c r="A10" s="233"/>
       <c r="B10" s="164" t="s">
         <v>393</v>
       </c>
@@ -44197,12 +44206,14 @@
         <v>394</v>
       </c>
       <c r="E10" s="164"/>
-      <c r="F10" s="164"/>
+      <c r="F10" s="164" t="s">
+        <v>538</v>
+      </c>
       <c r="G10" s="186"/>
       <c r="H10" s="165"/>
     </row>
     <row r="11" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="239"/>
+      <c r="A11" s="233"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
         <v>395</v>
@@ -44218,7 +44229,7 @@
       <c r="H11" s="165"/>
     </row>
     <row r="12" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="239"/>
+      <c r="A12" s="233"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
         <v>396</v>
@@ -44234,7 +44245,7 @@
       <c r="H12" s="165"/>
     </row>
     <row r="13" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="239"/>
+      <c r="A13" s="233"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
         <v>397</v>
@@ -44250,7 +44261,7 @@
       <c r="H13" s="165"/>
     </row>
     <row r="14" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="239"/>
+      <c r="A14" s="233"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
         <v>398</v>
@@ -44266,7 +44277,7 @@
       <c r="H14" s="165"/>
     </row>
     <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="239"/>
+      <c r="A15" s="233"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
         <v>400</v>
@@ -44282,7 +44293,7 @@
       <c r="H15" s="165"/>
     </row>
     <row r="16" spans="1:20" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="239"/>
+      <c r="A16" s="233"/>
       <c r="B16" s="164" t="s">
         <v>402</v>
       </c>
@@ -44291,12 +44302,14 @@
         <v>394</v>
       </c>
       <c r="E16" s="164"/>
-      <c r="F16" s="164"/>
+      <c r="F16" s="164" t="s">
+        <v>539</v>
+      </c>
       <c r="G16" s="186"/>
       <c r="H16" s="165"/>
     </row>
     <row r="17" spans="1:19" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="240"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
         <v>400</v>
@@ -44312,7 +44325,7 @@
       <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:19" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="241" t="s">
+      <c r="A18" s="235" t="s">
         <v>404</v>
       </c>
       <c r="B18" s="168"/>
@@ -44344,7 +44357,9 @@
         <v>394</v>
       </c>
       <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
+      <c r="F19" s="158" t="s">
+        <v>540</v>
+      </c>
       <c r="G19" s="183" t="s">
         <v>43</v>
       </c>
@@ -44441,16 +44456,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="238" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -45495,7 +45510,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="235" t="s">
         <v>413</v>
       </c>
       <c r="B3" s="172"/>
@@ -54795,7 +54810,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="238" t="s">
+      <c r="A13" s="232" t="s">
         <v>428</v>
       </c>
       <c r="B13" s="175"/>
@@ -54808,7 +54823,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="239"/>
+      <c r="A14" s="233"/>
       <c r="B14" s="69" t="s">
         <v>207</v>
       </c>
@@ -54824,7 +54839,7 @@
       <c r="H14" s="177"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="239"/>
+      <c r="A15" s="233"/>
       <c r="B15" s="69" t="s">
         <v>268</v>
       </c>
@@ -54840,7 +54855,7 @@
       <c r="H15" s="177"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="239"/>
+      <c r="A16" s="233"/>
       <c r="B16" s="69" t="s">
         <v>213</v>
       </c>
@@ -54856,7 +54871,7 @@
       <c r="H16" s="177"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="239"/>
+      <c r="A17" s="233"/>
       <c r="B17" s="69" t="s">
         <v>274</v>
       </c>
@@ -54872,7 +54887,7 @@
       <c r="H17" s="177"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="239"/>
+      <c r="A18" s="233"/>
       <c r="B18" s="69" t="s">
         <v>210</v>
       </c>
@@ -54888,7 +54903,7 @@
       <c r="H18" s="177"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="239"/>
+      <c r="A19" s="233"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -54904,7 +54919,7 @@
       <c r="H19" s="177"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="239"/>
+      <c r="A20" s="233"/>
       <c r="B20" s="69" t="s">
         <v>434</v>
       </c>
@@ -54920,7 +54935,7 @@
       <c r="H20" s="177"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="239"/>
+      <c r="A21" s="233"/>
       <c r="B21" s="69" t="s">
         <v>334</v>
       </c>
@@ -54936,7 +54951,7 @@
       <c r="H21" s="177"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="239"/>
+      <c r="A22" s="233"/>
       <c r="B22" s="69" t="s">
         <v>437</v>
       </c>
@@ -54952,7 +54967,7 @@
       <c r="H22" s="177"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="239"/>
+      <c r="A23" s="233"/>
       <c r="B23" s="69" t="s">
         <v>439</v>
       </c>
@@ -54968,7 +54983,7 @@
       <c r="H23" s="177"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="240"/>
+      <c r="A24" s="234"/>
       <c r="B24" s="73" t="s">
         <v>441</v>
       </c>
@@ -54984,7 +54999,7 @@
       <c r="H24" s="178"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="241" t="s">
+      <c r="A25" s="235" t="s">
         <v>370</v>
       </c>
       <c r="B25" s="179"/>
@@ -55172,7 +55187,7 @@
       <c r="H36" s="181"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="238" t="s">
+      <c r="A37" s="232" t="s">
         <v>290</v>
       </c>
       <c r="B37" s="175"/>
@@ -55185,7 +55200,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="239"/>
+      <c r="A38" s="233"/>
       <c r="B38" s="69" t="s">
         <v>207</v>
       </c>
@@ -55201,7 +55216,7 @@
       <c r="H38" s="177"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="239"/>
+      <c r="A39" s="233"/>
       <c r="B39" s="69" t="s">
         <v>268</v>
       </c>
@@ -55217,7 +55232,7 @@
       <c r="H39" s="177"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="239"/>
+      <c r="A40" s="233"/>
       <c r="B40" s="69" t="s">
         <v>213</v>
       </c>
@@ -55233,7 +55248,7 @@
       <c r="H40" s="177"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="239"/>
+      <c r="A41" s="233"/>
       <c r="B41" s="69" t="s">
         <v>274</v>
       </c>
@@ -55249,7 +55264,7 @@
       <c r="H41" s="177"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="239"/>
+      <c r="A42" s="233"/>
       <c r="B42" s="69" t="s">
         <v>460</v>
       </c>
@@ -55265,7 +55280,7 @@
       <c r="H42" s="177"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="239"/>
+      <c r="A43" s="233"/>
       <c r="B43" s="69" t="s">
         <v>370</v>
       </c>
@@ -55281,7 +55296,7 @@
       <c r="H43" s="177"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="239"/>
+      <c r="A44" s="233"/>
       <c r="B44" s="69" t="s">
         <v>210</v>
       </c>
@@ -55297,7 +55312,7 @@
       <c r="H44" s="177"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="239"/>
+      <c r="A45" s="233"/>
       <c r="B45" s="69" t="s">
         <v>424</v>
       </c>
@@ -55313,7 +55328,7 @@
       <c r="H45" s="177"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="239"/>
+      <c r="A46" s="233"/>
       <c r="B46" s="69" t="s">
         <v>465</v>
       </c>
@@ -55329,7 +55344,7 @@
       <c r="H46" s="177"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="239"/>
+      <c r="A47" s="233"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -55345,7 +55360,7 @@
       <c r="H47" s="177"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="240"/>
+      <c r="A48" s="234"/>
       <c r="B48" s="73" t="s">
         <v>437</v>
       </c>

</xml_diff>

<commit_message>
Add DATA_SCHEMA_URL to Data
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahajnal/Documents/github/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D1C529-52F7-1141-B053-543E98528845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9522CA-23D0-FB4D-9099-EFF84BE7E171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="24080" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="500" windowWidth="28360" windowHeight="14020" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="567">
   <si>
     <t>Concept</t>
   </si>
@@ -1060,9 +1060,6 @@
     <t>mandatory (WP6)</t>
   </si>
   <si>
-    <t>DATA_URI (pseudo vars: DATA_PROTOCOL, DATA_HOST, DATA_PORT, DATA_PATH, DATA_QUERY, DATA_FRAGMENT)</t>
-  </si>
-  <si>
     <t>mandatory (WP6 open)</t>
   </si>
   <si>
@@ -1528,13 +1525,7 @@
     <t>HTTP, HTTPS, TCP, UDP</t>
   </si>
   <si>
-    <t>database schema file contents (or URL?)</t>
-  </si>
-  <si>
     <t>[ { none , userpass , accesskey_secretkey , ssl_certificate , tls_mutual, access_token , rclone_config }+ ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accessibility of the data resource, including host, port information, protocol, and other fields (path is protocol dependent, can be a topic name). GUI may show host, port, path separately. Hidden at search. Format: protocol://host:port/path </t>
   </si>
   <si>
     <t>This sensor measures temperature in Celsius, sends data via ConSenses edge device via an MQTT broker</t>
@@ -1809,6 +1800,21 @@
   </si>
   <si>
     <t>For co-simulation Type only</t>
+  </si>
+  <si>
+    <t>DATA_URI</t>
+  </si>
+  <si>
+    <t>Accessibility of the data resource, including host, port information, protocol, and other fields (path is protocol dependent, can be a topic name). GUI may show host, port, path separately. Hidden at search. Format: protocol://host:port/path.  Pseudo vars: DATA_PROTOCOL, DATA_HOST, DATA_PORT, DATA_PATH, DATA_QUERY, DATA_FRAGMENT.</t>
+  </si>
+  <si>
+    <t>DATA_SCHEMA_URL</t>
+  </si>
+  <si>
+    <t>database schema URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database schema description/contents </t>
   </si>
 </sst>
 </file>
@@ -2338,7 +2344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3192,12 +3198,20 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3206,6 +3220,54 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3230,46 +3292,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3317,19 +3339,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4165,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -4187,16 +4197,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>499</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>496</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4225,7 +4235,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="244" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4237,7 +4247,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="245"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4252,12 +4262,12 @@
         <v>11</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="245"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4277,7 +4287,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="245"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4297,13 +4307,13 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="245"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="47" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>20</v>
@@ -4312,12 +4322,12 @@
         <v>21</v>
       </c>
       <c r="G7" s="183" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="245"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4337,7 +4347,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4346,10 +4356,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="49" t="s">
+        <v>474</v>
+      </c>
+      <c r="F9" s="47" t="s">
         <v>475</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>476</v>
       </c>
       <c r="G9" s="183" t="s">
         <v>12</v>
@@ -4357,7 +4367,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4377,7 +4387,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="232"/>
+      <c r="A11" s="246"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4397,7 +4407,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="233" t="s">
+      <c r="A12" s="247" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="217"/>
@@ -4409,7 +4419,7 @@
       <c r="H12" s="220"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="234"/>
+      <c r="A13" s="248"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4418,7 +4428,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F13" s="55" t="s">
         <v>37</v>
@@ -4429,19 +4439,19 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="234"/>
+      <c r="A14" s="248"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="55" t="s">
+        <v>456</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>471</v>
+      </c>
+      <c r="F14" s="55" t="s">
         <v>457</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>472</v>
-      </c>
-      <c r="F14" s="55" t="s">
-        <v>458</v>
       </c>
       <c r="G14" s="188" t="s">
         <v>12</v>
@@ -4449,19 +4459,19 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="234"/>
+      <c r="A15" s="248"/>
       <c r="B15" s="55" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="55" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F15" s="55" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G15" s="188" t="s">
         <v>43</v>
@@ -5485,19 +5495,19 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="234"/>
+      <c r="A16" s="248"/>
       <c r="B16" s="55" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="55" t="s">
+        <v>461</v>
+      </c>
+      <c r="E16" s="57" t="s">
         <v>462</v>
       </c>
-      <c r="E16" s="57" t="s">
-        <v>463</v>
-      </c>
       <c r="F16" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G16" s="188" t="s">
         <v>43</v>
@@ -6521,19 +6531,19 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="235"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="221" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C17" s="222"/>
       <c r="D17" s="221" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E17" s="223" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F17" s="221" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G17" s="224" t="s">
         <v>43</v>
@@ -7557,7 +7567,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="236" t="s">
+      <c r="A18" s="240" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="59"/>
@@ -7569,7 +7579,7 @@
       <c r="H18" s="61"/>
     </row>
     <row r="19" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="236"/>
+      <c r="A19" s="240"/>
       <c r="B19" s="47" t="s">
         <v>40</v>
       </c>
@@ -7589,7 +7599,7 @@
       <c r="H19" s="50"/>
     </row>
     <row r="20" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="236"/>
+      <c r="A20" s="240"/>
       <c r="B20" s="47" t="s">
         <v>44</v>
       </c>
@@ -7609,7 +7619,7 @@
       <c r="H20" s="50"/>
     </row>
     <row r="21" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="236"/>
+      <c r="A21" s="240"/>
       <c r="B21" s="47" t="s">
         <v>46</v>
       </c>
@@ -7629,7 +7639,7 @@
       <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="236"/>
+      <c r="A22" s="240"/>
       <c r="B22" s="47" t="s">
         <v>48</v>
       </c>
@@ -7649,7 +7659,7 @@
       <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="236"/>
+      <c r="A23" s="240"/>
       <c r="B23" s="47" t="s">
         <v>50</v>
       </c>
@@ -7669,7 +7679,7 @@
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="236"/>
+      <c r="A24" s="240"/>
       <c r="B24" s="47" t="s">
         <v>53</v>
       </c>
@@ -7689,7 +7699,7 @@
       <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="236"/>
+      <c r="A25" s="240"/>
       <c r="B25" s="47" t="s">
         <v>57</v>
       </c>
@@ -7709,7 +7719,7 @@
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="236"/>
+      <c r="A26" s="240"/>
       <c r="B26" s="47" t="s">
         <v>61</v>
       </c>
@@ -7729,7 +7739,7 @@
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="236"/>
+      <c r="A27" s="240"/>
       <c r="B27" s="47" t="s">
         <v>63</v>
       </c>
@@ -7749,7 +7759,7 @@
       <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="236"/>
+      <c r="A28" s="240"/>
       <c r="B28" s="47" t="s">
         <v>65</v>
       </c>
@@ -7769,7 +7779,7 @@
       <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="236"/>
+      <c r="A29" s="240"/>
       <c r="B29" s="47" t="s">
         <v>67</v>
       </c>
@@ -7789,7 +7799,7 @@
       <c r="H29" s="50"/>
     </row>
     <row r="30" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="237"/>
+      <c r="A30" s="241"/>
       <c r="B30" s="51" t="s">
         <v>69</v>
       </c>
@@ -7809,7 +7819,7 @@
       <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="238" t="s">
+      <c r="A31" s="236" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="62"/>
@@ -7821,7 +7831,7 @@
       <c r="H31" s="64"/>
     </row>
     <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="239"/>
+      <c r="A32" s="237"/>
       <c r="B32" s="65" t="s">
         <v>73</v>
       </c>
@@ -7841,7 +7851,7 @@
       <c r="H32" s="68"/>
     </row>
     <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="239"/>
+      <c r="A33" s="237"/>
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -7861,7 +7871,7 @@
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="239"/>
+      <c r="A34" s="237"/>
       <c r="B34" s="69" t="s">
         <v>79</v>
       </c>
@@ -7881,7 +7891,7 @@
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="240"/>
+      <c r="A35" s="238"/>
       <c r="B35" s="73" t="s">
         <v>82</v>
       </c>
@@ -7901,7 +7911,7 @@
       <c r="H35" s="76"/>
     </row>
     <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="241" t="s">
+      <c r="A36" s="239" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="59"/>
@@ -7913,7 +7923,7 @@
       <c r="H36" s="61"/>
     </row>
     <row r="37" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="236"/>
+      <c r="A37" s="240"/>
       <c r="B37" s="47" t="s">
         <v>86</v>
       </c>
@@ -8949,8 +8959,8 @@
       <c r="AMJ37" s="4"/>
     </row>
     <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="236"/>
-      <c r="B38" s="228" t="s">
+      <c r="A38" s="240"/>
+      <c r="B38" s="230" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -9987,8 +9997,8 @@
       <c r="AMJ38" s="4"/>
     </row>
     <row r="39" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="236"/>
-      <c r="B39" s="228"/>
+      <c r="A39" s="240"/>
+      <c r="B39" s="230"/>
       <c r="C39" s="47" t="s">
         <v>94</v>
       </c>
@@ -11023,8 +11033,8 @@
       <c r="AMJ39" s="4"/>
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="236"/>
-      <c r="B40" s="228"/>
+      <c r="A40" s="240"/>
+      <c r="B40" s="230"/>
       <c r="C40" s="47" t="s">
         <v>98</v>
       </c>
@@ -12059,8 +12069,8 @@
       <c r="AMJ40" s="4"/>
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A41" s="236"/>
-      <c r="B41" s="228"/>
+      <c r="A41" s="240"/>
+      <c r="B41" s="230"/>
       <c r="C41" s="47" t="s">
         <v>102</v>
       </c>
@@ -13095,8 +13105,8 @@
       <c r="AMJ41" s="4"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="236"/>
-      <c r="B42" s="228"/>
+      <c r="A42" s="240"/>
+      <c r="B42" s="230"/>
       <c r="C42" s="47" t="s">
         <v>106</v>
       </c>
@@ -14131,8 +14141,8 @@
       <c r="AMJ42" s="4"/>
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="236"/>
-      <c r="B43" s="228"/>
+      <c r="A43" s="240"/>
+      <c r="B43" s="230"/>
       <c r="C43" s="47" t="s">
         <v>110</v>
       </c>
@@ -15167,8 +15177,8 @@
       <c r="AMJ43" s="4"/>
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="236"/>
-      <c r="B44" s="228"/>
+      <c r="A44" s="240"/>
+      <c r="B44" s="230"/>
       <c r="C44" s="47" t="s">
         <v>114</v>
       </c>
@@ -16203,8 +16213,8 @@
       <c r="AMJ44" s="4"/>
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="236"/>
-      <c r="B45" s="228"/>
+      <c r="A45" s="240"/>
+      <c r="B45" s="230"/>
       <c r="C45" s="47" t="s">
         <v>118</v>
       </c>
@@ -17239,8 +17249,8 @@
       <c r="AMJ45" s="4"/>
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="236"/>
-      <c r="B46" s="228"/>
+      <c r="A46" s="240"/>
+      <c r="B46" s="230"/>
       <c r="C46" s="47" t="s">
         <v>122</v>
       </c>
@@ -18275,8 +18285,8 @@
       <c r="AMJ46" s="4"/>
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="236"/>
-      <c r="B47" s="228"/>
+      <c r="A47" s="240"/>
+      <c r="B47" s="230"/>
       <c r="C47" s="47" t="s">
         <v>126</v>
       </c>
@@ -19311,8 +19321,8 @@
       <c r="AMJ47" s="4"/>
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="236"/>
-      <c r="B48" s="228"/>
+      <c r="A48" s="240"/>
+      <c r="B48" s="230"/>
       <c r="C48" s="47" t="s">
         <v>130</v>
       </c>
@@ -20347,8 +20357,8 @@
       <c r="AMJ48" s="4"/>
     </row>
     <row r="49" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="237"/>
-      <c r="B49" s="229"/>
+      <c r="A49" s="241"/>
+      <c r="B49" s="231"/>
       <c r="C49" s="51" t="s">
         <v>134</v>
       </c>
@@ -20359,7 +20369,7 @@
         <v>136</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G49" s="184" t="s">
         <v>43</v>
@@ -21383,7 +21393,7 @@
       <c r="AMJ49" s="15"/>
     </row>
     <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="238" t="s">
+      <c r="A50" s="236" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="77"/>
@@ -21395,7 +21405,7 @@
       <c r="H50" s="79"/>
     </row>
     <row r="51" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="239"/>
+      <c r="A51" s="237"/>
       <c r="B51" s="80" t="s">
         <v>138</v>
       </c>
@@ -21415,8 +21425,8 @@
       <c r="H51" s="83"/>
     </row>
     <row r="52" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="239"/>
-      <c r="B52" s="242" t="s">
+      <c r="A52" s="237"/>
+      <c r="B52" s="232" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
@@ -21437,8 +21447,8 @@
       <c r="H52" s="83"/>
     </row>
     <row r="53" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="239"/>
-      <c r="B53" s="242"/>
+      <c r="A53" s="237"/>
+      <c r="B53" s="232"/>
       <c r="C53" s="80" t="s">
         <v>94</v>
       </c>
@@ -21457,8 +21467,8 @@
       <c r="H53" s="83"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="239"/>
-      <c r="B54" s="242"/>
+      <c r="A54" s="237"/>
+      <c r="B54" s="232"/>
       <c r="C54" s="80" t="s">
         <v>98</v>
       </c>
@@ -21477,8 +21487,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A55" s="239"/>
-      <c r="B55" s="242"/>
+      <c r="A55" s="237"/>
+      <c r="B55" s="232"/>
       <c r="C55" s="80" t="s">
         <v>102</v>
       </c>
@@ -21497,8 +21507,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="239"/>
-      <c r="B56" s="242"/>
+      <c r="A56" s="237"/>
+      <c r="B56" s="232"/>
       <c r="C56" s="80" t="s">
         <v>106</v>
       </c>
@@ -21517,8 +21527,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="239"/>
-      <c r="B57" s="242"/>
+      <c r="A57" s="237"/>
+      <c r="B57" s="232"/>
       <c r="C57" s="80" t="s">
         <v>110</v>
       </c>
@@ -21537,8 +21547,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="239"/>
-      <c r="B58" s="242"/>
+      <c r="A58" s="237"/>
+      <c r="B58" s="232"/>
       <c r="C58" s="80" t="s">
         <v>114</v>
       </c>
@@ -21557,8 +21567,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A59" s="239"/>
-      <c r="B59" s="242"/>
+      <c r="A59" s="237"/>
+      <c r="B59" s="232"/>
       <c r="C59" s="80" t="s">
         <v>118</v>
       </c>
@@ -21577,8 +21587,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="239"/>
-      <c r="B60" s="242"/>
+      <c r="A60" s="237"/>
+      <c r="B60" s="232"/>
       <c r="C60" s="80" t="s">
         <v>122</v>
       </c>
@@ -21597,8 +21607,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="239"/>
-      <c r="B61" s="242"/>
+      <c r="A61" s="237"/>
+      <c r="B61" s="232"/>
       <c r="C61" s="80" t="s">
         <v>126</v>
       </c>
@@ -21617,8 +21627,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="239"/>
-      <c r="B62" s="242"/>
+      <c r="A62" s="237"/>
+      <c r="B62" s="232"/>
       <c r="C62" s="80" t="s">
         <v>130</v>
       </c>
@@ -21637,8 +21647,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="240"/>
-      <c r="B63" s="243"/>
+      <c r="A63" s="238"/>
+      <c r="B63" s="233"/>
       <c r="C63" s="85" t="s">
         <v>134</v>
       </c>
@@ -21649,7 +21659,7 @@
         <v>136</v>
       </c>
       <c r="F63" s="85" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G63" s="187" t="s">
         <v>43</v>
@@ -21657,7 +21667,7 @@
       <c r="H63" s="87"/>
     </row>
     <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="241" t="s">
+      <c r="A64" s="239" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="59"/>
@@ -22685,7 +22695,7 @@
       <c r="AMJ64" s="13"/>
     </row>
     <row r="65" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="236"/>
+      <c r="A65" s="240"/>
       <c r="B65" s="89" t="s">
         <v>146</v>
       </c>
@@ -23721,7 +23731,7 @@
       <c r="AMJ65" s="13"/>
     </row>
     <row r="66" spans="1:1024" s="14" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="237"/>
+      <c r="A66" s="241"/>
       <c r="B66" s="93" t="s">
         <v>150</v>
       </c>
@@ -24757,7 +24767,7 @@
       <c r="AMJ66" s="13"/>
     </row>
     <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="238" t="s">
+      <c r="A67" s="236" t="s">
         <v>154</v>
       </c>
       <c r="B67" s="29"/>
@@ -24769,7 +24779,7 @@
       <c r="H67" s="64"/>
     </row>
     <row r="68" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="239"/>
+      <c r="A68" s="237"/>
       <c r="B68" s="69" t="s">
         <v>155</v>
       </c>
@@ -24787,8 +24797,8 @@
       <c r="H68" s="72"/>
     </row>
     <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="239"/>
-      <c r="B69" s="244" t="s">
+      <c r="A69" s="237"/>
+      <c r="B69" s="234" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="69" t="s">
@@ -24809,8 +24819,8 @@
       <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="239"/>
-      <c r="B70" s="244"/>
+      <c r="A70" s="237"/>
+      <c r="B70" s="234"/>
       <c r="C70" s="69" t="s">
         <v>30</v>
       </c>
@@ -24829,8 +24839,8 @@
       <c r="H70" s="72"/>
     </row>
     <row r="71" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="239"/>
-      <c r="B71" s="244"/>
+      <c r="A71" s="237"/>
+      <c r="B71" s="234"/>
       <c r="C71" s="69" t="s">
         <v>12</v>
       </c>
@@ -24849,8 +24859,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="239"/>
-      <c r="B72" s="244"/>
+      <c r="A72" s="237"/>
+      <c r="B72" s="234"/>
       <c r="C72" s="69" t="s">
         <v>167</v>
       </c>
@@ -24869,8 +24879,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="240"/>
-      <c r="B73" s="245"/>
+      <c r="A73" s="238"/>
+      <c r="B73" s="235"/>
       <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
@@ -24889,7 +24899,7 @@
       <c r="H73" s="76"/>
     </row>
     <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="241" t="s">
+      <c r="A74" s="239" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="31"/>
@@ -25917,7 +25927,7 @@
       <c r="AMJ74" s="13"/>
     </row>
     <row r="75" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="236"/>
+      <c r="A75" s="240"/>
       <c r="B75" s="47" t="s">
         <v>173</v>
       </c>
@@ -26951,8 +26961,8 @@
       <c r="AMJ75" s="13"/>
     </row>
     <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="236"/>
-      <c r="B76" s="228" t="s">
+      <c r="A76" s="240"/>
+      <c r="B76" s="230" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="47" t="s">
@@ -27989,8 +27999,8 @@
       <c r="AMJ76" s="13"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="236"/>
-      <c r="B77" s="228"/>
+      <c r="A77" s="240"/>
+      <c r="B77" s="230"/>
       <c r="C77" s="47" t="s">
         <v>179</v>
       </c>
@@ -29025,8 +29035,8 @@
       <c r="AMJ77" s="13"/>
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="236"/>
-      <c r="B78" s="228"/>
+      <c r="A78" s="240"/>
+      <c r="B78" s="230"/>
       <c r="C78" s="47" t="s">
         <v>182</v>
       </c>
@@ -30061,8 +30071,8 @@
       <c r="AMJ78" s="13"/>
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="236"/>
-      <c r="B79" s="228"/>
+      <c r="A79" s="240"/>
+      <c r="B79" s="230"/>
       <c r="C79" s="47" t="s">
         <v>185</v>
       </c>
@@ -31097,8 +31107,8 @@
       <c r="AMJ79" s="13"/>
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="237"/>
-      <c r="B80" s="229"/>
+      <c r="A80" s="241"/>
+      <c r="B80" s="231"/>
       <c r="C80" s="51" t="s">
         <v>25</v>
       </c>
@@ -32207,6 +32217,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A49"/>
     <mergeCell ref="B76:B80"/>
     <mergeCell ref="B52:B63"/>
     <mergeCell ref="B69:B73"/>
@@ -32214,13 +32231,6 @@
     <mergeCell ref="A64:A66"/>
     <mergeCell ref="A67:A73"/>
     <mergeCell ref="A74:A80"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A49"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32260,16 +32270,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32298,7 +32308,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="244" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -32310,7 +32320,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="245"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -32325,12 +32335,12 @@
         <v>192</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="245"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -32350,7 +32360,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="245"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -32370,7 +32380,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="245"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -32390,7 +32400,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="245"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -32410,7 +32420,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -32430,13 +32440,13 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="47" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>20</v>
@@ -32445,12 +32455,12 @@
         <v>201</v>
       </c>
       <c r="G10" s="183" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="232"/>
+      <c r="A11" s="246"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -32470,7 +32480,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="246" t="s">
+      <c r="A12" s="250" t="s">
         <v>203</v>
       </c>
       <c r="B12" s="98"/>
@@ -32482,7 +32492,7 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="247"/>
+      <c r="A13" s="251"/>
       <c r="B13" s="103" t="s">
         <v>204</v>
       </c>
@@ -32502,19 +32512,19 @@
       <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="247"/>
+      <c r="A14" s="251"/>
       <c r="B14" s="103" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103" t="s">
+        <v>453</v>
+      </c>
+      <c r="E14" s="104" t="s">
         <v>454</v>
       </c>
-      <c r="E14" s="104" t="s">
-        <v>455</v>
-      </c>
       <c r="F14" s="103" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="G14" s="186" t="s">
         <v>12</v>
@@ -32560,16 +32570,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>501</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -32598,7 +32608,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="244" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -32648,7 +32658,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="231"/>
+      <c r="A4" s="245"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -32661,12 +32671,12 @@
         <v>209</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="231"/>
+      <c r="A5" s="245"/>
       <c r="B5" s="105" t="s">
         <v>210</v>
       </c>
@@ -32682,23 +32692,23 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="231"/>
+      <c r="A6" s="245"/>
       <c r="B6" s="105" t="s">
         <v>213</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="231"/>
+      <c r="A7" s="245"/>
       <c r="B7" s="105" t="s">
         <v>214</v>
       </c>
@@ -32708,13 +32718,13 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G7" s="197"/>
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="231"/>
+      <c r="A8" s="245"/>
       <c r="B8" s="105" t="s">
         <v>215</v>
       </c>
@@ -32730,7 +32740,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="231"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="105" t="s">
         <v>217</v>
       </c>
@@ -32740,7 +32750,7 @@
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G9" s="197" t="s">
         <v>43</v>
@@ -32748,7 +32758,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="231"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="105" t="s">
         <v>219</v>
       </c>
@@ -32777,7 +32787,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="231"/>
+      <c r="A11" s="245"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -32793,7 +32803,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="231"/>
+      <c r="A12" s="245"/>
       <c r="B12" s="105" t="s">
         <v>223</v>
       </c>
@@ -32803,7 +32813,7 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="G12" s="197" t="s">
         <v>43</v>
@@ -32811,7 +32821,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="231"/>
+      <c r="A13" s="245"/>
       <c r="B13" s="105" t="s">
         <v>225</v>
       </c>
@@ -32829,9 +32839,9 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="231"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="105" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
@@ -32839,7 +32849,7 @@
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="105" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G14" s="197" t="s">
         <v>43</v>
@@ -32847,7 +32857,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="232"/>
+      <c r="A15" s="246"/>
       <c r="B15" s="108" t="s">
         <v>229</v>
       </c>
@@ -32863,7 +32873,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="238" t="s">
+      <c r="A16" s="236" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -32876,13 +32886,13 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="239"/>
+      <c r="A17" s="237"/>
       <c r="B17" s="113" t="s">
         <v>232</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E17" s="114"/>
       <c r="F17" s="113" t="s">
@@ -32892,7 +32902,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="239"/>
+      <c r="A18" s="237"/>
       <c r="B18" s="113"/>
       <c r="C18" s="114" t="s">
         <v>1</v>
@@ -32902,13 +32912,13 @@
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="G18" s="200"/>
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="239"/>
+      <c r="A19" s="237"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>210</v>
@@ -32918,163 +32928,163 @@
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G19" s="200"/>
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="239"/>
+      <c r="A20" s="237"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D20" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="G20" s="200"/>
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="239"/>
+      <c r="A21" s="237"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D21" s="113" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G21" s="200"/>
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="239"/>
+      <c r="A22" s="237"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G22" s="200"/>
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="239"/>
+      <c r="A23" s="237"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D23" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G23" s="200"/>
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="239"/>
+      <c r="A24" s="237"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G24" s="200"/>
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="239"/>
+      <c r="A25" s="237"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D25" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G25" s="200"/>
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="239"/>
+      <c r="A26" s="237"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G26" s="200"/>
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="239"/>
+      <c r="A27" s="237"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D27" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="G27" s="200"/>
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="239"/>
+      <c r="A28" s="237"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
+        <v>538</v>
+      </c>
+      <c r="D28" s="113" t="s">
         <v>541</v>
-      </c>
-      <c r="D28" s="113" t="s">
-        <v>544</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="G28" s="200"/>
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="239"/>
+      <c r="A29" s="237"/>
       <c r="B29" s="113" t="s">
         <v>234</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="113" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
@@ -33084,183 +33094,183 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="239"/>
-      <c r="B30" s="257"/>
+      <c r="A30" s="237"/>
+      <c r="B30" s="226"/>
       <c r="C30" s="114" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="113" t="s">
         <v>211</v>
       </c>
-      <c r="E30" s="258"/>
+      <c r="E30" s="227"/>
       <c r="F30" s="113" t="s">
-        <v>556</v>
-      </c>
-      <c r="G30" s="259"/>
-      <c r="H30" s="260"/>
+        <v>553</v>
+      </c>
+      <c r="G30" s="228"/>
+      <c r="H30" s="229"/>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="239"/>
-      <c r="B31" s="257"/>
+      <c r="A31" s="237"/>
+      <c r="B31" s="226"/>
       <c r="C31" s="114" t="s">
         <v>210</v>
       </c>
       <c r="D31" s="113" t="s">
         <v>211</v>
       </c>
-      <c r="E31" s="258"/>
+      <c r="E31" s="227"/>
       <c r="F31" s="113" t="s">
-        <v>557</v>
-      </c>
-      <c r="G31" s="259"/>
-      <c r="H31" s="260"/>
+        <v>554</v>
+      </c>
+      <c r="G31" s="228"/>
+      <c r="H31" s="229"/>
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="239"/>
-      <c r="B32" s="257"/>
+      <c r="A32" s="237"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="114" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D32" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="258"/>
+      <c r="E32" s="227"/>
       <c r="F32" s="113" t="s">
-        <v>558</v>
-      </c>
-      <c r="G32" s="259"/>
-      <c r="H32" s="260"/>
+        <v>555</v>
+      </c>
+      <c r="G32" s="228"/>
+      <c r="H32" s="229"/>
     </row>
     <row r="33" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="239"/>
-      <c r="B33" s="257"/>
+      <c r="A33" s="237"/>
+      <c r="B33" s="226"/>
       <c r="C33" s="114" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>542</v>
-      </c>
-      <c r="E33" s="258"/>
+        <v>539</v>
+      </c>
+      <c r="E33" s="227"/>
       <c r="F33" s="113" t="s">
-        <v>559</v>
-      </c>
-      <c r="G33" s="259"/>
-      <c r="H33" s="260"/>
+        <v>556</v>
+      </c>
+      <c r="G33" s="228"/>
+      <c r="H33" s="229"/>
     </row>
     <row r="34" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="239"/>
-      <c r="B34" s="257"/>
+      <c r="A34" s="237"/>
+      <c r="B34" s="226"/>
       <c r="C34" s="114" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D34" s="113" t="s">
-        <v>543</v>
-      </c>
-      <c r="E34" s="258"/>
+        <v>540</v>
+      </c>
+      <c r="E34" s="227"/>
       <c r="F34" s="113" t="s">
-        <v>560</v>
-      </c>
-      <c r="G34" s="259"/>
-      <c r="H34" s="260"/>
+        <v>557</v>
+      </c>
+      <c r="G34" s="228"/>
+      <c r="H34" s="229"/>
     </row>
     <row r="35" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="239"/>
-      <c r="B35" s="257"/>
+      <c r="A35" s="237"/>
+      <c r="B35" s="226"/>
       <c r="C35" s="114" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D35" s="113" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="258"/>
+      <c r="E35" s="227"/>
       <c r="F35" s="113" t="s">
-        <v>561</v>
-      </c>
-      <c r="G35" s="259"/>
-      <c r="H35" s="260"/>
+        <v>558</v>
+      </c>
+      <c r="G35" s="228"/>
+      <c r="H35" s="229"/>
     </row>
     <row r="36" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="239"/>
-      <c r="B36" s="257"/>
+      <c r="A36" s="237"/>
+      <c r="B36" s="226"/>
       <c r="C36" s="114" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>544</v>
-      </c>
-      <c r="E36" s="258"/>
+        <v>541</v>
+      </c>
+      <c r="E36" s="227"/>
       <c r="F36" s="113" t="s">
-        <v>551</v>
-      </c>
-      <c r="G36" s="259"/>
-      <c r="H36" s="260"/>
+        <v>548</v>
+      </c>
+      <c r="G36" s="228"/>
+      <c r="H36" s="229"/>
     </row>
     <row r="37" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="239"/>
-      <c r="B37" s="257"/>
+      <c r="A37" s="237"/>
+      <c r="B37" s="226"/>
       <c r="C37" s="114" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D37" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="E37" s="258"/>
+      <c r="E37" s="227"/>
       <c r="F37" s="113" t="s">
-        <v>552</v>
-      </c>
-      <c r="G37" s="259"/>
-      <c r="H37" s="260"/>
+        <v>549</v>
+      </c>
+      <c r="G37" s="228"/>
+      <c r="H37" s="229"/>
     </row>
     <row r="38" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="239"/>
-      <c r="B38" s="257"/>
+      <c r="A38" s="237"/>
+      <c r="B38" s="226"/>
       <c r="C38" s="114" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D38" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="E38" s="258"/>
+      <c r="E38" s="227"/>
       <c r="F38" s="113" t="s">
-        <v>553</v>
-      </c>
-      <c r="G38" s="259"/>
-      <c r="H38" s="260"/>
+        <v>550</v>
+      </c>
+      <c r="G38" s="228"/>
+      <c r="H38" s="229"/>
     </row>
     <row r="39" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="239"/>
-      <c r="B39" s="257"/>
+      <c r="A39" s="237"/>
+      <c r="B39" s="226"/>
       <c r="C39" s="114" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D39" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="E39" s="258"/>
+      <c r="E39" s="227"/>
       <c r="F39" s="113" t="s">
-        <v>562</v>
-      </c>
-      <c r="G39" s="259"/>
-      <c r="H39" s="260"/>
+        <v>559</v>
+      </c>
+      <c r="G39" s="228"/>
+      <c r="H39" s="229"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="239"/>
-      <c r="B40" s="257"/>
+      <c r="A40" s="237"/>
+      <c r="B40" s="226"/>
       <c r="C40" s="114" t="s">
+        <v>538</v>
+      </c>
+      <c r="D40" s="113" t="s">
         <v>541</v>
       </c>
-      <c r="D40" s="113" t="s">
-        <v>544</v>
-      </c>
-      <c r="E40" s="258"/>
+      <c r="E40" s="227"/>
       <c r="F40" s="113" t="s">
-        <v>563</v>
-      </c>
-      <c r="G40" s="259"/>
-      <c r="H40" s="260"/>
+        <v>560</v>
+      </c>
+      <c r="G40" s="228"/>
+      <c r="H40" s="229"/>
     </row>
     <row r="41" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="240"/>
+      <c r="A41" s="238"/>
       <c r="B41" s="116" t="s">
         <v>236</v>
       </c>
@@ -33270,7 +33280,7 @@
       </c>
       <c r="E41" s="117"/>
       <c r="F41" s="116" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="G41" s="201" t="s">
         <v>43</v>
@@ -33278,7 +33288,7 @@
       <c r="H41" s="118"/>
     </row>
     <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="241" t="s">
+      <c r="A42" s="239" t="s">
         <v>237</v>
       </c>
       <c r="B42" s="119"/>
@@ -33328,7 +33338,7 @@
       <c r="AMJ42" s="5"/>
     </row>
     <row r="43" spans="1:1024" s="9" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="237"/>
+      <c r="A43" s="241"/>
       <c r="B43" s="108" t="s">
         <v>238</v>
       </c>
@@ -33365,7 +33375,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="238" t="s">
+      <c r="A44" s="236" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="111"/>
@@ -33378,7 +33388,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="239"/>
+      <c r="A45" s="237"/>
       <c r="B45" s="113" t="s">
         <v>73</v>
       </c>
@@ -33396,7 +33406,7 @@
       <c r="H45" s="115"/>
     </row>
     <row r="46" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="239"/>
+      <c r="A46" s="237"/>
       <c r="B46" s="113" t="s">
         <v>76</v>
       </c>
@@ -33414,7 +33424,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="240"/>
+      <c r="A47" s="238"/>
       <c r="B47" s="116" t="s">
         <v>79</v>
       </c>
@@ -33432,7 +33442,7 @@
       <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="241" t="s">
+      <c r="A48" s="239" t="s">
         <v>244</v>
       </c>
       <c r="B48" s="121"/>
@@ -33463,7 +33473,7 @@
       <c r="AMJ48" s="5"/>
     </row>
     <row r="49" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="236"/>
+      <c r="A49" s="240"/>
       <c r="B49" s="105" t="s">
         <v>245</v>
       </c>
@@ -33481,7 +33491,7 @@
       <c r="H49" s="107"/>
     </row>
     <row r="50" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="236"/>
+      <c r="A50" s="240"/>
       <c r="B50" s="105" t="s">
         <v>247</v>
       </c>
@@ -33499,7 +33509,7 @@
       <c r="H50" s="107"/>
     </row>
     <row r="51" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="236"/>
+      <c r="A51" s="240"/>
       <c r="B51" s="105" t="s">
         <v>46</v>
       </c>
@@ -33517,7 +33527,7 @@
       <c r="H51" s="107"/>
     </row>
     <row r="52" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="236"/>
+      <c r="A52" s="240"/>
       <c r="B52" s="105" t="s">
         <v>48</v>
       </c>
@@ -33535,7 +33545,7 @@
       <c r="H52" s="107"/>
     </row>
     <row r="53" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="236"/>
+      <c r="A53" s="240"/>
       <c r="B53" s="105" t="s">
         <v>61</v>
       </c>
@@ -33573,7 +33583,7 @@
       <c r="AMJ53" s="5"/>
     </row>
     <row r="54" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="236"/>
+      <c r="A54" s="240"/>
       <c r="B54" s="105" t="s">
         <v>63</v>
       </c>
@@ -33591,7 +33601,7 @@
       <c r="H54" s="107"/>
     </row>
     <row r="55" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="236"/>
+      <c r="A55" s="240"/>
       <c r="B55" s="105" t="s">
         <v>65</v>
       </c>
@@ -33609,7 +33619,7 @@
       <c r="H55" s="107"/>
     </row>
     <row r="56" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="236"/>
+      <c r="A56" s="240"/>
       <c r="B56" s="105" t="s">
         <v>67</v>
       </c>
@@ -33627,7 +33637,7 @@
       <c r="H56" s="107"/>
     </row>
     <row r="57" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="237"/>
+      <c r="A57" s="241"/>
       <c r="B57" s="108" t="s">
         <v>69</v>
       </c>
@@ -33645,8 +33655,8 @@
       <c r="H57" s="110"/>
     </row>
     <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="238" t="s">
-        <v>513</v>
+      <c r="A58" s="236" t="s">
+        <v>510</v>
       </c>
       <c r="B58" s="123"/>
       <c r="C58" s="123"/>
@@ -33658,7 +33668,7 @@
       <c r="AMJ58" s="5"/>
     </row>
     <row r="59" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="240"/>
+      <c r="A59" s="238"/>
       <c r="B59" s="116" t="s">
         <v>5</v>
       </c>
@@ -33696,14 +33706,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" sqref="A1:H1"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -33720,16 +33730,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>502</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -34774,8 +34784,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="248" t="s">
-        <v>514</v>
+      <c r="A3" s="252" t="s">
+        <v>511</v>
       </c>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
@@ -34799,7 +34809,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="249"/>
+      <c r="A4" s="253"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -34814,12 +34824,12 @@
         <v>305</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="249"/>
+      <c r="A5" s="253"/>
       <c r="B5" s="105" t="s">
         <v>306</v>
       </c>
@@ -34834,14 +34844,14 @@
         <v>307</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="249"/>
+      <c r="A6" s="253"/>
       <c r="B6" s="105" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
@@ -34854,12 +34864,12 @@
         <v>308</v>
       </c>
       <c r="G6" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H6" s="126"/>
     </row>
     <row r="7" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="249"/>
+      <c r="A7" s="253"/>
       <c r="B7" s="105" t="s">
         <v>309</v>
       </c>
@@ -34868,18 +34878,18 @@
         <v>310</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F7" s="105" t="s">
         <v>311</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H7" s="126"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="251" t="s">
+      <c r="A8" s="255" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="123"/>
@@ -34892,7 +34902,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="257"/>
       <c r="B9" s="113" t="s">
         <v>312</v>
       </c>
@@ -34901,7 +34911,7 @@
         <v>211</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>313</v>
@@ -35928,19 +35938,19 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="257"/>
       <c r="B10" s="113" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G10" s="200" t="s">
         <v>43</v>
@@ -36964,7 +36974,7 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="253"/>
+      <c r="A11" s="257"/>
       <c r="B11" s="113" t="s">
         <v>317</v>
       </c>
@@ -36973,7 +36983,7 @@
         <v>211</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F11" s="113" t="s">
         <v>318</v>
@@ -38000,16 +38010,16 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="253"/>
+      <c r="A12" s="257"/>
       <c r="B12" s="113" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
         <v>319</v>
       </c>
       <c r="E12" s="117" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F12" s="116" t="s">
         <v>320</v>
@@ -39036,7 +39046,7 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="253"/>
+      <c r="A13" s="257"/>
       <c r="B13" s="113" t="s">
         <v>314</v>
       </c>
@@ -39045,7 +39055,7 @@
         <v>315</v>
       </c>
       <c r="E13" s="114" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F13" s="113" t="s">
         <v>316</v>
@@ -40072,8 +40082,8 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="248" t="s">
-        <v>515</v>
+      <c r="A14" s="252" t="s">
+        <v>512</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="121"/>
@@ -40093,7 +40103,7 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="250"/>
+      <c r="A15" s="254"/>
       <c r="B15" s="108" t="s">
         <v>321</v>
       </c>
@@ -40102,7 +40112,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="109" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F15" s="108" t="s">
         <v>323</v>
@@ -41129,7 +41139,7 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="251" t="s">
+      <c r="A16" s="255" t="s">
         <v>324</v>
       </c>
       <c r="B16" s="111"/>
@@ -42157,7 +42167,7 @@
       <c r="AMJ16" s="39"/>
     </row>
     <row r="17" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="253"/>
+      <c r="A17" s="257"/>
       <c r="B17" s="113" t="s">
         <v>94</v>
       </c>
@@ -42166,7 +42176,7 @@
         <v>220</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>325</v>
@@ -42177,7 +42187,7 @@
       <c r="H17" s="129"/>
     </row>
     <row r="18" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="253"/>
+      <c r="A18" s="257"/>
       <c r="B18" s="113" t="s">
         <v>98</v>
       </c>
@@ -42186,7 +42196,7 @@
         <v>220</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F18" s="113" t="s">
         <v>326</v>
@@ -42197,7 +42207,7 @@
       <c r="H18" s="129"/>
     </row>
     <row r="19" spans="1:1024" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="252"/>
+      <c r="A19" s="256"/>
       <c r="B19" s="116" t="s">
         <v>102</v>
       </c>
@@ -42206,7 +42216,7 @@
         <v>322</v>
       </c>
       <c r="E19" s="117" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F19" s="116" t="s">
         <v>327</v>
@@ -42217,7 +42227,7 @@
       <c r="H19" s="130"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="248" t="s">
+      <c r="A20" s="252" t="s">
         <v>329</v>
       </c>
       <c r="B20" s="121"/>
@@ -42237,7 +42247,7 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="249"/>
+      <c r="A21" s="253"/>
       <c r="B21" s="105" t="s">
         <v>106</v>
       </c>
@@ -42246,7 +42256,7 @@
         <v>211</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F21" s="105" t="s">
         <v>330</v>
@@ -42257,39 +42267,39 @@
       <c r="H21" s="126"/>
     </row>
     <row r="22" spans="1:1024" ht="146.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="249"/>
+      <c r="A22" s="253"/>
       <c r="B22" s="105" t="s">
-        <v>332</v>
+        <v>562</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
         <v>226</v>
       </c>
       <c r="E22" s="106" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>490</v>
+        <v>563</v>
       </c>
       <c r="G22" s="197" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="250"/>
+      <c r="A23" s="254"/>
       <c r="B23" s="108" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
+        <v>333</v>
+      </c>
+      <c r="E23" s="109" t="s">
+        <v>487</v>
+      </c>
+      <c r="F23" s="108" t="s">
         <v>334</v>
-      </c>
-      <c r="E23" s="109" t="s">
-        <v>489</v>
-      </c>
-      <c r="F23" s="108" t="s">
-        <v>335</v>
       </c>
       <c r="G23" s="198" t="s">
         <v>328</v>
@@ -42297,8 +42307,8 @@
       <c r="H23" s="127"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="251" t="s">
-        <v>516</v>
+      <c r="A24" s="255" t="s">
+        <v>513</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
@@ -42310,26 +42320,26 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="252"/>
+      <c r="A25" s="256"/>
       <c r="B25" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C25" s="117"/>
       <c r="D25" s="116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E25" s="117"/>
       <c r="F25" s="116" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G25" s="201" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H25" s="130"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="248" t="s">
-        <v>339</v>
+      <c r="A26" s="252" t="s">
+        <v>338</v>
       </c>
       <c r="B26" s="121"/>
       <c r="C26" s="121"/>
@@ -42348,7 +42358,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="249"/>
+      <c r="A27" s="253"/>
       <c r="B27" s="105" t="s">
         <v>110</v>
       </c>
@@ -42357,10 +42367,10 @@
         <v>211</v>
       </c>
       <c r="E27" s="106" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G27" s="197" t="s">
         <v>43</v>
@@ -42368,7 +42378,7 @@
       <c r="H27" s="126"/>
     </row>
     <row r="28" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="249"/>
+      <c r="A28" s="253"/>
       <c r="B28" s="105" t="s">
         <v>118</v>
       </c>
@@ -42377,10 +42387,10 @@
         <v>211</v>
       </c>
       <c r="E28" s="106" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G28" s="197" t="s">
         <v>43</v>
@@ -42388,7 +42398,7 @@
       <c r="H28" s="126"/>
     </row>
     <row r="29" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="249"/>
+      <c r="A29" s="253"/>
       <c r="B29" s="105" t="s">
         <v>122</v>
       </c>
@@ -42397,10 +42407,10 @@
         <v>211</v>
       </c>
       <c r="E29" s="106" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F29" s="105" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G29" s="197" t="s">
         <v>43</v>
@@ -42408,7 +42418,7 @@
       <c r="H29" s="126"/>
     </row>
     <row r="30" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="249"/>
+      <c r="A30" s="253"/>
       <c r="B30" s="105" t="s">
         <v>126</v>
       </c>
@@ -42417,10 +42427,10 @@
         <v>211</v>
       </c>
       <c r="E30" s="106" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G30" s="197" t="s">
         <v>43</v>
@@ -42428,7 +42438,7 @@
       <c r="H30" s="126"/>
     </row>
     <row r="31" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="250"/>
+      <c r="A31" s="254"/>
       <c r="B31" s="108" t="s">
         <v>130</v>
       </c>
@@ -42437,10 +42447,10 @@
         <v>211</v>
       </c>
       <c r="E31" s="109" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F31" s="108" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G31" s="198" t="s">
         <v>43</v>
@@ -42448,8 +42458,8 @@
       <c r="H31" s="127"/>
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="251" t="s">
-        <v>345</v>
+      <c r="A32" s="255" t="s">
+        <v>344</v>
       </c>
       <c r="B32" s="123"/>
       <c r="C32" s="123"/>
@@ -42461,7 +42471,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="89.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="253"/>
+      <c r="A33" s="257"/>
       <c r="B33" s="113" t="s">
         <v>134</v>
       </c>
@@ -42470,43 +42480,61 @@
         <v>211</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>488</v>
+        <v>566</v>
       </c>
       <c r="F33" s="113" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G33" s="200" t="s">
         <v>43</v>
       </c>
       <c r="H33" s="129"/>
     </row>
-    <row r="34" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="252"/>
-      <c r="B34" s="116" t="s">
+    <row r="34" spans="1:8" ht="89.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="257"/>
+      <c r="B34" s="113" t="s">
+        <v>564</v>
+      </c>
+      <c r="C34" s="227"/>
+      <c r="D34" s="226" t="s">
+        <v>319</v>
+      </c>
+      <c r="E34" s="114" t="s">
+        <v>565</v>
+      </c>
+      <c r="F34" s="226"/>
+      <c r="G34" s="228" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="261"/>
+    </row>
+    <row r="35" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="256"/>
+      <c r="B35" s="116" t="s">
+        <v>345</v>
+      </c>
+      <c r="C35" s="117"/>
+      <c r="D35" s="116" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" s="117"/>
+      <c r="F35" s="116" t="s">
         <v>346</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="116" t="s">
-        <v>211</v>
-      </c>
-      <c r="E34" s="117"/>
-      <c r="F34" s="116" t="s">
-        <v>347</v>
-      </c>
-      <c r="G34" s="201" t="s">
+      <c r="G35" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="130"/>
+      <c r="H35" s="130"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="9">
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:A13"/>
@@ -42550,16 +42578,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -42588,8 +42616,8 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
-        <v>517</v>
+      <c r="A3" s="239" t="s">
+        <v>514</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -42615,7 +42643,7 @@
       <c r="AMJ3" s="134"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="236"/>
+      <c r="A4" s="240"/>
       <c r="B4" s="106" t="s">
         <v>207</v>
       </c>
@@ -42627,15 +42655,15 @@
         <v>258</v>
       </c>
       <c r="F4" s="136" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="137"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="236"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="106" t="s">
         <v>260</v>
       </c>
@@ -42650,12 +42678,12 @@
         <v>263</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H5" s="137"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="236"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="106" t="s">
         <v>213</v>
       </c>
@@ -42667,13 +42695,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="136" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="137"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="236"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="106" t="s">
         <v>266</v>
       </c>
@@ -42688,12 +42716,12 @@
         <v>268</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H7" s="137"/>
     </row>
     <row r="8" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="236"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="106" t="s">
         <v>269</v>
       </c>
@@ -42705,15 +42733,15 @@
         <v>270</v>
       </c>
       <c r="F8" s="136" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G8" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H8" s="137"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="236"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="106" t="s">
         <v>272</v>
       </c>
@@ -42722,18 +42750,18 @@
         <v>208</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F9" s="136" t="s">
         <v>275</v>
       </c>
       <c r="G9" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H9" s="137"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="236"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="106" t="s">
         <v>210</v>
       </c>
@@ -42742,16 +42770,16 @@
         <v>276</v>
       </c>
       <c r="E10" s="106" t="s">
+        <v>351</v>
+      </c>
+      <c r="F10" s="136" t="s">
         <v>352</v>
-      </c>
-      <c r="F10" s="136" t="s">
-        <v>353</v>
       </c>
       <c r="G10" s="197"/>
       <c r="H10" s="137"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="236"/>
+      <c r="A11" s="240"/>
       <c r="B11" s="106" t="s">
         <v>279</v>
       </c>
@@ -42763,37 +42791,37 @@
         <v>280</v>
       </c>
       <c r="F11" s="136" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G11" s="197"/>
       <c r="H11" s="137"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="236"/>
+      <c r="A12" s="240"/>
       <c r="B12" s="106" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="136" t="s">
         <v>208</v>
       </c>
       <c r="E12" s="106" t="s">
+        <v>355</v>
+      </c>
+      <c r="F12" s="136" t="s">
         <v>356</v>
-      </c>
-      <c r="F12" s="136" t="s">
-        <v>357</v>
       </c>
       <c r="G12" s="197"/>
       <c r="H12" s="137"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="236"/>
+      <c r="A13" s="240"/>
       <c r="B13" s="106" t="s">
         <v>285</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="136" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E13" s="106" t="s">
         <v>287</v>
@@ -42805,63 +42833,63 @@
       <c r="H13" s="137"/>
     </row>
     <row r="14" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="236"/>
+      <c r="A14" s="240"/>
       <c r="B14" s="106" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="136" t="s">
         <v>208</v>
       </c>
       <c r="E14" s="136" t="s">
+        <v>359</v>
+      </c>
+      <c r="F14" s="136" t="s">
         <v>360</v>
-      </c>
-      <c r="F14" s="136" t="s">
-        <v>361</v>
       </c>
       <c r="G14" s="197"/>
       <c r="H14" s="137"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="236"/>
+      <c r="A15" s="240"/>
       <c r="B15" s="106" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="136" t="s">
         <v>208</v>
       </c>
       <c r="E15" s="136" t="s">
+        <v>362</v>
+      </c>
+      <c r="F15" s="136" t="s">
         <v>363</v>
-      </c>
-      <c r="F15" s="136" t="s">
-        <v>364</v>
       </c>
       <c r="G15" s="197"/>
       <c r="H15" s="137"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="236"/>
+      <c r="A16" s="240"/>
       <c r="B16" s="106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="136" t="s">
+        <v>365</v>
+      </c>
+      <c r="E16" s="136" t="s">
         <v>366</v>
       </c>
-      <c r="E16" s="136" t="s">
+      <c r="F16" s="136" t="s">
         <v>367</v>
-      </c>
-      <c r="F16" s="136" t="s">
-        <v>368</v>
       </c>
       <c r="G16" s="197"/>
       <c r="H16" s="137"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="236"/>
+      <c r="A17" s="240"/>
       <c r="B17" s="106" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
@@ -42871,13 +42899,13 @@
         <v>12</v>
       </c>
       <c r="F17" s="136" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G17" s="197"/>
       <c r="H17" s="137"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="237"/>
+      <c r="A18" s="241"/>
       <c r="B18" s="109" t="s">
         <v>302</v>
       </c>
@@ -42886,7 +42914,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="109" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F18" s="138" t="s">
         <v>304</v>
@@ -42938,16 +42966,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>504</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>501</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -42976,8 +43004,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="254" t="s">
-        <v>517</v>
+      <c r="A3" s="258" t="s">
+        <v>514</v>
       </c>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
@@ -42988,7 +43016,7 @@
       <c r="H3" s="143"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="255"/>
+      <c r="A4" s="259"/>
       <c r="B4" s="106" t="s">
         <v>207</v>
       </c>
@@ -43003,7 +43031,7 @@
         <v>259</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="145"/>
       <c r="I4" s="144"/>
@@ -43017,7 +43045,7 @@
       <c r="Q4" s="144"/>
     </row>
     <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="255"/>
+      <c r="A5" s="259"/>
       <c r="B5" s="106" t="s">
         <v>260</v>
       </c>
@@ -43032,7 +43060,7 @@
         <v>263</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H5" s="145"/>
       <c r="I5" s="144"/>
@@ -43046,7 +43074,7 @@
       <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="255"/>
+      <c r="A6" s="259"/>
       <c r="B6" s="106" t="s">
         <v>213</v>
       </c>
@@ -43073,7 +43101,7 @@
       <c r="Q6" s="144"/>
     </row>
     <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="255"/>
+      <c r="A7" s="259"/>
       <c r="B7" s="106" t="s">
         <v>266</v>
       </c>
@@ -43088,7 +43116,7 @@
         <v>268</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="144"/>
@@ -43102,7 +43130,7 @@
       <c r="Q7" s="144"/>
     </row>
     <row r="8" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="255"/>
+      <c r="A8" s="259"/>
       <c r="B8" s="106" t="s">
         <v>269</v>
       </c>
@@ -43117,7 +43145,7 @@
         <v>271</v>
       </c>
       <c r="G8" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H8" s="145"/>
       <c r="I8" s="144"/>
@@ -43131,7 +43159,7 @@
       <c r="Q8" s="144"/>
     </row>
     <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="255"/>
+      <c r="A9" s="259"/>
       <c r="B9" s="106" t="s">
         <v>272</v>
       </c>
@@ -43146,7 +43174,7 @@
         <v>275</v>
       </c>
       <c r="G9" s="197" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H9" s="149"/>
       <c r="I9" s="144"/>
@@ -43160,7 +43188,7 @@
       <c r="Q9" s="144"/>
     </row>
     <row r="10" spans="1:17" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="255"/>
+      <c r="A10" s="259"/>
       <c r="B10" s="106" t="s">
         <v>210</v>
       </c>
@@ -43187,7 +43215,7 @@
       <c r="Q10" s="144"/>
     </row>
     <row r="11" spans="1:17" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="255"/>
+      <c r="A11" s="259"/>
       <c r="B11" s="106" t="s">
         <v>279</v>
       </c>
@@ -43214,7 +43242,7 @@
       <c r="Q11" s="144"/>
     </row>
     <row r="12" spans="1:17" s="151" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="255"/>
+      <c r="A12" s="259"/>
       <c r="B12" s="106" t="s">
         <v>282</v>
       </c>
@@ -43241,7 +43269,7 @@
       <c r="Q12" s="144"/>
     </row>
     <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="255"/>
+      <c r="A13" s="259"/>
       <c r="B13" s="106" t="s">
         <v>285</v>
       </c>
@@ -43268,7 +43296,7 @@
       <c r="Q13" s="144"/>
     </row>
     <row r="14" spans="1:17" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="255"/>
+      <c r="A14" s="259"/>
       <c r="B14" s="106" t="s">
         <v>289</v>
       </c>
@@ -43295,7 +43323,7 @@
       <c r="Q14" s="144"/>
     </row>
     <row r="15" spans="1:17" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="255"/>
+      <c r="A15" s="259"/>
       <c r="B15" s="106" t="s">
         <v>292</v>
       </c>
@@ -43322,13 +43350,13 @@
       <c r="Q15" s="144"/>
     </row>
     <row r="16" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="255"/>
+      <c r="A16" s="259"/>
       <c r="B16" s="106" t="s">
         <v>295</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="105" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E16" s="136" t="s">
         <v>296</v>
@@ -43349,7 +43377,7 @@
       <c r="Q16" s="144"/>
     </row>
     <row r="17" spans="1:17" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="255"/>
+      <c r="A17" s="259"/>
       <c r="B17" s="106" t="s">
         <v>298</v>
       </c>
@@ -43376,7 +43404,7 @@
       <c r="Q17" s="144"/>
     </row>
     <row r="18" spans="1:17" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="256"/>
+      <c r="A18" s="260"/>
       <c r="B18" s="109" t="s">
         <v>302</v>
       </c>
@@ -43444,16 +43472,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>505</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>502</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -43482,7 +43510,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="239" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="154"/>
@@ -43506,7 +43534,7 @@
       <c r="T3" s="156"/>
     </row>
     <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="236"/>
+      <c r="A4" s="240"/>
       <c r="B4" s="158" t="s">
         <v>8</v>
       </c>
@@ -43516,15 +43544,15 @@
       </c>
       <c r="E4" s="158"/>
       <c r="F4" s="158" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H4" s="159"/>
     </row>
     <row r="5" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="236"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="158" t="s">
         <v>13</v>
       </c>
@@ -43534,7 +43562,7 @@
       </c>
       <c r="E5" s="158"/>
       <c r="F5" s="158" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G5" s="183" t="s">
         <v>12</v>
@@ -43542,7 +43570,7 @@
       <c r="H5" s="159"/>
     </row>
     <row r="6" spans="1:20" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="236"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="158" t="s">
         <v>16</v>
       </c>
@@ -43552,7 +43580,7 @@
       </c>
       <c r="E6" s="158"/>
       <c r="F6" s="158" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G6" s="183" t="s">
         <v>12</v>
@@ -43560,25 +43588,25 @@
       <c r="H6" s="159"/>
     </row>
     <row r="7" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="237"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="160" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="160"/>
       <c r="D7" s="160" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E7" s="160"/>
       <c r="F7" s="160" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G7" s="184" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="238" t="s">
+      <c r="A8" s="236" t="s">
         <v>295</v>
       </c>
       <c r="B8" s="162"/>
@@ -43590,17 +43618,17 @@
       <c r="H8" s="163"/>
     </row>
     <row r="9" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="239"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="164" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E9" s="164"/>
       <c r="F9" s="164" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G9" s="214" t="s">
         <v>12</v>
@@ -43608,136 +43636,136 @@
       <c r="H9" s="165"/>
     </row>
     <row r="10" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="239"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C10" s="164"/>
       <c r="D10" s="164" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E10" s="164"/>
       <c r="F10" s="164" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="G10" s="186"/>
       <c r="H10" s="165"/>
     </row>
     <row r="11" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="239"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D11" s="164" t="s">
         <v>208</v>
       </c>
       <c r="E11" s="164"/>
       <c r="F11" s="164" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="G11" s="186"/>
       <c r="H11" s="165"/>
     </row>
     <row r="12" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="239"/>
+      <c r="A12" s="237"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D12" s="164" t="s">
         <v>208</v>
       </c>
       <c r="E12" s="164"/>
       <c r="F12" s="164" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="G12" s="186"/>
       <c r="H12" s="165"/>
     </row>
     <row r="13" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="239"/>
+      <c r="A13" s="237"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D13" s="164" t="s">
         <v>208</v>
       </c>
       <c r="E13" s="164"/>
       <c r="F13" s="164" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="G13" s="186"/>
       <c r="H13" s="165"/>
     </row>
     <row r="14" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="239"/>
+      <c r="A14" s="237"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D14" s="164" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E14" s="164"/>
       <c r="F14" s="164" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G14" s="186"/>
       <c r="H14" s="165"/>
     </row>
     <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="239"/>
+      <c r="A15" s="237"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D15" s="164" t="s">
         <v>319</v>
       </c>
       <c r="E15" s="164"/>
       <c r="F15" s="164" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G15" s="186"/>
       <c r="H15" s="165"/>
     </row>
     <row r="16" spans="1:20" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="239"/>
+      <c r="A16" s="237"/>
       <c r="B16" s="164" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C16" s="164"/>
       <c r="D16" s="164" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E16" s="164"/>
       <c r="F16" s="164" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="G16" s="186"/>
       <c r="H16" s="165"/>
     </row>
     <row r="17" spans="1:19" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="240"/>
+      <c r="A17" s="238"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D17" s="166" t="s">
         <v>319</v>
       </c>
       <c r="E17" s="166"/>
       <c r="F17" s="166" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G17" s="187"/>
       <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:19" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="241" t="s">
-        <v>389</v>
+      <c r="A18" s="239" t="s">
+        <v>388</v>
       </c>
       <c r="B18" s="168"/>
       <c r="C18" s="168"/>
@@ -43759,17 +43787,17 @@
       <c r="S18" s="156"/>
     </row>
     <row r="19" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="236"/>
+      <c r="A19" s="240"/>
       <c r="B19" s="158" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C19" s="158"/>
       <c r="D19" s="158" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E19" s="158"/>
       <c r="F19" s="158" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G19" s="183" t="s">
         <v>43</v>
@@ -43777,49 +43805,49 @@
       <c r="H19" s="159"/>
     </row>
     <row r="20" spans="1:19" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="236"/>
+      <c r="A20" s="240"/>
       <c r="B20" s="158"/>
       <c r="C20" s="158" t="s">
+        <v>390</v>
+      </c>
+      <c r="D20" s="158" t="s">
         <v>391</v>
-      </c>
-      <c r="D20" s="158" t="s">
-        <v>392</v>
       </c>
       <c r="E20" s="158"/>
       <c r="F20" s="158" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G20" s="183"/>
       <c r="H20" s="159"/>
     </row>
     <row r="21" spans="1:19" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="236"/>
+      <c r="A21" s="240"/>
       <c r="B21" s="158"/>
       <c r="C21" s="158" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D21" s="158" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E21" s="158"/>
       <c r="F21" s="158" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G21" s="183"/>
       <c r="H21" s="159"/>
     </row>
     <row r="22" spans="1:19" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="237"/>
+      <c r="A22" s="241"/>
       <c r="B22" s="160"/>
       <c r="C22" s="160" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D22" s="160" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E22" s="160"/>
       <c r="F22" s="160" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G22" s="184"/>
       <c r="H22" s="161"/>
@@ -43867,16 +43895,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>506</v>
-      </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="242" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -44921,8 +44949,8 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="241" t="s">
-        <v>398</v>
+      <c r="A3" s="239" t="s">
+        <v>397</v>
       </c>
       <c r="B3" s="172"/>
       <c r="C3" s="172"/>
@@ -44933,7 +44961,7 @@
       <c r="H3" s="173"/>
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="236"/>
+      <c r="A4" s="240"/>
       <c r="B4" s="47" t="s">
         <v>207</v>
       </c>
@@ -44943,7 +44971,7 @@
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="158" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="159"/>
@@ -45965,7 +45993,7 @@
       <c r="AMJ4" s="23"/>
     </row>
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="236"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="47" t="s">
         <v>260</v>
       </c>
@@ -46997,7 +47025,7 @@
       <c r="AMJ5" s="23"/>
     </row>
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="236"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="47" t="s">
         <v>213</v>
       </c>
@@ -47007,7 +47035,7 @@
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="158" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="174"/>
@@ -48029,9 +48057,9 @@
       <c r="AMJ6" s="23"/>
     </row>
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="236"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C7" s="158"/>
       <c r="D7" s="47" t="s">
@@ -48039,7 +48067,7 @@
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="158" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="159"/>
@@ -49061,9 +49089,9 @@
       <c r="AMJ7" s="23"/>
     </row>
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="236"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C8" s="158"/>
       <c r="D8" s="47" t="s">
@@ -49071,7 +49099,7 @@
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="158" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="159"/>
@@ -50093,17 +50121,17 @@
       <c r="AMJ8" s="23"/>
     </row>
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="236"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C9" s="158"/>
       <c r="D9" s="47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="158" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G9" s="47"/>
       <c r="H9" s="159"/>
@@ -51125,9 +51153,9 @@
       <c r="AMJ9" s="23"/>
     </row>
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="236"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C10" s="158"/>
       <c r="D10" s="47" t="s">
@@ -51135,7 +51163,7 @@
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="158" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="159"/>
@@ -52157,17 +52185,17 @@
       <c r="AMJ10" s="23"/>
     </row>
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="236"/>
+      <c r="A11" s="240"/>
       <c r="B11" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C11" s="158"/>
       <c r="D11" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="158" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="159"/>
@@ -53189,9 +53217,9 @@
       <c r="AMJ11" s="23"/>
     </row>
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="237"/>
+      <c r="A12" s="241"/>
       <c r="B12" s="51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C12" s="160"/>
       <c r="D12" s="51" t="s">
@@ -53199,7 +53227,7 @@
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="160" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G12" s="51"/>
       <c r="H12" s="161"/>
@@ -54221,8 +54249,8 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="238" t="s">
-        <v>413</v>
+      <c r="A13" s="236" t="s">
+        <v>412</v>
       </c>
       <c r="B13" s="175"/>
       <c r="C13" s="175"/>
@@ -54234,7 +54262,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="239"/>
+      <c r="A14" s="237"/>
       <c r="B14" s="69" t="s">
         <v>207</v>
       </c>
@@ -54244,13 +54272,13 @@
       </c>
       <c r="E14" s="69"/>
       <c r="F14" s="69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G14" s="69"/>
       <c r="H14" s="177"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="239"/>
+      <c r="A15" s="237"/>
       <c r="B15" s="69" t="s">
         <v>260</v>
       </c>
@@ -54266,7 +54294,7 @@
       <c r="H15" s="177"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="239"/>
+      <c r="A16" s="237"/>
       <c r="B16" s="69" t="s">
         <v>213</v>
       </c>
@@ -54276,13 +54304,13 @@
       </c>
       <c r="E16" s="69"/>
       <c r="F16" s="69" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G16" s="69"/>
       <c r="H16" s="177"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="239"/>
+      <c r="A17" s="237"/>
       <c r="B17" s="69" t="s">
         <v>266</v>
       </c>
@@ -54292,13 +54320,13 @@
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="69" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="177"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="239"/>
+      <c r="A18" s="237"/>
       <c r="B18" s="69" t="s">
         <v>210</v>
       </c>
@@ -54308,13 +54336,13 @@
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="69" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G18" s="69"/>
       <c r="H18" s="177"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="239"/>
+      <c r="A19" s="237"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -54324,29 +54352,29 @@
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="69" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G19" s="69"/>
       <c r="H19" s="177"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="239"/>
+      <c r="A20" s="237"/>
       <c r="B20" s="69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="69" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G20" s="69"/>
       <c r="H20" s="177"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="239"/>
+      <c r="A21" s="237"/>
       <c r="B21" s="69" t="s">
         <v>319</v>
       </c>
@@ -54356,15 +54384,15 @@
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="69" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G21" s="69"/>
       <c r="H21" s="177"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="239"/>
+      <c r="A22" s="237"/>
       <c r="B22" s="69" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C22" s="69"/>
       <c r="D22" s="69" t="s">
@@ -54372,15 +54400,15 @@
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="69" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G22" s="69"/>
       <c r="H22" s="177"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="239"/>
+      <c r="A23" s="237"/>
       <c r="B23" s="69" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69" t="s">
@@ -54388,15 +54416,15 @@
       </c>
       <c r="E23" s="69"/>
       <c r="F23" s="69" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G23" s="69"/>
       <c r="H23" s="177"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="240"/>
+      <c r="A24" s="238"/>
       <c r="B24" s="73" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73" t="s">
@@ -54404,14 +54432,14 @@
       </c>
       <c r="E24" s="73"/>
       <c r="F24" s="73" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G24" s="73"/>
       <c r="H24" s="178"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="241" t="s">
-        <v>355</v>
+      <c r="A25" s="239" t="s">
+        <v>354</v>
       </c>
       <c r="B25" s="179"/>
       <c r="C25" s="179"/>
@@ -54422,7 +54450,7 @@
       <c r="H25" s="180"/>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="236"/>
+      <c r="A26" s="240"/>
       <c r="B26" s="47" t="s">
         <v>207</v>
       </c>
@@ -54432,13 +54460,13 @@
       </c>
       <c r="E26" s="47"/>
       <c r="F26" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="174"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="236"/>
+      <c r="A27" s="240"/>
       <c r="B27" s="47" t="s">
         <v>260</v>
       </c>
@@ -54454,7 +54482,7 @@
       <c r="H27" s="174"/>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="236"/>
+      <c r="A28" s="240"/>
       <c r="B28" s="47" t="s">
         <v>213</v>
       </c>
@@ -54464,13 +54492,13 @@
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="174"/>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="236"/>
+      <c r="A29" s="240"/>
       <c r="B29" s="47" t="s">
         <v>266</v>
       </c>
@@ -54480,15 +54508,15 @@
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="174"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="236"/>
+      <c r="A30" s="240"/>
       <c r="B30" s="47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47" t="s">
@@ -54496,13 +54524,13 @@
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="174"/>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="236"/>
+      <c r="A31" s="240"/>
       <c r="B31" s="47" t="s">
         <v>210</v>
       </c>
@@ -54512,31 +54540,31 @@
       </c>
       <c r="E31" s="47"/>
       <c r="F31" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="174"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="236"/>
+      <c r="A32" s="240"/>
       <c r="B32" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E32" s="47"/>
       <c r="F32" s="47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="174"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="236"/>
+      <c r="A33" s="240"/>
       <c r="B33" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="47" t="s">
@@ -54544,13 +54572,13 @@
       </c>
       <c r="E33" s="47"/>
       <c r="F33" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="174"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="236"/>
+      <c r="A34" s="240"/>
       <c r="B34" s="47" t="s">
         <v>5</v>
       </c>
@@ -54560,15 +54588,15 @@
       </c>
       <c r="E34" s="47"/>
       <c r="F34" s="47" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="174"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="236"/>
+      <c r="A35" s="240"/>
       <c r="B35" s="47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47" t="s">
@@ -54576,15 +54604,15 @@
       </c>
       <c r="E35" s="47"/>
       <c r="F35" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="174"/>
     </row>
     <row r="36" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="237"/>
+      <c r="A36" s="241"/>
       <c r="B36" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="51" t="s">
@@ -54592,13 +54620,13 @@
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G36" s="51"/>
       <c r="H36" s="181"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="238" t="s">
+      <c r="A37" s="236" t="s">
         <v>282</v>
       </c>
       <c r="B37" s="175"/>
@@ -54611,7 +54639,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="239"/>
+      <c r="A38" s="237"/>
       <c r="B38" s="69" t="s">
         <v>207</v>
       </c>
@@ -54621,13 +54649,13 @@
       </c>
       <c r="E38" s="69"/>
       <c r="F38" s="69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="177"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="239"/>
+      <c r="A39" s="237"/>
       <c r="B39" s="69" t="s">
         <v>260</v>
       </c>
@@ -54643,7 +54671,7 @@
       <c r="H39" s="177"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="239"/>
+      <c r="A40" s="237"/>
       <c r="B40" s="69" t="s">
         <v>213</v>
       </c>
@@ -54653,13 +54681,13 @@
       </c>
       <c r="E40" s="69"/>
       <c r="F40" s="69" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G40" s="69"/>
       <c r="H40" s="177"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="239"/>
+      <c r="A41" s="237"/>
       <c r="B41" s="69" t="s">
         <v>266</v>
       </c>
@@ -54669,15 +54697,15 @@
       </c>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G41" s="69"/>
       <c r="H41" s="177"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="239"/>
+      <c r="A42" s="237"/>
       <c r="B42" s="69" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="69" t="s">
@@ -54685,15 +54713,15 @@
       </c>
       <c r="E42" s="69"/>
       <c r="F42" s="69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G42" s="69"/>
       <c r="H42" s="177"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="239"/>
+      <c r="A43" s="237"/>
       <c r="B43" s="69" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C43" s="69"/>
       <c r="D43" s="69" t="s">
@@ -54701,13 +54729,13 @@
       </c>
       <c r="E43" s="69"/>
       <c r="F43" s="69" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G43" s="69"/>
       <c r="H43" s="177"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="239"/>
+      <c r="A44" s="237"/>
       <c r="B44" s="69" t="s">
         <v>210</v>
       </c>
@@ -54717,31 +54745,31 @@
       </c>
       <c r="E44" s="69"/>
       <c r="F44" s="69" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="177"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="239"/>
+      <c r="A45" s="237"/>
       <c r="B45" s="69" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C45" s="69"/>
       <c r="D45" s="69" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E45" s="69"/>
       <c r="F45" s="69" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G45" s="69"/>
       <c r="H45" s="177"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="239"/>
+      <c r="A46" s="237"/>
       <c r="B46" s="69" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="69" t="s">
@@ -54749,13 +54777,13 @@
       </c>
       <c r="E46" s="69"/>
       <c r="F46" s="69" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G46" s="69"/>
       <c r="H46" s="177"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="239"/>
+      <c r="A47" s="237"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -54765,15 +54793,15 @@
       </c>
       <c r="E47" s="69"/>
       <c r="F47" s="69" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G47" s="69"/>
       <c r="H47" s="177"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="240"/>
+      <c r="A48" s="238"/>
       <c r="B48" s="73" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="73" t="s">
@@ -54781,7 +54809,7 @@
       </c>
       <c r="E48" s="73"/>
       <c r="F48" s="73" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G48" s="73"/>
       <c r="H48" s="178"/>

</xml_diff>

<commit_message>
fix: more info on data_source_mapping
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahajnal/Documents/github/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9522CA-23D0-FB4D-9099-EFF84BE7E171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CA294C-C57D-4AA1-ABB1-366C51C7DACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="500" windowWidth="28360" windowHeight="14020" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Deployment" sheetId="7" r:id="rId7"/>
     <sheet name="Supporting Metadata" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1670,9 +1669,6 @@
     <t>Connection data for a bring-your-own edge</t>
   </si>
   <si>
-    <t>Mapping Microservices to Data assets, as available in the DMA Tuple</t>
-  </si>
-  <si>
     <t>PROVIDER</t>
   </si>
   <si>
@@ -1815,6 +1811,9 @@
   </si>
   <si>
     <t xml:space="preserve">database schema description/contents </t>
+  </si>
+  <si>
+    <t>Mapping the available Data assets in this DMA Tuple to available Microservices. One Microservice may require several Data assets, specified by their UUIDs.</t>
   </si>
 </sst>
 </file>
@@ -3214,6 +3213,10 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3336,10 +3339,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4175,40 +4174,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A11"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="2" customWidth="1"/>
     <col min="9" max="1024" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1025" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>496</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -4234,8 +4233,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="244" t="s">
+    <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="245" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4246,8 +4245,8 @@
       <c r="G3" s="182"/>
       <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="245"/>
+    <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="246"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4266,8 +4265,8 @@
       </c>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="245"/>
+    <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="246"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4286,8 +4285,8 @@
       </c>
       <c r="H5" s="50"/>
     </row>
-    <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="245"/>
+    <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="246"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4306,8 +4305,8 @@
       </c>
       <c r="H6" s="50"/>
     </row>
-    <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="245"/>
+    <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="246"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4326,8 +4325,8 @@
       </c>
       <c r="H7" s="50"/>
     </row>
-    <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="245"/>
+    <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="246"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4346,8 +4345,8 @@
       </c>
       <c r="H8" s="50"/>
     </row>
-    <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="245"/>
+    <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="246"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4366,8 +4365,8 @@
       </c>
       <c r="H9" s="50"/>
     </row>
-    <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+    <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="246"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4386,8 +4385,8 @@
       </c>
       <c r="H10" s="50"/>
     </row>
-    <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246"/>
+    <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="247"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4406,8 +4405,8 @@
       </c>
       <c r="H11" s="54"/>
     </row>
-    <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="247" t="s">
+    <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="248" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="217"/>
@@ -4418,8 +4417,8 @@
       <c r="G12" s="219"/>
       <c r="H12" s="220"/>
     </row>
-    <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="248"/>
+    <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="249"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4438,8 +4437,8 @@
       </c>
       <c r="H13" s="58"/>
     </row>
-    <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="248"/>
+    <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="249"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4458,8 +4457,8 @@
       </c>
       <c r="H14" s="58"/>
     </row>
-    <row r="15" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="248"/>
+    <row r="15" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="249"/>
       <c r="B15" s="55" t="s">
         <v>466</v>
       </c>
@@ -5494,8 +5493,8 @@
       <c r="AMI15" s="4"/>
       <c r="AMJ15" s="4"/>
     </row>
-    <row r="16" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="248"/>
+    <row r="16" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="249"/>
       <c r="B16" s="55" t="s">
         <v>459</v>
       </c>
@@ -6530,8 +6529,8 @@
       <c r="AMI16" s="4"/>
       <c r="AMJ16" s="4"/>
     </row>
-    <row r="17" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249"/>
+    <row r="17" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="250"/>
       <c r="B17" s="221" t="s">
         <v>460</v>
       </c>
@@ -7566,8 +7565,8 @@
       <c r="AMI17" s="4"/>
       <c r="AMJ17" s="4"/>
     </row>
-    <row r="18" spans="1:1024" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="240" t="s">
+    <row r="18" spans="1:1024" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="241" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="59"/>
@@ -7578,8 +7577,8 @@
       <c r="G18" s="189"/>
       <c r="H18" s="61"/>
     </row>
-    <row r="19" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="240"/>
+    <row r="19" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="241"/>
       <c r="B19" s="47" t="s">
         <v>40</v>
       </c>
@@ -7598,8 +7597,8 @@
       </c>
       <c r="H19" s="50"/>
     </row>
-    <row r="20" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="240"/>
+    <row r="20" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="241"/>
       <c r="B20" s="47" t="s">
         <v>44</v>
       </c>
@@ -7618,8 +7617,8 @@
       </c>
       <c r="H20" s="50"/>
     </row>
-    <row r="21" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="240"/>
+    <row r="21" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="241"/>
       <c r="B21" s="47" t="s">
         <v>46</v>
       </c>
@@ -7638,8 +7637,8 @@
       </c>
       <c r="H21" s="50"/>
     </row>
-    <row r="22" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="240"/>
+    <row r="22" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="241"/>
       <c r="B22" s="47" t="s">
         <v>48</v>
       </c>
@@ -7658,8 +7657,8 @@
       </c>
       <c r="H22" s="50"/>
     </row>
-    <row r="23" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="240"/>
+    <row r="23" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="241"/>
       <c r="B23" s="47" t="s">
         <v>50</v>
       </c>
@@ -7678,8 +7677,8 @@
       </c>
       <c r="H23" s="50"/>
     </row>
-    <row r="24" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="240"/>
+    <row r="24" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="241"/>
       <c r="B24" s="47" t="s">
         <v>53</v>
       </c>
@@ -7698,8 +7697,8 @@
       </c>
       <c r="H24" s="50"/>
     </row>
-    <row r="25" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="240"/>
+    <row r="25" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
+      <c r="A25" s="241"/>
       <c r="B25" s="47" t="s">
         <v>57</v>
       </c>
@@ -7718,8 +7717,8 @@
       </c>
       <c r="H25" s="50"/>
     </row>
-    <row r="26" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="240"/>
+    <row r="26" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="241"/>
       <c r="B26" s="47" t="s">
         <v>61</v>
       </c>
@@ -7738,8 +7737,8 @@
       </c>
       <c r="H26" s="50"/>
     </row>
-    <row r="27" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="240"/>
+    <row r="27" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="241"/>
       <c r="B27" s="47" t="s">
         <v>63</v>
       </c>
@@ -7758,8 +7757,8 @@
       </c>
       <c r="H27" s="50"/>
     </row>
-    <row r="28" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="240"/>
+    <row r="28" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="241"/>
       <c r="B28" s="47" t="s">
         <v>65</v>
       </c>
@@ -7778,8 +7777,8 @@
       </c>
       <c r="H28" s="50"/>
     </row>
-    <row r="29" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="240"/>
+    <row r="29" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="241"/>
       <c r="B29" s="47" t="s">
         <v>67</v>
       </c>
@@ -7798,8 +7797,8 @@
       </c>
       <c r="H29" s="50"/>
     </row>
-    <row r="30" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="241"/>
+    <row r="30" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="242"/>
       <c r="B30" s="51" t="s">
         <v>69</v>
       </c>
@@ -7818,8 +7817,8 @@
       </c>
       <c r="H30" s="54"/>
     </row>
-    <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="236" t="s">
+    <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="237" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="62"/>
@@ -7830,8 +7829,8 @@
       <c r="G31" s="190"/>
       <c r="H31" s="64"/>
     </row>
-    <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="237"/>
+    <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="238"/>
       <c r="B32" s="65" t="s">
         <v>73</v>
       </c>
@@ -7850,8 +7849,8 @@
       </c>
       <c r="H32" s="68"/>
     </row>
-    <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="237"/>
+    <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="238"/>
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -7870,8 +7869,8 @@
       </c>
       <c r="H33" s="72"/>
     </row>
-    <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="237"/>
+    <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="238"/>
       <c r="B34" s="69" t="s">
         <v>79</v>
       </c>
@@ -7890,8 +7889,8 @@
       </c>
       <c r="H34" s="72"/>
     </row>
-    <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="238"/>
+    <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="239"/>
       <c r="B35" s="73" t="s">
         <v>82</v>
       </c>
@@ -7910,8 +7909,8 @@
       </c>
       <c r="H35" s="76"/>
     </row>
-    <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="239" t="s">
+    <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="240" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="59"/>
@@ -7922,8 +7921,8 @@
       <c r="G36" s="189"/>
       <c r="H36" s="61"/>
     </row>
-    <row r="37" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="240"/>
+    <row r="37" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="241"/>
       <c r="B37" s="47" t="s">
         <v>86</v>
       </c>
@@ -8958,9 +8957,9 @@
       <c r="AMI37" s="4"/>
       <c r="AMJ37" s="4"/>
     </row>
-    <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="240"/>
-      <c r="B38" s="230" t="s">
+    <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="241"/>
+      <c r="B38" s="231" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -9996,9 +9995,9 @@
       <c r="AMI38" s="4"/>
       <c r="AMJ38" s="4"/>
     </row>
-    <row r="39" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="240"/>
-      <c r="B39" s="230"/>
+    <row r="39" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="241"/>
+      <c r="B39" s="231"/>
       <c r="C39" s="47" t="s">
         <v>94</v>
       </c>
@@ -11032,9 +11031,9 @@
       <c r="AMI39" s="4"/>
       <c r="AMJ39" s="4"/>
     </row>
-    <row r="40" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="240"/>
-      <c r="B40" s="230"/>
+    <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="241"/>
+      <c r="B40" s="231"/>
       <c r="C40" s="47" t="s">
         <v>98</v>
       </c>
@@ -12068,9 +12067,9 @@
       <c r="AMI40" s="4"/>
       <c r="AMJ40" s="4"/>
     </row>
-    <row r="41" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A41" s="240"/>
-      <c r="B41" s="230"/>
+    <row r="41" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="241"/>
+      <c r="B41" s="231"/>
       <c r="C41" s="47" t="s">
         <v>102</v>
       </c>
@@ -13104,9 +13103,9 @@
       <c r="AMI41" s="4"/>
       <c r="AMJ41" s="4"/>
     </row>
-    <row r="42" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="240"/>
-      <c r="B42" s="230"/>
+    <row r="42" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="241"/>
+      <c r="B42" s="231"/>
       <c r="C42" s="47" t="s">
         <v>106</v>
       </c>
@@ -14140,9 +14139,9 @@
       <c r="AMI42" s="4"/>
       <c r="AMJ42" s="4"/>
     </row>
-    <row r="43" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="240"/>
-      <c r="B43" s="230"/>
+    <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="241"/>
+      <c r="B43" s="231"/>
       <c r="C43" s="47" t="s">
         <v>110</v>
       </c>
@@ -15176,9 +15175,9 @@
       <c r="AMI43" s="4"/>
       <c r="AMJ43" s="4"/>
     </row>
-    <row r="44" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="240"/>
-      <c r="B44" s="230"/>
+    <row r="44" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="241"/>
+      <c r="B44" s="231"/>
       <c r="C44" s="47" t="s">
         <v>114</v>
       </c>
@@ -16212,9 +16211,9 @@
       <c r="AMI44" s="4"/>
       <c r="AMJ44" s="4"/>
     </row>
-    <row r="45" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="240"/>
-      <c r="B45" s="230"/>
+    <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="241"/>
+      <c r="B45" s="231"/>
       <c r="C45" s="47" t="s">
         <v>118</v>
       </c>
@@ -17248,9 +17247,9 @@
       <c r="AMI45" s="4"/>
       <c r="AMJ45" s="4"/>
     </row>
-    <row r="46" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="240"/>
-      <c r="B46" s="230"/>
+    <row r="46" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="241"/>
+      <c r="B46" s="231"/>
       <c r="C46" s="47" t="s">
         <v>122</v>
       </c>
@@ -18284,9 +18283,9 @@
       <c r="AMI46" s="4"/>
       <c r="AMJ46" s="4"/>
     </row>
-    <row r="47" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="240"/>
-      <c r="B47" s="230"/>
+    <row r="47" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="241"/>
+      <c r="B47" s="231"/>
       <c r="C47" s="47" t="s">
         <v>126</v>
       </c>
@@ -19320,9 +19319,9 @@
       <c r="AMI47" s="4"/>
       <c r="AMJ47" s="4"/>
     </row>
-    <row r="48" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="240"/>
-      <c r="B48" s="230"/>
+    <row r="48" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="241"/>
+      <c r="B48" s="231"/>
       <c r="C48" s="47" t="s">
         <v>130</v>
       </c>
@@ -20356,9 +20355,9 @@
       <c r="AMI48" s="4"/>
       <c r="AMJ48" s="4"/>
     </row>
-    <row r="49" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="241"/>
-      <c r="B49" s="231"/>
+    <row r="49" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="242"/>
+      <c r="B49" s="232"/>
       <c r="C49" s="51" t="s">
         <v>134</v>
       </c>
@@ -21392,8 +21391,8 @@
       <c r="AMI49" s="15"/>
       <c r="AMJ49" s="15"/>
     </row>
-    <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="236" t="s">
+    <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="237" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="77"/>
@@ -21404,8 +21403,8 @@
       <c r="G50" s="192"/>
       <c r="H50" s="79"/>
     </row>
-    <row r="51" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="237"/>
+    <row r="51" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="238"/>
       <c r="B51" s="80" t="s">
         <v>138</v>
       </c>
@@ -21424,9 +21423,9 @@
       </c>
       <c r="H51" s="83"/>
     </row>
-    <row r="52" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="237"/>
-      <c r="B52" s="232" t="s">
+    <row r="52" spans="1:1024" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="238"/>
+      <c r="B52" s="233" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
@@ -21446,9 +21445,9 @@
       </c>
       <c r="H52" s="83"/>
     </row>
-    <row r="53" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="237"/>
-      <c r="B53" s="232"/>
+    <row r="53" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
+      <c r="A53" s="238"/>
+      <c r="B53" s="233"/>
       <c r="C53" s="80" t="s">
         <v>94</v>
       </c>
@@ -21466,9 +21465,9 @@
       </c>
       <c r="H53" s="83"/>
     </row>
-    <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="237"/>
-      <c r="B54" s="232"/>
+    <row r="54" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="238"/>
+      <c r="B54" s="233"/>
       <c r="C54" s="80" t="s">
         <v>98</v>
       </c>
@@ -21486,9 +21485,9 @@
       </c>
       <c r="H54" s="83"/>
     </row>
-    <row r="55" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A55" s="237"/>
-      <c r="B55" s="232"/>
+    <row r="55" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="238"/>
+      <c r="B55" s="233"/>
       <c r="C55" s="80" t="s">
         <v>102</v>
       </c>
@@ -21506,9 +21505,9 @@
       </c>
       <c r="H55" s="83"/>
     </row>
-    <row r="56" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="237"/>
-      <c r="B56" s="232"/>
+    <row r="56" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="238"/>
+      <c r="B56" s="233"/>
       <c r="C56" s="80" t="s">
         <v>106</v>
       </c>
@@ -21526,9 +21525,9 @@
       </c>
       <c r="H56" s="83"/>
     </row>
-    <row r="57" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="237"/>
-      <c r="B57" s="232"/>
+    <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="238"/>
+      <c r="B57" s="233"/>
       <c r="C57" s="80" t="s">
         <v>110</v>
       </c>
@@ -21546,9 +21545,9 @@
       </c>
       <c r="H57" s="83"/>
     </row>
-    <row r="58" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="237"/>
-      <c r="B58" s="232"/>
+    <row r="58" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="238"/>
+      <c r="B58" s="233"/>
       <c r="C58" s="80" t="s">
         <v>114</v>
       </c>
@@ -21566,9 +21565,9 @@
       </c>
       <c r="H58" s="83"/>
     </row>
-    <row r="59" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A59" s="237"/>
-      <c r="B59" s="232"/>
+    <row r="59" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="238"/>
+      <c r="B59" s="233"/>
       <c r="C59" s="80" t="s">
         <v>118</v>
       </c>
@@ -21586,9 +21585,9 @@
       </c>
       <c r="H59" s="83"/>
     </row>
-    <row r="60" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="237"/>
-      <c r="B60" s="232"/>
+    <row r="60" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="238"/>
+      <c r="B60" s="233"/>
       <c r="C60" s="80" t="s">
         <v>122</v>
       </c>
@@ -21606,9 +21605,9 @@
       </c>
       <c r="H60" s="83"/>
     </row>
-    <row r="61" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="237"/>
-      <c r="B61" s="232"/>
+    <row r="61" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="238"/>
+      <c r="B61" s="233"/>
       <c r="C61" s="80" t="s">
         <v>126</v>
       </c>
@@ -21626,9 +21625,9 @@
       </c>
       <c r="H61" s="83"/>
     </row>
-    <row r="62" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="237"/>
-      <c r="B62" s="232"/>
+    <row r="62" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="238"/>
+      <c r="B62" s="233"/>
       <c r="C62" s="80" t="s">
         <v>130</v>
       </c>
@@ -21646,9 +21645,9 @@
       </c>
       <c r="H62" s="83"/>
     </row>
-    <row r="63" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="238"/>
-      <c r="B63" s="233"/>
+    <row r="63" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="239"/>
+      <c r="B63" s="234"/>
       <c r="C63" s="85" t="s">
         <v>134</v>
       </c>
@@ -21666,8 +21665,8 @@
       </c>
       <c r="H63" s="87"/>
     </row>
-    <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="239" t="s">
+    <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="240" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="59"/>
@@ -22694,8 +22693,8 @@
       <c r="AMI64" s="13"/>
       <c r="AMJ64" s="13"/>
     </row>
-    <row r="65" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="240"/>
+    <row r="65" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="241"/>
       <c r="B65" s="89" t="s">
         <v>146</v>
       </c>
@@ -23730,8 +23729,8 @@
       <c r="AMI65" s="13"/>
       <c r="AMJ65" s="13"/>
     </row>
-    <row r="66" spans="1:1024" s="14" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="241"/>
+    <row r="66" spans="1:1024" s="14" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="242"/>
       <c r="B66" s="93" t="s">
         <v>150</v>
       </c>
@@ -24766,8 +24765,8 @@
       <c r="AMI66" s="13"/>
       <c r="AMJ66" s="13"/>
     </row>
-    <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="236" t="s">
+    <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="237" t="s">
         <v>154</v>
       </c>
       <c r="B67" s="29"/>
@@ -24778,8 +24777,8 @@
       <c r="G67" s="194"/>
       <c r="H67" s="64"/>
     </row>
-    <row r="68" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="237"/>
+    <row r="68" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="238"/>
       <c r="B68" s="69" t="s">
         <v>155</v>
       </c>
@@ -24796,9 +24795,9 @@
       </c>
       <c r="H68" s="72"/>
     </row>
-    <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="237"/>
-      <c r="B69" s="234" t="s">
+    <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="238"/>
+      <c r="B69" s="235" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="69" t="s">
@@ -24818,9 +24817,9 @@
       </c>
       <c r="H69" s="72"/>
     </row>
-    <row r="70" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="237"/>
-      <c r="B70" s="234"/>
+    <row r="70" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="238"/>
+      <c r="B70" s="235"/>
       <c r="C70" s="69" t="s">
         <v>30</v>
       </c>
@@ -24838,9 +24837,9 @@
       </c>
       <c r="H70" s="72"/>
     </row>
-    <row r="71" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="237"/>
-      <c r="B71" s="234"/>
+    <row r="71" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="238"/>
+      <c r="B71" s="235"/>
       <c r="C71" s="69" t="s">
         <v>12</v>
       </c>
@@ -24858,9 +24857,9 @@
       </c>
       <c r="H71" s="72"/>
     </row>
-    <row r="72" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="237"/>
-      <c r="B72" s="234"/>
+    <row r="72" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="238"/>
+      <c r="B72" s="235"/>
       <c r="C72" s="69" t="s">
         <v>167</v>
       </c>
@@ -24878,9 +24877,9 @@
       </c>
       <c r="H72" s="72"/>
     </row>
-    <row r="73" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="238"/>
-      <c r="B73" s="235"/>
+    <row r="73" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="239"/>
+      <c r="B73" s="236"/>
       <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
@@ -24898,8 +24897,8 @@
       </c>
       <c r="H73" s="76"/>
     </row>
-    <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="239" t="s">
+    <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="240" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="31"/>
@@ -25926,8 +25925,8 @@
       <c r="AMI74" s="13"/>
       <c r="AMJ74" s="13"/>
     </row>
-    <row r="75" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="240"/>
+    <row r="75" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="241"/>
       <c r="B75" s="47" t="s">
         <v>173</v>
       </c>
@@ -26960,9 +26959,9 @@
       <c r="AMI75" s="13"/>
       <c r="AMJ75" s="13"/>
     </row>
-    <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="240"/>
-      <c r="B76" s="230" t="s">
+    <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="241"/>
+      <c r="B76" s="231" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="47" t="s">
@@ -27998,9 +27997,9 @@
       <c r="AMI76" s="13"/>
       <c r="AMJ76" s="13"/>
     </row>
-    <row r="77" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="240"/>
-      <c r="B77" s="230"/>
+    <row r="77" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="241"/>
+      <c r="B77" s="231"/>
       <c r="C77" s="47" t="s">
         <v>179</v>
       </c>
@@ -29034,9 +29033,9 @@
       <c r="AMI77" s="13"/>
       <c r="AMJ77" s="13"/>
     </row>
-    <row r="78" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="240"/>
-      <c r="B78" s="230"/>
+    <row r="78" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="241"/>
+      <c r="B78" s="231"/>
       <c r="C78" s="47" t="s">
         <v>182</v>
       </c>
@@ -30070,9 +30069,9 @@
       <c r="AMI78" s="13"/>
       <c r="AMJ78" s="13"/>
     </row>
-    <row r="79" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="240"/>
-      <c r="B79" s="230"/>
+    <row r="79" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="241"/>
+      <c r="B79" s="231"/>
       <c r="C79" s="47" t="s">
         <v>185</v>
       </c>
@@ -31106,9 +31105,9 @@
       <c r="AMI79" s="13"/>
       <c r="AMJ79" s="13"/>
     </row>
-    <row r="80" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="241"/>
-      <c r="B80" s="231"/>
+    <row r="80" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="242"/>
+      <c r="B80" s="232"/>
       <c r="C80" s="51" t="s">
         <v>25</v>
       </c>
@@ -32142,76 +32141,76 @@
       <c r="AMI80" s="13"/>
       <c r="AMJ80" s="13"/>
     </row>
-    <row r="81" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H96" s="4"/>
     </row>
-    <row r="97" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H97" s="4"/>
     </row>
-    <row r="98" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="8:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="8:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="H104" s="4"/>
     </row>
   </sheetData>
@@ -32255,33 +32254,33 @@
       <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
-    <col min="9" max="1023" width="8.5" style="1" hidden="1"/>
-    <col min="1024" max="1024" width="9.1640625" style="1" hidden="1"/>
-    <col min="16384" max="16384" width="3.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
+    <col min="9" max="1023" width="8.42578125" style="1" hidden="1"/>
+    <col min="1024" max="1024" width="9.140625" style="1" hidden="1"/>
+    <col min="16384" max="16384" width="3.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>497</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -32307,8 +32306,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="244" t="s">
+    <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="245" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -32319,8 +32318,8 @@
       <c r="G3" s="182"/>
       <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="245"/>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="246"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -32339,8 +32338,8 @@
       </c>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="245"/>
+    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="246"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -32359,8 +32358,8 @@
       </c>
       <c r="H5" s="50"/>
     </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="245"/>
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="246"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -32379,8 +32378,8 @@
       </c>
       <c r="H6" s="50"/>
     </row>
-    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="245"/>
+    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="246"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -32399,8 +32398,8 @@
       </c>
       <c r="H7" s="50"/>
     </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="245"/>
+    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="246"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -32419,8 +32418,8 @@
       </c>
       <c r="H8" s="50"/>
     </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="245"/>
+    <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="246"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -32439,8 +32438,8 @@
       </c>
       <c r="H9" s="50"/>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="246"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -32459,8 +32458,8 @@
       </c>
       <c r="H10" s="50"/>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246"/>
+    <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="247"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -32479,8 +32478,8 @@
       </c>
       <c r="H11" s="54"/>
     </row>
-    <row r="12" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="250" t="s">
+    <row r="12" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="251" t="s">
         <v>203</v>
       </c>
       <c r="B12" s="98"/>
@@ -32491,8 +32490,8 @@
       <c r="G12" s="185"/>
       <c r="H12" s="102"/>
     </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="251"/>
+    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="252"/>
       <c r="B13" s="103" t="s">
         <v>204</v>
       </c>
@@ -32511,8 +32510,8 @@
       </c>
       <c r="H13" s="72"/>
     </row>
-    <row r="14" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="251"/>
+    <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="252"/>
       <c r="B14" s="103" t="s">
         <v>452</v>
       </c>
@@ -32556,32 +32555,32 @@
       <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="205" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="205" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" customWidth="1"/>
     <col min="9" max="1024" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1025" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -32607,8 +32606,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="244" t="s">
+    <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="245" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -32657,8 +32656,8 @@
       <c r="AS3" s="7"/>
       <c r="AMJ3" s="5"/>
     </row>
-    <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="245"/>
+    <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="246"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -32675,8 +32674,8 @@
       </c>
       <c r="H4" s="107"/>
     </row>
-    <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="245"/>
+    <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="246"/>
       <c r="B5" s="105" t="s">
         <v>210</v>
       </c>
@@ -32691,24 +32690,24 @@
       <c r="G5" s="197"/>
       <c r="H5" s="107"/>
     </row>
-    <row r="6" spans="1:1024" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="245"/>
+    <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="246"/>
       <c r="B6" s="105" t="s">
         <v>213</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="107"/>
     </row>
-    <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="245"/>
+    <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="246"/>
       <c r="B7" s="105" t="s">
         <v>214</v>
       </c>
@@ -32718,13 +32717,13 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G7" s="197"/>
       <c r="H7" s="107"/>
     </row>
-    <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="245"/>
+    <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="246"/>
       <c r="B8" s="105" t="s">
         <v>215</v>
       </c>
@@ -32739,8 +32738,8 @@
       <c r="G8" s="197"/>
       <c r="H8" s="107"/>
     </row>
-    <row r="9" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="245"/>
+    <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="246"/>
       <c r="B9" s="105" t="s">
         <v>217</v>
       </c>
@@ -32750,15 +32749,15 @@
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G9" s="197" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="107"/>
     </row>
-    <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+    <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="246"/>
       <c r="B10" s="105" t="s">
         <v>219</v>
       </c>
@@ -32786,8 +32785,8 @@
       <c r="T10" s="8"/>
       <c r="AMJ10" s="5"/>
     </row>
-    <row r="11" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="245"/>
+    <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="246"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -32802,8 +32801,8 @@
       <c r="G11" s="197"/>
       <c r="H11" s="107"/>
     </row>
-    <row r="12" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="245"/>
+    <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="246"/>
       <c r="B12" s="105" t="s">
         <v>223</v>
       </c>
@@ -32813,15 +32812,15 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G12" s="197" t="s">
         <v>43</v>
       </c>
       <c r="H12" s="107"/>
     </row>
-    <row r="13" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="245"/>
+    <row r="13" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="246"/>
       <c r="B13" s="105" t="s">
         <v>225</v>
       </c>
@@ -32838,8 +32837,8 @@
       </c>
       <c r="H13" s="107"/>
     </row>
-    <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+    <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="246"/>
       <c r="B14" s="105" t="s">
         <v>469</v>
       </c>
@@ -32856,8 +32855,8 @@
       </c>
       <c r="H14" s="107"/>
     </row>
-    <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="246"/>
+    <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="247"/>
       <c r="B15" s="108" t="s">
         <v>229</v>
       </c>
@@ -32872,8 +32871,8 @@
       <c r="G15" s="198"/>
       <c r="H15" s="110"/>
     </row>
-    <row r="16" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="236" t="s">
+    <row r="16" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="237" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -32885,14 +32884,14 @@
       <c r="H16" s="112"/>
       <c r="AMJ16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="237"/>
+    <row r="17" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="238"/>
       <c r="B17" s="113" t="s">
         <v>232</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E17" s="114"/>
       <c r="F17" s="113" t="s">
@@ -32901,8 +32900,8 @@
       <c r="G17" s="200"/>
       <c r="H17" s="115"/>
     </row>
-    <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="237"/>
+    <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="238"/>
       <c r="B18" s="113"/>
       <c r="C18" s="114" t="s">
         <v>1</v>
@@ -32912,13 +32911,13 @@
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G18" s="200"/>
       <c r="H18" s="115"/>
     </row>
-    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="237"/>
+    <row r="19" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="238"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>210</v>
@@ -32928,163 +32927,163 @@
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G19" s="200"/>
       <c r="H19" s="115"/>
     </row>
-    <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="237"/>
+    <row r="20" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="238"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D20" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G20" s="200"/>
       <c r="H20" s="115"/>
     </row>
-    <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="237"/>
+    <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="238"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D21" s="113" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G21" s="200"/>
       <c r="H21" s="115"/>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="237"/>
+    <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="238"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G22" s="200"/>
       <c r="H22" s="115"/>
     </row>
-    <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="237"/>
+    <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="238"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D23" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G23" s="200"/>
       <c r="H23" s="115"/>
     </row>
-    <row r="24" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="237"/>
+    <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="238"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G24" s="200"/>
       <c r="H24" s="115"/>
     </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="237"/>
+    <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="238"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D25" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G25" s="200"/>
       <c r="H25" s="115"/>
     </row>
-    <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="237"/>
+    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="238"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G26" s="200"/>
       <c r="H26" s="115"/>
     </row>
-    <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="237"/>
+    <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="238"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D27" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G27" s="200"/>
       <c r="H27" s="115"/>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="237"/>
+    <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="238"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G28" s="200"/>
       <c r="H28" s="115"/>
     </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="237"/>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="238"/>
       <c r="B29" s="113" t="s">
         <v>234</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="113" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
@@ -33093,8 +33092,8 @@
       <c r="G29" s="200"/>
       <c r="H29" s="115"/>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="237"/>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="238"/>
       <c r="B30" s="226"/>
       <c r="C30" s="114" t="s">
         <v>1</v>
@@ -33104,13 +33103,13 @@
       </c>
       <c r="E30" s="227"/>
       <c r="F30" s="113" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G30" s="228"/>
       <c r="H30" s="229"/>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="237"/>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="238"/>
       <c r="B31" s="226"/>
       <c r="C31" s="114" t="s">
         <v>210</v>
@@ -33120,157 +33119,157 @@
       </c>
       <c r="E31" s="227"/>
       <c r="F31" s="113" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G31" s="228"/>
       <c r="H31" s="229"/>
     </row>
-    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="237"/>
+    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="238"/>
       <c r="B32" s="226"/>
       <c r="C32" s="114" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D32" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E32" s="227"/>
       <c r="F32" s="113" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G32" s="228"/>
       <c r="H32" s="229"/>
     </row>
-    <row r="33" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="237"/>
+    <row r="33" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="238"/>
       <c r="B33" s="226"/>
       <c r="C33" s="114" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E33" s="227"/>
       <c r="F33" s="113" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G33" s="228"/>
       <c r="H33" s="229"/>
     </row>
-    <row r="34" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="237"/>
+    <row r="34" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="238"/>
       <c r="B34" s="226"/>
       <c r="C34" s="114" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D34" s="113" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E34" s="227"/>
       <c r="F34" s="113" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G34" s="228"/>
       <c r="H34" s="229"/>
     </row>
-    <row r="35" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="237"/>
+    <row r="35" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="238"/>
       <c r="B35" s="226"/>
       <c r="C35" s="114" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D35" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E35" s="227"/>
       <c r="F35" s="113" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G35" s="228"/>
       <c r="H35" s="229"/>
     </row>
-    <row r="36" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="237"/>
+    <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="238"/>
       <c r="B36" s="226"/>
       <c r="C36" s="114" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E36" s="227"/>
       <c r="F36" s="113" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G36" s="228"/>
       <c r="H36" s="229"/>
     </row>
-    <row r="37" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="237"/>
+    <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="238"/>
       <c r="B37" s="226"/>
       <c r="C37" s="114" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D37" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E37" s="227"/>
       <c r="F37" s="113" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G37" s="228"/>
       <c r="H37" s="229"/>
     </row>
-    <row r="38" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="237"/>
+    <row r="38" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="238"/>
       <c r="B38" s="226"/>
       <c r="C38" s="114" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D38" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E38" s="227"/>
       <c r="F38" s="113" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G38" s="228"/>
       <c r="H38" s="229"/>
     </row>
-    <row r="39" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="237"/>
+    <row r="39" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="238"/>
       <c r="B39" s="226"/>
       <c r="C39" s="114" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D39" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E39" s="227"/>
       <c r="F39" s="113" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G39" s="228"/>
       <c r="H39" s="229"/>
     </row>
-    <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="237"/>
+    <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="238"/>
       <c r="B40" s="226"/>
       <c r="C40" s="114" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D40" s="113" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E40" s="227"/>
       <c r="F40" s="113" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G40" s="228"/>
       <c r="H40" s="229"/>
     </row>
-    <row r="41" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="238"/>
+    <row r="41" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="239"/>
       <c r="B41" s="116" t="s">
         <v>236</v>
       </c>
@@ -33280,15 +33279,15 @@
       </c>
       <c r="E41" s="117"/>
       <c r="F41" s="116" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G41" s="201" t="s">
         <v>43</v>
       </c>
       <c r="H41" s="118"/>
     </row>
-    <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="239" t="s">
+    <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="240" t="s">
         <v>237</v>
       </c>
       <c r="B42" s="119"/>
@@ -33337,8 +33336,8 @@
       <c r="AS42" s="7"/>
       <c r="AMJ42" s="5"/>
     </row>
-    <row r="43" spans="1:1024" s="9" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="241"/>
+    <row r="43" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="242"/>
       <c r="B43" s="108" t="s">
         <v>238</v>
       </c>
@@ -33374,8 +33373,8 @@
       <c r="Z43" s="8"/>
       <c r="AMJ43" s="5"/>
     </row>
-    <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="236" t="s">
+    <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="237" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="111"/>
@@ -33387,8 +33386,8 @@
       <c r="H44" s="112"/>
       <c r="AMJ44" s="5"/>
     </row>
-    <row r="45" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="237"/>
+    <row r="45" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="238"/>
       <c r="B45" s="113" t="s">
         <v>73</v>
       </c>
@@ -33405,8 +33404,8 @@
       </c>
       <c r="H45" s="115"/>
     </row>
-    <row r="46" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="237"/>
+    <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="238"/>
       <c r="B46" s="113" t="s">
         <v>76</v>
       </c>
@@ -33423,8 +33422,8 @@
       </c>
       <c r="H46" s="115"/>
     </row>
-    <row r="47" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="238"/>
+    <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="239"/>
       <c r="B47" s="116" t="s">
         <v>79</v>
       </c>
@@ -33441,8 +33440,8 @@
       </c>
       <c r="H47" s="118"/>
     </row>
-    <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="239" t="s">
+    <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="240" t="s">
         <v>244</v>
       </c>
       <c r="B48" s="121"/>
@@ -33472,8 +33471,8 @@
       <c r="Z48" s="7"/>
       <c r="AMJ48" s="5"/>
     </row>
-    <row r="49" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="240"/>
+    <row r="49" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="241"/>
       <c r="B49" s="105" t="s">
         <v>245</v>
       </c>
@@ -33490,8 +33489,8 @@
       </c>
       <c r="H49" s="107"/>
     </row>
-    <row r="50" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="240"/>
+    <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="241"/>
       <c r="B50" s="105" t="s">
         <v>247</v>
       </c>
@@ -33508,8 +33507,8 @@
       </c>
       <c r="H50" s="107"/>
     </row>
-    <row r="51" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="240"/>
+    <row r="51" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="241"/>
       <c r="B51" s="105" t="s">
         <v>46</v>
       </c>
@@ -33526,8 +33525,8 @@
       </c>
       <c r="H51" s="107"/>
     </row>
-    <row r="52" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="240"/>
+    <row r="52" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="241"/>
       <c r="B52" s="105" t="s">
         <v>48</v>
       </c>
@@ -33544,8 +33543,8 @@
       </c>
       <c r="H52" s="107"/>
     </row>
-    <row r="53" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="240"/>
+    <row r="53" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="241"/>
       <c r="B53" s="105" t="s">
         <v>61</v>
       </c>
@@ -33582,8 +33581,8 @@
       <c r="AA53" s="8"/>
       <c r="AMJ53" s="5"/>
     </row>
-    <row r="54" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="240"/>
+    <row r="54" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="241"/>
       <c r="B54" s="105" t="s">
         <v>63</v>
       </c>
@@ -33600,8 +33599,8 @@
       </c>
       <c r="H54" s="107"/>
     </row>
-    <row r="55" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="240"/>
+    <row r="55" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="241"/>
       <c r="B55" s="105" t="s">
         <v>65</v>
       </c>
@@ -33618,8 +33617,8 @@
       </c>
       <c r="H55" s="107"/>
     </row>
-    <row r="56" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="240"/>
+    <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="241"/>
       <c r="B56" s="105" t="s">
         <v>67</v>
       </c>
@@ -33636,8 +33635,8 @@
       </c>
       <c r="H56" s="107"/>
     </row>
-    <row r="57" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="241"/>
+    <row r="57" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="242"/>
       <c r="B57" s="108" t="s">
         <v>69</v>
       </c>
@@ -33654,8 +33653,8 @@
       </c>
       <c r="H57" s="110"/>
     </row>
-    <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="236" t="s">
+    <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="237" t="s">
         <v>510</v>
       </c>
       <c r="B58" s="123"/>
@@ -33667,8 +33666,8 @@
       <c r="H58" s="124"/>
       <c r="AMJ58" s="5"/>
     </row>
-    <row r="59" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="238"/>
+    <row r="59" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="239"/>
       <c r="B59" s="116" t="s">
         <v>5</v>
       </c>
@@ -33708,40 +33707,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="A34:XFD34"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="205" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="205" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" customWidth="1"/>
     <col min="9" max="1024" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1025" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
@@ -34783,8 +34782,8 @@
       <c r="AMI2" s="17"/>
       <c r="AMJ2" s="17"/>
     </row>
-    <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+    <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="253" t="s">
         <v>511</v>
       </c>
       <c r="B3" s="121"/>
@@ -34808,8 +34807,8 @@
       <c r="T3" s="7"/>
       <c r="AMJ3" s="5"/>
     </row>
-    <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+    <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="254"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -34828,8 +34827,8 @@
       </c>
       <c r="H4" s="126"/>
     </row>
-    <row r="5" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+    <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="254"/>
       <c r="B5" s="105" t="s">
         <v>306</v>
       </c>
@@ -34848,10 +34847,10 @@
       </c>
       <c r="H5" s="126"/>
     </row>
-    <row r="6" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+    <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="254"/>
       <c r="B6" s="105" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
@@ -34868,8 +34867,8 @@
       </c>
       <c r="H6" s="126"/>
     </row>
-    <row r="7" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="253"/>
+    <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="254"/>
       <c r="B7" s="105" t="s">
         <v>309</v>
       </c>
@@ -34888,8 +34887,8 @@
       </c>
       <c r="H7" s="126"/>
     </row>
-    <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="255" t="s">
+    <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="256" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="123"/>
@@ -34901,8 +34900,8 @@
       <c r="H8" s="128"/>
       <c r="AMJ8" s="5"/>
     </row>
-    <row r="9" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="257"/>
+    <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="258"/>
       <c r="B9" s="113" t="s">
         <v>312</v>
       </c>
@@ -35937,10 +35936,10 @@
       <c r="AMI9" s="8"/>
       <c r="AMJ9" s="8"/>
     </row>
-    <row r="10" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="257"/>
+    <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="258"/>
       <c r="B10" s="113" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
@@ -36973,8 +36972,8 @@
       <c r="AMI10" s="8"/>
       <c r="AMJ10" s="8"/>
     </row>
-    <row r="11" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="257"/>
+    <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="258"/>
       <c r="B11" s="113" t="s">
         <v>317</v>
       </c>
@@ -38009,10 +38008,10 @@
       <c r="AMI11" s="8"/>
       <c r="AMJ11" s="8"/>
     </row>
-    <row r="12" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="257"/>
+    <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="258"/>
       <c r="B12" s="113" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
@@ -39045,8 +39044,8 @@
       <c r="AMI12" s="8"/>
       <c r="AMJ12" s="8"/>
     </row>
-    <row r="13" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="257"/>
+    <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="258"/>
       <c r="B13" s="113" t="s">
         <v>314</v>
       </c>
@@ -40081,8 +40080,8 @@
       <c r="AMI13" s="8"/>
       <c r="AMJ13" s="8"/>
     </row>
-    <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="252" t="s">
+    <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="253" t="s">
         <v>512</v>
       </c>
       <c r="B14" s="121"/>
@@ -40102,8 +40101,8 @@
       <c r="P14" s="7"/>
       <c r="AMJ14" s="5"/>
     </row>
-    <row r="15" spans="1:1024" s="16" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="254"/>
+    <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="255"/>
       <c r="B15" s="108" t="s">
         <v>321</v>
       </c>
@@ -41138,8 +41137,8 @@
       <c r="AMI15" s="17"/>
       <c r="AMJ15" s="17"/>
     </row>
-    <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="255" t="s">
+    <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="256" t="s">
         <v>324</v>
       </c>
       <c r="B16" s="111"/>
@@ -42166,8 +42165,8 @@
       <c r="AMI16" s="39"/>
       <c r="AMJ16" s="39"/>
     </row>
-    <row r="17" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="257"/>
+    <row r="17" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="258"/>
       <c r="B17" s="113" t="s">
         <v>94</v>
       </c>
@@ -42176,7 +42175,7 @@
         <v>220</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>325</v>
@@ -42186,8 +42185,8 @@
       </c>
       <c r="H17" s="129"/>
     </row>
-    <row r="18" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="257"/>
+    <row r="18" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="258"/>
       <c r="B18" s="113" t="s">
         <v>98</v>
       </c>
@@ -42206,8 +42205,8 @@
       </c>
       <c r="H18" s="129"/>
     </row>
-    <row r="19" spans="1:1024" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="256"/>
+    <row r="19" spans="1:1024" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="257"/>
       <c r="B19" s="116" t="s">
         <v>102</v>
       </c>
@@ -42226,8 +42225,8 @@
       </c>
       <c r="H19" s="130"/>
     </row>
-    <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="252" t="s">
+    <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="253" t="s">
         <v>329</v>
       </c>
       <c r="B20" s="121"/>
@@ -42246,8 +42245,8 @@
       <c r="O20" s="7"/>
       <c r="AMJ20" s="5"/>
     </row>
-    <row r="21" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="253"/>
+    <row r="21" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="254"/>
       <c r="B21" s="105" t="s">
         <v>106</v>
       </c>
@@ -42266,10 +42265,10 @@
       </c>
       <c r="H21" s="126"/>
     </row>
-    <row r="22" spans="1:1024" ht="146.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="253"/>
+    <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="254"/>
       <c r="B22" s="105" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
@@ -42279,17 +42278,17 @@
         <v>493</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G22" s="197" t="s">
         <v>332</v>
       </c>
       <c r="H22" s="126"/>
     </row>
-    <row r="23" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="254"/>
+    <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="255"/>
       <c r="B23" s="108" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
@@ -42306,8 +42305,8 @@
       </c>
       <c r="H23" s="127"/>
     </row>
-    <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="255" t="s">
+    <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="256" t="s">
         <v>513</v>
       </c>
       <c r="B24" s="132"/>
@@ -42319,8 +42318,8 @@
       <c r="H24" s="133"/>
       <c r="AMJ24" s="5"/>
     </row>
-    <row r="25" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="256"/>
+    <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="257"/>
       <c r="B25" s="116" t="s">
         <v>335</v>
       </c>
@@ -42337,8 +42336,8 @@
       </c>
       <c r="H25" s="130"/>
     </row>
-    <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="252" t="s">
+    <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="253" t="s">
         <v>338</v>
       </c>
       <c r="B26" s="121"/>
@@ -42357,8 +42356,8 @@
       <c r="O26" s="7"/>
       <c r="AMJ26" s="5"/>
     </row>
-    <row r="27" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="253"/>
+    <row r="27" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
+      <c r="A27" s="254"/>
       <c r="B27" s="105" t="s">
         <v>110</v>
       </c>
@@ -42377,8 +42376,8 @@
       </c>
       <c r="H27" s="126"/>
     </row>
-    <row r="28" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="253"/>
+    <row r="28" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="254"/>
       <c r="B28" s="105" t="s">
         <v>118</v>
       </c>
@@ -42397,8 +42396,8 @@
       </c>
       <c r="H28" s="126"/>
     </row>
-    <row r="29" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="253"/>
+    <row r="29" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="254"/>
       <c r="B29" s="105" t="s">
         <v>122</v>
       </c>
@@ -42417,8 +42416,8 @@
       </c>
       <c r="H29" s="126"/>
     </row>
-    <row r="30" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="253"/>
+    <row r="30" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="254"/>
       <c r="B30" s="105" t="s">
         <v>126</v>
       </c>
@@ -42437,8 +42436,8 @@
       </c>
       <c r="H30" s="126"/>
     </row>
-    <row r="31" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="254"/>
+    <row r="31" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="255"/>
       <c r="B31" s="108" t="s">
         <v>130</v>
       </c>
@@ -42457,8 +42456,8 @@
       </c>
       <c r="H31" s="127"/>
     </row>
-    <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="255" t="s">
+    <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="256" t="s">
         <v>344</v>
       </c>
       <c r="B32" s="123"/>
@@ -42470,8 +42469,8 @@
       <c r="H32" s="128"/>
       <c r="AMJ32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="89.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="257"/>
+    <row r="33" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="258"/>
       <c r="B33" s="113" t="s">
         <v>134</v>
       </c>
@@ -42480,7 +42479,7 @@
         <v>211</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F33" s="113" t="s">
         <v>494</v>
@@ -42490,26 +42489,26 @@
       </c>
       <c r="H33" s="129"/>
     </row>
-    <row r="34" spans="1:8" ht="89.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="257"/>
+    <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="258"/>
       <c r="B34" s="113" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C34" s="227"/>
       <c r="D34" s="226" t="s">
         <v>319</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F34" s="226"/>
       <c r="G34" s="228" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="261"/>
+      <c r="H34" s="230"/>
     </row>
-    <row r="35" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="256"/>
+    <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="257"/>
       <c r="B35" s="116" t="s">
         <v>345</v>
       </c>
@@ -42526,8 +42525,8 @@
       </c>
       <c r="H35" s="130"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="9">
@@ -42563,33 +42562,33 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="134" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="134" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="134" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="134" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="134" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="209" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="134" customWidth="1"/>
-    <col min="9" max="67" width="10.5" style="134" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="134" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="134" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="134" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="134" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="134" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="209" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="134" customWidth="1"/>
+    <col min="9" max="67" width="10.42578125" style="134" hidden="1" customWidth="1"/>
     <col min="68" max="1024" width="0" style="134" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="9.1640625" style="135" hidden="1"/>
+    <col min="1025" max="16384" width="9.140625" style="135" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>500</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -42615,8 +42614,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="239" t="s">
+    <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="240" t="s">
         <v>514</v>
       </c>
       <c r="B3" s="18"/>
@@ -42642,8 +42641,8 @@
       <c r="V3" s="12"/>
       <c r="AMJ3" s="134"/>
     </row>
-    <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="240"/>
+    <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="241"/>
       <c r="B4" s="106" t="s">
         <v>207</v>
       </c>
@@ -42662,8 +42661,8 @@
       </c>
       <c r="H4" s="137"/>
     </row>
-    <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="240"/>
+    <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="241"/>
       <c r="B5" s="106" t="s">
         <v>260</v>
       </c>
@@ -42682,8 +42681,8 @@
       </c>
       <c r="H5" s="137"/>
     </row>
-    <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="240"/>
+    <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="241"/>
       <c r="B6" s="106" t="s">
         <v>213</v>
       </c>
@@ -42700,8 +42699,8 @@
       <c r="G6" s="197"/>
       <c r="H6" s="137"/>
     </row>
-    <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="240"/>
+    <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="241"/>
       <c r="B7" s="106" t="s">
         <v>266</v>
       </c>
@@ -42720,8 +42719,8 @@
       </c>
       <c r="H7" s="137"/>
     </row>
-    <row r="8" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="240"/>
+    <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="241"/>
       <c r="B8" s="106" t="s">
         <v>269</v>
       </c>
@@ -42740,8 +42739,8 @@
       </c>
       <c r="H8" s="137"/>
     </row>
-    <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="240"/>
+    <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="241"/>
       <c r="B9" s="106" t="s">
         <v>272</v>
       </c>
@@ -42760,8 +42759,8 @@
       </c>
       <c r="H9" s="137"/>
     </row>
-    <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="240"/>
+    <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="241"/>
       <c r="B10" s="106" t="s">
         <v>210</v>
       </c>
@@ -42778,8 +42777,8 @@
       <c r="G10" s="197"/>
       <c r="H10" s="137"/>
     </row>
-    <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="240"/>
+    <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="241"/>
       <c r="B11" s="106" t="s">
         <v>279</v>
       </c>
@@ -42796,8 +42795,8 @@
       <c r="G11" s="197"/>
       <c r="H11" s="137"/>
     </row>
-    <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="240"/>
+    <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="241"/>
       <c r="B12" s="106" t="s">
         <v>354</v>
       </c>
@@ -42814,8 +42813,8 @@
       <c r="G12" s="197"/>
       <c r="H12" s="137"/>
     </row>
-    <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="240"/>
+    <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="241"/>
       <c r="B13" s="106" t="s">
         <v>285</v>
       </c>
@@ -42832,8 +42831,8 @@
       <c r="G13" s="197"/>
       <c r="H13" s="137"/>
     </row>
-    <row r="14" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="240"/>
+    <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="241"/>
       <c r="B14" s="106" t="s">
         <v>358</v>
       </c>
@@ -42850,8 +42849,8 @@
       <c r="G14" s="197"/>
       <c r="H14" s="137"/>
     </row>
-    <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="240"/>
+    <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="241"/>
       <c r="B15" s="106" t="s">
         <v>361</v>
       </c>
@@ -42868,8 +42867,8 @@
       <c r="G15" s="197"/>
       <c r="H15" s="137"/>
     </row>
-    <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="240"/>
+    <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="241"/>
       <c r="B16" s="106" t="s">
         <v>364</v>
       </c>
@@ -42886,8 +42885,8 @@
       <c r="G16" s="197"/>
       <c r="H16" s="137"/>
     </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="240"/>
+    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="241"/>
       <c r="B17" s="106" t="s">
         <v>368</v>
       </c>
@@ -42904,8 +42903,8 @@
       <c r="G17" s="197"/>
       <c r="H17" s="137"/>
     </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="241"/>
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="242"/>
       <c r="B18" s="109" t="s">
         <v>302</v>
       </c>
@@ -42922,10 +42921,10 @@
       <c r="G18" s="198"/>
       <c r="H18" s="139"/>
     </row>
-    <row r="20" spans="1:8" ht="23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="F20" s="140"/>
     </row>
-    <row r="28" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="D28" s="141"/>
     </row>
   </sheetData>
@@ -42949,35 +42948,35 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A18"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="135" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="135" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="135" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="135" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="135" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="211" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="135" customWidth="1"/>
-    <col min="9" max="62" width="10.5" style="135" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="135" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="135" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="135" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="135" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="135" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="211" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="135" customWidth="1"/>
+    <col min="9" max="62" width="10.42578125" style="135" hidden="1" customWidth="1"/>
     <col min="63" max="16384" width="0" style="135" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>501</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -43003,8 +43002,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="144" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="258" t="s">
+    <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="259" t="s">
         <v>514</v>
       </c>
       <c r="B3" s="142"/>
@@ -43015,8 +43014,8 @@
       <c r="G3" s="210"/>
       <c r="H3" s="143"/>
     </row>
-    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="259"/>
+    <row r="4" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="260"/>
       <c r="B4" s="106" t="s">
         <v>207</v>
       </c>
@@ -43044,8 +43043,8 @@
       <c r="P4" s="144"/>
       <c r="Q4" s="144"/>
     </row>
-    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="259"/>
+    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="260"/>
       <c r="B5" s="106" t="s">
         <v>260</v>
       </c>
@@ -43073,8 +43072,8 @@
       <c r="P5" s="144"/>
       <c r="Q5" s="144"/>
     </row>
-    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="259"/>
+    <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="260"/>
       <c r="B6" s="106" t="s">
         <v>213</v>
       </c>
@@ -43100,8 +43099,8 @@
       <c r="P6" s="144"/>
       <c r="Q6" s="144"/>
     </row>
-    <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="259"/>
+    <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="260"/>
       <c r="B7" s="106" t="s">
         <v>266</v>
       </c>
@@ -43129,8 +43128,8 @@
       <c r="P7" s="144"/>
       <c r="Q7" s="144"/>
     </row>
-    <row r="8" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="259"/>
+    <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="260"/>
       <c r="B8" s="106" t="s">
         <v>269</v>
       </c>
@@ -43158,8 +43157,8 @@
       <c r="P8" s="144"/>
       <c r="Q8" s="144"/>
     </row>
-    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="259"/>
+    <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="260"/>
       <c r="B9" s="106" t="s">
         <v>272</v>
       </c>
@@ -43187,8 +43186,8 @@
       <c r="P9" s="144"/>
       <c r="Q9" s="144"/>
     </row>
-    <row r="10" spans="1:17" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259"/>
+    <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="260"/>
       <c r="B10" s="106" t="s">
         <v>210</v>
       </c>
@@ -43214,8 +43213,8 @@
       <c r="P10" s="144"/>
       <c r="Q10" s="144"/>
     </row>
-    <row r="11" spans="1:17" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="259"/>
+    <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="260"/>
       <c r="B11" s="106" t="s">
         <v>279</v>
       </c>
@@ -43241,8 +43240,8 @@
       <c r="P11" s="144"/>
       <c r="Q11" s="144"/>
     </row>
-    <row r="12" spans="1:17" s="151" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="259"/>
+    <row r="12" spans="1:17" s="151" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="260"/>
       <c r="B12" s="106" t="s">
         <v>282</v>
       </c>
@@ -43268,8 +43267,8 @@
       <c r="P12" s="144"/>
       <c r="Q12" s="144"/>
     </row>
-    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="259"/>
+    <row r="13" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="260"/>
       <c r="B13" s="106" t="s">
         <v>285</v>
       </c>
@@ -43295,8 +43294,8 @@
       <c r="P13" s="144"/>
       <c r="Q13" s="144"/>
     </row>
-    <row r="14" spans="1:17" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="259"/>
+    <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="260"/>
       <c r="B14" s="106" t="s">
         <v>289</v>
       </c>
@@ -43322,8 +43321,8 @@
       <c r="P14" s="144"/>
       <c r="Q14" s="144"/>
     </row>
-    <row r="15" spans="1:17" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="259"/>
+    <row r="15" spans="1:17" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="260"/>
       <c r="B15" s="106" t="s">
         <v>292</v>
       </c>
@@ -43349,8 +43348,8 @@
       <c r="P15" s="144"/>
       <c r="Q15" s="144"/>
     </row>
-    <row r="16" spans="1:17" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="259"/>
+    <row r="16" spans="1:17" ht="94.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="260"/>
       <c r="B16" s="106" t="s">
         <v>295</v>
       </c>
@@ -43376,8 +43375,8 @@
       <c r="P16" s="144"/>
       <c r="Q16" s="144"/>
     </row>
-    <row r="17" spans="1:17" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="259"/>
+    <row r="17" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="260"/>
       <c r="B17" s="106" t="s">
         <v>298</v>
       </c>
@@ -43403,8 +43402,8 @@
       <c r="P17" s="144"/>
       <c r="Q17" s="144"/>
     </row>
-    <row r="18" spans="1:17" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="260"/>
+    <row r="18" spans="1:17" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="261"/>
       <c r="B18" s="109" t="s">
         <v>302</v>
       </c>
@@ -43430,7 +43429,7 @@
       <c r="P18" s="144"/>
       <c r="Q18" s="144"/>
     </row>
-    <row r="22" spans="1:17" ht="23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="25.5" hidden="1" x14ac:dyDescent="0.5">
       <c r="F22" s="152"/>
     </row>
   </sheetData>
@@ -43457,33 +43456,33 @@
       <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="170" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="170" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="171" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="171" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="171" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="216" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="135" customWidth="1"/>
-    <col min="9" max="1023" width="10.5" style="135" hidden="1" customWidth="1"/>
-    <col min="1024" max="1024" width="9.1640625" style="135" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="10.5" style="135" hidden="1"/>
+    <col min="1" max="1" width="30.7109375" style="170" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="170" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="171" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="171" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="171" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="216" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="135" customWidth="1"/>
+    <col min="9" max="1023" width="10.42578125" style="135" hidden="1" customWidth="1"/>
+    <col min="1024" max="1024" width="9.140625" style="135" hidden="1" customWidth="1"/>
+    <col min="1025" max="16384" width="10.42578125" style="135" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>502</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -43509,8 +43508,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="239" t="s">
+    <row r="3" spans="1:20" s="157" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="154"/>
@@ -43533,8 +43532,8 @@
       <c r="S3" s="156"/>
       <c r="T3" s="156"/>
     </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="240"/>
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="241"/>
       <c r="B4" s="158" t="s">
         <v>8</v>
       </c>
@@ -43551,8 +43550,8 @@
       </c>
       <c r="H4" s="159"/>
     </row>
-    <row r="5" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="240"/>
+    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="241"/>
       <c r="B5" s="158" t="s">
         <v>13</v>
       </c>
@@ -43569,8 +43568,8 @@
       </c>
       <c r="H5" s="159"/>
     </row>
-    <row r="6" spans="1:20" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="240"/>
+    <row r="6" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="241"/>
       <c r="B6" s="158" t="s">
         <v>16</v>
       </c>
@@ -43587,8 +43586,8 @@
       </c>
       <c r="H6" s="159"/>
     </row>
-    <row r="7" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="242"/>
       <c r="B7" s="160" t="s">
         <v>19</v>
       </c>
@@ -43605,8 +43604,8 @@
       </c>
       <c r="H7" s="161"/>
     </row>
-    <row r="8" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="236" t="s">
+    <row r="8" spans="1:20" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="237" t="s">
         <v>295</v>
       </c>
       <c r="B8" s="162"/>
@@ -43617,8 +43616,8 @@
       <c r="G8" s="213"/>
       <c r="H8" s="163"/>
     </row>
-    <row r="9" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="237"/>
+    <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="238"/>
       <c r="B9" s="164" t="s">
         <v>30</v>
       </c>
@@ -43635,8 +43634,8 @@
       </c>
       <c r="H9" s="165"/>
     </row>
-    <row r="10" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="237"/>
+    <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="238"/>
       <c r="B10" s="164" t="s">
         <v>377</v>
       </c>
@@ -43651,8 +43650,8 @@
       <c r="G10" s="186"/>
       <c r="H10" s="165"/>
     </row>
-    <row r="11" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="237"/>
+    <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="238"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
         <v>379</v>
@@ -43667,8 +43666,8 @@
       <c r="G11" s="186"/>
       <c r="H11" s="165"/>
     </row>
-    <row r="12" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="237"/>
+    <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="238"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
         <v>380</v>
@@ -43683,8 +43682,8 @@
       <c r="G12" s="186"/>
       <c r="H12" s="165"/>
     </row>
-    <row r="13" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="237"/>
+    <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="238"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
         <v>381</v>
@@ -43699,8 +43698,8 @@
       <c r="G13" s="186"/>
       <c r="H13" s="165"/>
     </row>
-    <row r="14" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="237"/>
+    <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="238"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
         <v>382</v>
@@ -43715,8 +43714,8 @@
       <c r="G14" s="186"/>
       <c r="H14" s="165"/>
     </row>
-    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="237"/>
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="238"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
         <v>384</v>
@@ -43731,8 +43730,8 @@
       <c r="G15" s="186"/>
       <c r="H15" s="165"/>
     </row>
-    <row r="16" spans="1:20" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="237"/>
+    <row r="16" spans="1:20" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="238"/>
       <c r="B16" s="164" t="s">
         <v>386</v>
       </c>
@@ -43747,8 +43746,8 @@
       <c r="G16" s="186"/>
       <c r="H16" s="165"/>
     </row>
-    <row r="17" spans="1:19" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="238"/>
+    <row r="17" spans="1:19" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="239"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
         <v>384</v>
@@ -43763,8 +43762,8 @@
       <c r="G17" s="187"/>
       <c r="H17" s="167"/>
     </row>
-    <row r="18" spans="1:19" s="157" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="239" t="s">
+    <row r="18" spans="1:19" s="157" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="240" t="s">
         <v>388</v>
       </c>
       <c r="B18" s="168"/>
@@ -43786,8 +43785,8 @@
       <c r="R18" s="156"/>
       <c r="S18" s="156"/>
     </row>
-    <row r="19" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="240"/>
+    <row r="19" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="241"/>
       <c r="B19" s="158" t="s">
         <v>389</v>
       </c>
@@ -43797,15 +43796,15 @@
       </c>
       <c r="E19" s="158"/>
       <c r="F19" s="158" t="s">
-        <v>518</v>
+        <v>566</v>
       </c>
       <c r="G19" s="183" t="s">
         <v>43</v>
       </c>
       <c r="H19" s="159"/>
     </row>
-    <row r="20" spans="1:19" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="240"/>
+    <row r="20" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="241"/>
       <c r="B20" s="158"/>
       <c r="C20" s="158" t="s">
         <v>390</v>
@@ -43820,8 +43819,8 @@
       <c r="G20" s="183"/>
       <c r="H20" s="159"/>
     </row>
-    <row r="21" spans="1:19" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="240"/>
+    <row r="21" spans="1:19" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="241"/>
       <c r="B21" s="158"/>
       <c r="C21" s="158" t="s">
         <v>393</v>
@@ -43836,8 +43835,8 @@
       <c r="G21" s="183"/>
       <c r="H21" s="159"/>
     </row>
-    <row r="22" spans="1:19" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="241"/>
+    <row r="22" spans="1:19" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="242"/>
       <c r="B22" s="160"/>
       <c r="C22" s="160" t="s">
         <v>395</v>
@@ -43881,32 +43880,32 @@
       <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="21" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="21" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="21" customWidth="1"/>
     <col min="9" max="1024" width="0" style="21" hidden="1" customWidth="1"/>
-    <col min="1025" max="16384" width="9.1640625" style="22" hidden="1"/>
+    <col min="1025" max="16384" width="9.140625" style="22" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="242" t="s">
+    <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="243" t="s">
         <v>503</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
-    <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -44948,8 +44947,8 @@
       <c r="AMI2" s="41"/>
       <c r="AMJ2" s="41"/>
     </row>
-    <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="239" t="s">
+    <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="240" t="s">
         <v>397</v>
       </c>
       <c r="B3" s="172"/>
@@ -44960,8 +44959,8 @@
       <c r="G3" s="172"/>
       <c r="H3" s="173"/>
     </row>
-    <row r="4" spans="1:1024" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="240"/>
+    <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
         <v>207</v>
       </c>
@@ -45992,8 +45991,8 @@
       <c r="AMI4" s="23"/>
       <c r="AMJ4" s="23"/>
     </row>
-    <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="240"/>
+    <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
         <v>260</v>
       </c>
@@ -47024,8 +47023,8 @@
       <c r="AMI5" s="23"/>
       <c r="AMJ5" s="23"/>
     </row>
-    <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="240"/>
+    <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
         <v>213</v>
       </c>
@@ -48056,8 +48055,8 @@
       <c r="AMI6" s="23"/>
       <c r="AMJ6" s="23"/>
     </row>
-    <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="240"/>
+    <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
         <v>400</v>
       </c>
@@ -49088,8 +49087,8 @@
       <c r="AMI7" s="23"/>
       <c r="AMJ7" s="23"/>
     </row>
-    <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="240"/>
+    <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
         <v>402</v>
       </c>
@@ -50120,8 +50119,8 @@
       <c r="AMI8" s="23"/>
       <c r="AMJ8" s="23"/>
     </row>
-    <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="240"/>
+    <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
         <v>404</v>
       </c>
@@ -51152,8 +51151,8 @@
       <c r="AMI9" s="23"/>
       <c r="AMJ9" s="23"/>
     </row>
-    <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="240"/>
+    <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
         <v>406</v>
       </c>
@@ -52184,8 +52183,8 @@
       <c r="AMI10" s="23"/>
       <c r="AMJ10" s="23"/>
     </row>
-    <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="240"/>
+    <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="241"/>
       <c r="B11" s="47" t="s">
         <v>408</v>
       </c>
@@ -53216,8 +53215,8 @@
       <c r="AMI11" s="23"/>
       <c r="AMJ11" s="23"/>
     </row>
-    <row r="12" spans="1:1024" s="26" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="241"/>
+    <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="242"/>
       <c r="B12" s="51" t="s">
         <v>410</v>
       </c>
@@ -54248,8 +54247,8 @@
       <c r="AMI12" s="25"/>
       <c r="AMJ12" s="25"/>
     </row>
-    <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="236" t="s">
+    <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="237" t="s">
         <v>412</v>
       </c>
       <c r="B13" s="175"/>
@@ -54261,8 +54260,8 @@
       <c r="H13" s="176"/>
       <c r="AMJ13" s="21"/>
     </row>
-    <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="237"/>
+    <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="238"/>
       <c r="B14" s="69" t="s">
         <v>207</v>
       </c>
@@ -54277,8 +54276,8 @@
       <c r="G14" s="69"/>
       <c r="H14" s="177"/>
     </row>
-    <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="237"/>
+    <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="238"/>
       <c r="B15" s="69" t="s">
         <v>260</v>
       </c>
@@ -54293,8 +54292,8 @@
       <c r="G15" s="69"/>
       <c r="H15" s="177"/>
     </row>
-    <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="237"/>
+    <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="238"/>
       <c r="B16" s="69" t="s">
         <v>213</v>
       </c>
@@ -54309,8 +54308,8 @@
       <c r="G16" s="69"/>
       <c r="H16" s="177"/>
     </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="237"/>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="238"/>
       <c r="B17" s="69" t="s">
         <v>266</v>
       </c>
@@ -54325,8 +54324,8 @@
       <c r="G17" s="69"/>
       <c r="H17" s="177"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="237"/>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="238"/>
       <c r="B18" s="69" t="s">
         <v>210</v>
       </c>
@@ -54341,8 +54340,8 @@
       <c r="G18" s="69"/>
       <c r="H18" s="177"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="237"/>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="238"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -54357,8 +54356,8 @@
       <c r="G19" s="69"/>
       <c r="H19" s="177"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="237"/>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="238"/>
       <c r="B20" s="69" t="s">
         <v>418</v>
       </c>
@@ -54373,8 +54372,8 @@
       <c r="G20" s="69"/>
       <c r="H20" s="177"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="237"/>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="238"/>
       <c r="B21" s="69" t="s">
         <v>319</v>
       </c>
@@ -54389,8 +54388,8 @@
       <c r="G21" s="69"/>
       <c r="H21" s="177"/>
     </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="237"/>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="238"/>
       <c r="B22" s="69" t="s">
         <v>421</v>
       </c>
@@ -54405,8 +54404,8 @@
       <c r="G22" s="69"/>
       <c r="H22" s="177"/>
     </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="237"/>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="238"/>
       <c r="B23" s="69" t="s">
         <v>423</v>
       </c>
@@ -54421,8 +54420,8 @@
       <c r="G23" s="69"/>
       <c r="H23" s="177"/>
     </row>
-    <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="238"/>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="239"/>
       <c r="B24" s="73" t="s">
         <v>425</v>
       </c>
@@ -54437,8 +54436,8 @@
       <c r="G24" s="73"/>
       <c r="H24" s="178"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="239" t="s">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="240" t="s">
         <v>354</v>
       </c>
       <c r="B25" s="179"/>
@@ -54449,8 +54448,8 @@
       <c r="G25" s="179"/>
       <c r="H25" s="180"/>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="240"/>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="241"/>
       <c r="B26" s="47" t="s">
         <v>207</v>
       </c>
@@ -54465,8 +54464,8 @@
       <c r="G26" s="47"/>
       <c r="H26" s="174"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="240"/>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="241"/>
       <c r="B27" s="47" t="s">
         <v>260</v>
       </c>
@@ -54481,8 +54480,8 @@
       <c r="G27" s="47"/>
       <c r="H27" s="174"/>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="240"/>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="241"/>
       <c r="B28" s="47" t="s">
         <v>213</v>
       </c>
@@ -54497,8 +54496,8 @@
       <c r="G28" s="47"/>
       <c r="H28" s="174"/>
     </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="240"/>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="241"/>
       <c r="B29" s="47" t="s">
         <v>266</v>
       </c>
@@ -54513,8 +54512,8 @@
       <c r="G29" s="47"/>
       <c r="H29" s="174"/>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="240"/>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="241"/>
       <c r="B30" s="47" t="s">
         <v>430</v>
       </c>
@@ -54529,8 +54528,8 @@
       <c r="G30" s="47"/>
       <c r="H30" s="174"/>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="240"/>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="241"/>
       <c r="B31" s="47" t="s">
         <v>210</v>
       </c>
@@ -54545,8 +54544,8 @@
       <c r="G31" s="47"/>
       <c r="H31" s="174"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="240"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="241"/>
       <c r="B32" s="47" t="s">
         <v>408</v>
       </c>
@@ -54561,8 +54560,8 @@
       <c r="G32" s="47"/>
       <c r="H32" s="174"/>
     </row>
-    <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="240"/>
+    <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="241"/>
       <c r="B33" s="47" t="s">
         <v>434</v>
       </c>
@@ -54577,8 +54576,8 @@
       <c r="G33" s="47"/>
       <c r="H33" s="174"/>
     </row>
-    <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="240"/>
+    <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="241"/>
       <c r="B34" s="47" t="s">
         <v>5</v>
       </c>
@@ -54593,8 +54592,8 @@
       <c r="G34" s="47"/>
       <c r="H34" s="174"/>
     </row>
-    <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="240"/>
+    <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="241"/>
       <c r="B35" s="47" t="s">
         <v>437</v>
       </c>
@@ -54609,8 +54608,8 @@
       <c r="G35" s="47"/>
       <c r="H35" s="174"/>
     </row>
-    <row r="36" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="241"/>
+    <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="242"/>
       <c r="B36" s="51" t="s">
         <v>439</v>
       </c>
@@ -54625,8 +54624,8 @@
       <c r="G36" s="51"/>
       <c r="H36" s="181"/>
     </row>
-    <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="236" t="s">
+    <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="237" t="s">
         <v>282</v>
       </c>
       <c r="B37" s="175"/>
@@ -54638,8 +54637,8 @@
       <c r="H37" s="176"/>
       <c r="AMJ37" s="21"/>
     </row>
-    <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="237"/>
+    <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="238"/>
       <c r="B38" s="69" t="s">
         <v>207</v>
       </c>
@@ -54654,8 +54653,8 @@
       <c r="G38" s="69"/>
       <c r="H38" s="177"/>
     </row>
-    <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="237"/>
+    <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="238"/>
       <c r="B39" s="69" t="s">
         <v>260</v>
       </c>
@@ -54670,8 +54669,8 @@
       <c r="G39" s="69"/>
       <c r="H39" s="177"/>
     </row>
-    <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="237"/>
+    <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="238"/>
       <c r="B40" s="69" t="s">
         <v>213</v>
       </c>
@@ -54686,8 +54685,8 @@
       <c r="G40" s="69"/>
       <c r="H40" s="177"/>
     </row>
-    <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="237"/>
+    <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="238"/>
       <c r="B41" s="69" t="s">
         <v>266</v>
       </c>
@@ -54702,8 +54701,8 @@
       <c r="G41" s="69"/>
       <c r="H41" s="177"/>
     </row>
-    <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="237"/>
+    <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="238"/>
       <c r="B42" s="69" t="s">
         <v>444</v>
       </c>
@@ -54718,8 +54717,8 @@
       <c r="G42" s="69"/>
       <c r="H42" s="177"/>
     </row>
-    <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="237"/>
+    <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="238"/>
       <c r="B43" s="69" t="s">
         <v>354</v>
       </c>
@@ -54734,8 +54733,8 @@
       <c r="G43" s="69"/>
       <c r="H43" s="177"/>
     </row>
-    <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="237"/>
+    <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="238"/>
       <c r="B44" s="69" t="s">
         <v>210</v>
       </c>
@@ -54750,8 +54749,8 @@
       <c r="G44" s="69"/>
       <c r="H44" s="177"/>
     </row>
-    <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="237"/>
+    <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="238"/>
       <c r="B45" s="69" t="s">
         <v>408</v>
       </c>
@@ -54766,8 +54765,8 @@
       <c r="G45" s="69"/>
       <c r="H45" s="177"/>
     </row>
-    <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="237"/>
+    <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="238"/>
       <c r="B46" s="69" t="s">
         <v>449</v>
       </c>
@@ -54782,8 +54781,8 @@
       <c r="G46" s="69"/>
       <c r="H46" s="177"/>
     </row>
-    <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="237"/>
+    <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="238"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -54798,8 +54797,8 @@
       <c r="G47" s="69"/>
       <c r="H47" s="177"/>
     </row>
-    <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="238"/>
+    <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="239"/>
       <c r="B48" s="73" t="s">
         <v>421</v>
       </c>

</xml_diff>

<commit_message>
fix: improve mounted in/out descriptions
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CA294C-C57D-4AA1-ABB1-366C51C7DACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3519BDEC-F0BF-4FDF-B47F-DDF5E48412EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="24270" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -1449,18 +1449,6 @@
     <t>List(String)</t>
   </si>
   <si>
-    <t>/data</t>
-  </si>
-  <si>
-    <t>/data_out</t>
-  </si>
-  <si>
-    <t>directories shared on the host where this microservice can find required inputs</t>
-  </si>
-  <si>
-    <t>directories shared on the host where this microservice can find required outputs</t>
-  </si>
-  <si>
     <t>configurationData</t>
   </si>
   <si>
@@ -1814,6 +1802,18 @@
   </si>
   <si>
     <t>Mapping the available Data assets in this DMA Tuple to available Microservices. One Microservice may require several Data assets, specified by their UUIDs.</t>
+  </si>
+  <si>
+    <t>["/data", "/cfg"]</t>
+  </si>
+  <si>
+    <t>["/data_out", "/results"]</t>
+  </si>
+  <si>
+    <t>A note for developers of co-operating Microservices. A list of directories that should be shared to the host by where this microservice can find required inputs</t>
+  </si>
+  <si>
+    <t>A note for developers of co-operating Microservices.  A list of directories that are shared on the host where this microservice will store its outputs</t>
   </si>
 </sst>
 </file>
@@ -3217,60 +3217,20 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3295,6 +3255,46 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4175,11 +4175,11 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4196,16 +4196,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>496</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>492</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -4234,7 +4234,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="235" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4246,7 +4246,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="236"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4261,12 +4261,12 @@
         <v>11</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="236"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4286,7 +4286,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="236"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4306,13 +4306,13 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="246"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="47" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>20</v>
@@ -4321,12 +4321,12 @@
         <v>21</v>
       </c>
       <c r="G7" s="183" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="246"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4346,7 +4346,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="246"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4355,10 +4355,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="G9" s="183" t="s">
         <v>12</v>
@@ -4366,7 +4366,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="246"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4386,7 +4386,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="247"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4406,7 +4406,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="248" t="s">
+      <c r="A12" s="238" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="217"/>
@@ -4418,7 +4418,7 @@
       <c r="H12" s="220"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="249"/>
+      <c r="A13" s="239"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="249"/>
+      <c r="A14" s="239"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>456</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F14" s="55" t="s">
         <v>457</v>
@@ -4458,19 +4458,19 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="249"/>
+      <c r="A15" s="239"/>
       <c r="B15" s="55" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="55" t="s">
+        <v>464</v>
+      </c>
+      <c r="E15" s="57" t="s">
         <v>468</v>
       </c>
-      <c r="E15" s="57" t="s">
-        <v>472</v>
-      </c>
       <c r="F15" s="55" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G15" s="188" t="s">
         <v>43</v>
@@ -5493,8 +5493,8 @@
       <c r="AMI15" s="4"/>
       <c r="AMJ15" s="4"/>
     </row>
-    <row r="16" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="249"/>
+    <row r="16" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A16" s="239"/>
       <c r="B16" s="55" t="s">
         <v>459</v>
       </c>
@@ -5503,10 +5503,10 @@
         <v>461</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>462</v>
+        <v>563</v>
       </c>
       <c r="F16" s="55" t="s">
-        <v>464</v>
+        <v>565</v>
       </c>
       <c r="G16" s="188" t="s">
         <v>43</v>
@@ -6529,8 +6529,8 @@
       <c r="AMI16" s="4"/>
       <c r="AMJ16" s="4"/>
     </row>
-    <row r="17" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="250"/>
+    <row r="17" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="240"/>
       <c r="B17" s="221" t="s">
         <v>460</v>
       </c>
@@ -6539,10 +6539,10 @@
         <v>461</v>
       </c>
       <c r="E17" s="223" t="s">
-        <v>463</v>
+        <v>564</v>
       </c>
       <c r="F17" s="221" t="s">
-        <v>465</v>
+        <v>566</v>
       </c>
       <c r="G17" s="224" t="s">
         <v>43</v>
@@ -7818,7 +7818,7 @@
       <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="237" t="s">
+      <c r="A31" s="243" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="62"/>
@@ -7830,7 +7830,7 @@
       <c r="H31" s="64"/>
     </row>
     <row r="32" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="238"/>
+      <c r="A32" s="244"/>
       <c r="B32" s="65" t="s">
         <v>73</v>
       </c>
@@ -7850,7 +7850,7 @@
       <c r="H32" s="68"/>
     </row>
     <row r="33" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="238"/>
+      <c r="A33" s="244"/>
       <c r="B33" s="69" t="s">
         <v>76</v>
       </c>
@@ -7870,7 +7870,7 @@
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="238"/>
+      <c r="A34" s="244"/>
       <c r="B34" s="69" t="s">
         <v>79</v>
       </c>
@@ -7890,7 +7890,7 @@
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="239"/>
+      <c r="A35" s="245"/>
       <c r="B35" s="73" t="s">
         <v>82</v>
       </c>
@@ -7910,7 +7910,7 @@
       <c r="H35" s="76"/>
     </row>
     <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="240" t="s">
+      <c r="A36" s="246" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="59"/>
@@ -8959,7 +8959,7 @@
     </row>
     <row r="38" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="241"/>
-      <c r="B38" s="231" t="s">
+      <c r="B38" s="233" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -9997,7 +9997,7 @@
     </row>
     <row r="39" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="241"/>
-      <c r="B39" s="231"/>
+      <c r="B39" s="233"/>
       <c r="C39" s="47" t="s">
         <v>94</v>
       </c>
@@ -11033,7 +11033,7 @@
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="241"/>
-      <c r="B40" s="231"/>
+      <c r="B40" s="233"/>
       <c r="C40" s="47" t="s">
         <v>98</v>
       </c>
@@ -12069,7 +12069,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A41" s="241"/>
-      <c r="B41" s="231"/>
+      <c r="B41" s="233"/>
       <c r="C41" s="47" t="s">
         <v>102</v>
       </c>
@@ -13105,7 +13105,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="241"/>
-      <c r="B42" s="231"/>
+      <c r="B42" s="233"/>
       <c r="C42" s="47" t="s">
         <v>106</v>
       </c>
@@ -14141,7 +14141,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="241"/>
-      <c r="B43" s="231"/>
+      <c r="B43" s="233"/>
       <c r="C43" s="47" t="s">
         <v>110</v>
       </c>
@@ -15177,7 +15177,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="241"/>
-      <c r="B44" s="231"/>
+      <c r="B44" s="233"/>
       <c r="C44" s="47" t="s">
         <v>114</v>
       </c>
@@ -16213,7 +16213,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A45" s="241"/>
-      <c r="B45" s="231"/>
+      <c r="B45" s="233"/>
       <c r="C45" s="47" t="s">
         <v>118</v>
       </c>
@@ -17249,7 +17249,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="241"/>
-      <c r="B46" s="231"/>
+      <c r="B46" s="233"/>
       <c r="C46" s="47" t="s">
         <v>122</v>
       </c>
@@ -18285,7 +18285,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A47" s="241"/>
-      <c r="B47" s="231"/>
+      <c r="B47" s="233"/>
       <c r="C47" s="47" t="s">
         <v>126</v>
       </c>
@@ -19321,7 +19321,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="241"/>
-      <c r="B48" s="231"/>
+      <c r="B48" s="233"/>
       <c r="C48" s="47" t="s">
         <v>130</v>
       </c>
@@ -20357,7 +20357,7 @@
     </row>
     <row r="49" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="242"/>
-      <c r="B49" s="232"/>
+      <c r="B49" s="234"/>
       <c r="C49" s="51" t="s">
         <v>134</v>
       </c>
@@ -20368,7 +20368,7 @@
         <v>136</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G49" s="184" t="s">
         <v>43</v>
@@ -21392,7 +21392,7 @@
       <c r="AMJ49" s="15"/>
     </row>
     <row r="50" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="237" t="s">
+      <c r="A50" s="243" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="77"/>
@@ -21404,7 +21404,7 @@
       <c r="H50" s="79"/>
     </row>
     <row r="51" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="238"/>
+      <c r="A51" s="244"/>
       <c r="B51" s="80" t="s">
         <v>138</v>
       </c>
@@ -21424,8 +21424,8 @@
       <c r="H51" s="83"/>
     </row>
     <row r="52" spans="1:1024" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="238"/>
-      <c r="B52" s="233" t="s">
+      <c r="A52" s="244"/>
+      <c r="B52" s="247" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
@@ -21446,8 +21446,8 @@
       <c r="H52" s="83"/>
     </row>
     <row r="53" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A53" s="238"/>
-      <c r="B53" s="233"/>
+      <c r="A53" s="244"/>
+      <c r="B53" s="247"/>
       <c r="C53" s="80" t="s">
         <v>94</v>
       </c>
@@ -21466,8 +21466,8 @@
       <c r="H53" s="83"/>
     </row>
     <row r="54" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="238"/>
-      <c r="B54" s="233"/>
+      <c r="A54" s="244"/>
+      <c r="B54" s="247"/>
       <c r="C54" s="80" t="s">
         <v>98</v>
       </c>
@@ -21486,8 +21486,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="238"/>
-      <c r="B55" s="233"/>
+      <c r="A55" s="244"/>
+      <c r="B55" s="247"/>
       <c r="C55" s="80" t="s">
         <v>102</v>
       </c>
@@ -21506,8 +21506,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="238"/>
-      <c r="B56" s="233"/>
+      <c r="A56" s="244"/>
+      <c r="B56" s="247"/>
       <c r="C56" s="80" t="s">
         <v>106</v>
       </c>
@@ -21526,8 +21526,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="238"/>
-      <c r="B57" s="233"/>
+      <c r="A57" s="244"/>
+      <c r="B57" s="247"/>
       <c r="C57" s="80" t="s">
         <v>110</v>
       </c>
@@ -21546,8 +21546,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="238"/>
-      <c r="B58" s="233"/>
+      <c r="A58" s="244"/>
+      <c r="B58" s="247"/>
       <c r="C58" s="80" t="s">
         <v>114</v>
       </c>
@@ -21566,8 +21566,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="238"/>
-      <c r="B59" s="233"/>
+      <c r="A59" s="244"/>
+      <c r="B59" s="247"/>
       <c r="C59" s="80" t="s">
         <v>118</v>
       </c>
@@ -21586,8 +21586,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="238"/>
-      <c r="B60" s="233"/>
+      <c r="A60" s="244"/>
+      <c r="B60" s="247"/>
       <c r="C60" s="80" t="s">
         <v>122</v>
       </c>
@@ -21606,8 +21606,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="238"/>
-      <c r="B61" s="233"/>
+      <c r="A61" s="244"/>
+      <c r="B61" s="247"/>
       <c r="C61" s="80" t="s">
         <v>126</v>
       </c>
@@ -21626,8 +21626,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="238"/>
-      <c r="B62" s="233"/>
+      <c r="A62" s="244"/>
+      <c r="B62" s="247"/>
       <c r="C62" s="80" t="s">
         <v>130</v>
       </c>
@@ -21646,8 +21646,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="239"/>
-      <c r="B63" s="234"/>
+      <c r="A63" s="245"/>
+      <c r="B63" s="248"/>
       <c r="C63" s="85" t="s">
         <v>134</v>
       </c>
@@ -21658,7 +21658,7 @@
         <v>136</v>
       </c>
       <c r="F63" s="85" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G63" s="187" t="s">
         <v>43</v>
@@ -21666,7 +21666,7 @@
       <c r="H63" s="87"/>
     </row>
     <row r="64" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="240" t="s">
+      <c r="A64" s="246" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="59"/>
@@ -24766,7 +24766,7 @@
       <c r="AMJ66" s="13"/>
     </row>
     <row r="67" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="237" t="s">
+      <c r="A67" s="243" t="s">
         <v>154</v>
       </c>
       <c r="B67" s="29"/>
@@ -24778,7 +24778,7 @@
       <c r="H67" s="64"/>
     </row>
     <row r="68" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="238"/>
+      <c r="A68" s="244"/>
       <c r="B68" s="69" t="s">
         <v>155</v>
       </c>
@@ -24796,8 +24796,8 @@
       <c r="H68" s="72"/>
     </row>
     <row r="69" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="238"/>
-      <c r="B69" s="235" t="s">
+      <c r="A69" s="244"/>
+      <c r="B69" s="249" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="69" t="s">
@@ -24818,8 +24818,8 @@
       <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="238"/>
-      <c r="B70" s="235"/>
+      <c r="A70" s="244"/>
+      <c r="B70" s="249"/>
       <c r="C70" s="69" t="s">
         <v>30</v>
       </c>
@@ -24838,8 +24838,8 @@
       <c r="H70" s="72"/>
     </row>
     <row r="71" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="238"/>
-      <c r="B71" s="235"/>
+      <c r="A71" s="244"/>
+      <c r="B71" s="249"/>
       <c r="C71" s="69" t="s">
         <v>12</v>
       </c>
@@ -24858,8 +24858,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="238"/>
-      <c r="B72" s="235"/>
+      <c r="A72" s="244"/>
+      <c r="B72" s="249"/>
       <c r="C72" s="69" t="s">
         <v>167</v>
       </c>
@@ -24878,8 +24878,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="239"/>
-      <c r="B73" s="236"/>
+      <c r="A73" s="245"/>
+      <c r="B73" s="250"/>
       <c r="C73" s="73" t="s">
         <v>25</v>
       </c>
@@ -24898,7 +24898,7 @@
       <c r="H73" s="76"/>
     </row>
     <row r="74" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="240" t="s">
+      <c r="A74" s="246" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="31"/>
@@ -26961,7 +26961,7 @@
     </row>
     <row r="76" spans="1:1024" s="14" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="241"/>
-      <c r="B76" s="231" t="s">
+      <c r="B76" s="233" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="47" t="s">
@@ -27999,7 +27999,7 @@
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A77" s="241"/>
-      <c r="B77" s="231"/>
+      <c r="B77" s="233"/>
       <c r="C77" s="47" t="s">
         <v>179</v>
       </c>
@@ -29035,7 +29035,7 @@
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="241"/>
-      <c r="B78" s="231"/>
+      <c r="B78" s="233"/>
       <c r="C78" s="47" t="s">
         <v>182</v>
       </c>
@@ -30071,7 +30071,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="241"/>
-      <c r="B79" s="231"/>
+      <c r="B79" s="233"/>
       <c r="C79" s="47" t="s">
         <v>185</v>
       </c>
@@ -31107,7 +31107,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="242"/>
-      <c r="B80" s="232"/>
+      <c r="B80" s="234"/>
       <c r="C80" s="51" t="s">
         <v>25</v>
       </c>
@@ -32216,6 +32216,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="B52:B63"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="A50:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A74:A80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A3:A11"/>
@@ -32223,13 +32230,6 @@
     <mergeCell ref="A18:A30"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A36:A49"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B52:B63"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="A50:A63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A74:A80"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -32269,16 +32269,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>497</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -32307,7 +32307,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="235" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -32319,7 +32319,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="236"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -32334,12 +32334,12 @@
         <v>192</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="236"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -32359,7 +32359,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="236"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -32379,7 +32379,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="246"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -32399,7 +32399,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="246"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -32419,7 +32419,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="246"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -32439,13 +32439,13 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="246"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="47" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>20</v>
@@ -32454,12 +32454,12 @@
         <v>201</v>
       </c>
       <c r="G10" s="183" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="247"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -32523,7 +32523,7 @@
         <v>454</v>
       </c>
       <c r="F14" s="103" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G14" s="186" t="s">
         <v>12</v>
@@ -32569,16 +32569,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>498</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -32607,7 +32607,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="235" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -32657,7 +32657,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="236"/>
       <c r="B4" s="105" t="s">
         <v>207</v>
       </c>
@@ -32670,12 +32670,12 @@
         <v>209</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="236"/>
       <c r="B5" s="105" t="s">
         <v>210</v>
       </c>
@@ -32691,23 +32691,23 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="236"/>
       <c r="B6" s="105" t="s">
         <v>213</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="246"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="105" t="s">
         <v>214</v>
       </c>
@@ -32717,13 +32717,13 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G7" s="197"/>
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="246"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="105" t="s">
         <v>215</v>
       </c>
@@ -32739,7 +32739,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="246"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="105" t="s">
         <v>217</v>
       </c>
@@ -32749,7 +32749,7 @@
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="G9" s="197" t="s">
         <v>43</v>
@@ -32757,7 +32757,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="246"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="105" t="s">
         <v>219</v>
       </c>
@@ -32786,7 +32786,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246"/>
+      <c r="A11" s="236"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -32802,7 +32802,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="246"/>
+      <c r="A12" s="236"/>
       <c r="B12" s="105" t="s">
         <v>223</v>
       </c>
@@ -32812,7 +32812,7 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G12" s="197" t="s">
         <v>43</v>
@@ -32820,7 +32820,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="246"/>
+      <c r="A13" s="236"/>
       <c r="B13" s="105" t="s">
         <v>225</v>
       </c>
@@ -32838,9 +32838,9 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="246"/>
+      <c r="A14" s="236"/>
       <c r="B14" s="105" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
@@ -32848,7 +32848,7 @@
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="105" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G14" s="197" t="s">
         <v>43</v>
@@ -32856,7 +32856,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="247"/>
+      <c r="A15" s="237"/>
       <c r="B15" s="108" t="s">
         <v>229</v>
       </c>
@@ -32872,7 +32872,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="237" t="s">
+      <c r="A16" s="243" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -32885,13 +32885,13 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="238"/>
+      <c r="A17" s="244"/>
       <c r="B17" s="113" t="s">
         <v>232</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E17" s="114"/>
       <c r="F17" s="113" t="s">
@@ -32901,7 +32901,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="238"/>
+      <c r="A18" s="244"/>
       <c r="B18" s="113"/>
       <c r="C18" s="114" t="s">
         <v>1</v>
@@ -32911,13 +32911,13 @@
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="G18" s="200"/>
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="238"/>
+      <c r="A19" s="244"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>210</v>
@@ -32927,163 +32927,163 @@
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="G19" s="200"/>
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="238"/>
+      <c r="A20" s="244"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D20" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G20" s="200"/>
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="238"/>
+      <c r="A21" s="244"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D21" s="113" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G21" s="200"/>
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="238"/>
+      <c r="A22" s="244"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G22" s="200"/>
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="238"/>
+      <c r="A23" s="244"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D23" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="G23" s="200"/>
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="238"/>
+      <c r="A24" s="244"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G24" s="200"/>
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="238"/>
+      <c r="A25" s="244"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="D25" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G25" s="200"/>
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="238"/>
+      <c r="A26" s="244"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G26" s="200"/>
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="238"/>
+      <c r="A27" s="244"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D27" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="G27" s="200"/>
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="238"/>
+      <c r="A28" s="244"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="G28" s="200"/>
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="238"/>
+      <c r="A29" s="244"/>
       <c r="B29" s="113" t="s">
         <v>234</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="113" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
@@ -33093,7 +33093,7 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="238"/>
+      <c r="A30" s="244"/>
       <c r="B30" s="226"/>
       <c r="C30" s="114" t="s">
         <v>1</v>
@@ -33103,13 +33103,13 @@
       </c>
       <c r="E30" s="227"/>
       <c r="F30" s="113" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G30" s="228"/>
       <c r="H30" s="229"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="238"/>
+      <c r="A31" s="244"/>
       <c r="B31" s="226"/>
       <c r="C31" s="114" t="s">
         <v>210</v>
@@ -33119,157 +33119,157 @@
       </c>
       <c r="E31" s="227"/>
       <c r="F31" s="113" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="G31" s="228"/>
       <c r="H31" s="229"/>
     </row>
     <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="238"/>
+      <c r="A32" s="244"/>
       <c r="B32" s="226"/>
       <c r="C32" s="114" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D32" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E32" s="227"/>
       <c r="F32" s="113" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="G32" s="228"/>
       <c r="H32" s="229"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="238"/>
+      <c r="A33" s="244"/>
       <c r="B33" s="226"/>
       <c r="C33" s="114" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="E33" s="227"/>
       <c r="F33" s="113" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="G33" s="228"/>
       <c r="H33" s="229"/>
     </row>
     <row r="34" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="238"/>
+      <c r="A34" s="244"/>
       <c r="B34" s="226"/>
       <c r="C34" s="114" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D34" s="113" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E34" s="227"/>
       <c r="F34" s="113" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="G34" s="228"/>
       <c r="H34" s="229"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="238"/>
+      <c r="A35" s="244"/>
       <c r="B35" s="226"/>
       <c r="C35" s="114" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D35" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E35" s="227"/>
       <c r="F35" s="113" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G35" s="228"/>
       <c r="H35" s="229"/>
     </row>
     <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="238"/>
+      <c r="A36" s="244"/>
       <c r="B36" s="226"/>
       <c r="C36" s="114" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E36" s="227"/>
       <c r="F36" s="113" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G36" s="228"/>
       <c r="H36" s="229"/>
     </row>
     <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="238"/>
+      <c r="A37" s="244"/>
       <c r="B37" s="226"/>
       <c r="C37" s="114" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="D37" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E37" s="227"/>
       <c r="F37" s="113" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G37" s="228"/>
       <c r="H37" s="229"/>
     </row>
     <row r="38" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="238"/>
+      <c r="A38" s="244"/>
       <c r="B38" s="226"/>
       <c r="C38" s="114" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D38" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E38" s="227"/>
       <c r="F38" s="113" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G38" s="228"/>
       <c r="H38" s="229"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="238"/>
+      <c r="A39" s="244"/>
       <c r="B39" s="226"/>
       <c r="C39" s="114" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D39" s="113" t="s">
         <v>224</v>
       </c>
       <c r="E39" s="227"/>
       <c r="F39" s="113" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="G39" s="228"/>
       <c r="H39" s="229"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="238"/>
+      <c r="A40" s="244"/>
       <c r="B40" s="226"/>
       <c r="C40" s="114" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D40" s="113" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E40" s="227"/>
       <c r="F40" s="113" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="G40" s="228"/>
       <c r="H40" s="229"/>
     </row>
     <row r="41" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="239"/>
+      <c r="A41" s="245"/>
       <c r="B41" s="116" t="s">
         <v>236</v>
       </c>
@@ -33279,7 +33279,7 @@
       </c>
       <c r="E41" s="117"/>
       <c r="F41" s="116" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="G41" s="201" t="s">
         <v>43</v>
@@ -33287,7 +33287,7 @@
       <c r="H41" s="118"/>
     </row>
     <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="240" t="s">
+      <c r="A42" s="246" t="s">
         <v>237</v>
       </c>
       <c r="B42" s="119"/>
@@ -33374,7 +33374,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="237" t="s">
+      <c r="A44" s="243" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="111"/>
@@ -33387,7 +33387,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="238"/>
+      <c r="A45" s="244"/>
       <c r="B45" s="113" t="s">
         <v>73</v>
       </c>
@@ -33405,7 +33405,7 @@
       <c r="H45" s="115"/>
     </row>
     <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="238"/>
+      <c r="A46" s="244"/>
       <c r="B46" s="113" t="s">
         <v>76</v>
       </c>
@@ -33423,7 +33423,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="239"/>
+      <c r="A47" s="245"/>
       <c r="B47" s="116" t="s">
         <v>79</v>
       </c>
@@ -33441,7 +33441,7 @@
       <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="240" t="s">
+      <c r="A48" s="246" t="s">
         <v>244</v>
       </c>
       <c r="B48" s="121"/>
@@ -33654,8 +33654,8 @@
       <c r="H57" s="110"/>
     </row>
     <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="237" t="s">
-        <v>510</v>
+      <c r="A58" s="243" t="s">
+        <v>506</v>
       </c>
       <c r="B58" s="123"/>
       <c r="C58" s="123"/>
@@ -33667,7 +33667,7 @@
       <c r="AMJ58" s="5"/>
     </row>
     <row r="59" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="239"/>
+      <c r="A59" s="245"/>
       <c r="B59" s="116" t="s">
         <v>5</v>
       </c>
@@ -33729,16 +33729,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>499</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -34784,7 +34784,7 @@
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="253" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
@@ -34823,7 +34823,7 @@
         <v>305</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="126"/>
     </row>
@@ -34843,14 +34843,14 @@
         <v>307</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="254"/>
       <c r="B6" s="105" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
@@ -34863,7 +34863,7 @@
         <v>308</v>
       </c>
       <c r="G6" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H6" s="126"/>
     </row>
@@ -34877,13 +34877,13 @@
         <v>310</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F7" s="105" t="s">
         <v>311</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H7" s="126"/>
     </row>
@@ -34910,7 +34910,7 @@
         <v>211</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>313</v>
@@ -35939,17 +35939,17 @@
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="258"/>
       <c r="B10" s="113" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
         <v>211</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G10" s="200" t="s">
         <v>43</v>
@@ -36982,7 +36982,7 @@
         <v>211</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F11" s="113" t="s">
         <v>318</v>
@@ -38011,14 +38011,14 @@
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="258"/>
       <c r="B12" s="113" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
         <v>319</v>
       </c>
       <c r="E12" s="117" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F12" s="116" t="s">
         <v>320</v>
@@ -39054,7 +39054,7 @@
         <v>315</v>
       </c>
       <c r="E13" s="114" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F13" s="113" t="s">
         <v>316</v>
@@ -40082,7 +40082,7 @@
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="253" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="121"/>
@@ -40111,7 +40111,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="109" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F15" s="108" t="s">
         <v>323</v>
@@ -42175,7 +42175,7 @@
         <v>220</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>325</v>
@@ -42195,7 +42195,7 @@
         <v>220</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F18" s="113" t="s">
         <v>326</v>
@@ -42215,7 +42215,7 @@
         <v>322</v>
       </c>
       <c r="E19" s="117" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F19" s="116" t="s">
         <v>327</v>
@@ -42255,7 +42255,7 @@
         <v>211</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F21" s="105" t="s">
         <v>330</v>
@@ -42268,17 +42268,17 @@
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="254"/>
       <c r="B22" s="105" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
         <v>226</v>
       </c>
       <c r="E22" s="106" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="G22" s="197" t="s">
         <v>332</v>
@@ -42288,14 +42288,14 @@
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="255"/>
       <c r="B23" s="108" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
         <v>333</v>
       </c>
       <c r="E23" s="109" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F23" s="108" t="s">
         <v>334</v>
@@ -42307,7 +42307,7 @@
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="256" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
@@ -42332,7 +42332,7 @@
         <v>337</v>
       </c>
       <c r="G25" s="201" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="H25" s="130"/>
     </row>
@@ -42366,7 +42366,7 @@
         <v>211</v>
       </c>
       <c r="E27" s="106" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F27" s="105" t="s">
         <v>339</v>
@@ -42386,7 +42386,7 @@
         <v>211</v>
       </c>
       <c r="E28" s="106" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F28" s="105" t="s">
         <v>340</v>
@@ -42406,7 +42406,7 @@
         <v>211</v>
       </c>
       <c r="E29" s="106" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F29" s="105" t="s">
         <v>341</v>
@@ -42426,7 +42426,7 @@
         <v>211</v>
       </c>
       <c r="E30" s="106" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F30" s="105" t="s">
         <v>342</v>
@@ -42446,7 +42446,7 @@
         <v>211</v>
       </c>
       <c r="E31" s="109" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F31" s="108" t="s">
         <v>343</v>
@@ -42479,10 +42479,10 @@
         <v>211</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F33" s="113" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="G33" s="200" t="s">
         <v>43</v>
@@ -42492,14 +42492,14 @@
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="258"/>
       <c r="B34" s="113" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C34" s="227"/>
       <c r="D34" s="226" t="s">
         <v>319</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F34" s="226"/>
       <c r="G34" s="228" t="s">
@@ -42577,16 +42577,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>500</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>496</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -42615,8 +42615,8 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
-        <v>514</v>
+      <c r="A3" s="246" t="s">
+        <v>510</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -42657,7 +42657,7 @@
         <v>347</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="137"/>
     </row>
@@ -42677,7 +42677,7 @@
         <v>263</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H5" s="137"/>
     </row>
@@ -42715,7 +42715,7 @@
         <v>268</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H7" s="137"/>
     </row>
@@ -42735,7 +42735,7 @@
         <v>349</v>
       </c>
       <c r="G8" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H8" s="137"/>
     </row>
@@ -42755,7 +42755,7 @@
         <v>275</v>
       </c>
       <c r="G9" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H9" s="137"/>
     </row>
@@ -42965,16 +42965,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>501</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -43004,7 +43004,7 @@
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="259" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
@@ -43030,7 +43030,7 @@
         <v>259</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="145"/>
       <c r="I4" s="144"/>
@@ -43059,7 +43059,7 @@
         <v>263</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H5" s="145"/>
       <c r="I5" s="144"/>
@@ -43115,7 +43115,7 @@
         <v>268</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="144"/>
@@ -43144,7 +43144,7 @@
         <v>271</v>
       </c>
       <c r="G8" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H8" s="145"/>
       <c r="I8" s="144"/>
@@ -43173,7 +43173,7 @@
         <v>275</v>
       </c>
       <c r="G9" s="197" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H9" s="149"/>
       <c r="I9" s="144"/>
@@ -43471,16 +43471,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>502</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:20" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -43509,7 +43509,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="157" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="246" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="154"/>
@@ -43546,7 +43546,7 @@
         <v>371</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H4" s="159"/>
     </row>
@@ -43593,19 +43593,19 @@
       </c>
       <c r="C7" s="160"/>
       <c r="D7" s="160" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E7" s="160"/>
       <c r="F7" s="160" t="s">
         <v>374</v>
       </c>
       <c r="G7" s="184" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237" t="s">
+      <c r="A8" s="243" t="s">
         <v>295</v>
       </c>
       <c r="B8" s="162"/>
@@ -43617,7 +43617,7 @@
       <c r="H8" s="163"/>
     </row>
     <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="238"/>
+      <c r="A9" s="244"/>
       <c r="B9" s="164" t="s">
         <v>30</v>
       </c>
@@ -43635,7 +43635,7 @@
       <c r="H9" s="165"/>
     </row>
     <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="238"/>
+      <c r="A10" s="244"/>
       <c r="B10" s="164" t="s">
         <v>377</v>
       </c>
@@ -43645,13 +43645,13 @@
       </c>
       <c r="E10" s="164"/>
       <c r="F10" s="164" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="G10" s="186"/>
       <c r="H10" s="165"/>
     </row>
     <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="238"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
         <v>379</v>
@@ -43661,13 +43661,13 @@
       </c>
       <c r="E11" s="164"/>
       <c r="F11" s="164" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="G11" s="186"/>
       <c r="H11" s="165"/>
     </row>
     <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="238"/>
+      <c r="A12" s="244"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
         <v>380</v>
@@ -43677,13 +43677,13 @@
       </c>
       <c r="E12" s="164"/>
       <c r="F12" s="164" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="G12" s="186"/>
       <c r="H12" s="165"/>
     </row>
     <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="238"/>
+      <c r="A13" s="244"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
         <v>381</v>
@@ -43693,19 +43693,19 @@
       </c>
       <c r="E13" s="164"/>
       <c r="F13" s="164" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G13" s="186"/>
       <c r="H13" s="165"/>
     </row>
     <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="238"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
         <v>382</v>
       </c>
       <c r="D14" s="164" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E14" s="164"/>
       <c r="F14" s="164" t="s">
@@ -43715,7 +43715,7 @@
       <c r="H14" s="165"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="238"/>
+      <c r="A15" s="244"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
         <v>384</v>
@@ -43731,7 +43731,7 @@
       <c r="H15" s="165"/>
     </row>
     <row r="16" spans="1:20" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="238"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="164" t="s">
         <v>386</v>
       </c>
@@ -43741,13 +43741,13 @@
       </c>
       <c r="E16" s="164"/>
       <c r="F16" s="164" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G16" s="186"/>
       <c r="H16" s="165"/>
     </row>
     <row r="17" spans="1:19" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="239"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
         <v>384</v>
@@ -43763,7 +43763,7 @@
       <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:19" s="157" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="240" t="s">
+      <c r="A18" s="246" t="s">
         <v>388</v>
       </c>
       <c r="B18" s="168"/>
@@ -43796,7 +43796,7 @@
       </c>
       <c r="E19" s="158"/>
       <c r="F19" s="158" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="G19" s="183" t="s">
         <v>43</v>
@@ -43894,16 +43894,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="243" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="244"/>
+      <c r="A1" s="231" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -44948,7 +44948,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="246" t="s">
         <v>397</v>
       </c>
       <c r="B3" s="172"/>
@@ -54248,7 +54248,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="237" t="s">
+      <c r="A13" s="243" t="s">
         <v>412</v>
       </c>
       <c r="B13" s="175"/>
@@ -54261,7 +54261,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="238"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="69" t="s">
         <v>207</v>
       </c>
@@ -54277,7 +54277,7 @@
       <c r="H14" s="177"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="238"/>
+      <c r="A15" s="244"/>
       <c r="B15" s="69" t="s">
         <v>260</v>
       </c>
@@ -54293,7 +54293,7 @@
       <c r="H15" s="177"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="238"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="69" t="s">
         <v>213</v>
       </c>
@@ -54309,7 +54309,7 @@
       <c r="H16" s="177"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="238"/>
+      <c r="A17" s="244"/>
       <c r="B17" s="69" t="s">
         <v>266</v>
       </c>
@@ -54325,7 +54325,7 @@
       <c r="H17" s="177"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="238"/>
+      <c r="A18" s="244"/>
       <c r="B18" s="69" t="s">
         <v>210</v>
       </c>
@@ -54341,7 +54341,7 @@
       <c r="H18" s="177"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="238"/>
+      <c r="A19" s="244"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -54357,7 +54357,7 @@
       <c r="H19" s="177"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="238"/>
+      <c r="A20" s="244"/>
       <c r="B20" s="69" t="s">
         <v>418</v>
       </c>
@@ -54373,7 +54373,7 @@
       <c r="H20" s="177"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="238"/>
+      <c r="A21" s="244"/>
       <c r="B21" s="69" t="s">
         <v>319</v>
       </c>
@@ -54389,7 +54389,7 @@
       <c r="H21" s="177"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="238"/>
+      <c r="A22" s="244"/>
       <c r="B22" s="69" t="s">
         <v>421</v>
       </c>
@@ -54405,7 +54405,7 @@
       <c r="H22" s="177"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="238"/>
+      <c r="A23" s="244"/>
       <c r="B23" s="69" t="s">
         <v>423</v>
       </c>
@@ -54421,7 +54421,7 @@
       <c r="H23" s="177"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="239"/>
+      <c r="A24" s="245"/>
       <c r="B24" s="73" t="s">
         <v>425</v>
       </c>
@@ -54437,7 +54437,7 @@
       <c r="H24" s="178"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="240" t="s">
+      <c r="A25" s="246" t="s">
         <v>354</v>
       </c>
       <c r="B25" s="179"/>
@@ -54625,7 +54625,7 @@
       <c r="H36" s="181"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="237" t="s">
+      <c r="A37" s="243" t="s">
         <v>282</v>
       </c>
       <c r="B37" s="175"/>
@@ -54638,7 +54638,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="238"/>
+      <c r="A38" s="244"/>
       <c r="B38" s="69" t="s">
         <v>207</v>
       </c>
@@ -54654,7 +54654,7 @@
       <c r="H38" s="177"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="238"/>
+      <c r="A39" s="244"/>
       <c r="B39" s="69" t="s">
         <v>260</v>
       </c>
@@ -54670,7 +54670,7 @@
       <c r="H39" s="177"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="238"/>
+      <c r="A40" s="244"/>
       <c r="B40" s="69" t="s">
         <v>213</v>
       </c>
@@ -54686,7 +54686,7 @@
       <c r="H40" s="177"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="238"/>
+      <c r="A41" s="244"/>
       <c r="B41" s="69" t="s">
         <v>266</v>
       </c>
@@ -54702,7 +54702,7 @@
       <c r="H41" s="177"/>
     </row>
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="238"/>
+      <c r="A42" s="244"/>
       <c r="B42" s="69" t="s">
         <v>444</v>
       </c>
@@ -54718,7 +54718,7 @@
       <c r="H42" s="177"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="238"/>
+      <c r="A43" s="244"/>
       <c r="B43" s="69" t="s">
         <v>354</v>
       </c>
@@ -54734,7 +54734,7 @@
       <c r="H43" s="177"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="238"/>
+      <c r="A44" s="244"/>
       <c r="B44" s="69" t="s">
         <v>210</v>
       </c>
@@ -54750,7 +54750,7 @@
       <c r="H44" s="177"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="238"/>
+      <c r="A45" s="244"/>
       <c r="B45" s="69" t="s">
         <v>408</v>
       </c>
@@ -54766,7 +54766,7 @@
       <c r="H45" s="177"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="238"/>
+      <c r="A46" s="244"/>
       <c r="B46" s="69" t="s">
         <v>449</v>
       </c>
@@ -54782,7 +54782,7 @@
       <c r="H46" s="177"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="238"/>
+      <c r="A47" s="244"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -54798,7 +54798,7 @@
       <c r="H47" s="177"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="239"/>
+      <c r="A48" s="245"/>
       <c r="B48" s="73" t="s">
         <v>421</v>
       </c>

</xml_diff>

<commit_message>
fix: update list/map microservice examples
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3519BDEC-F0BF-4FDF-B47F-DDF5E48412EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02E9736-1C64-4F72-8515-53AF49E0AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="24270" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5745" yWindow="2085" windowWidth="24270" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -678,9 +678,6 @@
     <t>listOfMicroservices</t>
   </si>
   <si>
-    <t>{microserviceAsset_id_121241241}</t>
-  </si>
-  <si>
     <t>a list of Microservice Asset IDs, which are contained in the algorithm</t>
   </si>
   <si>
@@ -1423,9 +1420,6 @@
   </si>
   <si>
     <t>Map( String: String)</t>
-  </si>
-  <si>
-    <t>{microserviceA:hostB, microserviceB:hostB, microserviceC:hostC}</t>
   </si>
   <si>
     <t>docker-compose</t>
@@ -1814,6 +1808,12 @@
   </si>
   <si>
     <t>A note for developers of co-operating Microservices.  A list of directories that are shared on the host where this microservice will store its outputs</t>
+  </si>
+  <si>
+    <t>[microservice.microservice_id_A, microservice.microservice_id_B]</t>
+  </si>
+  <si>
+    <t>{microservice.microservice_id_A: deployment.microservice_id_B, microservice.microservice_id_B: deployment.microservice_id_B}</t>
   </si>
 </sst>
 </file>
@@ -4174,8 +4174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
@@ -4197,7 +4197,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -4261,7 +4261,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="50"/>
     </row>
@@ -4312,7 +4312,7 @@
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="47" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>20</v>
@@ -4321,7 +4321,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H7" s="50"/>
     </row>
@@ -4355,10 +4355,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G9" s="183" t="s">
         <v>12</v>
@@ -4427,7 +4427,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F13" s="55" t="s">
         <v>37</v>
@@ -4444,13 +4444,13 @@
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="55" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G14" s="188" t="s">
         <v>12</v>
@@ -4460,17 +4460,17 @@
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="239"/>
       <c r="B15" s="55" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="55" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F15" s="55" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G15" s="188" t="s">
         <v>43</v>
@@ -5496,17 +5496,17 @@
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="239"/>
       <c r="B16" s="55" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="55" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E16" s="57" t="s">
+        <v>561</v>
+      </c>
+      <c r="F16" s="55" t="s">
         <v>563</v>
-      </c>
-      <c r="F16" s="55" t="s">
-        <v>565</v>
       </c>
       <c r="G16" s="188" t="s">
         <v>43</v>
@@ -6532,17 +6532,17 @@
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="240"/>
       <c r="B17" s="221" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C17" s="222"/>
       <c r="D17" s="221" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E17" s="223" t="s">
+        <v>562</v>
+      </c>
+      <c r="F17" s="221" t="s">
         <v>564</v>
-      </c>
-      <c r="F17" s="221" t="s">
-        <v>566</v>
       </c>
       <c r="G17" s="224" t="s">
         <v>43</v>
@@ -20368,7 +20368,7 @@
         <v>136</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G49" s="184" t="s">
         <v>43</v>
@@ -21658,7 +21658,7 @@
         <v>136</v>
       </c>
       <c r="F63" s="85" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G63" s="187" t="s">
         <v>43</v>
@@ -32246,8 +32246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
@@ -32270,7 +32270,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -32334,7 +32334,7 @@
         <v>192</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="50"/>
     </row>
@@ -32445,7 +32445,7 @@
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="47" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>20</v>
@@ -32454,7 +32454,7 @@
         <v>201</v>
       </c>
       <c r="G10" s="183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H10" s="50"/>
     </row>
@@ -32500,10 +32500,10 @@
         <v>31</v>
       </c>
       <c r="E13" s="104" t="s">
+        <v>565</v>
+      </c>
+      <c r="F13" s="103" t="s">
         <v>205</v>
-      </c>
-      <c r="F13" s="103" t="s">
-        <v>206</v>
       </c>
       <c r="G13" s="186" t="s">
         <v>12</v>
@@ -32513,17 +32513,17 @@
     <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="252"/>
       <c r="B14" s="103" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E14" s="104" t="s">
-        <v>454</v>
+        <v>566</v>
       </c>
       <c r="F14" s="103" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G14" s="186" t="s">
         <v>12</v>
@@ -32570,7 +32570,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -32659,33 +32659,33 @@
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="236"/>
       <c r="B4" s="105" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="105" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="106"/>
       <c r="F4" s="105" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="236"/>
       <c r="B5" s="105" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="106"/>
       <c r="D5" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E5" s="106"/>
       <c r="F5" s="105" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G5" s="197"/>
       <c r="H5" s="107"/>
@@ -32693,15 +32693,15 @@
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="236"/>
       <c r="B6" s="105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="107"/>
@@ -32709,15 +32709,15 @@
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="236"/>
       <c r="B7" s="105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" s="106"/>
       <c r="D7" s="105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="G7" s="197"/>
       <c r="H7" s="107"/>
@@ -32725,15 +32725,15 @@
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="236"/>
       <c r="B8" s="105" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="106"/>
       <c r="F8" s="105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G8" s="197"/>
       <c r="H8" s="107"/>
@@ -32741,15 +32741,15 @@
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="236"/>
       <c r="B9" s="105" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="106"/>
       <c r="D9" s="105" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G9" s="197" t="s">
         <v>43</v>
@@ -32759,15 +32759,15 @@
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="236"/>
       <c r="B10" s="105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="106"/>
       <c r="D10" s="105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" s="106"/>
       <c r="F10" s="105" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G10" s="197"/>
       <c r="H10" s="107"/>
@@ -32792,11 +32792,11 @@
       </c>
       <c r="C11" s="106"/>
       <c r="D11" s="105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" s="106"/>
       <c r="F11" s="105" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G11" s="197"/>
       <c r="H11" s="107"/>
@@ -32804,15 +32804,15 @@
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="236"/>
       <c r="B12" s="105" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G12" s="197" t="s">
         <v>43</v>
@@ -32822,33 +32822,33 @@
     <row r="13" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="236"/>
       <c r="B13" s="105" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="105" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="G13" s="197" t="s">
         <v>227</v>
-      </c>
-      <c r="G13" s="197" t="s">
-        <v>228</v>
       </c>
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="236"/>
       <c r="B14" s="105" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="105" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G14" s="197" t="s">
         <v>43</v>
@@ -32858,15 +32858,15 @@
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="237"/>
       <c r="B15" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="109"/>
       <c r="D15" s="108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E15" s="109"/>
       <c r="F15" s="108" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G15" s="198"/>
       <c r="H15" s="110"/>
@@ -32887,15 +32887,15 @@
     <row r="17" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="244"/>
       <c r="B17" s="113" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E17" s="114"/>
       <c r="F17" s="113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G17" s="200"/>
       <c r="H17" s="115"/>
@@ -32907,11 +32907,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G18" s="200"/>
       <c r="H18" s="115"/>
@@ -32920,14 +32920,14 @@
       <c r="A19" s="244"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="113" t="s">
         <v>210</v>
-      </c>
-      <c r="D19" s="113" t="s">
-        <v>211</v>
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G19" s="200"/>
       <c r="H19" s="115"/>
@@ -32936,14 +32936,14 @@
       <c r="A20" s="244"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D20" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="G20" s="200"/>
       <c r="H20" s="115"/>
@@ -32952,14 +32952,14 @@
       <c r="A21" s="244"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D21" s="113" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="G21" s="200"/>
       <c r="H21" s="115"/>
@@ -32968,14 +32968,14 @@
       <c r="A22" s="244"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="G22" s="200"/>
       <c r="H22" s="115"/>
@@ -32984,14 +32984,14 @@
       <c r="A23" s="244"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D23" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G23" s="200"/>
       <c r="H23" s="115"/>
@@ -33000,14 +33000,14 @@
       <c r="A24" s="244"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G24" s="200"/>
       <c r="H24" s="115"/>
@@ -33016,14 +33016,14 @@
       <c r="A25" s="244"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D25" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="G25" s="200"/>
       <c r="H25" s="115"/>
@@ -33032,14 +33032,14 @@
       <c r="A26" s="244"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D26" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G26" s="200"/>
       <c r="H26" s="115"/>
@@ -33048,14 +33048,14 @@
       <c r="A27" s="244"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D27" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G27" s="200"/>
       <c r="H27" s="115"/>
@@ -33064,14 +33064,14 @@
       <c r="A28" s="244"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G28" s="200"/>
       <c r="H28" s="115"/>
@@ -33079,15 +33079,15 @@
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="244"/>
       <c r="B29" s="113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="113" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G29" s="200"/>
       <c r="H29" s="115"/>
@@ -33099,11 +33099,11 @@
         <v>1</v>
       </c>
       <c r="D30" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="227"/>
       <c r="F30" s="113" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="G30" s="228"/>
       <c r="H30" s="229"/>
@@ -33112,14 +33112,14 @@
       <c r="A31" s="244"/>
       <c r="B31" s="226"/>
       <c r="C31" s="114" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="113" t="s">
         <v>210</v>
-      </c>
-      <c r="D31" s="113" t="s">
-        <v>211</v>
       </c>
       <c r="E31" s="227"/>
       <c r="F31" s="113" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G31" s="228"/>
       <c r="H31" s="229"/>
@@ -33128,14 +33128,14 @@
       <c r="A32" s="244"/>
       <c r="B32" s="226"/>
       <c r="C32" s="114" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D32" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E32" s="227"/>
       <c r="F32" s="113" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="G32" s="228"/>
       <c r="H32" s="229"/>
@@ -33144,14 +33144,14 @@
       <c r="A33" s="244"/>
       <c r="B33" s="226"/>
       <c r="C33" s="114" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E33" s="227"/>
       <c r="F33" s="113" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G33" s="228"/>
       <c r="H33" s="229"/>
@@ -33160,14 +33160,14 @@
       <c r="A34" s="244"/>
       <c r="B34" s="226"/>
       <c r="C34" s="114" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D34" s="113" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E34" s="227"/>
       <c r="F34" s="113" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G34" s="228"/>
       <c r="H34" s="229"/>
@@ -33176,14 +33176,14 @@
       <c r="A35" s="244"/>
       <c r="B35" s="226"/>
       <c r="C35" s="114" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D35" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E35" s="227"/>
       <c r="F35" s="113" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G35" s="228"/>
       <c r="H35" s="229"/>
@@ -33192,14 +33192,14 @@
       <c r="A36" s="244"/>
       <c r="B36" s="226"/>
       <c r="C36" s="114" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E36" s="227"/>
       <c r="F36" s="113" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G36" s="228"/>
       <c r="H36" s="229"/>
@@ -33208,14 +33208,14 @@
       <c r="A37" s="244"/>
       <c r="B37" s="226"/>
       <c r="C37" s="114" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D37" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E37" s="227"/>
       <c r="F37" s="113" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="G37" s="228"/>
       <c r="H37" s="229"/>
@@ -33224,14 +33224,14 @@
       <c r="A38" s="244"/>
       <c r="B38" s="226"/>
       <c r="C38" s="114" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D38" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E38" s="227"/>
       <c r="F38" s="113" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G38" s="228"/>
       <c r="H38" s="229"/>
@@ -33240,14 +33240,14 @@
       <c r="A39" s="244"/>
       <c r="B39" s="226"/>
       <c r="C39" s="114" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D39" s="113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E39" s="227"/>
       <c r="F39" s="113" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G39" s="228"/>
       <c r="H39" s="229"/>
@@ -33256,14 +33256,14 @@
       <c r="A40" s="244"/>
       <c r="B40" s="226"/>
       <c r="C40" s="114" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D40" s="113" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E40" s="227"/>
       <c r="F40" s="113" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G40" s="228"/>
       <c r="H40" s="229"/>
@@ -33271,15 +33271,15 @@
     <row r="41" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="245"/>
       <c r="B41" s="116" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C41" s="117"/>
       <c r="D41" s="116" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E41" s="117"/>
       <c r="F41" s="116" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G41" s="201" t="s">
         <v>43</v>
@@ -33288,7 +33288,7 @@
     </row>
     <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="246" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B42" s="119"/>
       <c r="C42" s="119"/>
@@ -33339,15 +33339,15 @@
     <row r="43" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="242"/>
       <c r="B43" s="108" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C43" s="109"/>
       <c r="D43" s="108" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E43" s="109"/>
       <c r="F43" s="108" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G43" s="201" t="s">
         <v>43</v>
@@ -33393,11 +33393,11 @@
       </c>
       <c r="C45" s="114"/>
       <c r="D45" s="113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E45" s="114"/>
       <c r="F45" s="113" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G45" s="201" t="s">
         <v>43</v>
@@ -33411,11 +33411,11 @@
       </c>
       <c r="C46" s="114"/>
       <c r="D46" s="113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E46" s="114"/>
       <c r="F46" s="113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G46" s="201" t="s">
         <v>43</v>
@@ -33429,11 +33429,11 @@
       </c>
       <c r="C47" s="117"/>
       <c r="D47" s="116" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E47" s="117"/>
       <c r="F47" s="116" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G47" s="201" t="s">
         <v>43</v>
@@ -33442,7 +33442,7 @@
     </row>
     <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="246" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B48" s="121"/>
       <c r="C48" s="121"/>
@@ -33474,15 +33474,15 @@
     <row r="49" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="241"/>
       <c r="B49" s="105" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C49" s="106"/>
       <c r="D49" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E49" s="106"/>
       <c r="F49" s="105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G49" s="197" t="s">
         <v>43</v>
@@ -33492,15 +33492,15 @@
     <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="241"/>
       <c r="B50" s="105" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C50" s="106"/>
       <c r="D50" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E50" s="106"/>
       <c r="F50" s="105" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G50" s="197" t="s">
         <v>43</v>
@@ -33514,11 +33514,11 @@
       </c>
       <c r="C51" s="106"/>
       <c r="D51" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E51" s="106"/>
       <c r="F51" s="105" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G51" s="197" t="s">
         <v>43</v>
@@ -33532,11 +33532,11 @@
       </c>
       <c r="C52" s="106"/>
       <c r="D52" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E52" s="106"/>
       <c r="F52" s="105" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G52" s="197" t="s">
         <v>43</v>
@@ -33550,11 +33550,11 @@
       </c>
       <c r="C53" s="106"/>
       <c r="D53" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E53" s="106"/>
       <c r="F53" s="105" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G53" s="197" t="s">
         <v>43</v>
@@ -33588,11 +33588,11 @@
       </c>
       <c r="C54" s="106"/>
       <c r="D54" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E54" s="106"/>
       <c r="F54" s="105" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G54" s="197" t="s">
         <v>43</v>
@@ -33606,11 +33606,11 @@
       </c>
       <c r="C55" s="106"/>
       <c r="D55" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E55" s="106"/>
       <c r="F55" s="105" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G55" s="197" t="s">
         <v>43</v>
@@ -33624,11 +33624,11 @@
       </c>
       <c r="C56" s="106"/>
       <c r="D56" s="105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E56" s="106"/>
       <c r="F56" s="105" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G56" s="197" t="s">
         <v>43</v>
@@ -33642,11 +33642,11 @@
       </c>
       <c r="C57" s="109"/>
       <c r="D57" s="108" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E57" s="109"/>
       <c r="F57" s="108" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G57" s="198" t="s">
         <v>43</v>
@@ -33655,7 +33655,7 @@
     </row>
     <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="243" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B58" s="123"/>
       <c r="C58" s="123"/>
@@ -33673,11 +33673,11 @@
       </c>
       <c r="C59" s="117"/>
       <c r="D59" s="116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E59" s="117"/>
       <c r="F59" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G59" s="201"/>
       <c r="H59" s="118"/>
@@ -33730,7 +33730,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -34784,7 +34784,7 @@
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="253" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
@@ -34810,80 +34810,80 @@
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="254"/>
       <c r="B4" s="105" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="105" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="106" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F4" s="105" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="254"/>
       <c r="B5" s="105" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C5" s="106"/>
       <c r="D5" s="105" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="106" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F5" s="105" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="254"/>
       <c r="B6" s="105" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="106" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H6" s="126"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="254"/>
       <c r="B7" s="105" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C7" s="106"/>
       <c r="D7" s="105" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>470</v>
+      </c>
+      <c r="F7" s="105" t="s">
         <v>310</v>
       </c>
-      <c r="E7" s="106" t="s">
-        <v>472</v>
-      </c>
-      <c r="F7" s="105" t="s">
-        <v>311</v>
-      </c>
       <c r="G7" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H7" s="126"/>
     </row>
@@ -34903,17 +34903,17 @@
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="258"/>
       <c r="B9" s="113" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" s="114"/>
       <c r="D9" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F9" s="113" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G9" s="206" t="s">
         <v>12</v>
@@ -35939,17 +35939,17 @@
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="258"/>
       <c r="B10" s="113" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G10" s="200" t="s">
         <v>43</v>
@@ -36975,17 +36975,17 @@
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="258"/>
       <c r="B11" s="113" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C11" s="114"/>
       <c r="D11" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F11" s="113" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G11" s="200" t="s">
         <v>43</v>
@@ -38011,17 +38011,17 @@
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="258"/>
       <c r="B12" s="113" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="117" t="s">
+        <v>483</v>
+      </c>
+      <c r="F12" s="116" t="s">
         <v>319</v>
-      </c>
-      <c r="E12" s="117" t="s">
-        <v>485</v>
-      </c>
-      <c r="F12" s="116" t="s">
-        <v>320</v>
       </c>
       <c r="G12" s="200" t="s">
         <v>43</v>
@@ -39047,17 +39047,17 @@
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="258"/>
       <c r="B13" s="113" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C13" s="114"/>
       <c r="D13" s="113" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="114" t="s">
+        <v>474</v>
+      </c>
+      <c r="F13" s="113" t="s">
         <v>315</v>
-      </c>
-      <c r="E13" s="114" t="s">
-        <v>476</v>
-      </c>
-      <c r="F13" s="113" t="s">
-        <v>316</v>
       </c>
       <c r="G13" s="200" t="s">
         <v>43</v>
@@ -40082,7 +40082,7 @@
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="253" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="121"/>
@@ -40104,17 +40104,17 @@
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="255"/>
       <c r="B15" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" s="109"/>
       <c r="D15" s="108" t="s">
+        <v>321</v>
+      </c>
+      <c r="E15" s="109" t="s">
+        <v>484</v>
+      </c>
+      <c r="F15" s="108" t="s">
         <v>322</v>
-      </c>
-      <c r="E15" s="109" t="s">
-        <v>486</v>
-      </c>
-      <c r="F15" s="108" t="s">
-        <v>323</v>
       </c>
       <c r="G15" s="198" t="s">
         <v>43</v>
@@ -41139,7 +41139,7 @@
     </row>
     <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="256" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="111"/>
@@ -42172,13 +42172,13 @@
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F17" s="113" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G17" s="206" t="s">
         <v>12</v>
@@ -42192,13 +42192,13 @@
       </c>
       <c r="C18" s="114"/>
       <c r="D18" s="113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F18" s="113" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G18" s="206" t="s">
         <v>12</v>
@@ -42212,22 +42212,22 @@
       </c>
       <c r="C19" s="117"/>
       <c r="D19" s="116" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E19" s="117" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F19" s="116" t="s">
+        <v>326</v>
+      </c>
+      <c r="G19" s="201" t="s">
         <v>327</v>
-      </c>
-      <c r="G19" s="201" t="s">
-        <v>328</v>
       </c>
       <c r="H19" s="130"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="253" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20" s="121"/>
       <c r="C20" s="121"/>
@@ -42252,62 +42252,62 @@
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F21" s="105" t="s">
+        <v>329</v>
+      </c>
+      <c r="G21" s="197" t="s">
         <v>330</v>
-      </c>
-      <c r="G21" s="197" t="s">
-        <v>331</v>
       </c>
       <c r="H21" s="126"/>
     </row>
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="254"/>
       <c r="B22" s="105" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E22" s="106" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G22" s="197" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="255"/>
       <c r="B23" s="108" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
+        <v>332</v>
+      </c>
+      <c r="E23" s="109" t="s">
+        <v>481</v>
+      </c>
+      <c r="F23" s="108" t="s">
         <v>333</v>
       </c>
-      <c r="E23" s="109" t="s">
-        <v>483</v>
-      </c>
-      <c r="F23" s="108" t="s">
-        <v>334</v>
-      </c>
       <c r="G23" s="198" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H23" s="127"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="256" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
@@ -42321,24 +42321,24 @@
     <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="257"/>
       <c r="B25" s="116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C25" s="117"/>
       <c r="D25" s="116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" s="117"/>
       <c r="F25" s="116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G25" s="201" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H25" s="130"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="253" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B26" s="121"/>
       <c r="C26" s="121"/>
@@ -42363,13 +42363,13 @@
       </c>
       <c r="C27" s="106"/>
       <c r="D27" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E27" s="106" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G27" s="197" t="s">
         <v>43</v>
@@ -42383,13 +42383,13 @@
       </c>
       <c r="C28" s="106"/>
       <c r="D28" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E28" s="106" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G28" s="197" t="s">
         <v>43</v>
@@ -42403,13 +42403,13 @@
       </c>
       <c r="C29" s="106"/>
       <c r="D29" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E29" s="106" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F29" s="105" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G29" s="197" t="s">
         <v>43</v>
@@ -42423,13 +42423,13 @@
       </c>
       <c r="C30" s="106"/>
       <c r="D30" s="105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="106" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G30" s="197" t="s">
         <v>43</v>
@@ -42443,13 +42443,13 @@
       </c>
       <c r="C31" s="109"/>
       <c r="D31" s="108" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E31" s="109" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F31" s="108" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G31" s="198" t="s">
         <v>43</v>
@@ -42458,7 +42458,7 @@
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="256" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B32" s="123"/>
       <c r="C32" s="123"/>
@@ -42476,13 +42476,13 @@
       </c>
       <c r="C33" s="114"/>
       <c r="D33" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F33" s="113" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G33" s="200" t="s">
         <v>43</v>
@@ -42492,14 +42492,14 @@
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="258"/>
       <c r="B34" s="113" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C34" s="227"/>
       <c r="D34" s="226" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F34" s="226"/>
       <c r="G34" s="228" t="s">
@@ -42510,15 +42510,15 @@
     <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="257"/>
       <c r="B35" s="116" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C35" s="117"/>
       <c r="D35" s="116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E35" s="117"/>
       <c r="F35" s="116" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G35" s="201" t="s">
         <v>43</v>
@@ -42578,7 +42578,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -42616,7 +42616,7 @@
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="246" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -42644,47 +42644,47 @@
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="241"/>
       <c r="B4" s="106" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="106" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F4" s="136" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G4" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="137"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="241"/>
       <c r="B5" s="106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="106"/>
       <c r="D5" s="136" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="106" t="s">
         <v>261</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="F5" s="136" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="136" t="s">
-        <v>263</v>
-      </c>
       <c r="G5" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H5" s="137"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="241"/>
       <c r="B6" s="106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="136" t="s">
@@ -42694,7 +42694,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="136" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="137"/>
@@ -42702,77 +42702,77 @@
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="241"/>
       <c r="B7" s="106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="106"/>
       <c r="D7" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7" s="106" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="136" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="136" t="s">
-        <v>268</v>
-      </c>
       <c r="G7" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H7" s="137"/>
     </row>
     <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="241"/>
       <c r="B8" s="106" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E8" s="106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F8" s="136" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G8" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H8" s="137"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="241"/>
       <c r="B9" s="106" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" s="106"/>
       <c r="D9" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F9" s="136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G9" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H9" s="137"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="241"/>
       <c r="B10" s="106" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="106"/>
       <c r="D10" s="136" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E10" s="106" t="s">
+        <v>350</v>
+      </c>
+      <c r="F10" s="136" t="s">
         <v>351</v>
-      </c>
-      <c r="F10" s="136" t="s">
-        <v>352</v>
       </c>
       <c r="G10" s="197"/>
       <c r="H10" s="137"/>
@@ -42780,17 +42780,17 @@
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="241"/>
       <c r="B11" s="106" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" s="106"/>
       <c r="D11" s="106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="106" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="136" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G11" s="197"/>
       <c r="H11" s="137"/>
@@ -42798,17 +42798,17 @@
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="241"/>
       <c r="B12" s="106" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E12" s="106" t="s">
+        <v>354</v>
+      </c>
+      <c r="F12" s="136" t="s">
         <v>355</v>
-      </c>
-      <c r="F12" s="136" t="s">
-        <v>356</v>
       </c>
       <c r="G12" s="197"/>
       <c r="H12" s="137"/>
@@ -42816,17 +42816,17 @@
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="241"/>
       <c r="B13" s="106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="136" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E13" s="106" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" s="136" t="s">
         <v>287</v>
-      </c>
-      <c r="F13" s="136" t="s">
-        <v>288</v>
       </c>
       <c r="G13" s="197"/>
       <c r="H13" s="137"/>
@@ -42834,17 +42834,17 @@
     <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="241"/>
       <c r="B14" s="106" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E14" s="136" t="s">
+        <v>358</v>
+      </c>
+      <c r="F14" s="136" t="s">
         <v>359</v>
-      </c>
-      <c r="F14" s="136" t="s">
-        <v>360</v>
       </c>
       <c r="G14" s="197"/>
       <c r="H14" s="137"/>
@@ -42852,17 +42852,17 @@
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="241"/>
       <c r="B15" s="106" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="136" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E15" s="136" t="s">
+        <v>361</v>
+      </c>
+      <c r="F15" s="136" t="s">
         <v>362</v>
-      </c>
-      <c r="F15" s="136" t="s">
-        <v>363</v>
       </c>
       <c r="G15" s="197"/>
       <c r="H15" s="137"/>
@@ -42870,17 +42870,17 @@
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="241"/>
       <c r="B16" s="106" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="136" t="s">
+        <v>364</v>
+      </c>
+      <c r="E16" s="136" t="s">
         <v>365</v>
       </c>
-      <c r="E16" s="136" t="s">
+      <c r="F16" s="136" t="s">
         <v>366</v>
-      </c>
-      <c r="F16" s="136" t="s">
-        <v>367</v>
       </c>
       <c r="G16" s="197"/>
       <c r="H16" s="137"/>
@@ -42888,7 +42888,7 @@
     <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="241"/>
       <c r="B17" s="106" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
@@ -42898,7 +42898,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="136" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G17" s="197"/>
       <c r="H17" s="137"/>
@@ -42906,17 +42906,17 @@
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="242"/>
       <c r="B18" s="109" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C18" s="109"/>
       <c r="D18" s="109" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="109" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F18" s="138" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G18" s="198"/>
       <c r="H18" s="139"/>
@@ -42966,7 +42966,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -43004,7 +43004,7 @@
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="259" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
@@ -43017,20 +43017,20 @@
     <row r="4" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A4" s="260"/>
       <c r="B4" s="106" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="136" t="s">
         <v>257</v>
       </c>
-      <c r="E4" s="136" t="s">
+      <c r="F4" s="105" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="105" t="s">
-        <v>259</v>
-      </c>
       <c r="G4" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="145"/>
       <c r="I4" s="144"/>
@@ -43046,20 +43046,20 @@
     <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="260"/>
       <c r="B5" s="106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="106"/>
       <c r="D5" s="105" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="136" t="s">
         <v>261</v>
       </c>
-      <c r="E5" s="136" t="s">
+      <c r="F5" s="106" t="s">
         <v>262</v>
       </c>
-      <c r="F5" s="106" t="s">
-        <v>263</v>
-      </c>
       <c r="G5" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H5" s="145"/>
       <c r="I5" s="144"/>
@@ -43075,17 +43075,17 @@
     <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="260"/>
       <c r="B6" s="106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
         <v>163</v>
       </c>
       <c r="E6" s="136" t="s">
+        <v>263</v>
+      </c>
+      <c r="F6" s="106" t="s">
         <v>264</v>
-      </c>
-      <c r="F6" s="106" t="s">
-        <v>265</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="145"/>
@@ -43102,20 +43102,20 @@
     <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A7" s="260"/>
       <c r="B7" s="106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="106"/>
       <c r="D7" s="105" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E7" s="136" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="106" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="106" t="s">
-        <v>268</v>
-      </c>
       <c r="G7" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="144"/>
@@ -43131,20 +43131,20 @@
     <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A8" s="260"/>
       <c r="B8" s="106" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="105" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E8" s="136" t="s">
+        <v>269</v>
+      </c>
+      <c r="F8" s="106" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="106" t="s">
-        <v>271</v>
-      </c>
       <c r="G8" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H8" s="145"/>
       <c r="I8" s="144"/>
@@ -43160,20 +43160,20 @@
     <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A9" s="260"/>
       <c r="B9" s="106" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" s="106"/>
       <c r="D9" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" s="148" t="s">
         <v>273</v>
       </c>
-      <c r="E9" s="148" t="s">
+      <c r="F9" s="106" t="s">
         <v>274</v>
       </c>
-      <c r="F9" s="106" t="s">
-        <v>275</v>
-      </c>
       <c r="G9" s="197" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H9" s="149"/>
       <c r="I9" s="144"/>
@@ -43189,17 +43189,17 @@
     <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="260"/>
       <c r="B10" s="106" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="106"/>
       <c r="D10" s="105" t="s">
+        <v>275</v>
+      </c>
+      <c r="E10" s="136" t="s">
         <v>276</v>
       </c>
-      <c r="E10" s="136" t="s">
+      <c r="F10" s="106" t="s">
         <v>277</v>
-      </c>
-      <c r="F10" s="106" t="s">
-        <v>278</v>
       </c>
       <c r="G10" s="197"/>
       <c r="H10" s="145"/>
@@ -43216,17 +43216,17 @@
     <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="260"/>
       <c r="B11" s="106" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" s="106"/>
       <c r="D11" s="105" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="136" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="106" t="s">
         <v>280</v>
-      </c>
-      <c r="F11" s="106" t="s">
-        <v>281</v>
       </c>
       <c r="G11" s="197"/>
       <c r="H11" s="145"/>
@@ -43243,17 +43243,17 @@
     <row r="12" spans="1:17" s="151" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A12" s="260"/>
       <c r="B12" s="106" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="105" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12" s="136" t="s">
+        <v>282</v>
+      </c>
+      <c r="F12" s="106" t="s">
         <v>283</v>
-      </c>
-      <c r="F12" s="106" t="s">
-        <v>284</v>
       </c>
       <c r="G12" s="197"/>
       <c r="H12" s="145"/>
@@ -43270,17 +43270,17 @@
     <row r="13" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A13" s="260"/>
       <c r="B13" s="106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="136" t="s">
+      <c r="F13" s="106" t="s">
         <v>287</v>
-      </c>
-      <c r="F13" s="106" t="s">
-        <v>288</v>
       </c>
       <c r="G13" s="197"/>
       <c r="H13" s="145"/>
@@ -43297,17 +43297,17 @@
     <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="260"/>
       <c r="B14" s="106" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14" s="136" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" s="106" t="s">
         <v>290</v>
-      </c>
-      <c r="F14" s="106" t="s">
-        <v>291</v>
       </c>
       <c r="G14" s="197"/>
       <c r="H14" s="145"/>
@@ -43324,17 +43324,17 @@
     <row r="15" spans="1:17" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="260"/>
       <c r="B15" s="106" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E15" s="136" t="s">
+        <v>292</v>
+      </c>
+      <c r="F15" s="106" t="s">
         <v>293</v>
-      </c>
-      <c r="F15" s="106" t="s">
-        <v>294</v>
       </c>
       <c r="G15" s="197"/>
       <c r="H15" s="145"/>
@@ -43351,17 +43351,17 @@
     <row r="16" spans="1:17" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A16" s="260"/>
       <c r="B16" s="106" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="105" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E16" s="136" t="s">
+        <v>295</v>
+      </c>
+      <c r="F16" s="106" t="s">
         <v>296</v>
-      </c>
-      <c r="F16" s="106" t="s">
-        <v>297</v>
       </c>
       <c r="G16" s="197"/>
       <c r="H16" s="145"/>
@@ -43378,17 +43378,17 @@
     <row r="17" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="260"/>
       <c r="B17" s="106" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
+        <v>298</v>
+      </c>
+      <c r="E17" s="106" t="s">
         <v>299</v>
       </c>
-      <c r="E17" s="106" t="s">
+      <c r="F17" s="106" t="s">
         <v>300</v>
-      </c>
-      <c r="F17" s="106" t="s">
-        <v>301</v>
       </c>
       <c r="G17" s="197"/>
       <c r="H17" s="137"/>
@@ -43405,17 +43405,17 @@
     <row r="18" spans="1:17" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="261"/>
       <c r="B18" s="109" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C18" s="109"/>
       <c r="D18" s="109" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="109" t="s">
+        <v>302</v>
+      </c>
+      <c r="F18" s="109" t="s">
         <v>303</v>
-      </c>
-      <c r="F18" s="109" t="s">
-        <v>304</v>
       </c>
       <c r="G18" s="198"/>
       <c r="H18" s="139"/>
@@ -43472,7 +43472,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -43539,14 +43539,14 @@
       </c>
       <c r="C4" s="158"/>
       <c r="D4" s="158" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="158"/>
       <c r="F4" s="158" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G4" s="183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="159"/>
     </row>
@@ -43561,7 +43561,7 @@
       </c>
       <c r="E5" s="158"/>
       <c r="F5" s="158" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G5" s="183" t="s">
         <v>12</v>
@@ -43579,7 +43579,7 @@
       </c>
       <c r="E6" s="158"/>
       <c r="F6" s="158" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G6" s="183" t="s">
         <v>12</v>
@@ -43593,20 +43593,20 @@
       </c>
       <c r="C7" s="160"/>
       <c r="D7" s="160" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E7" s="160"/>
       <c r="F7" s="160" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G7" s="184" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H7" s="161"/>
     </row>
     <row r="8" spans="1:20" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="243" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="162"/>
       <c r="C8" s="162"/>
@@ -43623,11 +43623,11 @@
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="164" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E9" s="164"/>
       <c r="F9" s="164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G9" s="214" t="s">
         <v>12</v>
@@ -43637,15 +43637,15 @@
     <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="244"/>
       <c r="B10" s="164" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C10" s="164"/>
       <c r="D10" s="164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E10" s="164"/>
       <c r="F10" s="164" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G10" s="186"/>
       <c r="H10" s="165"/>
@@ -43654,14 +43654,14 @@
       <c r="A11" s="244"/>
       <c r="B11" s="164"/>
       <c r="C11" s="164" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D11" s="164" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E11" s="164"/>
       <c r="F11" s="164" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G11" s="186"/>
       <c r="H11" s="165"/>
@@ -43670,14 +43670,14 @@
       <c r="A12" s="244"/>
       <c r="B12" s="164"/>
       <c r="C12" s="164" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D12" s="164" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E12" s="164"/>
       <c r="F12" s="164" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G12" s="186"/>
       <c r="H12" s="165"/>
@@ -43686,14 +43686,14 @@
       <c r="A13" s="244"/>
       <c r="B13" s="164"/>
       <c r="C13" s="164" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D13" s="164" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E13" s="164"/>
       <c r="F13" s="164" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G13" s="186"/>
       <c r="H13" s="165"/>
@@ -43702,14 +43702,14 @@
       <c r="A14" s="244"/>
       <c r="B14" s="164"/>
       <c r="C14" s="164" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D14" s="164" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E14" s="164"/>
       <c r="F14" s="164" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G14" s="186"/>
       <c r="H14" s="165"/>
@@ -43718,14 +43718,14 @@
       <c r="A15" s="244"/>
       <c r="B15" s="164"/>
       <c r="C15" s="164" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D15" s="164" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E15" s="164"/>
       <c r="F15" s="164" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G15" s="186"/>
       <c r="H15" s="165"/>
@@ -43733,15 +43733,15 @@
     <row r="16" spans="1:20" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="244"/>
       <c r="B16" s="164" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C16" s="164"/>
       <c r="D16" s="164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E16" s="164"/>
       <c r="F16" s="164" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G16" s="186"/>
       <c r="H16" s="165"/>
@@ -43750,21 +43750,21 @@
       <c r="A17" s="245"/>
       <c r="B17" s="166"/>
       <c r="C17" s="166" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D17" s="166" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E17" s="166"/>
       <c r="F17" s="166" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G17" s="187"/>
       <c r="H17" s="167"/>
     </row>
     <row r="18" spans="1:19" s="157" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="246" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B18" s="168"/>
       <c r="C18" s="168"/>
@@ -43788,15 +43788,15 @@
     <row r="19" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="241"/>
       <c r="B19" s="158" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C19" s="158"/>
       <c r="D19" s="158" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E19" s="158"/>
       <c r="F19" s="158" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G19" s="183" t="s">
         <v>43</v>
@@ -43807,14 +43807,14 @@
       <c r="A20" s="241"/>
       <c r="B20" s="158"/>
       <c r="C20" s="158" t="s">
+        <v>389</v>
+      </c>
+      <c r="D20" s="158" t="s">
         <v>390</v>
-      </c>
-      <c r="D20" s="158" t="s">
-        <v>391</v>
       </c>
       <c r="E20" s="158"/>
       <c r="F20" s="158" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G20" s="183"/>
       <c r="H20" s="159"/>
@@ -43823,14 +43823,14 @@
       <c r="A21" s="241"/>
       <c r="B21" s="158"/>
       <c r="C21" s="158" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D21" s="158" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E21" s="158"/>
       <c r="F21" s="158" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G21" s="183"/>
       <c r="H21" s="159"/>
@@ -43839,14 +43839,14 @@
       <c r="A22" s="242"/>
       <c r="B22" s="160"/>
       <c r="C22" s="160" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D22" s="160" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E22" s="160"/>
       <c r="F22" s="160" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G22" s="184"/>
       <c r="H22" s="161"/>
@@ -43895,7 +43895,7 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="231" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="231"/>
@@ -44949,7 +44949,7 @@
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="246" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B3" s="172"/>
       <c r="C3" s="172"/>
@@ -44962,15 +44962,15 @@
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="158"/>
       <c r="D4" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="158" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="159"/>
@@ -45994,15 +45994,15 @@
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="158"/>
       <c r="D5" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="158" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G5" s="47"/>
       <c r="H5" s="159"/>
@@ -47026,7 +47026,7 @@
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="158"/>
       <c r="D6" s="47" t="s">
@@ -47034,7 +47034,7 @@
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="158" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="174"/>
@@ -48058,15 +48058,15 @@
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C7" s="158"/>
       <c r="D7" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="158" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="159"/>
@@ -49090,15 +49090,15 @@
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C8" s="158"/>
       <c r="D8" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="158" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="159"/>
@@ -50122,15 +50122,15 @@
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C9" s="158"/>
       <c r="D9" s="47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="158" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G9" s="47"/>
       <c r="H9" s="159"/>
@@ -51154,15 +51154,15 @@
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C10" s="158"/>
       <c r="D10" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="158" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="159"/>
@@ -52186,15 +52186,15 @@
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="241"/>
       <c r="B11" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C11" s="158"/>
       <c r="D11" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="158" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="159"/>
@@ -53218,15 +53218,15 @@
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="242"/>
       <c r="B12" s="51" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C12" s="160"/>
       <c r="D12" s="51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="160" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G12" s="51"/>
       <c r="H12" s="161"/>
@@ -54249,7 +54249,7 @@
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="243" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B13" s="175"/>
       <c r="C13" s="175"/>
@@ -54263,15 +54263,15 @@
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="244"/>
       <c r="B14" s="69" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14" s="69"/>
       <c r="F14" s="69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G14" s="69"/>
       <c r="H14" s="177"/>
@@ -54279,15 +54279,15 @@
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="244"/>
       <c r="B15" s="69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" s="69"/>
       <c r="D15" s="69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E15" s="69"/>
       <c r="F15" s="69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G15" s="69"/>
       <c r="H15" s="177"/>
@@ -54295,7 +54295,7 @@
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="244"/>
       <c r="B16" s="69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C16" s="69"/>
       <c r="D16" s="69" t="s">
@@ -54303,7 +54303,7 @@
       </c>
       <c r="E16" s="69"/>
       <c r="F16" s="69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G16" s="69"/>
       <c r="H16" s="177"/>
@@ -54311,15 +54311,15 @@
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="244"/>
       <c r="B17" s="69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C17" s="69"/>
       <c r="D17" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="69" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="177"/>
@@ -54327,15 +54327,15 @@
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="244"/>
       <c r="B18" s="69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" s="69"/>
       <c r="D18" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="69" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G18" s="69"/>
       <c r="H18" s="177"/>
@@ -54347,11 +54347,11 @@
       </c>
       <c r="C19" s="69"/>
       <c r="D19" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="69" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G19" s="69"/>
       <c r="H19" s="177"/>
@@ -54359,15 +54359,15 @@
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="244"/>
       <c r="B20" s="69" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G20" s="69"/>
       <c r="H20" s="177"/>
@@ -54375,15 +54375,15 @@
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="244"/>
       <c r="B21" s="69" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C21" s="69"/>
       <c r="D21" s="69" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="69" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G21" s="69"/>
       <c r="H21" s="177"/>
@@ -54391,15 +54391,15 @@
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="244"/>
       <c r="B22" s="69" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C22" s="69"/>
       <c r="D22" s="69" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="69" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G22" s="69"/>
       <c r="H22" s="177"/>
@@ -54407,7 +54407,7 @@
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="244"/>
       <c r="B23" s="69" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69" t="s">
@@ -54415,7 +54415,7 @@
       </c>
       <c r="E23" s="69"/>
       <c r="F23" s="69" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G23" s="69"/>
       <c r="H23" s="177"/>
@@ -54423,7 +54423,7 @@
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="245"/>
       <c r="B24" s="73" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73" t="s">
@@ -54431,14 +54431,14 @@
       </c>
       <c r="E24" s="73"/>
       <c r="F24" s="73" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G24" s="73"/>
       <c r="H24" s="178"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="246" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B25" s="179"/>
       <c r="C25" s="179"/>
@@ -54451,15 +54451,15 @@
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="241"/>
       <c r="B26" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E26" s="47"/>
       <c r="F26" s="47" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="174"/>
@@ -54467,15 +54467,15 @@
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="241"/>
       <c r="B27" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C27" s="47"/>
       <c r="D27" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E27" s="47"/>
       <c r="F27" s="47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G27" s="47"/>
       <c r="H27" s="174"/>
@@ -54483,7 +54483,7 @@
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="241"/>
       <c r="B28" s="47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47" t="s">
@@ -54491,7 +54491,7 @@
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="174"/>
@@ -54499,15 +54499,15 @@
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="241"/>
       <c r="B29" s="47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="174"/>
@@ -54515,15 +54515,15 @@
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="241"/>
       <c r="B30" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="174"/>
@@ -54531,15 +54531,15 @@
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="241"/>
       <c r="B31" s="47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E31" s="47"/>
       <c r="F31" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="174"/>
@@ -54547,15 +54547,15 @@
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="241"/>
       <c r="B32" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E32" s="47"/>
       <c r="F32" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="174"/>
@@ -54563,15 +54563,15 @@
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="241"/>
       <c r="B33" s="47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E33" s="47"/>
       <c r="F33" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="174"/>
@@ -54583,11 +54583,11 @@
       </c>
       <c r="C34" s="47"/>
       <c r="D34" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E34" s="47"/>
       <c r="F34" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="174"/>
@@ -54595,15 +54595,15 @@
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="241"/>
       <c r="B35" s="47" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E35" s="47"/>
       <c r="F35" s="47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="174"/>
@@ -54611,22 +54611,22 @@
     <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="242"/>
       <c r="B36" s="51" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G36" s="51"/>
       <c r="H36" s="181"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="243" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B37" s="175"/>
       <c r="C37" s="175"/>
@@ -54640,15 +54640,15 @@
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="244"/>
       <c r="B38" s="69" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C38" s="69"/>
       <c r="D38" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E38" s="69"/>
       <c r="F38" s="69" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="177"/>
@@ -54656,15 +54656,15 @@
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="244"/>
       <c r="B39" s="69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C39" s="69"/>
       <c r="D39" s="69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E39" s="69"/>
       <c r="F39" s="69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G39" s="69"/>
       <c r="H39" s="177"/>
@@ -54672,7 +54672,7 @@
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="244"/>
       <c r="B40" s="69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C40" s="69"/>
       <c r="D40" s="69" t="s">
@@ -54680,7 +54680,7 @@
       </c>
       <c r="E40" s="69"/>
       <c r="F40" s="69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G40" s="69"/>
       <c r="H40" s="177"/>
@@ -54688,15 +54688,15 @@
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="244"/>
       <c r="B41" s="69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41" s="69"/>
       <c r="D41" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G41" s="69"/>
       <c r="H41" s="177"/>
@@ -54704,15 +54704,15 @@
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="244"/>
       <c r="B42" s="69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E42" s="69"/>
       <c r="F42" s="69" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G42" s="69"/>
       <c r="H42" s="177"/>
@@ -54720,15 +54720,15 @@
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="244"/>
       <c r="B43" s="69" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C43" s="69"/>
       <c r="D43" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E43" s="69"/>
       <c r="F43" s="69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G43" s="69"/>
       <c r="H43" s="177"/>
@@ -54736,15 +54736,15 @@
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="244"/>
       <c r="B44" s="69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C44" s="69"/>
       <c r="D44" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E44" s="69"/>
       <c r="F44" s="69" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="177"/>
@@ -54752,15 +54752,15 @@
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="244"/>
       <c r="B45" s="69" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C45" s="69"/>
       <c r="D45" s="69" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E45" s="69"/>
       <c r="F45" s="69" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G45" s="69"/>
       <c r="H45" s="177"/>
@@ -54768,15 +54768,15 @@
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="244"/>
       <c r="B46" s="69" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E46" s="69"/>
       <c r="F46" s="69" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G46" s="69"/>
       <c r="H46" s="177"/>
@@ -54788,11 +54788,11 @@
       </c>
       <c r="C47" s="69"/>
       <c r="D47" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E47" s="69"/>
       <c r="F47" s="69" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G47" s="69"/>
       <c r="H47" s="177"/>
@@ -54800,15 +54800,15 @@
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="245"/>
       <c r="B48" s="73" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E48" s="73"/>
       <c r="F48" s="73" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G48" s="73"/>
       <c r="H48" s="178"/>

</xml_diff>

<commit_message>
style: cleanup metadata excel
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D69C4-9477-49FA-B4BD-71DBE6D9B17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDC39DD-0486-4138-A4D6-C70033CDBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29100" windowHeight="13455" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29100" windowHeight="13455" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -4225,12 +4225,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ107"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -35406,7 +35406,7 @@
   <dimension ref="A1:XFC14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
@@ -36871,7 +36871,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A7"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -46102,7 +46102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -47030,7 +47030,7 @@
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E9" sqref="E9"/>

</xml_diff>

<commit_message>
feat(deployment): add field- cloud-init config
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDC39DD-0486-4138-A4D6-C70033CDBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83371CD-6847-4305-864F-F9D049C0CBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29100" windowHeight="13455" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="580">
   <si>
     <t>Concept</t>
   </si>
@@ -1845,6 +1845,15 @@
   <si>
     <t>UUIDs of required Data asset(s) for  MicroserviceC</t>
   </si>
+  <si>
+    <t>cloud_config</t>
+  </si>
+  <si>
+    <t>cloud-init configuration for contextualisation of the VM</t>
+  </si>
+  <si>
+    <t>#cloud-config\nruncmd:\n- [ sh, -xc, \"echo 'hello world!'\" ]</t>
+  </si>
 </sst>
 </file>
 
@@ -3232,52 +3241,40 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3286,6 +3283,14 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3310,6 +3315,46 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3354,42 +3399,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4247,16 +4256,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -4285,7 +4294,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4297,7 +4306,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="242"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4317,7 +4326,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="242"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4337,7 +4346,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="242"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4357,7 +4366,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="242"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4377,7 +4386,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="242"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4397,7 +4406,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="242"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4417,7 +4426,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="242"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4437,7 +4446,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="243"/>
+      <c r="A11" s="242"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4457,7 +4466,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="244" t="s">
+      <c r="A12" s="243" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="213"/>
@@ -4469,7 +4478,7 @@
       <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="245"/>
+      <c r="A13" s="244"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4489,7 +4498,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="245"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4508,8 +4517,8 @@
       </c>
       <c r="H14" s="58"/>
     </row>
-    <row r="15" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="245"/>
+    <row r="15" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="244"/>
       <c r="B15" s="55" t="s">
         <v>457</v>
       </c>
@@ -5545,7 +5554,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="245"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="55"/>
       <c r="C16" s="56" t="s">
         <v>562</v>
@@ -6581,7 +6590,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="245"/>
+      <c r="A17" s="244"/>
       <c r="B17" s="55"/>
       <c r="C17" s="56" t="s">
         <v>564</v>
@@ -7617,7 +7626,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="245"/>
+      <c r="A18" s="244"/>
       <c r="B18" s="55"/>
       <c r="C18" s="56" t="s">
         <v>563</v>
@@ -8653,7 +8662,7 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="245"/>
+      <c r="A19" s="244"/>
       <c r="B19" s="55" t="s">
         <v>454</v>
       </c>
@@ -9689,7 +9698,7 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="246"/>
+      <c r="A20" s="245"/>
       <c r="B20" s="217" t="s">
         <v>455</v>
       </c>
@@ -10725,7 +10734,7 @@
       <c r="AMJ20" s="4"/>
     </row>
     <row r="21" spans="1:1024" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="237" t="s">
+      <c r="A21" s="246" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="59"/>
@@ -10737,7 +10746,7 @@
       <c r="H21" s="61"/>
     </row>
     <row r="22" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="237"/>
+      <c r="A22" s="246"/>
       <c r="B22" s="47" t="s">
         <v>40</v>
       </c>
@@ -10757,7 +10766,7 @@
       <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="237"/>
+      <c r="A23" s="246"/>
       <c r="B23" s="47" t="s">
         <v>44</v>
       </c>
@@ -10777,7 +10786,7 @@
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="237"/>
+      <c r="A24" s="246"/>
       <c r="B24" s="47" t="s">
         <v>46</v>
       </c>
@@ -10797,7 +10806,7 @@
       <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="237"/>
+      <c r="A25" s="246"/>
       <c r="B25" s="47" t="s">
         <v>48</v>
       </c>
@@ -10817,7 +10826,7 @@
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="237"/>
+      <c r="A26" s="246"/>
       <c r="B26" s="47" t="s">
         <v>50</v>
       </c>
@@ -10837,7 +10846,7 @@
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="237"/>
+      <c r="A27" s="246"/>
       <c r="B27" s="47" t="s">
         <v>53</v>
       </c>
@@ -10857,7 +10866,7 @@
       <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="237"/>
+      <c r="A28" s="246"/>
       <c r="B28" s="47" t="s">
         <v>57</v>
       </c>
@@ -10877,7 +10886,7 @@
       <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="237"/>
+      <c r="A29" s="246"/>
       <c r="B29" s="47" t="s">
         <v>61</v>
       </c>
@@ -10897,7 +10906,7 @@
       <c r="H29" s="50"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="237"/>
+      <c r="A30" s="246"/>
       <c r="B30" s="47" t="s">
         <v>63</v>
       </c>
@@ -10917,7 +10926,7 @@
       <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="237"/>
+      <c r="A31" s="246"/>
       <c r="B31" s="47" t="s">
         <v>65</v>
       </c>
@@ -10937,7 +10946,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="237"/>
+      <c r="A32" s="246"/>
       <c r="B32" s="47" t="s">
         <v>67</v>
       </c>
@@ -10957,7 +10966,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="238"/>
+      <c r="A33" s="247"/>
       <c r="B33" s="51" t="s">
         <v>69</v>
       </c>
@@ -10977,7 +10986,7 @@
       <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="233" t="s">
+      <c r="A34" s="248" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="62"/>
@@ -10989,7 +10998,7 @@
       <c r="H34" s="64"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="234"/>
+      <c r="A35" s="249"/>
       <c r="B35" s="65" t="s">
         <v>73</v>
       </c>
@@ -11009,7 +11018,7 @@
       <c r="H35" s="68"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="234"/>
+      <c r="A36" s="249"/>
       <c r="B36" s="69" t="s">
         <v>76</v>
       </c>
@@ -11029,7 +11038,7 @@
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="234"/>
+      <c r="A37" s="249"/>
       <c r="B37" s="69" t="s">
         <v>79</v>
       </c>
@@ -11049,7 +11058,7 @@
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="235"/>
+      <c r="A38" s="250"/>
       <c r="B38" s="73" t="s">
         <v>82</v>
       </c>
@@ -11069,7 +11078,7 @@
       <c r="H38" s="76"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="236" t="s">
+      <c r="A39" s="251" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="59"/>
@@ -11081,7 +11090,7 @@
       <c r="H39" s="61"/>
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="237"/>
+      <c r="A40" s="246"/>
       <c r="B40" s="47" t="s">
         <v>86</v>
       </c>
@@ -12117,8 +12126,8 @@
       <c r="AMJ40" s="4"/>
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="237"/>
-      <c r="B41" s="227" t="s">
+      <c r="A41" s="246"/>
+      <c r="B41" s="238" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -13155,8 +13164,8 @@
       <c r="AMJ41" s="4"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A42" s="237"/>
-      <c r="B42" s="227"/>
+      <c r="A42" s="246"/>
+      <c r="B42" s="238"/>
       <c r="C42" s="47" t="s">
         <v>94</v>
       </c>
@@ -14191,8 +14200,8 @@
       <c r="AMJ42" s="4"/>
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="237"/>
-      <c r="B43" s="227"/>
+      <c r="A43" s="246"/>
+      <c r="B43" s="238"/>
       <c r="C43" s="47" t="s">
         <v>98</v>
       </c>
@@ -15227,8 +15236,8 @@
       <c r="AMJ43" s="4"/>
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="237"/>
-      <c r="B44" s="227"/>
+      <c r="A44" s="246"/>
+      <c r="B44" s="238"/>
       <c r="C44" s="47" t="s">
         <v>102</v>
       </c>
@@ -16263,8 +16272,8 @@
       <c r="AMJ44" s="4"/>
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="237"/>
-      <c r="B45" s="227"/>
+      <c r="A45" s="246"/>
+      <c r="B45" s="238"/>
       <c r="C45" s="47" t="s">
         <v>106</v>
       </c>
@@ -17299,8 +17308,8 @@
       <c r="AMJ45" s="4"/>
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="237"/>
-      <c r="B46" s="227"/>
+      <c r="A46" s="246"/>
+      <c r="B46" s="238"/>
       <c r="C46" s="47" t="s">
         <v>110</v>
       </c>
@@ -18335,8 +18344,8 @@
       <c r="AMJ46" s="4"/>
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="237"/>
-      <c r="B47" s="227"/>
+      <c r="A47" s="246"/>
+      <c r="B47" s="238"/>
       <c r="C47" s="47" t="s">
         <v>114</v>
       </c>
@@ -19371,8 +19380,8 @@
       <c r="AMJ47" s="4"/>
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="237"/>
-      <c r="B48" s="227"/>
+      <c r="A48" s="246"/>
+      <c r="B48" s="238"/>
       <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
@@ -20407,8 +20416,8 @@
       <c r="AMJ48" s="4"/>
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="237"/>
-      <c r="B49" s="227"/>
+      <c r="A49" s="246"/>
+      <c r="B49" s="238"/>
       <c r="C49" s="47" t="s">
         <v>122</v>
       </c>
@@ -21443,8 +21452,8 @@
       <c r="AMJ49" s="4"/>
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="237"/>
-      <c r="B50" s="227"/>
+      <c r="A50" s="246"/>
+      <c r="B50" s="238"/>
       <c r="C50" s="47" t="s">
         <v>126</v>
       </c>
@@ -22479,8 +22488,8 @@
       <c r="AMJ50" s="4"/>
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="237"/>
-      <c r="B51" s="227"/>
+      <c r="A51" s="246"/>
+      <c r="B51" s="238"/>
       <c r="C51" s="47" t="s">
         <v>130</v>
       </c>
@@ -23515,8 +23524,8 @@
       <c r="AMJ51" s="4"/>
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="238"/>
-      <c r="B52" s="228"/>
+      <c r="A52" s="247"/>
+      <c r="B52" s="239"/>
       <c r="C52" s="51" t="s">
         <v>134</v>
       </c>
@@ -24551,7 +24560,7 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="233" t="s">
+      <c r="A53" s="248" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="77"/>
@@ -24563,7 +24572,7 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="234"/>
+      <c r="A54" s="249"/>
       <c r="B54" s="80" t="s">
         <v>138</v>
       </c>
@@ -24583,8 +24592,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="234"/>
-      <c r="B55" s="229" t="s">
+      <c r="A55" s="249"/>
+      <c r="B55" s="252" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="84" t="s">
@@ -24605,8 +24614,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A56" s="234"/>
-      <c r="B56" s="229"/>
+      <c r="A56" s="249"/>
+      <c r="B56" s="252"/>
       <c r="C56" s="80" t="s">
         <v>94</v>
       </c>
@@ -24625,8 +24634,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="234"/>
-      <c r="B57" s="229"/>
+      <c r="A57" s="249"/>
+      <c r="B57" s="252"/>
       <c r="C57" s="80" t="s">
         <v>98</v>
       </c>
@@ -24645,8 +24654,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="234"/>
-      <c r="B58" s="229"/>
+      <c r="A58" s="249"/>
+      <c r="B58" s="252"/>
       <c r="C58" s="80" t="s">
         <v>102</v>
       </c>
@@ -24665,8 +24674,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="234"/>
-      <c r="B59" s="229"/>
+      <c r="A59" s="249"/>
+      <c r="B59" s="252"/>
       <c r="C59" s="80" t="s">
         <v>106</v>
       </c>
@@ -24685,8 +24694,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="234"/>
-      <c r="B60" s="229"/>
+      <c r="A60" s="249"/>
+      <c r="B60" s="252"/>
       <c r="C60" s="80" t="s">
         <v>110</v>
       </c>
@@ -24705,8 +24714,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="234"/>
-      <c r="B61" s="229"/>
+      <c r="A61" s="249"/>
+      <c r="B61" s="252"/>
       <c r="C61" s="80" t="s">
         <v>114</v>
       </c>
@@ -24725,8 +24734,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="234"/>
-      <c r="B62" s="229"/>
+      <c r="A62" s="249"/>
+      <c r="B62" s="252"/>
       <c r="C62" s="80" t="s">
         <v>118</v>
       </c>
@@ -24745,8 +24754,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="234"/>
-      <c r="B63" s="229"/>
+      <c r="A63" s="249"/>
+      <c r="B63" s="252"/>
       <c r="C63" s="80" t="s">
         <v>122</v>
       </c>
@@ -24765,8 +24774,8 @@
       <c r="H63" s="83"/>
     </row>
     <row r="64" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="234"/>
-      <c r="B64" s="229"/>
+      <c r="A64" s="249"/>
+      <c r="B64" s="252"/>
       <c r="C64" s="80" t="s">
         <v>126</v>
       </c>
@@ -24785,8 +24794,8 @@
       <c r="H64" s="83"/>
     </row>
     <row r="65" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="234"/>
-      <c r="B65" s="229"/>
+      <c r="A65" s="249"/>
+      <c r="B65" s="252"/>
       <c r="C65" s="80" t="s">
         <v>130</v>
       </c>
@@ -24805,8 +24814,8 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="235"/>
-      <c r="B66" s="230"/>
+      <c r="A66" s="250"/>
+      <c r="B66" s="253"/>
       <c r="C66" s="85" t="s">
         <v>134</v>
       </c>
@@ -24825,7 +24834,7 @@
       <c r="H66" s="87"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="236" t="s">
+      <c r="A67" s="251" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="59"/>
@@ -25853,7 +25862,7 @@
       <c r="AMJ67" s="13"/>
     </row>
     <row r="68" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="237"/>
+      <c r="A68" s="246"/>
       <c r="B68" s="89" t="s">
         <v>146</v>
       </c>
@@ -26889,7 +26898,7 @@
       <c r="AMJ68" s="13"/>
     </row>
     <row r="69" spans="1:1024" s="14" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="238"/>
+      <c r="A69" s="247"/>
       <c r="B69" s="93" t="s">
         <v>150</v>
       </c>
@@ -27925,7 +27934,7 @@
       <c r="AMJ69" s="13"/>
     </row>
     <row r="70" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="233" t="s">
+      <c r="A70" s="248" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="29"/>
@@ -27937,7 +27946,7 @@
       <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="234"/>
+      <c r="A71" s="249"/>
       <c r="B71" s="69" t="s">
         <v>155</v>
       </c>
@@ -27955,8 +27964,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="234"/>
-      <c r="B72" s="231" t="s">
+      <c r="A72" s="249"/>
+      <c r="B72" s="254" t="s">
         <v>158</v>
       </c>
       <c r="C72" s="69" t="s">
@@ -27977,8 +27986,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="234"/>
-      <c r="B73" s="231"/>
+      <c r="A73" s="249"/>
+      <c r="B73" s="254"/>
       <c r="C73" s="69" t="s">
         <v>30</v>
       </c>
@@ -27997,8 +28006,8 @@
       <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="234"/>
-      <c r="B74" s="231"/>
+      <c r="A74" s="249"/>
+      <c r="B74" s="254"/>
       <c r="C74" s="69" t="s">
         <v>12</v>
       </c>
@@ -28017,8 +28026,8 @@
       <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="234"/>
-      <c r="B75" s="231"/>
+      <c r="A75" s="249"/>
+      <c r="B75" s="254"/>
       <c r="C75" s="69" t="s">
         <v>167</v>
       </c>
@@ -28037,8 +28046,8 @@
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="235"/>
-      <c r="B76" s="232"/>
+      <c r="A76" s="250"/>
+      <c r="B76" s="255"/>
       <c r="C76" s="73" t="s">
         <v>25</v>
       </c>
@@ -28057,7 +28066,7 @@
       <c r="H76" s="76"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="236" t="s">
+      <c r="A77" s="251" t="s">
         <v>172</v>
       </c>
       <c r="B77" s="31"/>
@@ -29085,7 +29094,7 @@
       <c r="AMJ77" s="13"/>
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="237"/>
+      <c r="A78" s="246"/>
       <c r="B78" s="47" t="s">
         <v>173</v>
       </c>
@@ -30119,8 +30128,8 @@
       <c r="AMJ78" s="13"/>
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="237"/>
-      <c r="B79" s="227" t="s">
+      <c r="A79" s="246"/>
+      <c r="B79" s="238" t="s">
         <v>176</v>
       </c>
       <c r="C79" s="47" t="s">
@@ -31157,8 +31166,8 @@
       <c r="AMJ79" s="13"/>
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="237"/>
-      <c r="B80" s="227"/>
+      <c r="A80" s="246"/>
+      <c r="B80" s="238"/>
       <c r="C80" s="47" t="s">
         <v>179</v>
       </c>
@@ -32193,8 +32202,8 @@
       <c r="AMJ80" s="13"/>
     </row>
     <row r="81" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="237"/>
-      <c r="B81" s="227"/>
+      <c r="A81" s="246"/>
+      <c r="B81" s="238"/>
       <c r="C81" s="47" t="s">
         <v>182</v>
       </c>
@@ -33229,8 +33238,8 @@
       <c r="AMJ81" s="13"/>
     </row>
     <row r="82" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="237"/>
-      <c r="B82" s="227"/>
+      <c r="A82" s="246"/>
+      <c r="B82" s="238"/>
       <c r="C82" s="47" t="s">
         <v>185</v>
       </c>
@@ -34265,8 +34274,8 @@
       <c r="AMJ82" s="13"/>
     </row>
     <row r="83" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="238"/>
-      <c r="B83" s="228"/>
+      <c r="A83" s="247"/>
+      <c r="B83" s="239"/>
       <c r="C83" s="51" t="s">
         <v>25</v>
       </c>
@@ -35375,6 +35384,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B55:B66"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A77:A83"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B41:B52"/>
     <mergeCell ref="A3:A11"/>
@@ -35382,13 +35398,6 @@
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A52"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B55:B66"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A77:A83"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -35428,16 +35437,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -35466,7 +35475,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -35478,7 +35487,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="242"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -35498,7 +35507,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="242"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -35518,7 +35527,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="242"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -35538,7 +35547,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="242"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -35558,7 +35567,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="242"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -35578,7 +35587,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="242"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -35598,7 +35607,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="242"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -35618,7 +35627,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="243"/>
+      <c r="A11" s="242"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -35638,7 +35647,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="247" t="s">
+      <c r="A12" s="256" t="s">
         <v>203</v>
       </c>
       <c r="B12" s="98"/>
@@ -35650,7 +35659,7 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="248"/>
+      <c r="A13" s="257"/>
       <c r="B13" s="103" t="s">
         <v>204</v>
       </c>
@@ -35670,7 +35679,7 @@
       <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="248"/>
+      <c r="A14" s="257"/>
       <c r="B14" s="103" t="s">
         <v>448</v>
       </c>
@@ -35728,16 +35737,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>487</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -35766,7 +35775,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="240" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -35816,7 +35825,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="242"/>
+      <c r="A4" s="241"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -35834,7 +35843,7 @@
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="242"/>
+      <c r="A5" s="241"/>
       <c r="B5" s="105" t="s">
         <v>209</v>
       </c>
@@ -35850,7 +35859,7 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="242"/>
+      <c r="A6" s="241"/>
       <c r="B6" s="105" t="s">
         <v>212</v>
       </c>
@@ -35866,7 +35875,7 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="242"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="105" t="s">
         <v>213</v>
       </c>
@@ -35882,7 +35891,7 @@
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="242"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="105" t="s">
         <v>214</v>
       </c>
@@ -35898,7 +35907,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="242"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="105" t="s">
         <v>216</v>
       </c>
@@ -35916,7 +35925,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="242"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="105" t="s">
         <v>218</v>
       </c>
@@ -35945,7 +35954,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="242"/>
+      <c r="A11" s="241"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -35961,7 +35970,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="242"/>
+      <c r="A12" s="241"/>
       <c r="B12" s="105" t="s">
         <v>222</v>
       </c>
@@ -35979,7 +35988,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="242"/>
+      <c r="A13" s="241"/>
       <c r="B13" s="105" t="s">
         <v>224</v>
       </c>
@@ -35997,7 +36006,7 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="242"/>
+      <c r="A14" s="241"/>
       <c r="B14" s="105" t="s">
         <v>459</v>
       </c>
@@ -36015,7 +36024,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="243"/>
+      <c r="A15" s="242"/>
       <c r="B15" s="108" t="s">
         <v>228</v>
       </c>
@@ -36031,7 +36040,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="233" t="s">
+      <c r="A16" s="248" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -36044,7 +36053,7 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="234"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="113" t="s">
         <v>231</v>
       </c>
@@ -36060,7 +36069,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="234"/>
+      <c r="A18" s="249"/>
       <c r="B18" s="113"/>
       <c r="C18" s="114" t="s">
         <v>1</v>
@@ -36076,7 +36085,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="234"/>
+      <c r="A19" s="249"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>209</v>
@@ -36092,7 +36101,7 @@
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="234"/>
+      <c r="A20" s="249"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
         <v>518</v>
@@ -36108,7 +36117,7 @@
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="234"/>
+      <c r="A21" s="249"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
         <v>519</v>
@@ -36124,7 +36133,7 @@
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="234"/>
+      <c r="A22" s="249"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
         <v>520</v>
@@ -36140,7 +36149,7 @@
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="234"/>
+      <c r="A23" s="249"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
         <v>521</v>
@@ -36156,7 +36165,7 @@
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="234"/>
+      <c r="A24" s="249"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
         <v>522</v>
@@ -36172,7 +36181,7 @@
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="234"/>
+      <c r="A25" s="249"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
         <v>523</v>
@@ -36188,7 +36197,7 @@
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="234"/>
+      <c r="A26" s="249"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
         <v>524</v>
@@ -36204,7 +36213,7 @@
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="234"/>
+      <c r="A27" s="249"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
         <v>525</v>
@@ -36220,7 +36229,7 @@
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="234"/>
+      <c r="A28" s="249"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
         <v>526</v>
@@ -36236,7 +36245,7 @@
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="234"/>
+      <c r="A29" s="249"/>
       <c r="B29" s="113" t="s">
         <v>233</v>
       </c>
@@ -36252,7 +36261,7 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="234"/>
+      <c r="A30" s="249"/>
       <c r="B30" s="222"/>
       <c r="C30" s="114" t="s">
         <v>1</v>
@@ -36268,7 +36277,7 @@
       <c r="H30" s="225"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="234"/>
+      <c r="A31" s="249"/>
       <c r="B31" s="222"/>
       <c r="C31" s="114" t="s">
         <v>209</v>
@@ -36284,7 +36293,7 @@
       <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="234"/>
+      <c r="A32" s="249"/>
       <c r="B32" s="222"/>
       <c r="C32" s="114" t="s">
         <v>518</v>
@@ -36300,7 +36309,7 @@
       <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="234"/>
+      <c r="A33" s="249"/>
       <c r="B33" s="222"/>
       <c r="C33" s="114" t="s">
         <v>519</v>
@@ -36316,7 +36325,7 @@
       <c r="H33" s="225"/>
     </row>
     <row r="34" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="234"/>
+      <c r="A34" s="249"/>
       <c r="B34" s="222"/>
       <c r="C34" s="114" t="s">
         <v>520</v>
@@ -36332,7 +36341,7 @@
       <c r="H34" s="225"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="234"/>
+      <c r="A35" s="249"/>
       <c r="B35" s="222"/>
       <c r="C35" s="114" t="s">
         <v>521</v>
@@ -36348,7 +36357,7 @@
       <c r="H35" s="225"/>
     </row>
     <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="234"/>
+      <c r="A36" s="249"/>
       <c r="B36" s="222"/>
       <c r="C36" s="114" t="s">
         <v>522</v>
@@ -36364,7 +36373,7 @@
       <c r="H36" s="225"/>
     </row>
     <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="234"/>
+      <c r="A37" s="249"/>
       <c r="B37" s="222"/>
       <c r="C37" s="114" t="s">
         <v>523</v>
@@ -36380,7 +36389,7 @@
       <c r="H37" s="225"/>
     </row>
     <row r="38" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="234"/>
+      <c r="A38" s="249"/>
       <c r="B38" s="222"/>
       <c r="C38" s="114" t="s">
         <v>524</v>
@@ -36396,7 +36405,7 @@
       <c r="H38" s="225"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="234"/>
+      <c r="A39" s="249"/>
       <c r="B39" s="222"/>
       <c r="C39" s="114" t="s">
         <v>525</v>
@@ -36412,7 +36421,7 @@
       <c r="H39" s="225"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="234"/>
+      <c r="A40" s="249"/>
       <c r="B40" s="222"/>
       <c r="C40" s="114" t="s">
         <v>526</v>
@@ -36428,7 +36437,7 @@
       <c r="H40" s="225"/>
     </row>
     <row r="41" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="235"/>
+      <c r="A41" s="250"/>
       <c r="B41" s="116" t="s">
         <v>235</v>
       </c>
@@ -36446,7 +36455,7 @@
       <c r="H41" s="118"/>
     </row>
     <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="236" t="s">
+      <c r="A42" s="251" t="s">
         <v>236</v>
       </c>
       <c r="B42" s="119"/>
@@ -36496,7 +36505,7 @@
       <c r="AMJ42" s="5"/>
     </row>
     <row r="43" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="238"/>
+      <c r="A43" s="247"/>
       <c r="B43" s="108" t="s">
         <v>237</v>
       </c>
@@ -36533,7 +36542,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="233" t="s">
+      <c r="A44" s="248" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="111"/>
@@ -36546,7 +36555,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="234"/>
+      <c r="A45" s="249"/>
       <c r="B45" s="113" t="s">
         <v>73</v>
       </c>
@@ -36564,7 +36573,7 @@
       <c r="H45" s="115"/>
     </row>
     <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="234"/>
+      <c r="A46" s="249"/>
       <c r="B46" s="113" t="s">
         <v>76</v>
       </c>
@@ -36582,7 +36591,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="235"/>
+      <c r="A47" s="250"/>
       <c r="B47" s="116" t="s">
         <v>79</v>
       </c>
@@ -36600,7 +36609,7 @@
       <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="236" t="s">
+      <c r="A48" s="251" t="s">
         <v>243</v>
       </c>
       <c r="B48" s="121"/>
@@ -36631,7 +36640,7 @@
       <c r="AMJ48" s="5"/>
     </row>
     <row r="49" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="237"/>
+      <c r="A49" s="246"/>
       <c r="B49" s="105" t="s">
         <v>244</v>
       </c>
@@ -36649,7 +36658,7 @@
       <c r="H49" s="107"/>
     </row>
     <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="237"/>
+      <c r="A50" s="246"/>
       <c r="B50" s="105" t="s">
         <v>246</v>
       </c>
@@ -36667,7 +36676,7 @@
       <c r="H50" s="107"/>
     </row>
     <row r="51" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="237"/>
+      <c r="A51" s="246"/>
       <c r="B51" s="105" t="s">
         <v>46</v>
       </c>
@@ -36685,7 +36694,7 @@
       <c r="H51" s="107"/>
     </row>
     <row r="52" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="237"/>
+      <c r="A52" s="246"/>
       <c r="B52" s="105" t="s">
         <v>48</v>
       </c>
@@ -36703,7 +36712,7 @@
       <c r="H52" s="107"/>
     </row>
     <row r="53" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="237"/>
+      <c r="A53" s="246"/>
       <c r="B53" s="105" t="s">
         <v>61</v>
       </c>
@@ -36741,7 +36750,7 @@
       <c r="AMJ53" s="5"/>
     </row>
     <row r="54" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="237"/>
+      <c r="A54" s="246"/>
       <c r="B54" s="105" t="s">
         <v>63</v>
       </c>
@@ -36759,7 +36768,7 @@
       <c r="H54" s="107"/>
     </row>
     <row r="55" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="237"/>
+      <c r="A55" s="246"/>
       <c r="B55" s="105" t="s">
         <v>65</v>
       </c>
@@ -36777,7 +36786,7 @@
       <c r="H55" s="107"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="237"/>
+      <c r="A56" s="246"/>
       <c r="B56" s="105" t="s">
         <v>67</v>
       </c>
@@ -36795,7 +36804,7 @@
       <c r="H56" s="107"/>
     </row>
     <row r="57" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="238"/>
+      <c r="A57" s="247"/>
       <c r="B57" s="108" t="s">
         <v>69</v>
       </c>
@@ -36813,7 +36822,7 @@
       <c r="H57" s="110"/>
     </row>
     <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="233" t="s">
+      <c r="A58" s="248" t="s">
         <v>499</v>
       </c>
       <c r="B58" s="123"/>
@@ -36826,7 +36835,7 @@
       <c r="AMJ58" s="5"/>
     </row>
     <row r="59" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="235"/>
+      <c r="A59" s="250"/>
       <c r="B59" s="116" t="s">
         <v>5</v>
       </c>
@@ -36888,16 +36897,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -37942,7 +37951,7 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="249" t="s">
+      <c r="A3" s="258" t="s">
         <v>500</v>
       </c>
       <c r="B3" s="121"/>
@@ -37967,7 +37976,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="250"/>
+      <c r="A4" s="259"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -37987,7 +37996,7 @@
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="250"/>
+      <c r="A5" s="259"/>
       <c r="B5" s="105" t="s">
         <v>305</v>
       </c>
@@ -38007,7 +38016,7 @@
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="250"/>
+      <c r="A6" s="259"/>
       <c r="B6" s="105" t="s">
         <v>507</v>
       </c>
@@ -38027,7 +38036,7 @@
       <c r="H6" s="126"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="250"/>
+      <c r="A7" s="259"/>
       <c r="B7" s="105" t="s">
         <v>308</v>
       </c>
@@ -38047,7 +38056,7 @@
       <c r="H7" s="126"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="261" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="123"/>
@@ -38060,7 +38069,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="254"/>
+      <c r="A9" s="263"/>
       <c r="B9" s="113" t="s">
         <v>311</v>
       </c>
@@ -39096,7 +39105,7 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="254"/>
+      <c r="A10" s="263"/>
       <c r="B10" s="113" t="s">
         <v>508</v>
       </c>
@@ -40132,7 +40141,7 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="263"/>
       <c r="B11" s="113" t="s">
         <v>316</v>
       </c>
@@ -41168,7 +41177,7 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="254"/>
+      <c r="A12" s="263"/>
       <c r="B12" s="113" t="s">
         <v>509</v>
       </c>
@@ -42204,7 +42213,7 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="254"/>
+      <c r="A13" s="263"/>
       <c r="B13" s="113" t="s">
         <v>313</v>
       </c>
@@ -43240,7 +43249,7 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="249" t="s">
+      <c r="A14" s="258" t="s">
         <v>501</v>
       </c>
       <c r="B14" s="121"/>
@@ -43261,7 +43270,7 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="251"/>
+      <c r="A15" s="260"/>
       <c r="B15" s="108" t="s">
         <v>320</v>
       </c>
@@ -44297,7 +44306,7 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="252" t="s">
+      <c r="A16" s="261" t="s">
         <v>323</v>
       </c>
       <c r="B16" s="111"/>
@@ -45325,7 +45334,7 @@
       <c r="AMJ16" s="39"/>
     </row>
     <row r="17" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
+      <c r="A17" s="263"/>
       <c r="B17" s="113" t="s">
         <v>94</v>
       </c>
@@ -45345,7 +45354,7 @@
       <c r="H17" s="129"/>
     </row>
     <row r="18" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="254"/>
+      <c r="A18" s="263"/>
       <c r="B18" s="113" t="s">
         <v>98</v>
       </c>
@@ -45365,7 +45374,7 @@
       <c r="H18" s="129"/>
     </row>
     <row r="19" spans="1:1024" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="253"/>
+      <c r="A19" s="262"/>
       <c r="B19" s="116" t="s">
         <v>102</v>
       </c>
@@ -45385,7 +45394,7 @@
       <c r="H19" s="130"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="249" t="s">
+      <c r="A20" s="258" t="s">
         <v>328</v>
       </c>
       <c r="B20" s="121"/>
@@ -45405,7 +45414,7 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="250"/>
+      <c r="A21" s="259"/>
       <c r="B21" s="105" t="s">
         <v>106</v>
       </c>
@@ -45425,7 +45434,7 @@
       <c r="H21" s="126"/>
     </row>
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="250"/>
+      <c r="A22" s="259"/>
       <c r="B22" s="105" t="s">
         <v>550</v>
       </c>
@@ -45445,7 +45454,7 @@
       <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="251"/>
+      <c r="A23" s="260"/>
       <c r="B23" s="108" t="s">
         <v>511</v>
       </c>
@@ -45465,7 +45474,7 @@
       <c r="H23" s="127"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="252" t="s">
+      <c r="A24" s="261" t="s">
         <v>502</v>
       </c>
       <c r="B24" s="132"/>
@@ -45478,7 +45487,7 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="253"/>
+      <c r="A25" s="262"/>
       <c r="B25" s="116" t="s">
         <v>334</v>
       </c>
@@ -45496,7 +45505,7 @@
       <c r="H25" s="130"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="249" t="s">
+      <c r="A26" s="258" t="s">
         <v>337</v>
       </c>
       <c r="B26" s="121"/>
@@ -45516,7 +45525,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="250"/>
+      <c r="A27" s="259"/>
       <c r="B27" s="105" t="s">
         <v>110</v>
       </c>
@@ -45536,7 +45545,7 @@
       <c r="H27" s="126"/>
     </row>
     <row r="28" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="250"/>
+      <c r="A28" s="259"/>
       <c r="B28" s="105" t="s">
         <v>118</v>
       </c>
@@ -45556,7 +45565,7 @@
       <c r="H28" s="126"/>
     </row>
     <row r="29" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="250"/>
+      <c r="A29" s="259"/>
       <c r="B29" s="105" t="s">
         <v>122</v>
       </c>
@@ -45576,7 +45585,7 @@
       <c r="H29" s="126"/>
     </row>
     <row r="30" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="250"/>
+      <c r="A30" s="259"/>
       <c r="B30" s="105" t="s">
         <v>126</v>
       </c>
@@ -45596,7 +45605,7 @@
       <c r="H30" s="126"/>
     </row>
     <row r="31" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="251"/>
+      <c r="A31" s="260"/>
       <c r="B31" s="108" t="s">
         <v>130</v>
       </c>
@@ -45616,7 +45625,7 @@
       <c r="H31" s="127"/>
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="252" t="s">
+      <c r="A32" s="261" t="s">
         <v>343</v>
       </c>
       <c r="B32" s="123"/>
@@ -45629,7 +45638,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="254"/>
+      <c r="A33" s="263"/>
       <c r="B33" s="113" t="s">
         <v>134</v>
       </c>
@@ -45649,7 +45658,7 @@
       <c r="H33" s="129"/>
     </row>
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="254"/>
+      <c r="A34" s="263"/>
       <c r="B34" s="113" t="s">
         <v>552</v>
       </c>
@@ -45667,7 +45676,7 @@
       <c r="H34" s="226"/>
     </row>
     <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="253"/>
+      <c r="A35" s="262"/>
       <c r="B35" s="116" t="s">
         <v>344</v>
       </c>
@@ -45736,16 +45745,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -45774,7 +45783,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="251" t="s">
         <v>503</v>
       </c>
       <c r="B3" s="18"/>
@@ -45801,7 +45810,7 @@
       <c r="AMJ3" s="134"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
+      <c r="A4" s="246"/>
       <c r="B4" s="106" t="s">
         <v>206</v>
       </c>
@@ -45821,7 +45830,7 @@
       <c r="H4" s="137"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
+      <c r="A5" s="246"/>
       <c r="B5" s="106" t="s">
         <v>259</v>
       </c>
@@ -45841,7 +45850,7 @@
       <c r="H5" s="137"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
+      <c r="A6" s="246"/>
       <c r="B6" s="106" t="s">
         <v>212</v>
       </c>
@@ -45859,7 +45868,7 @@
       <c r="H6" s="137"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="237"/>
+      <c r="A7" s="246"/>
       <c r="B7" s="106" t="s">
         <v>265</v>
       </c>
@@ -45879,7 +45888,7 @@
       <c r="H7" s="137"/>
     </row>
     <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="237"/>
+      <c r="A8" s="246"/>
       <c r="B8" s="106" t="s">
         <v>268</v>
       </c>
@@ -45899,7 +45908,7 @@
       <c r="H8" s="137"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="237"/>
+      <c r="A9" s="246"/>
       <c r="B9" s="106" t="s">
         <v>271</v>
       </c>
@@ -45919,7 +45928,7 @@
       <c r="H9" s="137"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="237"/>
+      <c r="A10" s="246"/>
       <c r="B10" s="106" t="s">
         <v>209</v>
       </c>
@@ -45937,7 +45946,7 @@
       <c r="H10" s="137"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="237"/>
+      <c r="A11" s="246"/>
       <c r="B11" s="106" t="s">
         <v>278</v>
       </c>
@@ -45955,7 +45964,7 @@
       <c r="H11" s="137"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="237"/>
+      <c r="A12" s="246"/>
       <c r="B12" s="106" t="s">
         <v>353</v>
       </c>
@@ -45973,7 +45982,7 @@
       <c r="H12" s="137"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="237"/>
+      <c r="A13" s="246"/>
       <c r="B13" s="106" t="s">
         <v>284</v>
       </c>
@@ -45991,7 +46000,7 @@
       <c r="H13" s="137"/>
     </row>
     <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="237"/>
+      <c r="A14" s="246"/>
       <c r="B14" s="106" t="s">
         <v>357</v>
       </c>
@@ -46009,7 +46018,7 @@
       <c r="H14" s="137"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="237"/>
+      <c r="A15" s="246"/>
       <c r="B15" s="106" t="s">
         <v>360</v>
       </c>
@@ -46027,7 +46036,7 @@
       <c r="H15" s="137"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="237"/>
+      <c r="A16" s="246"/>
       <c r="B16" s="106" t="s">
         <v>363</v>
       </c>
@@ -46045,7 +46054,7 @@
       <c r="H16" s="137"/>
     </row>
     <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="237"/>
+      <c r="A17" s="246"/>
       <c r="B17" s="106" t="s">
         <v>367</v>
       </c>
@@ -46063,7 +46072,7 @@
       <c r="H17" s="137"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="238"/>
+      <c r="A18" s="247"/>
       <c r="B18" s="109" t="s">
         <v>301</v>
       </c>
@@ -46124,16 +46133,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>490</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -46162,7 +46171,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="264" t="s">
         <v>503</v>
       </c>
       <c r="B3" s="142"/>
@@ -46174,7 +46183,7 @@
       <c r="H3" s="143"/>
     </row>
     <row r="4" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="256"/>
+      <c r="A4" s="265"/>
       <c r="B4" s="106" t="s">
         <v>206</v>
       </c>
@@ -46203,7 +46212,7 @@
       <c r="Q4" s="144"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="256"/>
+      <c r="A5" s="265"/>
       <c r="B5" s="106" t="s">
         <v>259</v>
       </c>
@@ -46232,7 +46241,7 @@
       <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="256"/>
+      <c r="A6" s="265"/>
       <c r="B6" s="106" t="s">
         <v>212</v>
       </c>
@@ -46259,7 +46268,7 @@
       <c r="Q6" s="144"/>
     </row>
     <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="256"/>
+      <c r="A7" s="265"/>
       <c r="B7" s="106" t="s">
         <v>265</v>
       </c>
@@ -46288,7 +46297,7 @@
       <c r="Q7" s="144"/>
     </row>
     <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="256"/>
+      <c r="A8" s="265"/>
       <c r="B8" s="106" t="s">
         <v>268</v>
       </c>
@@ -46317,7 +46326,7 @@
       <c r="Q8" s="144"/>
     </row>
     <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="256"/>
+      <c r="A9" s="265"/>
       <c r="B9" s="106" t="s">
         <v>271</v>
       </c>
@@ -46346,7 +46355,7 @@
       <c r="Q9" s="144"/>
     </row>
     <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="256"/>
+      <c r="A10" s="265"/>
       <c r="B10" s="106" t="s">
         <v>209</v>
       </c>
@@ -46373,7 +46382,7 @@
       <c r="Q10" s="144"/>
     </row>
     <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="256"/>
+      <c r="A11" s="265"/>
       <c r="B11" s="106" t="s">
         <v>278</v>
       </c>
@@ -46400,7 +46409,7 @@
       <c r="Q11" s="144"/>
     </row>
     <row r="12" spans="1:17" s="151" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="256"/>
+      <c r="A12" s="265"/>
       <c r="B12" s="106" t="s">
         <v>281</v>
       </c>
@@ -46427,7 +46436,7 @@
       <c r="Q12" s="144"/>
     </row>
     <row r="13" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="256"/>
+      <c r="A13" s="265"/>
       <c r="B13" s="106" t="s">
         <v>284</v>
       </c>
@@ -46454,7 +46463,7 @@
       <c r="Q13" s="144"/>
     </row>
     <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="256"/>
+      <c r="A14" s="265"/>
       <c r="B14" s="106" t="s">
         <v>288</v>
       </c>
@@ -46481,7 +46490,7 @@
       <c r="Q14" s="144"/>
     </row>
     <row r="15" spans="1:17" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="256"/>
+      <c r="A15" s="265"/>
       <c r="B15" s="106" t="s">
         <v>291</v>
       </c>
@@ -46508,7 +46517,7 @@
       <c r="Q15" s="144"/>
     </row>
     <row r="16" spans="1:17" ht="94.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="256"/>
+      <c r="A16" s="265"/>
       <c r="B16" s="106" t="s">
         <v>294</v>
       </c>
@@ -46535,7 +46544,7 @@
       <c r="Q16" s="144"/>
     </row>
     <row r="17" spans="1:19" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="256"/>
+      <c r="A17" s="265"/>
       <c r="B17" s="106" t="s">
         <v>297</v>
       </c>
@@ -46562,7 +46571,7 @@
       <c r="Q17" s="144"/>
     </row>
     <row r="18" spans="1:19" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="257"/>
+      <c r="A18" s="266"/>
       <c r="B18" s="109" t="s">
         <v>301</v>
       </c>
@@ -46589,16 +46598,16 @@
       <c r="Q18" s="144"/>
     </row>
     <row r="19" spans="1:19" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="244" t="s">
+      <c r="A19" s="243" t="s">
         <v>387</v>
       </c>
-      <c r="B19" s="258"/>
-      <c r="C19" s="258"/>
-      <c r="D19" s="258"/>
-      <c r="E19" s="258"/>
-      <c r="F19" s="258"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="260"/>
+      <c r="B19" s="227"/>
+      <c r="C19" s="227"/>
+      <c r="D19" s="227"/>
+      <c r="E19" s="227"/>
+      <c r="F19" s="227"/>
+      <c r="G19" s="228"/>
+      <c r="H19" s="229"/>
       <c r="I19" s="155"/>
       <c r="J19" s="155"/>
       <c r="K19" s="155"/>
@@ -46612,70 +46621,70 @@
       <c r="S19" s="155"/>
     </row>
     <row r="20" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="245"/>
-      <c r="B20" s="261" t="s">
+      <c r="A20" s="244"/>
+      <c r="B20" s="230" t="s">
         <v>388</v>
       </c>
-      <c r="C20" s="261"/>
-      <c r="D20" s="261" t="s">
+      <c r="C20" s="230"/>
+      <c r="D20" s="230" t="s">
         <v>377</v>
       </c>
-      <c r="E20" s="261"/>
-      <c r="F20" s="261" t="s">
+      <c r="E20" s="230"/>
+      <c r="F20" s="230" t="s">
         <v>555</v>
       </c>
-      <c r="G20" s="262" t="s">
+      <c r="G20" s="231" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="263"/>
+      <c r="H20" s="232"/>
     </row>
     <row r="21" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="245"/>
-      <c r="B21" s="261"/>
-      <c r="C21" s="261" t="s">
+      <c r="A21" s="244"/>
+      <c r="B21" s="230"/>
+      <c r="C21" s="230" t="s">
         <v>389</v>
       </c>
-      <c r="D21" s="261" t="s">
+      <c r="D21" s="230" t="s">
         <v>390</v>
       </c>
-      <c r="E21" s="261"/>
-      <c r="F21" s="261" t="s">
+      <c r="E21" s="230"/>
+      <c r="F21" s="230" t="s">
         <v>574</v>
       </c>
-      <c r="G21" s="262"/>
-      <c r="H21" s="263"/>
+      <c r="G21" s="231"/>
+      <c r="H21" s="232"/>
     </row>
     <row r="22" spans="1:19" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="245"/>
-      <c r="B22" s="261"/>
-      <c r="C22" s="261" t="s">
+      <c r="A22" s="244"/>
+      <c r="B22" s="230"/>
+      <c r="C22" s="230" t="s">
         <v>391</v>
       </c>
-      <c r="D22" s="261" t="s">
+      <c r="D22" s="230" t="s">
         <v>390</v>
       </c>
-      <c r="E22" s="261"/>
-      <c r="F22" s="261" t="s">
+      <c r="E22" s="230"/>
+      <c r="F22" s="230" t="s">
         <v>575</v>
       </c>
-      <c r="G22" s="262"/>
-      <c r="H22" s="263"/>
+      <c r="G22" s="231"/>
+      <c r="H22" s="232"/>
     </row>
     <row r="23" spans="1:19" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="246"/>
-      <c r="B23" s="264"/>
-      <c r="C23" s="264" t="s">
+      <c r="A23" s="245"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233" t="s">
         <v>392</v>
       </c>
-      <c r="D23" s="264" t="s">
+      <c r="D23" s="233" t="s">
         <v>390</v>
       </c>
-      <c r="E23" s="264"/>
-      <c r="F23" s="264" t="s">
+      <c r="E23" s="233"/>
+      <c r="F23" s="233" t="s">
         <v>576</v>
       </c>
-      <c r="G23" s="265"/>
-      <c r="H23" s="266"/>
+      <c r="G23" s="234"/>
+      <c r="H23" s="235"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
@@ -46692,14 +46701,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMJ17"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -46717,16 +46726,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:20" s="152" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -46755,7 +46764,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="251" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="153"/>
@@ -46779,7 +46788,7 @@
       <c r="T3" s="155"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
+      <c r="A4" s="246"/>
       <c r="B4" s="157" t="s">
         <v>8</v>
       </c>
@@ -46797,7 +46806,7 @@
       <c r="H4" s="158"/>
     </row>
     <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
+      <c r="A5" s="246"/>
       <c r="B5" s="157" t="s">
         <v>13</v>
       </c>
@@ -46815,7 +46824,7 @@
       <c r="H5" s="158"/>
     </row>
     <row r="6" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
+      <c r="A6" s="246"/>
       <c r="B6" s="157" t="s">
         <v>16</v>
       </c>
@@ -46833,7 +46842,7 @@
       <c r="H6" s="158"/>
     </row>
     <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="247"/>
       <c r="B7" s="159" t="s">
         <v>19</v>
       </c>
@@ -46851,7 +46860,7 @@
       <c r="H7" s="160"/>
     </row>
     <row r="8" spans="1:20" s="155" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="233" t="s">
+      <c r="A8" s="248" t="s">
         <v>294</v>
       </c>
       <c r="B8" s="161"/>
@@ -46863,7 +46872,7 @@
       <c r="H8" s="162"/>
     </row>
     <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="234"/>
+      <c r="A9" s="249"/>
       <c r="B9" s="163" t="s">
         <v>30</v>
       </c>
@@ -46881,7 +46890,7 @@
       <c r="H9" s="164"/>
     </row>
     <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="234"/>
+      <c r="A10" s="249"/>
       <c r="B10" s="163" t="s">
         <v>376</v>
       </c>
@@ -46897,7 +46906,7 @@
       <c r="H10" s="164"/>
     </row>
     <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="234"/>
+      <c r="A11" s="249"/>
       <c r="B11" s="163"/>
       <c r="C11" s="163" t="s">
         <v>378</v>
@@ -46913,7 +46922,7 @@
       <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="234"/>
+      <c r="A12" s="249"/>
       <c r="B12" s="163"/>
       <c r="C12" s="163" t="s">
         <v>379</v>
@@ -46929,7 +46938,7 @@
       <c r="H12" s="164"/>
     </row>
     <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="234"/>
+      <c r="A13" s="249"/>
       <c r="B13" s="163"/>
       <c r="C13" s="163" t="s">
         <v>380</v>
@@ -46945,7 +46954,7 @@
       <c r="H13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="234"/>
+      <c r="A14" s="249"/>
       <c r="B14" s="163"/>
       <c r="C14" s="163" t="s">
         <v>381</v>
@@ -46961,7 +46970,7 @@
       <c r="H14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="234"/>
+      <c r="A15" s="249"/>
       <c r="B15" s="163"/>
       <c r="C15" s="163" t="s">
         <v>383</v>
@@ -46976,44 +46985,62 @@
       <c r="G15" s="183"/>
       <c r="H15" s="164"/>
     </row>
-    <row r="16" spans="1:20" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="234"/>
-      <c r="B16" s="163" t="s">
-        <v>385</v>
-      </c>
-      <c r="C16" s="163"/>
+    <row r="16" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="249"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="163" t="s">
+        <v>577</v>
+      </c>
       <c r="D16" s="163" t="s">
-        <v>377</v>
-      </c>
-      <c r="E16" s="163"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="163" t="s">
+        <v>579</v>
+      </c>
       <c r="F16" s="163" t="s">
-        <v>506</v>
+        <v>578</v>
       </c>
       <c r="G16" s="183"/>
       <c r="H16" s="164"/>
     </row>
-    <row r="17" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="235"/>
-      <c r="B17" s="165"/>
-      <c r="C17" s="165" t="s">
+    <row r="17" spans="1:8" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="249"/>
+      <c r="B17" s="163" t="s">
+        <v>385</v>
+      </c>
+      <c r="C17" s="163"/>
+      <c r="D17" s="163" t="s">
+        <v>377</v>
+      </c>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163" t="s">
+        <v>506</v>
+      </c>
+      <c r="G17" s="183"/>
+      <c r="H17" s="164"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="250"/>
+      <c r="B18" s="165"/>
+      <c r="C18" s="165" t="s">
         <v>383</v>
       </c>
-      <c r="D17" s="165" t="s">
+      <c r="D18" s="165" t="s">
         <v>318</v>
       </c>
-      <c r="E17" s="165"/>
-      <c r="F17" s="165" t="s">
+      <c r="E18" s="165"/>
+      <c r="F18" s="165" t="s">
         <v>386</v>
       </c>
-      <c r="G17" s="184"/>
-      <c r="H17" s="166"/>
+      <c r="G18" s="184"/>
+      <c r="H18" s="166"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="A8:A18"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -47050,16 +47077,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="236" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -48104,7 +48131,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="251" t="s">
         <v>393</v>
       </c>
       <c r="B3" s="169"/>
@@ -48116,7 +48143,7 @@
       <c r="H3" s="170"/>
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
+      <c r="A4" s="246"/>
       <c r="B4" s="47" t="s">
         <v>206</v>
       </c>
@@ -49148,7 +49175,7 @@
       <c r="AMJ4" s="23"/>
     </row>
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
+      <c r="A5" s="246"/>
       <c r="B5" s="47" t="s">
         <v>259</v>
       </c>
@@ -50180,7 +50207,7 @@
       <c r="AMJ5" s="23"/>
     </row>
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
+      <c r="A6" s="246"/>
       <c r="B6" s="47" t="s">
         <v>212</v>
       </c>
@@ -51212,7 +51239,7 @@
       <c r="AMJ6" s="23"/>
     </row>
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="237"/>
+      <c r="A7" s="246"/>
       <c r="B7" s="47" t="s">
         <v>396</v>
       </c>
@@ -52244,7 +52271,7 @@
       <c r="AMJ7" s="23"/>
     </row>
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="237"/>
+      <c r="A8" s="246"/>
       <c r="B8" s="47" t="s">
         <v>398</v>
       </c>
@@ -53276,7 +53303,7 @@
       <c r="AMJ8" s="23"/>
     </row>
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="237"/>
+      <c r="A9" s="246"/>
       <c r="B9" s="47" t="s">
         <v>400</v>
       </c>
@@ -54308,7 +54335,7 @@
       <c r="AMJ9" s="23"/>
     </row>
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="237"/>
+      <c r="A10" s="246"/>
       <c r="B10" s="47" t="s">
         <v>402</v>
       </c>
@@ -55340,7 +55367,7 @@
       <c r="AMJ10" s="23"/>
     </row>
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="237"/>
+      <c r="A11" s="246"/>
       <c r="B11" s="47" t="s">
         <v>404</v>
       </c>
@@ -56372,7 +56399,7 @@
       <c r="AMJ11" s="23"/>
     </row>
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="238"/>
+      <c r="A12" s="247"/>
       <c r="B12" s="51" t="s">
         <v>406</v>
       </c>
@@ -57404,7 +57431,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="233" t="s">
+      <c r="A13" s="248" t="s">
         <v>408</v>
       </c>
       <c r="B13" s="172"/>
@@ -57417,7 +57444,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="234"/>
+      <c r="A14" s="249"/>
       <c r="B14" s="69" t="s">
         <v>206</v>
       </c>
@@ -57433,7 +57460,7 @@
       <c r="H14" s="174"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="234"/>
+      <c r="A15" s="249"/>
       <c r="B15" s="69" t="s">
         <v>259</v>
       </c>
@@ -57449,7 +57476,7 @@
       <c r="H15" s="174"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="234"/>
+      <c r="A16" s="249"/>
       <c r="B16" s="69" t="s">
         <v>212</v>
       </c>
@@ -57465,7 +57492,7 @@
       <c r="H16" s="174"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="234"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="69" t="s">
         <v>265</v>
       </c>
@@ -57481,7 +57508,7 @@
       <c r="H17" s="174"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="234"/>
+      <c r="A18" s="249"/>
       <c r="B18" s="69" t="s">
         <v>209</v>
       </c>
@@ -57497,7 +57524,7 @@
       <c r="H18" s="174"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="234"/>
+      <c r="A19" s="249"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -57513,7 +57540,7 @@
       <c r="H19" s="174"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="234"/>
+      <c r="A20" s="249"/>
       <c r="B20" s="69" t="s">
         <v>414</v>
       </c>
@@ -57529,7 +57556,7 @@
       <c r="H20" s="174"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="234"/>
+      <c r="A21" s="249"/>
       <c r="B21" s="69" t="s">
         <v>318</v>
       </c>
@@ -57545,7 +57572,7 @@
       <c r="H21" s="174"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="234"/>
+      <c r="A22" s="249"/>
       <c r="B22" s="69" t="s">
         <v>417</v>
       </c>
@@ -57561,7 +57588,7 @@
       <c r="H22" s="174"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="234"/>
+      <c r="A23" s="249"/>
       <c r="B23" s="69" t="s">
         <v>419</v>
       </c>
@@ -57577,7 +57604,7 @@
       <c r="H23" s="174"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="235"/>
+      <c r="A24" s="250"/>
       <c r="B24" s="73" t="s">
         <v>421</v>
       </c>
@@ -57593,7 +57620,7 @@
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="236" t="s">
+      <c r="A25" s="251" t="s">
         <v>353</v>
       </c>
       <c r="B25" s="176"/>
@@ -57605,7 +57632,7 @@
       <c r="H25" s="177"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="237"/>
+      <c r="A26" s="246"/>
       <c r="B26" s="47" t="s">
         <v>206</v>
       </c>
@@ -57621,7 +57648,7 @@
       <c r="H26" s="171"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="237"/>
+      <c r="A27" s="246"/>
       <c r="B27" s="47" t="s">
         <v>259</v>
       </c>
@@ -57637,7 +57664,7 @@
       <c r="H27" s="171"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="237"/>
+      <c r="A28" s="246"/>
       <c r="B28" s="47" t="s">
         <v>212</v>
       </c>
@@ -57653,7 +57680,7 @@
       <c r="H28" s="171"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="237"/>
+      <c r="A29" s="246"/>
       <c r="B29" s="47" t="s">
         <v>265</v>
       </c>
@@ -57669,7 +57696,7 @@
       <c r="H29" s="171"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="237"/>
+      <c r="A30" s="246"/>
       <c r="B30" s="47" t="s">
         <v>426</v>
       </c>
@@ -57685,7 +57712,7 @@
       <c r="H30" s="171"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="237"/>
+      <c r="A31" s="246"/>
       <c r="B31" s="47" t="s">
         <v>209</v>
       </c>
@@ -57701,7 +57728,7 @@
       <c r="H31" s="171"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="237"/>
+      <c r="A32" s="246"/>
       <c r="B32" s="47" t="s">
         <v>404</v>
       </c>
@@ -57717,7 +57744,7 @@
       <c r="H32" s="171"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="237"/>
+      <c r="A33" s="246"/>
       <c r="B33" s="47" t="s">
         <v>430</v>
       </c>
@@ -57733,7 +57760,7 @@
       <c r="H33" s="171"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="237"/>
+      <c r="A34" s="246"/>
       <c r="B34" s="47" t="s">
         <v>5</v>
       </c>
@@ -57749,7 +57776,7 @@
       <c r="H34" s="171"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="237"/>
+      <c r="A35" s="246"/>
       <c r="B35" s="47" t="s">
         <v>433</v>
       </c>
@@ -57765,7 +57792,7 @@
       <c r="H35" s="171"/>
     </row>
     <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="238"/>
+      <c r="A36" s="247"/>
       <c r="B36" s="51" t="s">
         <v>435</v>
       </c>
@@ -57781,7 +57808,7 @@
       <c r="H36" s="178"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="233" t="s">
+      <c r="A37" s="248" t="s">
         <v>281</v>
       </c>
       <c r="B37" s="172"/>
@@ -57794,7 +57821,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="234"/>
+      <c r="A38" s="249"/>
       <c r="B38" s="69" t="s">
         <v>206</v>
       </c>
@@ -57810,7 +57837,7 @@
       <c r="H38" s="174"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="234"/>
+      <c r="A39" s="249"/>
       <c r="B39" s="69" t="s">
         <v>259</v>
       </c>
@@ -57826,7 +57853,7 @@
       <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="234"/>
+      <c r="A40" s="249"/>
       <c r="B40" s="69" t="s">
         <v>212</v>
       </c>
@@ -57842,7 +57869,7 @@
       <c r="H40" s="174"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="234"/>
+      <c r="A41" s="249"/>
       <c r="B41" s="69" t="s">
         <v>265</v>
       </c>
@@ -57858,7 +57885,7 @@
       <c r="H41" s="174"/>
     </row>
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="234"/>
+      <c r="A42" s="249"/>
       <c r="B42" s="69" t="s">
         <v>440</v>
       </c>
@@ -57874,7 +57901,7 @@
       <c r="H42" s="174"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="234"/>
+      <c r="A43" s="249"/>
       <c r="B43" s="69" t="s">
         <v>353</v>
       </c>
@@ -57890,7 +57917,7 @@
       <c r="H43" s="174"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="234"/>
+      <c r="A44" s="249"/>
       <c r="B44" s="69" t="s">
         <v>209</v>
       </c>
@@ -57906,7 +57933,7 @@
       <c r="H44" s="174"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="234"/>
+      <c r="A45" s="249"/>
       <c r="B45" s="69" t="s">
         <v>404</v>
       </c>
@@ -57922,7 +57949,7 @@
       <c r="H45" s="174"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="234"/>
+      <c r="A46" s="249"/>
       <c r="B46" s="69" t="s">
         <v>445</v>
       </c>
@@ -57938,7 +57965,7 @@
       <c r="H46" s="174"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="234"/>
+      <c r="A47" s="249"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -57954,7 +57981,7 @@
       <c r="H47" s="174"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="235"/>
+      <c r="A48" s="250"/>
       <c r="B48" s="73" t="s">
         <v>417</v>
       </c>

</xml_diff>

<commit_message>
feat(dma): replace D Assets with DataAssetsMapping
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83371CD-6847-4305-864F-F9D049C0CBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E35F95-B337-4CD8-9B19-A4590D33A16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,18 @@
     <sheet name="Deployment" sheetId="7" r:id="rId7"/>
     <sheet name="Supporting Metadata" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="574">
   <si>
     <t>Concept</t>
   </si>
@@ -936,13 +947,7 @@
     <t>Identifier of the MA Pair associated to the DMA Tuple</t>
   </si>
   <si>
-    <t>D Assets</t>
-  </si>
-  <si>
     <t>data_123e4567-e89b-12d3</t>
-  </si>
-  <si>
-    <t>Identifiers of the Data Assets associated to the DMA Tuple</t>
   </si>
   <si>
     <t>Deployments</t>
@@ -1222,24 +1227,6 @@
   </si>
   <si>
     <t>accesible IP or FQDN of edge device</t>
-  </si>
-  <si>
-    <t>Data Source Mapping</t>
-  </si>
-  <si>
-    <t>data_source_mapping</t>
-  </si>
-  <si>
-    <t>microserviceA_data</t>
-  </si>
-  <si>
-    <t>List of UUIDs</t>
-  </si>
-  <si>
-    <t>microserviceB_data</t>
-  </si>
-  <si>
-    <t>microserviceC_data</t>
   </si>
   <si>
     <t>Person</t>
@@ -1780,9 +1767,6 @@
     <t xml:space="preserve">database schema description/contents </t>
   </si>
   <si>
-    <t>Mapping the available Data assets in this DMA Tuple to available Microservices. One Microservice may require several Data assets, specified by their UUIDs.</t>
-  </si>
-  <si>
     <t>["/data", "/cfg"]</t>
   </si>
   <si>
@@ -1837,15 +1821,6 @@
     <t>https://github.com/UoW-CPC/ADTGenerator/blob/main/examples/metadata_RISTRA.json#L101</t>
   </si>
   <si>
-    <t>UUIDs of required Data asset(s) for MicroserviceA</t>
-  </si>
-  <si>
-    <t>UUIDs of required Data asset(s) for  MicroserviceB</t>
-  </si>
-  <si>
-    <t>UUIDs of required Data asset(s) for  MicroserviceC</t>
-  </si>
-  <si>
     <t>cloud_config</t>
   </si>
   <si>
@@ -1853,6 +1828,24 @@
   </si>
   <si>
     <t>#cloud-config\nruncmd:\n- [ sh, -xc, \"echo 'hello world!'\" ]</t>
+  </si>
+  <si>
+    <t>DataAssetsMapping</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>{ "microserviceA_ID": "data_123e4567-e89b-12d3", "microserviceB_ID": "data_234e4567-e89b-23d4"}</t>
+  </si>
+  <si>
+    <t>1:1 relationship between a Microservice and a Data asset, specified by their IDs</t>
+  </si>
+  <si>
+    <t>Mapping the available Data assets in this DMA Tuple to available Microservices. Required if Data assets are required. Not all microservices need a Data asset.</t>
+  </si>
+  <si>
+    <t>microserviceA_ID</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3241,40 +3234,52 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3283,14 +3288,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3315,46 +3312,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4234,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
@@ -4256,16 +4213,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>485</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -4294,7 +4251,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="241" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4306,7 +4263,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="241"/>
+      <c r="A4" s="242"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4321,12 +4278,12 @@
         <v>11</v>
       </c>
       <c r="G4" s="180" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="241"/>
+      <c r="A5" s="242"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4346,7 +4303,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
+      <c r="A6" s="242"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4366,13 +4323,13 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="47" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>20</v>
@@ -4381,12 +4338,12 @@
         <v>21</v>
       </c>
       <c r="G7" s="180" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="241"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4406,7 +4363,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="241"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4415,10 +4372,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G9" s="180" t="s">
         <v>12</v>
@@ -4426,7 +4383,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="241"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4446,7 +4403,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="242"/>
+      <c r="A11" s="243"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4466,7 +4423,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="243" t="s">
+      <c r="A12" s="244" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="213"/>
@@ -4478,7 +4435,7 @@
       <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="244"/>
+      <c r="A13" s="245"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4487,7 +4444,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="F13" s="55" t="s">
         <v>37</v>
@@ -4498,19 +4455,19 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="244"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="55" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="G14" s="185" t="s">
         <v>12</v>
@@ -4518,19 +4475,19 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="244"/>
+      <c r="A15" s="245"/>
       <c r="B15" s="55" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="55" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="F15" s="55" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="G15" s="185" t="s">
         <v>43</v>
@@ -5554,22 +5511,22 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="244"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="55"/>
       <c r="C16" s="56" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="F16" s="55" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="G16" s="185" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="4"/>
@@ -6590,22 +6547,22 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="244"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="55"/>
       <c r="C17" s="56" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="D17" s="55" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="F17" s="55" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="G17" s="185" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="4"/>
@@ -7626,19 +7583,19 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="244"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="55"/>
       <c r="C18" s="56" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="F18" s="55" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="G18" s="185" t="s">
         <v>43</v>
@@ -8662,19 +8619,19 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="244"/>
+      <c r="A19" s="245"/>
       <c r="B19" s="55" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="55" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="F19" s="55" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="G19" s="185" t="s">
         <v>43</v>
@@ -9698,19 +9655,19 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="245"/>
+      <c r="A20" s="246"/>
       <c r="B20" s="217" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C20" s="218"/>
       <c r="D20" s="217" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E20" s="219" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="F20" s="217" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="G20" s="220" t="s">
         <v>43</v>
@@ -10734,7 +10691,7 @@
       <c r="AMJ20" s="4"/>
     </row>
     <row r="21" spans="1:1024" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="246" t="s">
+      <c r="A21" s="237" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="59"/>
@@ -10746,7 +10703,7 @@
       <c r="H21" s="61"/>
     </row>
     <row r="22" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="246"/>
+      <c r="A22" s="237"/>
       <c r="B22" s="47" t="s">
         <v>40</v>
       </c>
@@ -10766,7 +10723,7 @@
       <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="246"/>
+      <c r="A23" s="237"/>
       <c r="B23" s="47" t="s">
         <v>44</v>
       </c>
@@ -10786,7 +10743,7 @@
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="246"/>
+      <c r="A24" s="237"/>
       <c r="B24" s="47" t="s">
         <v>46</v>
       </c>
@@ -10806,7 +10763,7 @@
       <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="246"/>
+      <c r="A25" s="237"/>
       <c r="B25" s="47" t="s">
         <v>48</v>
       </c>
@@ -10826,7 +10783,7 @@
       <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="246"/>
+      <c r="A26" s="237"/>
       <c r="B26" s="47" t="s">
         <v>50</v>
       </c>
@@ -10846,7 +10803,7 @@
       <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="246"/>
+      <c r="A27" s="237"/>
       <c r="B27" s="47" t="s">
         <v>53</v>
       </c>
@@ -10866,7 +10823,7 @@
       <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="246"/>
+      <c r="A28" s="237"/>
       <c r="B28" s="47" t="s">
         <v>57</v>
       </c>
@@ -10886,7 +10843,7 @@
       <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="246"/>
+      <c r="A29" s="237"/>
       <c r="B29" s="47" t="s">
         <v>61</v>
       </c>
@@ -10906,7 +10863,7 @@
       <c r="H29" s="50"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="246"/>
+      <c r="A30" s="237"/>
       <c r="B30" s="47" t="s">
         <v>63</v>
       </c>
@@ -10926,7 +10883,7 @@
       <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="246"/>
+      <c r="A31" s="237"/>
       <c r="B31" s="47" t="s">
         <v>65</v>
       </c>
@@ -10946,7 +10903,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="246"/>
+      <c r="A32" s="237"/>
       <c r="B32" s="47" t="s">
         <v>67</v>
       </c>
@@ -10966,7 +10923,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="247"/>
+      <c r="A33" s="238"/>
       <c r="B33" s="51" t="s">
         <v>69</v>
       </c>
@@ -10986,7 +10943,7 @@
       <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="248" t="s">
+      <c r="A34" s="233" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="62"/>
@@ -10998,7 +10955,7 @@
       <c r="H34" s="64"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="249"/>
+      <c r="A35" s="234"/>
       <c r="B35" s="65" t="s">
         <v>73</v>
       </c>
@@ -11018,7 +10975,7 @@
       <c r="H35" s="68"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="249"/>
+      <c r="A36" s="234"/>
       <c r="B36" s="69" t="s">
         <v>76</v>
       </c>
@@ -11038,7 +10995,7 @@
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="249"/>
+      <c r="A37" s="234"/>
       <c r="B37" s="69" t="s">
         <v>79</v>
       </c>
@@ -11058,7 +11015,7 @@
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="250"/>
+      <c r="A38" s="235"/>
       <c r="B38" s="73" t="s">
         <v>82</v>
       </c>
@@ -11078,7 +11035,7 @@
       <c r="H38" s="76"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="251" t="s">
+      <c r="A39" s="236" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="59"/>
@@ -11090,7 +11047,7 @@
       <c r="H39" s="61"/>
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="246"/>
+      <c r="A40" s="237"/>
       <c r="B40" s="47" t="s">
         <v>86</v>
       </c>
@@ -12126,8 +12083,8 @@
       <c r="AMJ40" s="4"/>
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="246"/>
-      <c r="B41" s="238" t="s">
+      <c r="A41" s="237"/>
+      <c r="B41" s="227" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -13164,8 +13121,8 @@
       <c r="AMJ41" s="4"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A42" s="246"/>
-      <c r="B42" s="238"/>
+      <c r="A42" s="237"/>
+      <c r="B42" s="227"/>
       <c r="C42" s="47" t="s">
         <v>94</v>
       </c>
@@ -14200,8 +14157,8 @@
       <c r="AMJ42" s="4"/>
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="246"/>
-      <c r="B43" s="238"/>
+      <c r="A43" s="237"/>
+      <c r="B43" s="227"/>
       <c r="C43" s="47" t="s">
         <v>98</v>
       </c>
@@ -15236,8 +15193,8 @@
       <c r="AMJ43" s="4"/>
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="246"/>
-      <c r="B44" s="238"/>
+      <c r="A44" s="237"/>
+      <c r="B44" s="227"/>
       <c r="C44" s="47" t="s">
         <v>102</v>
       </c>
@@ -16272,8 +16229,8 @@
       <c r="AMJ44" s="4"/>
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="246"/>
-      <c r="B45" s="238"/>
+      <c r="A45" s="237"/>
+      <c r="B45" s="227"/>
       <c r="C45" s="47" t="s">
         <v>106</v>
       </c>
@@ -17308,8 +17265,8 @@
       <c r="AMJ45" s="4"/>
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="246"/>
-      <c r="B46" s="238"/>
+      <c r="A46" s="237"/>
+      <c r="B46" s="227"/>
       <c r="C46" s="47" t="s">
         <v>110</v>
       </c>
@@ -18344,8 +18301,8 @@
       <c r="AMJ46" s="4"/>
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="246"/>
-      <c r="B47" s="238"/>
+      <c r="A47" s="237"/>
+      <c r="B47" s="227"/>
       <c r="C47" s="47" t="s">
         <v>114</v>
       </c>
@@ -19380,8 +19337,8 @@
       <c r="AMJ47" s="4"/>
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="246"/>
-      <c r="B48" s="238"/>
+      <c r="A48" s="237"/>
+      <c r="B48" s="227"/>
       <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
@@ -20416,8 +20373,8 @@
       <c r="AMJ48" s="4"/>
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="246"/>
-      <c r="B49" s="238"/>
+      <c r="A49" s="237"/>
+      <c r="B49" s="227"/>
       <c r="C49" s="47" t="s">
         <v>122</v>
       </c>
@@ -21452,8 +21409,8 @@
       <c r="AMJ49" s="4"/>
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="246"/>
-      <c r="B50" s="238"/>
+      <c r="A50" s="237"/>
+      <c r="B50" s="227"/>
       <c r="C50" s="47" t="s">
         <v>126</v>
       </c>
@@ -22488,8 +22445,8 @@
       <c r="AMJ50" s="4"/>
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="246"/>
-      <c r="B51" s="238"/>
+      <c r="A51" s="237"/>
+      <c r="B51" s="227"/>
       <c r="C51" s="47" t="s">
         <v>130</v>
       </c>
@@ -23524,8 +23481,8 @@
       <c r="AMJ51" s="4"/>
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="247"/>
-      <c r="B52" s="239"/>
+      <c r="A52" s="238"/>
+      <c r="B52" s="228"/>
       <c r="C52" s="51" t="s">
         <v>134</v>
       </c>
@@ -23536,7 +23493,7 @@
         <v>136</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="G52" s="181" t="s">
         <v>43</v>
@@ -24560,7 +24517,7 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="248" t="s">
+      <c r="A53" s="233" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="77"/>
@@ -24572,7 +24529,7 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="249"/>
+      <c r="A54" s="234"/>
       <c r="B54" s="80" t="s">
         <v>138</v>
       </c>
@@ -24592,8 +24549,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="249"/>
-      <c r="B55" s="252" t="s">
+      <c r="A55" s="234"/>
+      <c r="B55" s="229" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="84" t="s">
@@ -24614,8 +24571,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A56" s="249"/>
-      <c r="B56" s="252"/>
+      <c r="A56" s="234"/>
+      <c r="B56" s="229"/>
       <c r="C56" s="80" t="s">
         <v>94</v>
       </c>
@@ -24634,8 +24591,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="249"/>
-      <c r="B57" s="252"/>
+      <c r="A57" s="234"/>
+      <c r="B57" s="229"/>
       <c r="C57" s="80" t="s">
         <v>98</v>
       </c>
@@ -24654,8 +24611,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="249"/>
-      <c r="B58" s="252"/>
+      <c r="A58" s="234"/>
+      <c r="B58" s="229"/>
       <c r="C58" s="80" t="s">
         <v>102</v>
       </c>
@@ -24674,8 +24631,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="249"/>
-      <c r="B59" s="252"/>
+      <c r="A59" s="234"/>
+      <c r="B59" s="229"/>
       <c r="C59" s="80" t="s">
         <v>106</v>
       </c>
@@ -24694,8 +24651,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="249"/>
-      <c r="B60" s="252"/>
+      <c r="A60" s="234"/>
+      <c r="B60" s="229"/>
       <c r="C60" s="80" t="s">
         <v>110</v>
       </c>
@@ -24714,8 +24671,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="249"/>
-      <c r="B61" s="252"/>
+      <c r="A61" s="234"/>
+      <c r="B61" s="229"/>
       <c r="C61" s="80" t="s">
         <v>114</v>
       </c>
@@ -24734,8 +24691,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="249"/>
-      <c r="B62" s="252"/>
+      <c r="A62" s="234"/>
+      <c r="B62" s="229"/>
       <c r="C62" s="80" t="s">
         <v>118</v>
       </c>
@@ -24754,8 +24711,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="249"/>
-      <c r="B63" s="252"/>
+      <c r="A63" s="234"/>
+      <c r="B63" s="229"/>
       <c r="C63" s="80" t="s">
         <v>122</v>
       </c>
@@ -24774,8 +24731,8 @@
       <c r="H63" s="83"/>
     </row>
     <row r="64" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="249"/>
-      <c r="B64" s="252"/>
+      <c r="A64" s="234"/>
+      <c r="B64" s="229"/>
       <c r="C64" s="80" t="s">
         <v>126</v>
       </c>
@@ -24794,8 +24751,8 @@
       <c r="H64" s="83"/>
     </row>
     <row r="65" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="249"/>
-      <c r="B65" s="252"/>
+      <c r="A65" s="234"/>
+      <c r="B65" s="229"/>
       <c r="C65" s="80" t="s">
         <v>130</v>
       </c>
@@ -24814,8 +24771,8 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="250"/>
-      <c r="B66" s="253"/>
+      <c r="A66" s="235"/>
+      <c r="B66" s="230"/>
       <c r="C66" s="85" t="s">
         <v>134</v>
       </c>
@@ -24826,7 +24783,7 @@
         <v>136</v>
       </c>
       <c r="F66" s="85" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="G66" s="184" t="s">
         <v>43</v>
@@ -24834,7 +24791,7 @@
       <c r="H66" s="87"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="251" t="s">
+      <c r="A67" s="236" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="59"/>
@@ -25862,7 +25819,7 @@
       <c r="AMJ67" s="13"/>
     </row>
     <row r="68" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="246"/>
+      <c r="A68" s="237"/>
       <c r="B68" s="89" t="s">
         <v>146</v>
       </c>
@@ -26898,7 +26855,7 @@
       <c r="AMJ68" s="13"/>
     </row>
     <row r="69" spans="1:1024" s="14" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="247"/>
+      <c r="A69" s="238"/>
       <c r="B69" s="93" t="s">
         <v>150</v>
       </c>
@@ -27934,7 +27891,7 @@
       <c r="AMJ69" s="13"/>
     </row>
     <row r="70" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="248" t="s">
+      <c r="A70" s="233" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="29"/>
@@ -27946,7 +27903,7 @@
       <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="249"/>
+      <c r="A71" s="234"/>
       <c r="B71" s="69" t="s">
         <v>155</v>
       </c>
@@ -27964,8 +27921,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="249"/>
-      <c r="B72" s="254" t="s">
+      <c r="A72" s="234"/>
+      <c r="B72" s="231" t="s">
         <v>158</v>
       </c>
       <c r="C72" s="69" t="s">
@@ -27986,8 +27943,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="249"/>
-      <c r="B73" s="254"/>
+      <c r="A73" s="234"/>
+      <c r="B73" s="231"/>
       <c r="C73" s="69" t="s">
         <v>30</v>
       </c>
@@ -28006,8 +27963,8 @@
       <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="249"/>
-      <c r="B74" s="254"/>
+      <c r="A74" s="234"/>
+      <c r="B74" s="231"/>
       <c r="C74" s="69" t="s">
         <v>12</v>
       </c>
@@ -28026,8 +27983,8 @@
       <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="249"/>
-      <c r="B75" s="254"/>
+      <c r="A75" s="234"/>
+      <c r="B75" s="231"/>
       <c r="C75" s="69" t="s">
         <v>167</v>
       </c>
@@ -28046,8 +28003,8 @@
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="250"/>
-      <c r="B76" s="255"/>
+      <c r="A76" s="235"/>
+      <c r="B76" s="232"/>
       <c r="C76" s="73" t="s">
         <v>25</v>
       </c>
@@ -28066,7 +28023,7 @@
       <c r="H76" s="76"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="251" t="s">
+      <c r="A77" s="236" t="s">
         <v>172</v>
       </c>
       <c r="B77" s="31"/>
@@ -29094,7 +29051,7 @@
       <c r="AMJ77" s="13"/>
     </row>
     <row r="78" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="246"/>
+      <c r="A78" s="237"/>
       <c r="B78" s="47" t="s">
         <v>173</v>
       </c>
@@ -30128,8 +30085,8 @@
       <c r="AMJ78" s="13"/>
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="246"/>
-      <c r="B79" s="238" t="s">
+      <c r="A79" s="237"/>
+      <c r="B79" s="227" t="s">
         <v>176</v>
       </c>
       <c r="C79" s="47" t="s">
@@ -31166,8 +31123,8 @@
       <c r="AMJ79" s="13"/>
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="246"/>
-      <c r="B80" s="238"/>
+      <c r="A80" s="237"/>
+      <c r="B80" s="227"/>
       <c r="C80" s="47" t="s">
         <v>179</v>
       </c>
@@ -32202,8 +32159,8 @@
       <c r="AMJ80" s="13"/>
     </row>
     <row r="81" spans="1:1024" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="246"/>
-      <c r="B81" s="238"/>
+      <c r="A81" s="237"/>
+      <c r="B81" s="227"/>
       <c r="C81" s="47" t="s">
         <v>182</v>
       </c>
@@ -33238,8 +33195,8 @@
       <c r="AMJ81" s="13"/>
     </row>
     <row r="82" spans="1:1024" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="246"/>
-      <c r="B82" s="238"/>
+      <c r="A82" s="237"/>
+      <c r="B82" s="227"/>
       <c r="C82" s="47" t="s">
         <v>185</v>
       </c>
@@ -34274,8 +34231,8 @@
       <c r="AMJ82" s="13"/>
     </row>
     <row r="83" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="247"/>
-      <c r="B83" s="239"/>
+      <c r="A83" s="238"/>
+      <c r="B83" s="228"/>
       <c r="C83" s="51" t="s">
         <v>25</v>
       </c>
@@ -35384,6 +35341,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B41:B52"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A33"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A52"/>
     <mergeCell ref="B79:B83"/>
     <mergeCell ref="B55:B66"/>
     <mergeCell ref="B72:B76"/>
@@ -35391,13 +35355,6 @@
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="A70:A76"/>
     <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B41:B52"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A33"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A39:A52"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -35437,16 +35394,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>486</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>478</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -35475,7 +35432,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="241" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -35487,7 +35444,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="241"/>
+      <c r="A4" s="242"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -35502,12 +35459,12 @@
         <v>192</v>
       </c>
       <c r="G4" s="180" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="241"/>
+      <c r="A5" s="242"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -35527,7 +35484,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
+      <c r="A6" s="242"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -35547,7 +35504,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -35567,7 +35524,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="241"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -35587,7 +35544,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="241"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -35607,13 +35564,13 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="241"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="47" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>20</v>
@@ -35622,12 +35579,12 @@
         <v>201</v>
       </c>
       <c r="G10" s="180" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="242"/>
+      <c r="A11" s="243"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -35647,7 +35604,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="247" t="s">
         <v>203</v>
       </c>
       <c r="B12" s="98"/>
@@ -35659,7 +35616,7 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="257"/>
+      <c r="A13" s="248"/>
       <c r="B13" s="103" t="s">
         <v>204</v>
       </c>
@@ -35668,7 +35625,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="104" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="F13" s="103" t="s">
         <v>205</v>
@@ -35679,19 +35636,19 @@
       <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="257"/>
+      <c r="A14" s="248"/>
       <c r="B14" s="103" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="E14" s="104" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="F14" s="103" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="G14" s="183" t="s">
         <v>12</v>
@@ -35737,16 +35694,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>487</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>479</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -35775,7 +35732,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="241" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -35825,7 +35782,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="241"/>
+      <c r="A4" s="242"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -35838,12 +35795,12 @@
         <v>208</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="241"/>
+      <c r="A5" s="242"/>
       <c r="B5" s="105" t="s">
         <v>209</v>
       </c>
@@ -35859,23 +35816,23 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="241"/>
+      <c r="A6" s="242"/>
       <c r="B6" s="105" t="s">
         <v>212</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="G6" s="194"/>
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="241"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="105" t="s">
         <v>213</v>
       </c>
@@ -35885,13 +35842,13 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="G7" s="194"/>
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="241"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="105" t="s">
         <v>214</v>
       </c>
@@ -35907,7 +35864,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="241"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="105" t="s">
         <v>216</v>
       </c>
@@ -35917,7 +35874,7 @@
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="G9" s="194" t="s">
         <v>43</v>
@@ -35925,7 +35882,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="241"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="105" t="s">
         <v>218</v>
       </c>
@@ -35954,7 +35911,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="241"/>
+      <c r="A11" s="242"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -35970,7 +35927,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="241"/>
+      <c r="A12" s="242"/>
       <c r="B12" s="105" t="s">
         <v>222</v>
       </c>
@@ -35980,7 +35937,7 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="G12" s="194" t="s">
         <v>43</v>
@@ -35988,7 +35945,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="241"/>
+      <c r="A13" s="242"/>
       <c r="B13" s="105" t="s">
         <v>224</v>
       </c>
@@ -36006,9 +35963,9 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="241"/>
+      <c r="A14" s="242"/>
       <c r="B14" s="105" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
@@ -36016,7 +35973,7 @@
       </c>
       <c r="E14" s="106"/>
       <c r="F14" s="105" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="G14" s="194" t="s">
         <v>43</v>
@@ -36024,7 +35981,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="242"/>
+      <c r="A15" s="243"/>
       <c r="B15" s="108" t="s">
         <v>228</v>
       </c>
@@ -36040,7 +35997,7 @@
       <c r="H15" s="110"/>
     </row>
     <row r="16" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="248" t="s">
+      <c r="A16" s="233" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="111"/>
@@ -36053,13 +36010,13 @@
       <c r="AMJ16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="113" t="s">
         <v>231</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="113" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E17" s="114"/>
       <c r="F17" s="113" t="s">
@@ -36069,7 +36026,7 @@
       <c r="H17" s="115"/>
     </row>
     <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="249"/>
+      <c r="A18" s="234"/>
       <c r="B18" s="113"/>
       <c r="C18" s="114" t="s">
         <v>1</v>
@@ -36079,13 +36036,13 @@
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G18" s="197"/>
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="249"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>209</v>
@@ -36095,163 +36052,163 @@
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="G19" s="197"/>
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="249"/>
+      <c r="A20" s="234"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="D20" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="G20" s="197"/>
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="249"/>
+      <c r="A21" s="234"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
+        <v>511</v>
+      </c>
+      <c r="D21" s="113" t="s">
         <v>519</v>
-      </c>
-      <c r="D21" s="113" t="s">
-        <v>527</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="G21" s="197"/>
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="249"/>
+      <c r="A22" s="234"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
+        <v>512</v>
+      </c>
+      <c r="D22" s="113" t="s">
         <v>520</v>
-      </c>
-      <c r="D22" s="113" t="s">
-        <v>528</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="G22" s="197"/>
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="249"/>
+      <c r="A23" s="234"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="D23" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="G23" s="197"/>
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="249"/>
+      <c r="A24" s="234"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="G24" s="197"/>
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="249"/>
+      <c r="A25" s="234"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D25" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="G25" s="197"/>
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="249"/>
+      <c r="A26" s="234"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="G26" s="197"/>
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="249"/>
+      <c r="A27" s="234"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="D27" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="G27" s="197"/>
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="249"/>
+      <c r="A28" s="234"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="G28" s="197"/>
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="249"/>
+      <c r="A29" s="234"/>
       <c r="B29" s="113" t="s">
         <v>233</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="113" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
@@ -36261,7 +36218,7 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="249"/>
+      <c r="A30" s="234"/>
       <c r="B30" s="222"/>
       <c r="C30" s="114" t="s">
         <v>1</v>
@@ -36271,13 +36228,13 @@
       </c>
       <c r="E30" s="223"/>
       <c r="F30" s="113" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="G30" s="224"/>
       <c r="H30" s="225"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="249"/>
+      <c r="A31" s="234"/>
       <c r="B31" s="222"/>
       <c r="C31" s="114" t="s">
         <v>209</v>
@@ -36287,157 +36244,157 @@
       </c>
       <c r="E31" s="223"/>
       <c r="F31" s="113" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="G31" s="224"/>
       <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="249"/>
+      <c r="A32" s="234"/>
       <c r="B32" s="222"/>
       <c r="C32" s="114" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="D32" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E32" s="223"/>
       <c r="F32" s="113" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="G32" s="224"/>
       <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="249"/>
+      <c r="A33" s="234"/>
       <c r="B33" s="222"/>
       <c r="C33" s="114" t="s">
+        <v>511</v>
+      </c>
+      <c r="D33" s="113" t="s">
         <v>519</v>
-      </c>
-      <c r="D33" s="113" t="s">
-        <v>527</v>
       </c>
       <c r="E33" s="223"/>
       <c r="F33" s="113" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="G33" s="224"/>
       <c r="H33" s="225"/>
     </row>
     <row r="34" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="249"/>
+      <c r="A34" s="234"/>
       <c r="B34" s="222"/>
       <c r="C34" s="114" t="s">
+        <v>512</v>
+      </c>
+      <c r="D34" s="113" t="s">
         <v>520</v>
-      </c>
-      <c r="D34" s="113" t="s">
-        <v>528</v>
       </c>
       <c r="E34" s="223"/>
       <c r="F34" s="113" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="G34" s="224"/>
       <c r="H34" s="225"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="249"/>
+      <c r="A35" s="234"/>
       <c r="B35" s="222"/>
       <c r="C35" s="114" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="D35" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E35" s="223"/>
       <c r="F35" s="113" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="G35" s="224"/>
       <c r="H35" s="225"/>
     </row>
     <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="249"/>
+      <c r="A36" s="234"/>
       <c r="B36" s="222"/>
       <c r="C36" s="114" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E36" s="223"/>
       <c r="F36" s="113" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="G36" s="224"/>
       <c r="H36" s="225"/>
     </row>
     <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="249"/>
+      <c r="A37" s="234"/>
       <c r="B37" s="222"/>
       <c r="C37" s="114" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D37" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E37" s="223"/>
       <c r="F37" s="113" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="G37" s="224"/>
       <c r="H37" s="225"/>
     </row>
     <row r="38" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="249"/>
+      <c r="A38" s="234"/>
       <c r="B38" s="222"/>
       <c r="C38" s="114" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D38" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E38" s="223"/>
       <c r="F38" s="113" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="G38" s="224"/>
       <c r="H38" s="225"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="249"/>
+      <c r="A39" s="234"/>
       <c r="B39" s="222"/>
       <c r="C39" s="114" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="D39" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E39" s="223"/>
       <c r="F39" s="113" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="G39" s="224"/>
       <c r="H39" s="225"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="249"/>
+      <c r="A40" s="234"/>
       <c r="B40" s="222"/>
       <c r="C40" s="114" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D40" s="113" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E40" s="223"/>
       <c r="F40" s="113" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="G40" s="224"/>
       <c r="H40" s="225"/>
     </row>
     <row r="41" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="250"/>
+      <c r="A41" s="235"/>
       <c r="B41" s="116" t="s">
         <v>235</v>
       </c>
@@ -36447,7 +36404,7 @@
       </c>
       <c r="E41" s="117"/>
       <c r="F41" s="116" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="G41" s="198" t="s">
         <v>43</v>
@@ -36455,7 +36412,7 @@
       <c r="H41" s="118"/>
     </row>
     <row r="42" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="251" t="s">
+      <c r="A42" s="236" t="s">
         <v>236</v>
       </c>
       <c r="B42" s="119"/>
@@ -36505,7 +36462,7 @@
       <c r="AMJ42" s="5"/>
     </row>
     <row r="43" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="247"/>
+      <c r="A43" s="238"/>
       <c r="B43" s="108" t="s">
         <v>237</v>
       </c>
@@ -36542,7 +36499,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="248" t="s">
+      <c r="A44" s="233" t="s">
         <v>72</v>
       </c>
       <c r="B44" s="111"/>
@@ -36555,7 +36512,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="249"/>
+      <c r="A45" s="234"/>
       <c r="B45" s="113" t="s">
         <v>73</v>
       </c>
@@ -36573,7 +36530,7 @@
       <c r="H45" s="115"/>
     </row>
     <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="249"/>
+      <c r="A46" s="234"/>
       <c r="B46" s="113" t="s">
         <v>76</v>
       </c>
@@ -36591,7 +36548,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="250"/>
+      <c r="A47" s="235"/>
       <c r="B47" s="116" t="s">
         <v>79</v>
       </c>
@@ -36609,7 +36566,7 @@
       <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="251" t="s">
+      <c r="A48" s="236" t="s">
         <v>243</v>
       </c>
       <c r="B48" s="121"/>
@@ -36640,7 +36597,7 @@
       <c r="AMJ48" s="5"/>
     </row>
     <row r="49" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="246"/>
+      <c r="A49" s="237"/>
       <c r="B49" s="105" t="s">
         <v>244</v>
       </c>
@@ -36658,7 +36615,7 @@
       <c r="H49" s="107"/>
     </row>
     <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="246"/>
+      <c r="A50" s="237"/>
       <c r="B50" s="105" t="s">
         <v>246</v>
       </c>
@@ -36676,7 +36633,7 @@
       <c r="H50" s="107"/>
     </row>
     <row r="51" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="246"/>
+      <c r="A51" s="237"/>
       <c r="B51" s="105" t="s">
         <v>46</v>
       </c>
@@ -36694,7 +36651,7 @@
       <c r="H51" s="107"/>
     </row>
     <row r="52" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="246"/>
+      <c r="A52" s="237"/>
       <c r="B52" s="105" t="s">
         <v>48</v>
       </c>
@@ -36712,7 +36669,7 @@
       <c r="H52" s="107"/>
     </row>
     <row r="53" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="246"/>
+      <c r="A53" s="237"/>
       <c r="B53" s="105" t="s">
         <v>61</v>
       </c>
@@ -36750,7 +36707,7 @@
       <c r="AMJ53" s="5"/>
     </row>
     <row r="54" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="246"/>
+      <c r="A54" s="237"/>
       <c r="B54" s="105" t="s">
         <v>63</v>
       </c>
@@ -36768,7 +36725,7 @@
       <c r="H54" s="107"/>
     </row>
     <row r="55" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="246"/>
+      <c r="A55" s="237"/>
       <c r="B55" s="105" t="s">
         <v>65</v>
       </c>
@@ -36786,7 +36743,7 @@
       <c r="H55" s="107"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="246"/>
+      <c r="A56" s="237"/>
       <c r="B56" s="105" t="s">
         <v>67</v>
       </c>
@@ -36804,7 +36761,7 @@
       <c r="H56" s="107"/>
     </row>
     <row r="57" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="247"/>
+      <c r="A57" s="238"/>
       <c r="B57" s="108" t="s">
         <v>69</v>
       </c>
@@ -36822,8 +36779,8 @@
       <c r="H57" s="110"/>
     </row>
     <row r="58" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="248" t="s">
-        <v>499</v>
+      <c r="A58" s="233" t="s">
+        <v>491</v>
       </c>
       <c r="B58" s="123"/>
       <c r="C58" s="123"/>
@@ -36835,7 +36792,7 @@
       <c r="AMJ58" s="5"/>
     </row>
     <row r="59" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="250"/>
+      <c r="A59" s="235"/>
       <c r="B59" s="116" t="s">
         <v>5</v>
       </c>
@@ -36897,16 +36854,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>488</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>480</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -37951,8 +37908,8 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="258" t="s">
-        <v>500</v>
+      <c r="A3" s="249" t="s">
+        <v>492</v>
       </c>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
@@ -37976,7 +37933,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="259"/>
+      <c r="A4" s="250"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -37988,17 +37945,17 @@
         <v>207</v>
       </c>
       <c r="F4" s="105" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="126"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="259"/>
+      <c r="A5" s="250"/>
       <c r="B5" s="105" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C5" s="106"/>
       <c r="D5" s="105" t="s">
@@ -38008,17 +37965,17 @@
         <v>207</v>
       </c>
       <c r="F5" s="105" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="259"/>
+      <c r="A6" s="250"/>
       <c r="B6" s="105" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
@@ -38028,35 +37985,35 @@
         <v>207</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G6" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H6" s="126"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="259"/>
+      <c r="A7" s="250"/>
       <c r="B7" s="105" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C7" s="106"/>
       <c r="D7" s="105" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="F7" s="105" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H7" s="126"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="261" t="s">
+      <c r="A8" s="252" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="123"/>
@@ -38069,19 +38026,19 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="263"/>
+      <c r="A9" s="254"/>
       <c r="B9" s="113" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C9" s="114"/>
       <c r="D9" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="F9" s="113" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G9" s="203" t="s">
         <v>12</v>
@@ -39105,19 +39062,19 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="263"/>
+      <c r="A10" s="254"/>
       <c r="B10" s="113" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="G10" s="197" t="s">
         <v>43</v>
@@ -40141,19 +40098,19 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="263"/>
+      <c r="A11" s="254"/>
       <c r="B11" s="113" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C11" s="114"/>
       <c r="D11" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="F11" s="113" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G11" s="197" t="s">
         <v>43</v>
@@ -41177,19 +41134,19 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="263"/>
+      <c r="A12" s="254"/>
       <c r="B12" s="113" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E12" s="117" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="F12" s="116" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G12" s="197" t="s">
         <v>43</v>
@@ -42213,19 +42170,19 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="263"/>
+      <c r="A13" s="254"/>
       <c r="B13" s="113" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C13" s="114"/>
       <c r="D13" s="113" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E13" s="114" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="F13" s="113" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G13" s="197" t="s">
         <v>43</v>
@@ -43249,8 +43206,8 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="258" t="s">
-        <v>501</v>
+      <c r="A14" s="249" t="s">
+        <v>493</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="121"/>
@@ -43270,19 +43227,19 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="260"/>
+      <c r="A15" s="251"/>
       <c r="B15" s="108" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C15" s="109"/>
       <c r="D15" s="108" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E15" s="109" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="F15" s="108" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G15" s="195" t="s">
         <v>43</v>
@@ -44306,8 +44263,8 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="1:1024" s="40" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="261" t="s">
-        <v>323</v>
+      <c r="A16" s="252" t="s">
+        <v>321</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="111"/>
@@ -45334,7 +45291,7 @@
       <c r="AMJ16" s="39"/>
     </row>
     <row r="17" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="263"/>
+      <c r="A17" s="254"/>
       <c r="B17" s="113" t="s">
         <v>94</v>
       </c>
@@ -45343,10 +45300,10 @@
         <v>219</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="F17" s="113" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G17" s="203" t="s">
         <v>12</v>
@@ -45354,7 +45311,7 @@
       <c r="H17" s="129"/>
     </row>
     <row r="18" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="263"/>
+      <c r="A18" s="254"/>
       <c r="B18" s="113" t="s">
         <v>98</v>
       </c>
@@ -45363,10 +45320,10 @@
         <v>219</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="F18" s="113" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G18" s="203" t="s">
         <v>12</v>
@@ -45374,28 +45331,28 @@
       <c r="H18" s="129"/>
     </row>
     <row r="19" spans="1:1024" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="262"/>
+      <c r="A19" s="253"/>
       <c r="B19" s="116" t="s">
         <v>102</v>
       </c>
       <c r="C19" s="117"/>
       <c r="D19" s="116" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E19" s="117" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F19" s="116" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G19" s="198" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H19" s="130"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="258" t="s">
-        <v>328</v>
+      <c r="A20" s="249" t="s">
+        <v>326</v>
       </c>
       <c r="B20" s="121"/>
       <c r="C20" s="121"/>
@@ -45414,7 +45371,7 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="259"/>
+      <c r="A21" s="250"/>
       <c r="B21" s="105" t="s">
         <v>106</v>
       </c>
@@ -45423,59 +45380,59 @@
         <v>210</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="F21" s="105" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G21" s="194" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H21" s="126"/>
     </row>
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="259"/>
+      <c r="A22" s="250"/>
       <c r="B22" s="105" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
         <v>225</v>
       </c>
       <c r="E22" s="106" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="G22" s="194" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="260"/>
+      <c r="A23" s="251"/>
       <c r="B23" s="108" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E23" s="109" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="F23" s="108" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G23" s="195" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H23" s="127"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="261" t="s">
-        <v>502</v>
+      <c r="A24" s="252" t="s">
+        <v>494</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
@@ -45487,26 +45444,26 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="262"/>
+      <c r="A25" s="253"/>
       <c r="B25" s="116" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C25" s="117"/>
       <c r="D25" s="116" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E25" s="117"/>
       <c r="F25" s="116" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G25" s="198" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="H25" s="130"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="258" t="s">
-        <v>337</v>
+      <c r="A26" s="249" t="s">
+        <v>335</v>
       </c>
       <c r="B26" s="121"/>
       <c r="C26" s="121"/>
@@ -45525,7 +45482,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="259"/>
+      <c r="A27" s="250"/>
       <c r="B27" s="105" t="s">
         <v>110</v>
       </c>
@@ -45534,10 +45491,10 @@
         <v>210</v>
       </c>
       <c r="E27" s="106" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G27" s="194" t="s">
         <v>43</v>
@@ -45545,7 +45502,7 @@
       <c r="H27" s="126"/>
     </row>
     <row r="28" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="259"/>
+      <c r="A28" s="250"/>
       <c r="B28" s="105" t="s">
         <v>118</v>
       </c>
@@ -45554,10 +45511,10 @@
         <v>210</v>
       </c>
       <c r="E28" s="106" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G28" s="194" t="s">
         <v>43</v>
@@ -45565,7 +45522,7 @@
       <c r="H28" s="126"/>
     </row>
     <row r="29" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="259"/>
+      <c r="A29" s="250"/>
       <c r="B29" s="105" t="s">
         <v>122</v>
       </c>
@@ -45574,10 +45531,10 @@
         <v>210</v>
       </c>
       <c r="E29" s="106" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="F29" s="105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G29" s="194" t="s">
         <v>43</v>
@@ -45585,7 +45542,7 @@
       <c r="H29" s="126"/>
     </row>
     <row r="30" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="259"/>
+      <c r="A30" s="250"/>
       <c r="B30" s="105" t="s">
         <v>126</v>
       </c>
@@ -45594,10 +45551,10 @@
         <v>210</v>
       </c>
       <c r="E30" s="106" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G30" s="194" t="s">
         <v>43</v>
@@ -45605,7 +45562,7 @@
       <c r="H30" s="126"/>
     </row>
     <row r="31" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="260"/>
+      <c r="A31" s="251"/>
       <c r="B31" s="108" t="s">
         <v>130</v>
       </c>
@@ -45614,10 +45571,10 @@
         <v>210</v>
       </c>
       <c r="E31" s="109" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="F31" s="108" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G31" s="195" t="s">
         <v>43</v>
@@ -45625,8 +45582,8 @@
       <c r="H31" s="127"/>
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="261" t="s">
-        <v>343</v>
+      <c r="A32" s="252" t="s">
+        <v>341</v>
       </c>
       <c r="B32" s="123"/>
       <c r="C32" s="123"/>
@@ -45638,7 +45595,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="263"/>
+      <c r="A33" s="254"/>
       <c r="B33" s="113" t="s">
         <v>134</v>
       </c>
@@ -45647,10 +45604,10 @@
         <v>210</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="F33" s="113" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="G33" s="197" t="s">
         <v>43</v>
@@ -45658,16 +45615,16 @@
       <c r="H33" s="129"/>
     </row>
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="263"/>
+      <c r="A34" s="254"/>
       <c r="B34" s="113" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="C34" s="223"/>
       <c r="D34" s="222" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="F34" s="222"/>
       <c r="G34" s="224" t="s">
@@ -45676,9 +45633,9 @@
       <c r="H34" s="226"/>
     </row>
     <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="262"/>
+      <c r="A35" s="253"/>
       <c r="B35" s="116" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C35" s="117"/>
       <c r="D35" s="116" t="s">
@@ -45686,7 +45643,7 @@
       </c>
       <c r="E35" s="117"/>
       <c r="F35" s="116" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G35" s="198" t="s">
         <v>43</v>
@@ -45745,16 +45702,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>489</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -45783,8 +45740,8 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="251" t="s">
-        <v>503</v>
+      <c r="A3" s="236" t="s">
+        <v>495</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -45810,7 +45767,7 @@
       <c r="AMJ3" s="134"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="237"/>
       <c r="B4" s="106" t="s">
         <v>206</v>
       </c>
@@ -45822,15 +45779,15 @@
         <v>257</v>
       </c>
       <c r="F4" s="136" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="137"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="106" t="s">
         <v>259</v>
       </c>
@@ -45845,12 +45802,12 @@
         <v>262</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H5" s="137"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="106" t="s">
         <v>212</v>
       </c>
@@ -45862,13 +45819,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="136" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G6" s="194"/>
       <c r="H6" s="137"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="106" t="s">
         <v>265</v>
       </c>
@@ -45883,12 +45840,12 @@
         <v>267</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H7" s="137"/>
     </row>
     <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="246"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="106" t="s">
         <v>268</v>
       </c>
@@ -45900,15 +45857,15 @@
         <v>269</v>
       </c>
       <c r="F8" s="136" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G8" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H8" s="137"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="246"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="106" t="s">
         <v>271</v>
       </c>
@@ -45917,18 +45874,18 @@
         <v>207</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F9" s="136" t="s">
         <v>274</v>
       </c>
       <c r="G9" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H9" s="137"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="246"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="106" t="s">
         <v>209</v>
       </c>
@@ -45937,16 +45894,16 @@
         <v>275</v>
       </c>
       <c r="E10" s="106" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F10" s="136" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G10" s="194"/>
       <c r="H10" s="137"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="106" t="s">
         <v>278</v>
       </c>
@@ -45958,37 +45915,37 @@
         <v>279</v>
       </c>
       <c r="F11" s="136" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G11" s="194"/>
       <c r="H11" s="137"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="246"/>
+      <c r="A12" s="237"/>
       <c r="B12" s="106" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E12" s="106" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F12" s="136" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G12" s="194"/>
       <c r="H12" s="137"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="246"/>
+      <c r="A13" s="237"/>
       <c r="B13" s="106" t="s">
         <v>284</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="136" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E13" s="106" t="s">
         <v>286</v>
@@ -46000,63 +45957,63 @@
       <c r="H13" s="137"/>
     </row>
     <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="246"/>
+      <c r="A14" s="237"/>
       <c r="B14" s="106" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E14" s="136" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F14" s="136" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G14" s="194"/>
       <c r="H14" s="137"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="246"/>
+      <c r="A15" s="237"/>
       <c r="B15" s="106" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E15" s="136" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F15" s="136" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G15" s="194"/>
       <c r="H15" s="137"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="246"/>
+      <c r="A16" s="237"/>
       <c r="B16" s="106" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="136" t="s">
+        <v>362</v>
+      </c>
+      <c r="E16" s="136" t="s">
+        <v>363</v>
+      </c>
+      <c r="F16" s="136" t="s">
         <v>364</v>
-      </c>
-      <c r="E16" s="136" t="s">
-        <v>365</v>
-      </c>
-      <c r="F16" s="136" t="s">
-        <v>366</v>
       </c>
       <c r="G16" s="194"/>
       <c r="H16" s="137"/>
     </row>
     <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="246"/>
+      <c r="A17" s="237"/>
       <c r="B17" s="106" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
@@ -46066,25 +46023,25 @@
         <v>12</v>
       </c>
       <c r="F17" s="136" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G17" s="194"/>
       <c r="H17" s="137"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="247"/>
+      <c r="A18" s="238"/>
       <c r="B18" s="109" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="109"/>
       <c r="D18" s="109" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="109" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F18" s="138" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G18" s="195"/>
       <c r="H18" s="139"/>
@@ -46109,14 +46066,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BJ23"/>
+  <dimension ref="A1:BJ19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A18"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -46133,16 +46090,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>490</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -46171,8 +46128,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="264" t="s">
-        <v>503</v>
+      <c r="A3" s="255" t="s">
+        <v>495</v>
       </c>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
@@ -46183,7 +46140,7 @@
       <c r="H3" s="143"/>
     </row>
     <row r="4" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="265"/>
+      <c r="A4" s="256"/>
       <c r="B4" s="106" t="s">
         <v>206</v>
       </c>
@@ -46198,7 +46155,7 @@
         <v>258</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="145"/>
       <c r="I4" s="144"/>
@@ -46212,7 +46169,7 @@
       <c r="Q4" s="144"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="265"/>
+      <c r="A5" s="256"/>
       <c r="B5" s="106" t="s">
         <v>259</v>
       </c>
@@ -46227,7 +46184,7 @@
         <v>262</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H5" s="145"/>
       <c r="I5" s="144"/>
@@ -46241,7 +46198,7 @@
       <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="265"/>
+      <c r="A6" s="256"/>
       <c r="B6" s="106" t="s">
         <v>212</v>
       </c>
@@ -46268,7 +46225,7 @@
       <c r="Q6" s="144"/>
     </row>
     <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="265"/>
+      <c r="A7" s="256"/>
       <c r="B7" s="106" t="s">
         <v>265</v>
       </c>
@@ -46283,7 +46240,7 @@
         <v>267</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="144"/>
@@ -46297,7 +46254,7 @@
       <c r="Q7" s="144"/>
     </row>
     <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="265"/>
+      <c r="A8" s="256"/>
       <c r="B8" s="106" t="s">
         <v>268</v>
       </c>
@@ -46312,7 +46269,7 @@
         <v>270</v>
       </c>
       <c r="G8" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H8" s="145"/>
       <c r="I8" s="144"/>
@@ -46326,7 +46283,7 @@
       <c r="Q8" s="144"/>
     </row>
     <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="265"/>
+      <c r="A9" s="256"/>
       <c r="B9" s="106" t="s">
         <v>271</v>
       </c>
@@ -46341,7 +46298,7 @@
         <v>274</v>
       </c>
       <c r="G9" s="194" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H9" s="149"/>
       <c r="I9" s="144"/>
@@ -46355,7 +46312,7 @@
       <c r="Q9" s="144"/>
     </row>
     <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="265"/>
+      <c r="A10" s="256"/>
       <c r="B10" s="106" t="s">
         <v>209</v>
       </c>
@@ -46382,7 +46339,7 @@
       <c r="Q10" s="144"/>
     </row>
     <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="265"/>
+      <c r="A11" s="256"/>
       <c r="B11" s="106" t="s">
         <v>278</v>
       </c>
@@ -46409,7 +46366,7 @@
       <c r="Q11" s="144"/>
     </row>
     <row r="12" spans="1:17" s="151" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="265"/>
+      <c r="A12" s="256"/>
       <c r="B12" s="106" t="s">
         <v>281</v>
       </c>
@@ -46436,7 +46393,7 @@
       <c r="Q12" s="144"/>
     </row>
     <row r="13" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="265"/>
+      <c r="A13" s="256"/>
       <c r="B13" s="106" t="s">
         <v>284</v>
       </c>
@@ -46463,7 +46420,7 @@
       <c r="Q13" s="144"/>
     </row>
     <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="265"/>
+      <c r="A14" s="256"/>
       <c r="B14" s="106" t="s">
         <v>288</v>
       </c>
@@ -46489,20 +46446,20 @@
       <c r="P14" s="144"/>
       <c r="Q14" s="144"/>
     </row>
-    <row r="15" spans="1:17" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="265"/>
+    <row r="15" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="256"/>
       <c r="B15" s="106" t="s">
-        <v>291</v>
+        <v>568</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
-        <v>272</v>
+        <v>569</v>
       </c>
       <c r="E15" s="136" t="s">
-        <v>292</v>
+        <v>570</v>
       </c>
       <c r="F15" s="106" t="s">
-        <v>293</v>
+        <v>572</v>
       </c>
       <c r="G15" s="194"/>
       <c r="H15" s="145"/>
@@ -46516,20 +46473,18 @@
       <c r="P15" s="144"/>
       <c r="Q15" s="144"/>
     </row>
-    <row r="16" spans="1:17" ht="94.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="265"/>
-      <c r="B16" s="106" t="s">
-        <v>294</v>
-      </c>
-      <c r="C16" s="106"/>
-      <c r="D16" s="105" t="s">
-        <v>453</v>
-      </c>
+    <row r="16" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="256"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="106" t="s">
+        <v>573</v>
+      </c>
+      <c r="D16" s="105"/>
       <c r="E16" s="136" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F16" s="106" t="s">
-        <v>296</v>
+        <v>571</v>
       </c>
       <c r="G16" s="194"/>
       <c r="H16" s="145"/>
@@ -46543,50 +46498,50 @@
       <c r="P16" s="144"/>
       <c r="Q16" s="144"/>
     </row>
-    <row r="17" spans="1:19" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="265"/>
+    <row r="17" spans="1:17" ht="94.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="256"/>
       <c r="B17" s="106" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C17" s="106"/>
-      <c r="D17" s="106" t="s">
-        <v>298</v>
-      </c>
-      <c r="E17" s="106" t="s">
-        <v>299</v>
+      <c r="D17" s="105" t="s">
+        <v>445</v>
+      </c>
+      <c r="E17" s="136" t="s">
+        <v>293</v>
       </c>
       <c r="F17" s="106" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G17" s="194"/>
-      <c r="H17" s="137"/>
+      <c r="H17" s="145"/>
       <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
+      <c r="J17" s="146"/>
+      <c r="K17" s="147"/>
       <c r="L17" s="144"/>
       <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-      <c r="O17" s="144"/>
+      <c r="N17" s="146"/>
+      <c r="O17" s="147"/>
       <c r="P17" s="144"/>
       <c r="Q17" s="144"/>
     </row>
-    <row r="18" spans="1:19" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="266"/>
-      <c r="B18" s="109" t="s">
-        <v>301</v>
-      </c>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="109" t="s">
-        <v>302</v>
-      </c>
-      <c r="F18" s="109" t="s">
-        <v>303</v>
-      </c>
-      <c r="G18" s="195"/>
-      <c r="H18" s="139"/>
+    <row r="18" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="256"/>
+      <c r="B18" s="106" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="F18" s="106" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="194"/>
+      <c r="H18" s="137"/>
       <c r="I18" s="144"/>
       <c r="J18" s="144"/>
       <c r="K18" s="144"/>
@@ -46597,101 +46552,38 @@
       <c r="P18" s="144"/>
       <c r="Q18" s="144"/>
     </row>
-    <row r="19" spans="1:19" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="243" t="s">
-        <v>387</v>
-      </c>
-      <c r="B19" s="227"/>
-      <c r="C19" s="227"/>
-      <c r="D19" s="227"/>
-      <c r="E19" s="227"/>
-      <c r="F19" s="227"/>
-      <c r="G19" s="228"/>
-      <c r="H19" s="229"/>
-      <c r="I19" s="155"/>
-      <c r="J19" s="155"/>
-      <c r="K19" s="155"/>
-      <c r="L19" s="155"/>
-      <c r="M19" s="155"/>
-      <c r="N19" s="155"/>
-      <c r="O19" s="155"/>
-      <c r="P19" s="155"/>
-      <c r="Q19" s="155"/>
-      <c r="R19" s="155"/>
-      <c r="S19" s="155"/>
-    </row>
-    <row r="20" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="244"/>
-      <c r="B20" s="230" t="s">
-        <v>388</v>
-      </c>
-      <c r="C20" s="230"/>
-      <c r="D20" s="230" t="s">
-        <v>377</v>
-      </c>
-      <c r="E20" s="230"/>
-      <c r="F20" s="230" t="s">
-        <v>555</v>
-      </c>
-      <c r="G20" s="231" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="232"/>
-    </row>
-    <row r="21" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="244"/>
-      <c r="B21" s="230"/>
-      <c r="C21" s="230" t="s">
-        <v>389</v>
-      </c>
-      <c r="D21" s="230" t="s">
-        <v>390</v>
-      </c>
-      <c r="E21" s="230"/>
-      <c r="F21" s="230" t="s">
-        <v>574</v>
-      </c>
-      <c r="G21" s="231"/>
-      <c r="H21" s="232"/>
-    </row>
-    <row r="22" spans="1:19" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="244"/>
-      <c r="B22" s="230"/>
-      <c r="C22" s="230" t="s">
-        <v>391</v>
-      </c>
-      <c r="D22" s="230" t="s">
-        <v>390</v>
-      </c>
-      <c r="E22" s="230"/>
-      <c r="F22" s="230" t="s">
-        <v>575</v>
-      </c>
-      <c r="G22" s="231"/>
-      <c r="H22" s="232"/>
-    </row>
-    <row r="23" spans="1:19" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="245"/>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233" t="s">
-        <v>392</v>
-      </c>
-      <c r="D23" s="233" t="s">
-        <v>390</v>
-      </c>
-      <c r="E23" s="233"/>
-      <c r="F23" s="233" t="s">
-        <v>576</v>
-      </c>
-      <c r="G23" s="234"/>
-      <c r="H23" s="235"/>
+    <row r="19" spans="1:17" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="257"/>
+      <c r="B19" s="109" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="109" t="s">
+        <v>300</v>
+      </c>
+      <c r="F19" s="109" t="s">
+        <v>301</v>
+      </c>
+      <c r="G19" s="195"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="144"/>
+      <c r="K19" s="144"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="144"/>
+      <c r="N19" s="144"/>
+      <c r="O19" s="144"/>
+      <c r="P19" s="144"/>
+      <c r="Q19" s="144"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:A18"/>
-    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A3:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -46726,16 +46618,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>491</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:20" s="152" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -46764,7 +46656,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="156" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="251" t="s">
+      <c r="A3" s="236" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="153"/>
@@ -46788,7 +46680,7 @@
       <c r="T3" s="155"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="237"/>
       <c r="B4" s="157" t="s">
         <v>8</v>
       </c>
@@ -46798,15 +46690,15 @@
       </c>
       <c r="E4" s="157"/>
       <c r="F4" s="157" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G4" s="180" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H4" s="158"/>
     </row>
     <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="157" t="s">
         <v>13</v>
       </c>
@@ -46816,7 +46708,7 @@
       </c>
       <c r="E5" s="157"/>
       <c r="F5" s="157" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G5" s="180" t="s">
         <v>12</v>
@@ -46824,7 +46716,7 @@
       <c r="H5" s="158"/>
     </row>
     <row r="6" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="157" t="s">
         <v>16</v>
       </c>
@@ -46834,7 +46726,7 @@
       </c>
       <c r="E6" s="157"/>
       <c r="F6" s="157" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G6" s="180" t="s">
         <v>12</v>
@@ -46842,26 +46734,26 @@
       <c r="H6" s="158"/>
     </row>
     <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="247"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="159" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="159"/>
       <c r="D7" s="159" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E7" s="159"/>
       <c r="F7" s="159" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G7" s="181" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="H7" s="160"/>
     </row>
     <row r="8" spans="1:20" s="155" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="248" t="s">
-        <v>294</v>
+      <c r="A8" s="233" t="s">
+        <v>292</v>
       </c>
       <c r="B8" s="161"/>
       <c r="C8" s="161"/>
@@ -46872,17 +46764,17 @@
       <c r="H8" s="162"/>
     </row>
     <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="249"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="163" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="163"/>
       <c r="D9" s="163" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="163" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G9" s="211" t="s">
         <v>12</v>
@@ -46890,147 +46782,147 @@
       <c r="H9" s="164"/>
     </row>
     <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="249"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="163" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C10" s="163"/>
       <c r="D10" s="163" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E10" s="163"/>
       <c r="F10" s="163" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="G10" s="183"/>
       <c r="H10" s="164"/>
     </row>
     <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="249"/>
+      <c r="A11" s="234"/>
       <c r="B11" s="163"/>
       <c r="C11" s="163" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D11" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E11" s="163"/>
       <c r="F11" s="163" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="G11" s="183"/>
       <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="249"/>
+      <c r="A12" s="234"/>
       <c r="B12" s="163"/>
       <c r="C12" s="163" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D12" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E12" s="163"/>
       <c r="F12" s="163" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="G12" s="183"/>
       <c r="H12" s="164"/>
     </row>
     <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="249"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="163"/>
       <c r="C13" s="163" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D13" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E13" s="163"/>
       <c r="F13" s="163" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="G13" s="183"/>
       <c r="H13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="249"/>
+      <c r="A14" s="234"/>
       <c r="B14" s="163"/>
       <c r="C14" s="163" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D14" s="163" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E14" s="163"/>
       <c r="F14" s="163" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G14" s="183"/>
       <c r="H14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="249"/>
+      <c r="A15" s="234"/>
       <c r="B15" s="163"/>
       <c r="C15" s="163" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D15" s="163" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E15" s="163"/>
       <c r="F15" s="163" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G15" s="183"/>
       <c r="H15" s="164"/>
     </row>
     <row r="16" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="249"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="163"/>
       <c r="C16" s="163" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="D16" s="163" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="163" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="F16" s="163" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="G16" s="183"/>
       <c r="H16" s="164"/>
     </row>
     <row r="17" spans="1:8" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="163" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C17" s="163"/>
       <c r="D17" s="163" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E17" s="163"/>
       <c r="F17" s="163" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="G17" s="183"/>
       <c r="H17" s="164"/>
     </row>
     <row r="18" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="250"/>
+      <c r="A18" s="235"/>
       <c r="B18" s="165"/>
       <c r="C18" s="165" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D18" s="165" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E18" s="165"/>
       <c r="F18" s="165" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G18" s="184"/>
       <c r="H18" s="166"/>
@@ -47077,16 +46969,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
-        <v>492</v>
-      </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="237"/>
+      <c r="A1" s="239" t="s">
+        <v>484</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -48131,8 +48023,8 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="251" t="s">
-        <v>393</v>
+      <c r="A3" s="236" t="s">
+        <v>385</v>
       </c>
       <c r="B3" s="169"/>
       <c r="C3" s="169"/>
@@ -48143,7 +48035,7 @@
       <c r="H3" s="170"/>
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="246"/>
+      <c r="A4" s="237"/>
       <c r="B4" s="47" t="s">
         <v>206</v>
       </c>
@@ -48153,7 +48045,7 @@
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="157" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="158"/>
@@ -49175,7 +49067,7 @@
       <c r="AMJ4" s="23"/>
     </row>
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="246"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="47" t="s">
         <v>259</v>
       </c>
@@ -50207,7 +50099,7 @@
       <c r="AMJ5" s="23"/>
     </row>
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="246"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="47" t="s">
         <v>212</v>
       </c>
@@ -50217,7 +50109,7 @@
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="157" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="171"/>
@@ -51239,9 +51131,9 @@
       <c r="AMJ6" s="23"/>
     </row>
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="246"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="47" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C7" s="157"/>
       <c r="D7" s="47" t="s">
@@ -51249,7 +51141,7 @@
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="157" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="158"/>
@@ -52271,9 +52163,9 @@
       <c r="AMJ7" s="23"/>
     </row>
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="246"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="47" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C8" s="157"/>
       <c r="D8" s="47" t="s">
@@ -52281,7 +52173,7 @@
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="157" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="158"/>
@@ -53303,17 +53195,17 @@
       <c r="AMJ8" s="23"/>
     </row>
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="246"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="47" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C9" s="157"/>
       <c r="D9" s="47" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="157" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="G9" s="47"/>
       <c r="H9" s="158"/>
@@ -54335,9 +54227,9 @@
       <c r="AMJ9" s="23"/>
     </row>
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="246"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="47" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C10" s="157"/>
       <c r="D10" s="47" t="s">
@@ -54345,7 +54237,7 @@
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="157" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="158"/>
@@ -55367,17 +55259,17 @@
       <c r="AMJ10" s="23"/>
     </row>
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="47" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C11" s="157"/>
       <c r="D11" s="47" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="157" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="158"/>
@@ -56399,9 +56291,9 @@
       <c r="AMJ11" s="23"/>
     </row>
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="247"/>
+      <c r="A12" s="238"/>
       <c r="B12" s="51" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C12" s="159"/>
       <c r="D12" s="51" t="s">
@@ -56409,7 +56301,7 @@
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="159" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="G12" s="51"/>
       <c r="H12" s="160"/>
@@ -57431,8 +57323,8 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="248" t="s">
-        <v>408</v>
+      <c r="A13" s="233" t="s">
+        <v>400</v>
       </c>
       <c r="B13" s="172"/>
       <c r="C13" s="172"/>
@@ -57444,7 +57336,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="249"/>
+      <c r="A14" s="234"/>
       <c r="B14" s="69" t="s">
         <v>206</v>
       </c>
@@ -57454,13 +57346,13 @@
       </c>
       <c r="E14" s="69"/>
       <c r="F14" s="69" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="G14" s="69"/>
       <c r="H14" s="174"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="249"/>
+      <c r="A15" s="234"/>
       <c r="B15" s="69" t="s">
         <v>259</v>
       </c>
@@ -57476,7 +57368,7 @@
       <c r="H15" s="174"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="249"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="69" t="s">
         <v>212</v>
       </c>
@@ -57486,13 +57378,13 @@
       </c>
       <c r="E16" s="69"/>
       <c r="F16" s="69" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="G16" s="69"/>
       <c r="H16" s="174"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="249"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="69" t="s">
         <v>265</v>
       </c>
@@ -57502,13 +57394,13 @@
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="69" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="174"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="249"/>
+      <c r="A18" s="234"/>
       <c r="B18" s="69" t="s">
         <v>209</v>
       </c>
@@ -57518,13 +57410,13 @@
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="69" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="G18" s="69"/>
       <c r="H18" s="174"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="249"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -57534,47 +57426,47 @@
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="69" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="G19" s="69"/>
       <c r="H19" s="174"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="249"/>
+      <c r="A20" s="234"/>
       <c r="B20" s="69" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="69" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="G20" s="69"/>
       <c r="H20" s="174"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="249"/>
+      <c r="A21" s="234"/>
       <c r="B21" s="69" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C21" s="69"/>
       <c r="D21" s="69" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="69" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="G21" s="69"/>
       <c r="H21" s="174"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="249"/>
+      <c r="A22" s="234"/>
       <c r="B22" s="69" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C22" s="69"/>
       <c r="D22" s="69" t="s">
@@ -57582,15 +57474,15 @@
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="69" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="G22" s="69"/>
       <c r="H22" s="174"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="249"/>
+      <c r="A23" s="234"/>
       <c r="B23" s="69" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69" t="s">
@@ -57598,15 +57490,15 @@
       </c>
       <c r="E23" s="69"/>
       <c r="F23" s="69" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="G23" s="69"/>
       <c r="H23" s="174"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="250"/>
+      <c r="A24" s="235"/>
       <c r="B24" s="73" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73" t="s">
@@ -57614,14 +57506,14 @@
       </c>
       <c r="E24" s="73"/>
       <c r="F24" s="73" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="G24" s="73"/>
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="251" t="s">
-        <v>353</v>
+      <c r="A25" s="236" t="s">
+        <v>351</v>
       </c>
       <c r="B25" s="176"/>
       <c r="C25" s="176"/>
@@ -57632,7 +57524,7 @@
       <c r="H25" s="177"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="246"/>
+      <c r="A26" s="237"/>
       <c r="B26" s="47" t="s">
         <v>206</v>
       </c>
@@ -57642,13 +57534,13 @@
       </c>
       <c r="E26" s="47"/>
       <c r="F26" s="47" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="171"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="246"/>
+      <c r="A27" s="237"/>
       <c r="B27" s="47" t="s">
         <v>259</v>
       </c>
@@ -57664,7 +57556,7 @@
       <c r="H27" s="171"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="246"/>
+      <c r="A28" s="237"/>
       <c r="B28" s="47" t="s">
         <v>212</v>
       </c>
@@ -57674,13 +57566,13 @@
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="47" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="171"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="246"/>
+      <c r="A29" s="237"/>
       <c r="B29" s="47" t="s">
         <v>265</v>
       </c>
@@ -57690,15 +57582,15 @@
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="47" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="171"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="246"/>
+      <c r="A30" s="237"/>
       <c r="B30" s="47" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47" t="s">
@@ -57706,13 +57598,13 @@
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="47" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="171"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="246"/>
+      <c r="A31" s="237"/>
       <c r="B31" s="47" t="s">
         <v>209</v>
       </c>
@@ -57722,31 +57614,31 @@
       </c>
       <c r="E31" s="47"/>
       <c r="F31" s="47" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="171"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="246"/>
+      <c r="A32" s="237"/>
       <c r="B32" s="47" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="47" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E32" s="47"/>
       <c r="F32" s="47" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="171"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="246"/>
+      <c r="A33" s="237"/>
       <c r="B33" s="47" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="47" t="s">
@@ -57754,13 +57646,13 @@
       </c>
       <c r="E33" s="47"/>
       <c r="F33" s="47" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="171"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="246"/>
+      <c r="A34" s="237"/>
       <c r="B34" s="47" t="s">
         <v>5</v>
       </c>
@@ -57770,15 +57662,15 @@
       </c>
       <c r="E34" s="47"/>
       <c r="F34" s="47" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="171"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="246"/>
+      <c r="A35" s="237"/>
       <c r="B35" s="47" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47" t="s">
@@ -57786,15 +57678,15 @@
       </c>
       <c r="E35" s="47"/>
       <c r="F35" s="47" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="171"/>
     </row>
     <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="247"/>
+      <c r="A36" s="238"/>
       <c r="B36" s="51" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="51" t="s">
@@ -57802,13 +57694,13 @@
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="G36" s="51"/>
       <c r="H36" s="178"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="248" t="s">
+      <c r="A37" s="233" t="s">
         <v>281</v>
       </c>
       <c r="B37" s="172"/>
@@ -57821,7 +57713,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="249"/>
+      <c r="A38" s="234"/>
       <c r="B38" s="69" t="s">
         <v>206</v>
       </c>
@@ -57831,13 +57723,13 @@
       </c>
       <c r="E38" s="69"/>
       <c r="F38" s="69" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="174"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="249"/>
+      <c r="A39" s="234"/>
       <c r="B39" s="69" t="s">
         <v>259</v>
       </c>
@@ -57853,7 +57745,7 @@
       <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="249"/>
+      <c r="A40" s="234"/>
       <c r="B40" s="69" t="s">
         <v>212</v>
       </c>
@@ -57863,13 +57755,13 @@
       </c>
       <c r="E40" s="69"/>
       <c r="F40" s="69" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="G40" s="69"/>
       <c r="H40" s="174"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="249"/>
+      <c r="A41" s="234"/>
       <c r="B41" s="69" t="s">
         <v>265</v>
       </c>
@@ -57879,15 +57771,15 @@
       </c>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="G41" s="69"/>
       <c r="H41" s="174"/>
     </row>
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="249"/>
+      <c r="A42" s="234"/>
       <c r="B42" s="69" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="69" t="s">
@@ -57895,15 +57787,15 @@
       </c>
       <c r="E42" s="69"/>
       <c r="F42" s="69" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G42" s="69"/>
       <c r="H42" s="174"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="249"/>
+      <c r="A43" s="234"/>
       <c r="B43" s="69" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C43" s="69"/>
       <c r="D43" s="69" t="s">
@@ -57911,13 +57803,13 @@
       </c>
       <c r="E43" s="69"/>
       <c r="F43" s="69" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="G43" s="69"/>
       <c r="H43" s="174"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="249"/>
+      <c r="A44" s="234"/>
       <c r="B44" s="69" t="s">
         <v>209</v>
       </c>
@@ -57927,31 +57819,31 @@
       </c>
       <c r="E44" s="69"/>
       <c r="F44" s="69" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="174"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="249"/>
+      <c r="A45" s="234"/>
       <c r="B45" s="69" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C45" s="69"/>
       <c r="D45" s="69" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E45" s="69"/>
       <c r="F45" s="69" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="G45" s="69"/>
       <c r="H45" s="174"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="249"/>
+      <c r="A46" s="234"/>
       <c r="B46" s="69" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="69" t="s">
@@ -57959,13 +57851,13 @@
       </c>
       <c r="E46" s="69"/>
       <c r="F46" s="69" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="G46" s="69"/>
       <c r="H46" s="174"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="249"/>
+      <c r="A47" s="234"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -57975,15 +57867,15 @@
       </c>
       <c r="E47" s="69"/>
       <c r="F47" s="69" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="G47" s="69"/>
       <c r="H47" s="174"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="250"/>
+      <c r="A48" s="235"/>
       <c r="B48" s="73" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="73" t="s">
@@ -57991,7 +57883,7 @@
       </c>
       <c r="E48" s="73"/>
       <c r="F48" s="73" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="G48" s="73"/>
       <c r="H48" s="175"/>

</xml_diff>

<commit_message>
Rename DATA_SOURCE_TYPE to DATA_STORE_TYPE (a store is not always a source, so was not general enough). Correct word 'protocol' to 'scheme' where it was not appropriate. This change affects fields in Micorservice metadata with the same previous name, to keep them in sync.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/digitbrain.github.io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahajnal/Documents/github/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AFA45-BD30-D54B-AB13-E6746A6042C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEFE86F-304F-0E47-97C5-313017B331B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="583">
   <si>
     <t>Concept</t>
   </si>
@@ -1038,9 +1038,6 @@
     <t>Data access specification</t>
   </si>
   <si>
-    <t>The exact type of the data resource. Typically corresponds to the scheme part (protocol://) of DATA_URI.</t>
-  </si>
-  <si>
     <t>mandatory (WP6)</t>
   </si>
   <si>
@@ -1063,9 +1060,6 @@
   </si>
   <si>
     <t>Further access clauses (extensible)</t>
-  </si>
-  <si>
-    <t>Protocol to use in communication with the data source, only if DATA_TYPE does not imply it (e.g. S3 over HTTP). Moved from to Data access specification.</t>
   </si>
   <si>
     <t>Protocol dialect to be used in communication with the database</t>
@@ -1726,9 +1720,6 @@
     <t>DATA_URI</t>
   </si>
   <si>
-    <t>Accessibility of the data resource, including host, port information, protocol, and other fields (path is protocol dependent, can be a topic name). GUI may show host, port, path separately. Hidden at search. Format: protocol://host:port/path.  Pseudo vars: DATA_PROTOCOL, DATA_HOST, DATA_PORT, DATA_PATH, DATA_QUERY, DATA_FRAGMENT.</t>
-  </si>
-  <si>
     <t>DATA_SCHEMA_URL</t>
   </si>
   <si>
@@ -1871,6 +1862,18 @@
   </si>
   <si>
     <t xml:space="preserve">*DATA_SOURCE_ID* </t>
+  </si>
+  <si>
+    <t>Protocol to use in communication with the data source, only if DATA_TYPE does not imply it (e.g. S3 over HTTP). Moved from to Data access specification. Note this is not necessarily the scheme part of the URI.</t>
+  </si>
+  <si>
+    <t>The exact type of the data resource. Typically corresponds to the scheme part (scheme://) of DATA_URI.</t>
+  </si>
+  <si>
+    <t>DATA_STORE_TYPE</t>
+  </si>
+  <si>
+    <t>Accessibility of the data resource, including host, port information, protocol, and other fields (path is protocol dependent, can be a topic name). GUI may show host, port, path separately. Hidden at search. Format: scheme://host:port/path.  Pseudo vars: DATA_PROTOCOL, DATA_HOST, DATA_PORT, DATA_PATH, DATA_QUERY, DATA_FRAGMENT.</t>
   </si>
 </sst>
 </file>
@@ -3326,60 +3329,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3404,6 +3367,46 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4343,7 +4346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -4365,16 +4368,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>468</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>466</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4403,7 +4406,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4415,7 +4418,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4430,12 +4433,12 @@
         <v>11</v>
       </c>
       <c r="G4" s="180" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4455,7 +4458,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4475,13 +4478,13 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="47" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>20</v>
@@ -4490,12 +4493,12 @@
         <v>21</v>
       </c>
       <c r="G7" s="180" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4515,7 +4518,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4524,10 +4527,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G9" s="180" t="s">
         <v>12</v>
@@ -4535,7 +4538,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4555,7 +4558,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4575,7 +4578,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="255" t="s">
+      <c r="A12" s="245" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="213"/>
@@ -4587,7 +4590,7 @@
       <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="256"/>
+      <c r="A13" s="246"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4596,7 +4599,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F13" s="55" t="s">
         <v>37</v>
@@ -4607,19 +4610,19 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="256"/>
+      <c r="A14" s="246"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="55" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G14" s="185" t="s">
         <v>12</v>
@@ -4627,19 +4630,19 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="256"/>
+      <c r="A15" s="246"/>
       <c r="B15" s="55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="55" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F15" s="55" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G15" s="185" t="s">
         <v>43</v>
@@ -5663,22 +5666,22 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="256"/>
+      <c r="A16" s="246"/>
       <c r="B16" s="55"/>
       <c r="C16" s="56" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F16" s="55" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="G16" s="185" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="4"/>
@@ -6699,22 +6702,22 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="256"/>
+      <c r="A17" s="246"/>
       <c r="B17" s="55"/>
       <c r="C17" s="56" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D17" s="55" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F17" s="55" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G17" s="185" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="4"/>
@@ -7735,19 +7738,19 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="256"/>
+      <c r="A18" s="246"/>
       <c r="B18" s="55"/>
       <c r="C18" s="56" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F18" s="55" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G18" s="185" t="s">
         <v>43</v>
@@ -8771,19 +8774,19 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="256"/>
+      <c r="A19" s="246"/>
       <c r="B19" s="55" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="55" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F19" s="55" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="G19" s="185" t="s">
         <v>43</v>
@@ -9807,19 +9810,19 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="257"/>
+      <c r="A20" s="247"/>
       <c r="B20" s="217" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C20" s="218"/>
       <c r="D20" s="217" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E20" s="219" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F20" s="217" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G20" s="220" t="s">
         <v>43</v>
@@ -11095,7 +11098,7 @@
       <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="244" t="s">
+      <c r="A34" s="250" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="62"/>
@@ -11107,7 +11110,7 @@
       <c r="H34" s="64"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="245"/>
+      <c r="A35" s="251"/>
       <c r="B35" s="65" t="s">
         <v>73</v>
       </c>
@@ -11127,7 +11130,7 @@
       <c r="H35" s="68"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="245"/>
+      <c r="A36" s="251"/>
       <c r="B36" s="69" t="s">
         <v>76</v>
       </c>
@@ -11147,7 +11150,7 @@
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="245"/>
+      <c r="A37" s="251"/>
       <c r="B37" s="69" t="s">
         <v>79</v>
       </c>
@@ -11167,7 +11170,7 @@
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="246"/>
+      <c r="A38" s="252"/>
       <c r="B38" s="73" t="s">
         <v>82</v>
       </c>
@@ -11187,7 +11190,7 @@
       <c r="H38" s="76"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="247" t="s">
+      <c r="A39" s="253" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="59"/>
@@ -12236,7 +12239,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="248"/>
-      <c r="B41" s="238" t="s">
+      <c r="B41" s="240" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -13274,7 +13277,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="248"/>
-      <c r="B42" s="238"/>
+      <c r="B42" s="240"/>
       <c r="C42" s="47" t="s">
         <v>94</v>
       </c>
@@ -14310,7 +14313,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="248"/>
-      <c r="B43" s="238"/>
+      <c r="B43" s="240"/>
       <c r="C43" s="47" t="s">
         <v>98</v>
       </c>
@@ -15346,7 +15349,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A44" s="248"/>
-      <c r="B44" s="238"/>
+      <c r="B44" s="240"/>
       <c r="C44" s="47" t="s">
         <v>102</v>
       </c>
@@ -16382,7 +16385,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="248"/>
-      <c r="B45" s="238"/>
+      <c r="B45" s="240"/>
       <c r="C45" s="47" t="s">
         <v>106</v>
       </c>
@@ -17418,7 +17421,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="248"/>
-      <c r="B46" s="238"/>
+      <c r="B46" s="240"/>
       <c r="C46" s="47" t="s">
         <v>110</v>
       </c>
@@ -18454,7 +18457,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="248"/>
-      <c r="B47" s="238"/>
+      <c r="B47" s="240"/>
       <c r="C47" s="47" t="s">
         <v>114</v>
       </c>
@@ -19490,7 +19493,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="248"/>
-      <c r="B48" s="238"/>
+      <c r="B48" s="240"/>
       <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
@@ -20526,7 +20529,7 @@
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="248"/>
-      <c r="B49" s="238"/>
+      <c r="B49" s="240"/>
       <c r="C49" s="47" t="s">
         <v>122</v>
       </c>
@@ -21562,7 +21565,7 @@
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="248"/>
-      <c r="B50" s="238"/>
+      <c r="B50" s="240"/>
       <c r="C50" s="47" t="s">
         <v>126</v>
       </c>
@@ -22598,7 +22601,7 @@
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="248"/>
-      <c r="B51" s="238"/>
+      <c r="B51" s="240"/>
       <c r="C51" s="47" t="s">
         <v>130</v>
       </c>
@@ -23634,7 +23637,7 @@
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="249"/>
-      <c r="B52" s="239"/>
+      <c r="B52" s="241"/>
       <c r="C52" s="51" t="s">
         <v>134</v>
       </c>
@@ -23645,7 +23648,7 @@
         <v>136</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G52" s="181" t="s">
         <v>43</v>
@@ -24669,7 +24672,7 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="244" t="s">
+      <c r="A53" s="250" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="77"/>
@@ -24681,7 +24684,7 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="245"/>
+      <c r="A54" s="251"/>
       <c r="B54" s="80" t="s">
         <v>138</v>
       </c>
@@ -24701,8 +24704,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="245"/>
-      <c r="B55" s="240" t="s">
+      <c r="A55" s="251"/>
+      <c r="B55" s="254" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="84" t="s">
@@ -24723,8 +24726,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="245"/>
-      <c r="B56" s="240"/>
+      <c r="A56" s="251"/>
+      <c r="B56" s="254"/>
       <c r="C56" s="80" t="s">
         <v>94</v>
       </c>
@@ -24743,8 +24746,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="245"/>
-      <c r="B57" s="240"/>
+      <c r="A57" s="251"/>
+      <c r="B57" s="254"/>
       <c r="C57" s="80" t="s">
         <v>98</v>
       </c>
@@ -24763,8 +24766,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A58" s="245"/>
-      <c r="B58" s="240"/>
+      <c r="A58" s="251"/>
+      <c r="B58" s="254"/>
       <c r="C58" s="80" t="s">
         <v>102</v>
       </c>
@@ -24783,8 +24786,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="245"/>
-      <c r="B59" s="240"/>
+      <c r="A59" s="251"/>
+      <c r="B59" s="254"/>
       <c r="C59" s="80" t="s">
         <v>106</v>
       </c>
@@ -24803,8 +24806,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="245"/>
-      <c r="B60" s="240"/>
+      <c r="A60" s="251"/>
+      <c r="B60" s="254"/>
       <c r="C60" s="80" t="s">
         <v>110</v>
       </c>
@@ -24823,8 +24826,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="245"/>
-      <c r="B61" s="240"/>
+      <c r="A61" s="251"/>
+      <c r="B61" s="254"/>
       <c r="C61" s="80" t="s">
         <v>114</v>
       </c>
@@ -24843,8 +24846,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A62" s="245"/>
-      <c r="B62" s="240"/>
+      <c r="A62" s="251"/>
+      <c r="B62" s="254"/>
       <c r="C62" s="80" t="s">
         <v>118</v>
       </c>
@@ -24863,8 +24866,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A63" s="245"/>
-      <c r="B63" s="240"/>
+      <c r="A63" s="251"/>
+      <c r="B63" s="254"/>
       <c r="C63" s="80" t="s">
         <v>122</v>
       </c>
@@ -24883,8 +24886,8 @@
       <c r="H63" s="83"/>
     </row>
     <row r="64" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A64" s="245"/>
-      <c r="B64" s="240"/>
+      <c r="A64" s="251"/>
+      <c r="B64" s="254"/>
       <c r="C64" s="80" t="s">
         <v>126</v>
       </c>
@@ -24903,8 +24906,8 @@
       <c r="H64" s="83"/>
     </row>
     <row r="65" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="245"/>
-      <c r="B65" s="240"/>
+      <c r="A65" s="251"/>
+      <c r="B65" s="254"/>
       <c r="C65" s="80" t="s">
         <v>130</v>
       </c>
@@ -24923,8 +24926,8 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="246"/>
-      <c r="B66" s="241"/>
+      <c r="A66" s="252"/>
+      <c r="B66" s="255"/>
       <c r="C66" s="85" t="s">
         <v>134</v>
       </c>
@@ -24935,7 +24938,7 @@
         <v>136</v>
       </c>
       <c r="F66" s="85" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G66" s="184" t="s">
         <v>43</v>
@@ -24943,7 +24946,7 @@
       <c r="H66" s="87"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="247" t="s">
+      <c r="A67" s="253" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="59"/>
@@ -28043,7 +28046,7 @@
       <c r="AMJ69" s="13"/>
     </row>
     <row r="70" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="244" t="s">
+      <c r="A70" s="250" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="29"/>
@@ -28055,7 +28058,7 @@
       <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="245"/>
+      <c r="A71" s="251"/>
       <c r="B71" s="69" t="s">
         <v>155</v>
       </c>
@@ -28073,8 +28076,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="245"/>
-      <c r="B72" s="242" t="s">
+      <c r="A72" s="251"/>
+      <c r="B72" s="256" t="s">
         <v>158</v>
       </c>
       <c r="C72" s="69" t="s">
@@ -28095,8 +28098,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="245"/>
-      <c r="B73" s="242"/>
+      <c r="A73" s="251"/>
+      <c r="B73" s="256"/>
       <c r="C73" s="69" t="s">
         <v>30</v>
       </c>
@@ -28115,8 +28118,8 @@
       <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="245"/>
-      <c r="B74" s="242"/>
+      <c r="A74" s="251"/>
+      <c r="B74" s="256"/>
       <c r="C74" s="69" t="s">
         <v>12</v>
       </c>
@@ -28135,8 +28138,8 @@
       <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="245"/>
-      <c r="B75" s="242"/>
+      <c r="A75" s="251"/>
+      <c r="B75" s="256"/>
       <c r="C75" s="69" t="s">
         <v>167</v>
       </c>
@@ -28155,8 +28158,8 @@
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="246"/>
-      <c r="B76" s="243"/>
+      <c r="A76" s="252"/>
+      <c r="B76" s="257"/>
       <c r="C76" s="73" t="s">
         <v>25</v>
       </c>
@@ -28175,7 +28178,7 @@
       <c r="H76" s="76"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="247" t="s">
+      <c r="A77" s="253" t="s">
         <v>172</v>
       </c>
       <c r="B77" s="31"/>
@@ -30238,7 +30241,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="248"/>
-      <c r="B79" s="238" t="s">
+      <c r="B79" s="240" t="s">
         <v>176</v>
       </c>
       <c r="C79" s="47" t="s">
@@ -31276,7 +31279,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="248"/>
-      <c r="B80" s="238"/>
+      <c r="B80" s="240"/>
       <c r="C80" s="47" t="s">
         <v>179</v>
       </c>
@@ -32312,7 +32315,7 @@
     </row>
     <row r="81" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="248"/>
-      <c r="B81" s="238"/>
+      <c r="B81" s="240"/>
       <c r="C81" s="47" t="s">
         <v>182</v>
       </c>
@@ -33348,7 +33351,7 @@
     </row>
     <row r="82" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="248"/>
-      <c r="B82" s="238"/>
+      <c r="B82" s="240"/>
       <c r="C82" s="47" t="s">
         <v>185</v>
       </c>
@@ -34384,7 +34387,7 @@
     </row>
     <row r="83" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="249"/>
-      <c r="B83" s="239"/>
+      <c r="B83" s="241"/>
       <c r="C83" s="51" t="s">
         <v>25</v>
       </c>
@@ -35493,6 +35496,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B55:B66"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A77:A83"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B41:B52"/>
     <mergeCell ref="A3:A11"/>
@@ -35500,13 +35510,6 @@
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A52"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B55:B66"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A77:A83"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -35546,16 +35549,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>469</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>467</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35584,7 +35587,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -35596,7 +35599,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -35611,12 +35614,12 @@
         <v>192</v>
       </c>
       <c r="G4" s="180" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -35636,7 +35639,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -35656,7 +35659,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -35676,7 +35679,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -35696,7 +35699,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -35716,13 +35719,13 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="47" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>20</v>
@@ -35731,12 +35734,12 @@
         <v>201</v>
       </c>
       <c r="G10" s="180" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -35777,7 +35780,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="104" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F13" s="103" t="s">
         <v>205</v>
@@ -35790,17 +35793,17 @@
     <row r="14" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="259"/>
       <c r="B14" s="103" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E14" s="104" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F14" s="103" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G14" s="183" t="s">
         <v>12</v>
@@ -35846,16 +35849,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>470</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35884,7 +35887,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -35934,7 +35937,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -35947,12 +35950,12 @@
         <v>208</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="105" t="s">
         <v>209</v>
       </c>
@@ -35968,23 +35971,23 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="105" t="s">
         <v>212</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E6" s="106"/>
       <c r="F6" s="105" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="G6" s="194"/>
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="105" t="s">
         <v>213</v>
       </c>
@@ -35994,13 +35997,13 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="105" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G7" s="194"/>
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="105" t="s">
         <v>214</v>
       </c>
@@ -36016,7 +36019,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="105" t="s">
         <v>216</v>
       </c>
@@ -36026,7 +36029,7 @@
       </c>
       <c r="E9" s="106"/>
       <c r="F9" s="105" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G9" s="194" t="s">
         <v>43</v>
@@ -36034,7 +36037,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="105" t="s">
         <v>218</v>
       </c>
@@ -36063,7 +36066,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="253"/>
+      <c r="A11" s="243"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -36079,7 +36082,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="253"/>
+      <c r="A12" s="243"/>
       <c r="B12" s="105" t="s">
         <v>222</v>
       </c>
@@ -36089,7 +36092,7 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G12" s="194" t="s">
         <v>43</v>
@@ -36097,19 +36100,19 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="253"/>
+      <c r="A13" s="243"/>
       <c r="B13" s="105" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="105" t="s">
         <v>224</v>
       </c>
       <c r="E13" s="106" t="s">
+        <v>561</v>
+      </c>
+      <c r="F13" s="105" t="s">
         <v>564</v>
-      </c>
-      <c r="F13" s="105" t="s">
-        <v>567</v>
       </c>
       <c r="G13" s="194" t="s">
         <v>12</v>
@@ -36117,19 +36120,19 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="253"/>
+      <c r="A14" s="243"/>
       <c r="B14" s="105" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E14" s="106" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F14" s="105" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="G14" s="194" t="s">
         <v>12</v>
@@ -36137,19 +36140,19 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="253"/>
+      <c r="A15" s="243"/>
       <c r="B15" s="105" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E15" s="106" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F15" s="105" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="G15" s="194" t="s">
         <v>12</v>
@@ -36157,7 +36160,7 @@
       <c r="H15" s="107"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="254"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="108" t="s">
         <v>225</v>
       </c>
@@ -36173,7 +36176,7 @@
       <c r="H16" s="110"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="244" t="s">
+      <c r="A17" s="250" t="s">
         <v>154</v>
       </c>
       <c r="B17" s="111"/>
@@ -36186,13 +36189,13 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="113" t="s">
         <v>228</v>
       </c>
       <c r="C18" s="114"/>
       <c r="D18" s="113" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E18" s="114"/>
       <c r="F18" s="113" t="s">
@@ -36202,7 +36205,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="245"/>
+      <c r="A19" s="251"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>1</v>
@@ -36212,13 +36215,13 @@
       </c>
       <c r="E19" s="114"/>
       <c r="F19" s="113" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G19" s="197"/>
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="245"/>
+      <c r="A20" s="251"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
         <v>209</v>
@@ -36228,163 +36231,163 @@
       </c>
       <c r="E20" s="114"/>
       <c r="F20" s="113" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G20" s="197"/>
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="245"/>
+      <c r="A21" s="251"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D21" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E21" s="114"/>
       <c r="F21" s="113" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G21" s="197"/>
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="245"/>
+      <c r="A22" s="251"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="113" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G22" s="197"/>
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="245"/>
+      <c r="A23" s="251"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D23" s="113" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E23" s="114"/>
       <c r="F23" s="113" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G23" s="197"/>
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="245"/>
+      <c r="A24" s="251"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D24" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E24" s="114"/>
       <c r="F24" s="113" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G24" s="197"/>
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="245"/>
+      <c r="A25" s="251"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D25" s="113" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E25" s="114"/>
       <c r="F25" s="113" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G25" s="197"/>
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="245"/>
+      <c r="A26" s="251"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="113" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G26" s="197"/>
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="245"/>
+      <c r="A27" s="251"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D27" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E27" s="114"/>
       <c r="F27" s="113" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G27" s="197"/>
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="245"/>
+      <c r="A28" s="251"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D28" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E28" s="114"/>
       <c r="F28" s="113" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="G28" s="197"/>
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="245"/>
+      <c r="A29" s="251"/>
       <c r="B29" s="113"/>
       <c r="C29" s="114" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D29" s="113" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E29" s="114"/>
       <c r="F29" s="113" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G29" s="197"/>
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="245"/>
+      <c r="A30" s="251"/>
       <c r="B30" s="113" t="s">
         <v>230</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="113" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E30" s="114"/>
       <c r="F30" s="113" t="s">
@@ -36394,7 +36397,7 @@
       <c r="H30" s="115"/>
     </row>
     <row r="31" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="245"/>
+      <c r="A31" s="251"/>
       <c r="B31" s="222"/>
       <c r="C31" s="114" t="s">
         <v>1</v>
@@ -36404,13 +36407,13 @@
       </c>
       <c r="E31" s="223"/>
       <c r="F31" s="113" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G31" s="224"/>
       <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="245"/>
+      <c r="A32" s="251"/>
       <c r="B32" s="222"/>
       <c r="C32" s="114" t="s">
         <v>209</v>
@@ -36420,157 +36423,157 @@
       </c>
       <c r="E32" s="223"/>
       <c r="F32" s="113" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G32" s="224"/>
       <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="245"/>
+      <c r="A33" s="251"/>
       <c r="B33" s="222"/>
       <c r="C33" s="114" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D33" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E33" s="223"/>
       <c r="F33" s="113" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G33" s="224"/>
       <c r="H33" s="225"/>
     </row>
     <row r="34" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="245"/>
+      <c r="A34" s="251"/>
       <c r="B34" s="222"/>
       <c r="C34" s="114" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D34" s="113" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E34" s="223"/>
       <c r="F34" s="113" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G34" s="224"/>
       <c r="H34" s="225"/>
     </row>
     <row r="35" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="245"/>
+      <c r="A35" s="251"/>
       <c r="B35" s="222"/>
       <c r="C35" s="114" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D35" s="113" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E35" s="223"/>
       <c r="F35" s="113" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G35" s="224"/>
       <c r="H35" s="225"/>
     </row>
     <row r="36" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="245"/>
+      <c r="A36" s="251"/>
       <c r="B36" s="222"/>
       <c r="C36" s="114" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D36" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E36" s="223"/>
       <c r="F36" s="113" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="G36" s="224"/>
       <c r="H36" s="225"/>
     </row>
     <row r="37" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="245"/>
+      <c r="A37" s="251"/>
       <c r="B37" s="222"/>
       <c r="C37" s="114" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D37" s="113" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E37" s="223"/>
       <c r="F37" s="113" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G37" s="224"/>
       <c r="H37" s="225"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="245"/>
+      <c r="A38" s="251"/>
       <c r="B38" s="222"/>
       <c r="C38" s="114" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D38" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E38" s="223"/>
       <c r="F38" s="113" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G38" s="224"/>
       <c r="H38" s="225"/>
     </row>
     <row r="39" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="245"/>
+      <c r="A39" s="251"/>
       <c r="B39" s="222"/>
       <c r="C39" s="114" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D39" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E39" s="223"/>
       <c r="F39" s="113" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G39" s="224"/>
       <c r="H39" s="225"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="245"/>
+      <c r="A40" s="251"/>
       <c r="B40" s="222"/>
       <c r="C40" s="114" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D40" s="113" t="s">
         <v>223</v>
       </c>
       <c r="E40" s="223"/>
       <c r="F40" s="113" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G40" s="224"/>
       <c r="H40" s="225"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="245"/>
+      <c r="A41" s="251"/>
       <c r="B41" s="222"/>
       <c r="C41" s="114" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D41" s="113" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E41" s="223"/>
       <c r="F41" s="113" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G41" s="224"/>
       <c r="H41" s="225"/>
     </row>
     <row r="42" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="246"/>
+      <c r="A42" s="252"/>
       <c r="B42" s="116" t="s">
         <v>232</v>
       </c>
@@ -36580,7 +36583,7 @@
       </c>
       <c r="E42" s="117"/>
       <c r="F42" s="116" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G42" s="198" t="s">
         <v>43</v>
@@ -36588,7 +36591,7 @@
       <c r="H42" s="118"/>
     </row>
     <row r="43" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="247" t="s">
+      <c r="A43" s="253" t="s">
         <v>233</v>
       </c>
       <c r="B43" s="119"/>
@@ -36675,7 +36678,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="244" t="s">
+      <c r="A45" s="250" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="111"/>
@@ -36688,7 +36691,7 @@
       <c r="AMJ45" s="5"/>
     </row>
     <row r="46" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="245"/>
+      <c r="A46" s="251"/>
       <c r="B46" s="113" t="s">
         <v>73</v>
       </c>
@@ -36706,7 +36709,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="245"/>
+      <c r="A47" s="251"/>
       <c r="B47" s="113" t="s">
         <v>76</v>
       </c>
@@ -36724,7 +36727,7 @@
       <c r="H47" s="115"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="246"/>
+      <c r="A48" s="252"/>
       <c r="B48" s="116" t="s">
         <v>79</v>
       </c>
@@ -36742,7 +36745,7 @@
       <c r="H48" s="118"/>
     </row>
     <row r="49" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="247" t="s">
+      <c r="A49" s="253" t="s">
         <v>240</v>
       </c>
       <c r="B49" s="121"/>
@@ -36955,8 +36958,8 @@
       <c r="H58" s="110"/>
     </row>
     <row r="59" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="244" t="s">
-        <v>481</v>
+      <c r="A59" s="250" t="s">
+        <v>479</v>
       </c>
       <c r="B59" s="123"/>
       <c r="C59" s="123"/>
@@ -36968,7 +36971,7 @@
       <c r="AMJ59" s="5"/>
     </row>
     <row r="60" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="246"/>
+      <c r="A60" s="252"/>
       <c r="B60" s="116" t="s">
         <v>5</v>
       </c>
@@ -37008,12 +37011,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -37030,16 +37033,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>471</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -38085,7 +38088,7 @@
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="260" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
@@ -38124,7 +38127,7 @@
         <v>296</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="126"/>
     </row>
@@ -38144,14 +38147,14 @@
         <v>298</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="261"/>
       <c r="B6" s="105" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="105" t="s">
@@ -38164,7 +38167,7 @@
         <v>299</v>
       </c>
       <c r="G6" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H6" s="126"/>
     </row>
@@ -38178,13 +38181,13 @@
         <v>301</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F7" s="105" t="s">
         <v>302</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H7" s="126"/>
     </row>
@@ -38211,7 +38214,7 @@
         <v>210</v>
       </c>
       <c r="E9" s="114" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>304</v>
@@ -39240,17 +39243,17 @@
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="265"/>
       <c r="B10" s="113" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C10" s="114"/>
       <c r="D10" s="113" t="s">
         <v>210</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G10" s="197" t="s">
         <v>43</v>
@@ -40283,7 +40286,7 @@
         <v>210</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F11" s="113" t="s">
         <v>309</v>
@@ -41312,14 +41315,14 @@
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="265"/>
       <c r="B12" s="113" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="113" t="s">
         <v>310</v>
       </c>
       <c r="E12" s="117" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F12" s="116" t="s">
         <v>311</v>
@@ -42355,7 +42358,7 @@
         <v>306</v>
       </c>
       <c r="E13" s="114" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F13" s="113" t="s">
         <v>307</v>
@@ -43383,7 +43386,7 @@
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="260" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="121"/>
@@ -43412,7 +43415,7 @@
         <v>313</v>
       </c>
       <c r="E15" s="109" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F15" s="108" t="s">
         <v>314</v>
@@ -45476,7 +45479,7 @@
         <v>219</v>
       </c>
       <c r="E17" s="114" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>316</v>
@@ -45496,7 +45499,7 @@
         <v>219</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F18" s="113" t="s">
         <v>317</v>
@@ -45516,7 +45519,7 @@
         <v>313</v>
       </c>
       <c r="E19" s="117" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F19" s="116" t="s">
         <v>318</v>
@@ -45549,57 +45552,57 @@
     <row r="21" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="261"/>
       <c r="B21" s="105" t="s">
-        <v>106</v>
+        <v>581</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F21" s="105" t="s">
+        <v>580</v>
+      </c>
+      <c r="G21" s="194" t="s">
         <v>321</v>
-      </c>
-      <c r="G21" s="194" t="s">
-        <v>322</v>
       </c>
       <c r="H21" s="126"/>
     </row>
     <row r="22" spans="1:1024" ht="146.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="261"/>
       <c r="B22" s="105" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="105" t="s">
         <v>224</v>
       </c>
       <c r="E22" s="106" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>533</v>
+        <v>582</v>
       </c>
       <c r="G22" s="194" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="262"/>
       <c r="B23" s="108" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C23" s="109"/>
       <c r="D23" s="108" t="s">
+        <v>323</v>
+      </c>
+      <c r="E23" s="109" t="s">
+        <v>457</v>
+      </c>
+      <c r="F23" s="108" t="s">
         <v>324</v>
-      </c>
-      <c r="E23" s="109" t="s">
-        <v>459</v>
-      </c>
-      <c r="F23" s="108" t="s">
-        <v>325</v>
       </c>
       <c r="G23" s="195" t="s">
         <v>319</v>
@@ -45608,7 +45611,7 @@
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="263" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="132"/>
@@ -45622,24 +45625,24 @@
     <row r="25" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="264"/>
       <c r="B25" s="116" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C25" s="117"/>
       <c r="D25" s="116" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E25" s="117"/>
       <c r="F25" s="116" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G25" s="198" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H25" s="130"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="260" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B26" s="121"/>
       <c r="C26" s="121"/>
@@ -45657,7 +45660,7 @@
       <c r="O26" s="7"/>
       <c r="AMJ26" s="5"/>
     </row>
-    <row r="27" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1024" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="261"/>
       <c r="B27" s="105" t="s">
         <v>110</v>
@@ -45667,10 +45670,10 @@
         <v>210</v>
       </c>
       <c r="E27" s="106" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>330</v>
+        <v>579</v>
       </c>
       <c r="G27" s="194" t="s">
         <v>43</v>
@@ -45687,10 +45690,10 @@
         <v>210</v>
       </c>
       <c r="E28" s="106" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G28" s="194" t="s">
         <v>43</v>
@@ -45707,10 +45710,10 @@
         <v>210</v>
       </c>
       <c r="E29" s="106" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F29" s="105" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G29" s="194" t="s">
         <v>43</v>
@@ -45727,10 +45730,10 @@
         <v>210</v>
       </c>
       <c r="E30" s="106" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G30" s="194" t="s">
         <v>43</v>
@@ -45747,10 +45750,10 @@
         <v>210</v>
       </c>
       <c r="E31" s="109" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F31" s="108" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G31" s="195" t="s">
         <v>43</v>
@@ -45759,7 +45762,7 @@
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="263" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B32" s="123"/>
       <c r="C32" s="123"/>
@@ -45780,10 +45783,10 @@
         <v>210</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F33" s="113" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G33" s="197" t="s">
         <v>43</v>
@@ -45793,14 +45796,14 @@
     <row r="34" spans="1:8" ht="89.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="265"/>
       <c r="B34" s="113" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C34" s="223"/>
       <c r="D34" s="222" t="s">
         <v>310</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F34" s="222"/>
       <c r="G34" s="224" t="s">
@@ -45811,7 +45814,7 @@
     <row r="35" spans="1:8" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="264"/>
       <c r="B35" s="116" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C35" s="117"/>
       <c r="D35" s="116" t="s">
@@ -45819,7 +45822,7 @@
       </c>
       <c r="E35" s="117"/>
       <c r="F35" s="116" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G35" s="198" t="s">
         <v>43</v>
@@ -45878,16 +45881,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>472</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>470</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -45916,8 +45919,8 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
-        <v>485</v>
+      <c r="A3" s="253" t="s">
+        <v>483</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -45955,10 +45958,10 @@
         <v>254</v>
       </c>
       <c r="F4" s="136" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="137"/>
     </row>
@@ -45978,7 +45981,7 @@
         <v>259</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H5" s="137"/>
     </row>
@@ -45995,7 +45998,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="136" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G6" s="194"/>
       <c r="H6" s="137"/>
@@ -46016,7 +46019,7 @@
         <v>264</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H7" s="137"/>
     </row>
@@ -46033,10 +46036,10 @@
         <v>266</v>
       </c>
       <c r="F8" s="136" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G8" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H8" s="137"/>
     </row>
@@ -46050,13 +46053,13 @@
         <v>207</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F9" s="136" t="s">
         <v>271</v>
       </c>
       <c r="G9" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H9" s="137"/>
     </row>
@@ -46070,10 +46073,10 @@
         <v>272</v>
       </c>
       <c r="E10" s="106" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F10" s="136" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G10" s="194"/>
       <c r="H10" s="137"/>
@@ -46091,7 +46094,7 @@
         <v>276</v>
       </c>
       <c r="F11" s="136" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G11" s="194"/>
       <c r="H11" s="137"/>
@@ -46099,17 +46102,17 @@
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="248"/>
       <c r="B12" s="106" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E12" s="106" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F12" s="136" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G12" s="194"/>
       <c r="H12" s="137"/>
@@ -46121,7 +46124,7 @@
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="136" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E13" s="106" t="s">
         <v>283</v>
@@ -46135,17 +46138,17 @@
     <row r="14" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="248"/>
       <c r="B14" s="106" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E14" s="136" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F14" s="136" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G14" s="194"/>
       <c r="H14" s="137"/>
@@ -46153,17 +46156,17 @@
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="248"/>
       <c r="B15" s="106" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="136" t="s">
         <v>207</v>
       </c>
       <c r="E15" s="136" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F15" s="136" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G15" s="194"/>
       <c r="H15" s="137"/>
@@ -46171,17 +46174,17 @@
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="248"/>
       <c r="B16" s="106" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="136" t="s">
+        <v>354</v>
+      </c>
+      <c r="E16" s="136" t="s">
+        <v>355</v>
+      </c>
+      <c r="F16" s="136" t="s">
         <v>356</v>
-      </c>
-      <c r="E16" s="136" t="s">
-        <v>357</v>
-      </c>
-      <c r="F16" s="136" t="s">
-        <v>358</v>
       </c>
       <c r="G16" s="194"/>
       <c r="H16" s="137"/>
@@ -46189,7 +46192,7 @@
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="248"/>
       <c r="B17" s="106" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
@@ -46199,7 +46202,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="136" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G17" s="194"/>
       <c r="H17" s="137"/>
@@ -46214,7 +46217,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="109" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F18" s="138" t="s">
         <v>295</v>
@@ -46266,16 +46269,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>473</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>471</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -46305,7 +46308,7 @@
     </row>
     <row r="3" spans="1:17" s="144" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="266" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
@@ -46331,7 +46334,7 @@
         <v>255</v>
       </c>
       <c r="G4" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H4" s="145"/>
       <c r="I4" s="144"/>
@@ -46360,7 +46363,7 @@
         <v>259</v>
       </c>
       <c r="G5" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H5" s="145"/>
       <c r="I5" s="144"/>
@@ -46416,7 +46419,7 @@
         <v>264</v>
       </c>
       <c r="G7" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="144"/>
@@ -46445,7 +46448,7 @@
         <v>267</v>
       </c>
       <c r="G8" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H8" s="145"/>
       <c r="I8" s="144"/>
@@ -46474,7 +46477,7 @@
         <v>271</v>
       </c>
       <c r="G9" s="194" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H9" s="149"/>
       <c r="I9" s="144"/>
@@ -46625,15 +46628,15 @@
     <row r="15" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="267"/>
       <c r="B15" s="106" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E15" s="136"/>
       <c r="F15" s="106" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G15" s="194"/>
       <c r="H15" s="145"/>
@@ -46654,11 +46657,11 @@
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="105" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E16" s="136"/>
       <c r="F16" s="106" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G16" s="194"/>
       <c r="H16" s="145"/>
@@ -46766,16 +46769,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>570</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:20" s="152" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -46805,7 +46808,7 @@
     </row>
     <row r="3" spans="1:20" s="152" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="230" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B3" s="227"/>
       <c r="C3" s="227"/>
@@ -46816,7 +46819,7 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="247" t="s">
+      <c r="A4" s="253" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="153"/>
@@ -46850,10 +46853,10 @@
       </c>
       <c r="E5" s="157"/>
       <c r="F5" s="157" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G5" s="180" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H5" s="158"/>
     </row>
@@ -46868,7 +46871,7 @@
       </c>
       <c r="E6" s="157"/>
       <c r="F6" s="157" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G6" s="180" t="s">
         <v>12</v>
@@ -46886,7 +46889,7 @@
       </c>
       <c r="E7" s="157"/>
       <c r="F7" s="157" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G7" s="180" t="s">
         <v>12</v>
@@ -46900,19 +46903,19 @@
       </c>
       <c r="C8" s="159"/>
       <c r="D8" s="159" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E8" s="159"/>
       <c r="F8" s="159" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G8" s="181" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H8" s="160"/>
     </row>
     <row r="9" spans="1:20" s="155" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="244" t="s">
+      <c r="A9" s="250" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="161"/>
@@ -46924,17 +46927,17 @@
       <c r="H9" s="162"/>
     </row>
     <row r="10" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+      <c r="A10" s="251"/>
       <c r="B10" s="163" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="163"/>
       <c r="D10" s="163" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E10" s="163"/>
       <c r="F10" s="163" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G10" s="211" t="s">
         <v>12</v>
@@ -46942,147 +46945,147 @@
       <c r="H10" s="164"/>
     </row>
     <row r="11" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="245"/>
+      <c r="A11" s="251"/>
       <c r="B11" s="163" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C11" s="163"/>
       <c r="D11" s="163" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E11" s="163"/>
       <c r="F11" s="163" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G11" s="183"/>
       <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="245"/>
+      <c r="A12" s="251"/>
       <c r="B12" s="163"/>
       <c r="C12" s="163" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D12" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E12" s="163"/>
       <c r="F12" s="163" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G12" s="183"/>
       <c r="H12" s="164"/>
     </row>
     <row r="13" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="245"/>
+      <c r="A13" s="251"/>
       <c r="B13" s="163"/>
       <c r="C13" s="163" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D13" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E13" s="163"/>
       <c r="F13" s="163" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G13" s="183"/>
       <c r="H13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+      <c r="A14" s="251"/>
       <c r="B14" s="163"/>
       <c r="C14" s="163" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D14" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E14" s="163"/>
       <c r="F14" s="163" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G14" s="183"/>
       <c r="H14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="245"/>
+      <c r="A15" s="251"/>
       <c r="B15" s="163"/>
       <c r="C15" s="163" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D15" s="163" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E15" s="163"/>
       <c r="F15" s="163" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G15" s="183"/>
       <c r="H15" s="164"/>
     </row>
     <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="245"/>
+      <c r="A16" s="251"/>
       <c r="B16" s="163"/>
       <c r="C16" s="163" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D16" s="163" t="s">
         <v>310</v>
       </c>
       <c r="E16" s="163"/>
       <c r="F16" s="163" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G16" s="183"/>
       <c r="H16" s="164"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="245"/>
+      <c r="A17" s="251"/>
       <c r="B17" s="163"/>
       <c r="C17" s="163" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D17" s="163" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="163" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F17" s="163" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="G17" s="183"/>
       <c r="H17" s="164"/>
     </row>
     <row r="18" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="163" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C18" s="163"/>
       <c r="D18" s="163" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E18" s="163"/>
       <c r="F18" s="163" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G18" s="183"/>
       <c r="H18" s="164"/>
     </row>
     <row r="19" spans="1:8" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="246"/>
+      <c r="A19" s="252"/>
       <c r="B19" s="165"/>
       <c r="C19" s="165" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D19" s="165" t="s">
         <v>310</v>
       </c>
       <c r="E19" s="165"/>
       <c r="F19" s="165" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G19" s="184"/>
       <c r="H19" s="166"/>
@@ -47135,7 +47138,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="269" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B1" s="269"/>
       <c r="C1" s="269"/>
@@ -47143,7 +47146,7 @@
       <c r="E1" s="269"/>
       <c r="F1" s="269"/>
       <c r="G1" s="269"/>
-      <c r="H1" s="251"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:20" s="232" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -47173,7 +47176,7 @@
     </row>
     <row r="3" spans="1:20" s="152" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="230" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B3" s="227"/>
       <c r="C3" s="227"/>
@@ -47184,8 +47187,8 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="236" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="247" t="s">
-        <v>558</v>
+      <c r="A4" s="253" t="s">
+        <v>555</v>
       </c>
       <c r="B4" s="153"/>
       <c r="C4" s="153"/>
@@ -47210,17 +47213,17 @@
     <row r="5" spans="1:20" s="151" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="248"/>
       <c r="B5" s="105" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C5" s="157"/>
       <c r="D5" s="157" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E5" s="157" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F5" s="157" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="G5" s="180" t="s">
         <v>12</v>
@@ -47231,16 +47234,16 @@
       <c r="A6" s="248"/>
       <c r="B6" s="157"/>
       <c r="C6" s="157" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D6" s="157" t="s">
         <v>207</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F6" s="157" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="G6" s="180" t="s">
         <v>12</v>
@@ -47311,16 +47314,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
-        <v>474</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="A1" s="238" t="s">
+        <v>472</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -48365,8 +48368,8 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
-        <v>379</v>
+      <c r="A3" s="253" t="s">
+        <v>377</v>
       </c>
       <c r="B3" s="169"/>
       <c r="C3" s="169"/>
@@ -48387,7 +48390,7 @@
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="157" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G4" s="47"/>
       <c r="H4" s="158"/>
@@ -50451,7 +50454,7 @@
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="157" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="171"/>
@@ -51475,7 +51478,7 @@
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="248"/>
       <c r="B7" s="47" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C7" s="157"/>
       <c r="D7" s="47" t="s">
@@ -51483,7 +51486,7 @@
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="157" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="158"/>
@@ -52507,7 +52510,7 @@
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="248"/>
       <c r="B8" s="47" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C8" s="157"/>
       <c r="D8" s="47" t="s">
@@ -52515,7 +52518,7 @@
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="157" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="158"/>
@@ -53539,15 +53542,15 @@
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="248"/>
       <c r="B9" s="47" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C9" s="157"/>
       <c r="D9" s="47" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="157" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G9" s="47"/>
       <c r="H9" s="158"/>
@@ -54571,7 +54574,7 @@
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="248"/>
       <c r="B10" s="47" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C10" s="157"/>
       <c r="D10" s="47" t="s">
@@ -54579,7 +54582,7 @@
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="157" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="158"/>
@@ -55603,15 +55606,15 @@
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="248"/>
       <c r="B11" s="47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C11" s="157"/>
       <c r="D11" s="47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="157" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="158"/>
@@ -56635,7 +56638,7 @@
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="249"/>
       <c r="B12" s="51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C12" s="159"/>
       <c r="D12" s="51" t="s">
@@ -56643,7 +56646,7 @@
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="159" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G12" s="51"/>
       <c r="H12" s="160"/>
@@ -57665,8 +57668,8 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="244" t="s">
-        <v>394</v>
+      <c r="A13" s="250" t="s">
+        <v>392</v>
       </c>
       <c r="B13" s="172"/>
       <c r="C13" s="172"/>
@@ -57678,7 +57681,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+      <c r="A14" s="251"/>
       <c r="B14" s="69" t="s">
         <v>206</v>
       </c>
@@ -57688,13 +57691,13 @@
       </c>
       <c r="E14" s="69"/>
       <c r="F14" s="69" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G14" s="69"/>
       <c r="H14" s="174"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="245"/>
+      <c r="A15" s="251"/>
       <c r="B15" s="69" t="s">
         <v>256</v>
       </c>
@@ -57710,7 +57713,7 @@
       <c r="H15" s="174"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="245"/>
+      <c r="A16" s="251"/>
       <c r="B16" s="69" t="s">
         <v>212</v>
       </c>
@@ -57720,13 +57723,13 @@
       </c>
       <c r="E16" s="69"/>
       <c r="F16" s="69" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G16" s="69"/>
       <c r="H16" s="174"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="245"/>
+      <c r="A17" s="251"/>
       <c r="B17" s="69" t="s">
         <v>262</v>
       </c>
@@ -57736,13 +57739,13 @@
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="69" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="174"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="69" t="s">
         <v>209</v>
       </c>
@@ -57752,13 +57755,13 @@
       </c>
       <c r="E18" s="69"/>
       <c r="F18" s="69" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G18" s="69"/>
       <c r="H18" s="174"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="245"/>
+      <c r="A19" s="251"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -57768,29 +57771,29 @@
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="69" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G19" s="69"/>
       <c r="H19" s="174"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="245"/>
+      <c r="A20" s="251"/>
       <c r="B20" s="69" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="69" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G20" s="69"/>
       <c r="H20" s="174"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="245"/>
+      <c r="A21" s="251"/>
       <c r="B21" s="69" t="s">
         <v>310</v>
       </c>
@@ -57800,15 +57803,15 @@
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="69" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G21" s="69"/>
       <c r="H21" s="174"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="245"/>
+      <c r="A22" s="251"/>
       <c r="B22" s="69" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C22" s="69"/>
       <c r="D22" s="69" t="s">
@@ -57816,15 +57819,15 @@
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="69" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G22" s="69"/>
       <c r="H22" s="174"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="245"/>
+      <c r="A23" s="251"/>
       <c r="B23" s="69" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="69" t="s">
@@ -57832,15 +57835,15 @@
       </c>
       <c r="E23" s="69"/>
       <c r="F23" s="69" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G23" s="69"/>
       <c r="H23" s="174"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="246"/>
+      <c r="A24" s="252"/>
       <c r="B24" s="73" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73" t="s">
@@ -57848,14 +57851,14 @@
       </c>
       <c r="E24" s="73"/>
       <c r="F24" s="73" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G24" s="73"/>
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="247" t="s">
-        <v>345</v>
+      <c r="A25" s="253" t="s">
+        <v>343</v>
       </c>
       <c r="B25" s="176"/>
       <c r="C25" s="176"/>
@@ -57876,7 +57879,7 @@
       </c>
       <c r="E26" s="47"/>
       <c r="F26" s="47" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="171"/>
@@ -57908,7 +57911,7 @@
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="47" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="171"/>
@@ -57924,7 +57927,7 @@
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="47" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="171"/>
@@ -57932,7 +57935,7 @@
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="248"/>
       <c r="B30" s="47" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47" t="s">
@@ -57940,7 +57943,7 @@
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="47" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="171"/>
@@ -57956,7 +57959,7 @@
       </c>
       <c r="E31" s="47"/>
       <c r="F31" s="47" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="171"/>
@@ -57964,15 +57967,15 @@
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="248"/>
       <c r="B32" s="47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E32" s="47"/>
       <c r="F32" s="47" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="171"/>
@@ -57980,7 +57983,7 @@
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="248"/>
       <c r="B33" s="47" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="47" t="s">
@@ -57988,7 +57991,7 @@
       </c>
       <c r="E33" s="47"/>
       <c r="F33" s="47" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="171"/>
@@ -58004,7 +58007,7 @@
       </c>
       <c r="E34" s="47"/>
       <c r="F34" s="47" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="171"/>
@@ -58012,7 +58015,7 @@
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="248"/>
       <c r="B35" s="47" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47" t="s">
@@ -58020,7 +58023,7 @@
       </c>
       <c r="E35" s="47"/>
       <c r="F35" s="47" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="171"/>
@@ -58028,7 +58031,7 @@
     <row r="36" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="249"/>
       <c r="B36" s="51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="51" t="s">
@@ -58036,13 +58039,13 @@
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G36" s="51"/>
       <c r="H36" s="178"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="244" t="s">
+      <c r="A37" s="250" t="s">
         <v>278</v>
       </c>
       <c r="B37" s="172"/>
@@ -58055,7 +58058,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="245"/>
+      <c r="A38" s="251"/>
       <c r="B38" s="69" t="s">
         <v>206</v>
       </c>
@@ -58065,13 +58068,13 @@
       </c>
       <c r="E38" s="69"/>
       <c r="F38" s="69" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G38" s="69"/>
       <c r="H38" s="174"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="245"/>
+      <c r="A39" s="251"/>
       <c r="B39" s="69" t="s">
         <v>256</v>
       </c>
@@ -58087,7 +58090,7 @@
       <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="245"/>
+      <c r="A40" s="251"/>
       <c r="B40" s="69" t="s">
         <v>212</v>
       </c>
@@ -58097,13 +58100,13 @@
       </c>
       <c r="E40" s="69"/>
       <c r="F40" s="69" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G40" s="69"/>
       <c r="H40" s="174"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="245"/>
+      <c r="A41" s="251"/>
       <c r="B41" s="69" t="s">
         <v>262</v>
       </c>
@@ -58113,15 +58116,15 @@
       </c>
       <c r="E41" s="69"/>
       <c r="F41" s="69" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G41" s="69"/>
       <c r="H41" s="174"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="245"/>
+      <c r="A42" s="251"/>
       <c r="B42" s="69" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="69" t="s">
@@ -58129,15 +58132,15 @@
       </c>
       <c r="E42" s="69"/>
       <c r="F42" s="69" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G42" s="69"/>
       <c r="H42" s="174"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="245"/>
+      <c r="A43" s="251"/>
       <c r="B43" s="69" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C43" s="69"/>
       <c r="D43" s="69" t="s">
@@ -58145,13 +58148,13 @@
       </c>
       <c r="E43" s="69"/>
       <c r="F43" s="69" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G43" s="69"/>
       <c r="H43" s="174"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="245"/>
+      <c r="A44" s="251"/>
       <c r="B44" s="69" t="s">
         <v>209</v>
       </c>
@@ -58161,31 +58164,31 @@
       </c>
       <c r="E44" s="69"/>
       <c r="F44" s="69" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G44" s="69"/>
       <c r="H44" s="174"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="245"/>
+      <c r="A45" s="251"/>
       <c r="B45" s="69" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C45" s="69"/>
       <c r="D45" s="69" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E45" s="69"/>
       <c r="F45" s="69" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G45" s="69"/>
       <c r="H45" s="174"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="245"/>
+      <c r="A46" s="251"/>
       <c r="B46" s="69" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C46" s="69"/>
       <c r="D46" s="69" t="s">
@@ -58193,13 +58196,13 @@
       </c>
       <c r="E46" s="69"/>
       <c r="F46" s="69" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G46" s="69"/>
       <c r="H46" s="174"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="245"/>
+      <c r="A47" s="251"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -58209,15 +58212,15 @@
       </c>
       <c r="E47" s="69"/>
       <c r="F47" s="69" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G47" s="69"/>
       <c r="H47" s="174"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="246"/>
+      <c r="A48" s="252"/>
       <c r="B48" s="73" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="73" t="s">
@@ -58225,7 +58228,7 @@
       </c>
       <c r="E48" s="73"/>
       <c r="F48" s="73" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G48" s="73"/>
       <c r="H48" s="175"/>

</xml_diff>

<commit_message>
feat(DMA): improve DataAssetsMapping examples
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahajnal/Documents/github/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/digitbrain.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEFE86F-304F-0E47-97C5-313017B331B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBD35E8-199E-8B48-A1C0-7CF8E93CBD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -1795,9 +1795,6 @@
     <t>DataAssetsMapping</t>
   </si>
   <si>
-    <t>Map</t>
-  </si>
-  <si>
     <t>Mapping the available Data assets in this DMA Tuple to available Microservices. Required if Data assets are required. Not all microservices need a Data asset.</t>
   </si>
   <si>
@@ -1849,13 +1846,7 @@
     <t>See above</t>
   </si>
   <si>
-    <t>Nested below each Microservice, these key(s) are UUID string(s) corresponding to the Data Source(s) of each Microservice. &lt;br&gt; The value for each key is the UUID of the Data Asset that corresponds to it.</t>
-  </si>
-  <si>
     <t>[DataAssetsMapping](dataassetsmapping.md)</t>
-  </si>
-  <si>
-    <t>"microservice_0dk": { &lt;br&gt;  "datasource_89d": "data_9d8", &lt;br&gt;  "datasource_dlo": "data_aij" &lt;br&gt; }</t>
   </si>
   <si>
     <t xml:space="preserve">*MICROSERVICE_ID* </t>
@@ -1874,6 +1865,15 @@
   </si>
   <si>
     <t>Accessibility of the data resource, including host, port information, protocol, and other fields (path is protocol dependent, can be a topic name). GUI may show host, port, path separately. Hidden at search. Format: scheme://host:port/path.  Pseudo vars: DATA_PROTOCOL, DATA_HOST, DATA_PORT, DATA_PATH, DATA_QUERY, DATA_FRAGMENT.</t>
+  </si>
+  <si>
+    <t>Map&lt;String, UUID&gt;</t>
+  </si>
+  <si>
+    <t>"microservice_0db_uuid": { &lt;br&gt;  "datasource_89d": "data_9d8_uuid", &lt;br&gt;  "datasource_dlo": "data_aij_uuid" &lt;br&gt; }</t>
+  </si>
+  <si>
+    <t>Nested below each Microservice, these key(s) are the String identifier(s) of the Data Source(s) of each Microservice. &lt;br&gt; The value for each key is the UUID of the Data Asset that corresponds to it.</t>
   </si>
 </sst>
 </file>
@@ -3329,20 +3329,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3367,46 +3407,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4346,7 +4346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ107"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -4368,16 +4368,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4406,7 +4406,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="252" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4418,7 +4418,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="243"/>
+      <c r="A4" s="253"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="243"/>
+      <c r="A5" s="253"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4458,7 +4458,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="243"/>
+      <c r="A6" s="253"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4478,7 +4478,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="243"/>
+      <c r="A7" s="253"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="243"/>
+      <c r="A8" s="253"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4518,7 +4518,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="243"/>
+      <c r="A9" s="253"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4538,7 +4538,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="243"/>
+      <c r="A10" s="253"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4558,7 +4558,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="244"/>
+      <c r="A11" s="254"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4578,7 +4578,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="245" t="s">
+      <c r="A12" s="255" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="213"/>
@@ -4590,7 +4590,7 @@
       <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="246"/>
+      <c r="A13" s="256"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4610,7 +4610,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="246"/>
+      <c r="A14" s="256"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4630,7 +4630,7 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="246"/>
+      <c r="A15" s="256"/>
       <c r="B15" s="55" t="s">
         <v>440</v>
       </c>
@@ -5666,7 +5666,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="246"/>
+      <c r="A16" s="256"/>
       <c r="B16" s="55"/>
       <c r="C16" s="56" t="s">
         <v>540</v>
@@ -6702,7 +6702,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="246"/>
+      <c r="A17" s="256"/>
       <c r="B17" s="55"/>
       <c r="C17" s="56" t="s">
         <v>542</v>
@@ -7738,7 +7738,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="246"/>
+      <c r="A18" s="256"/>
       <c r="B18" s="55"/>
       <c r="C18" s="56" t="s">
         <v>541</v>
@@ -8774,7 +8774,7 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="246"/>
+      <c r="A19" s="256"/>
       <c r="B19" s="55" t="s">
         <v>437</v>
       </c>
@@ -9810,7 +9810,7 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="247"/>
+      <c r="A20" s="257"/>
       <c r="B20" s="217" t="s">
         <v>438</v>
       </c>
@@ -11098,7 +11098,7 @@
       <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="250" t="s">
+      <c r="A34" s="244" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="62"/>
@@ -11110,7 +11110,7 @@
       <c r="H34" s="64"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="251"/>
+      <c r="A35" s="245"/>
       <c r="B35" s="65" t="s">
         <v>73</v>
       </c>
@@ -11130,7 +11130,7 @@
       <c r="H35" s="68"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="251"/>
+      <c r="A36" s="245"/>
       <c r="B36" s="69" t="s">
         <v>76</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="251"/>
+      <c r="A37" s="245"/>
       <c r="B37" s="69" t="s">
         <v>79</v>
       </c>
@@ -11170,7 +11170,7 @@
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="252"/>
+      <c r="A38" s="246"/>
       <c r="B38" s="73" t="s">
         <v>82</v>
       </c>
@@ -11190,7 +11190,7 @@
       <c r="H38" s="76"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="253" t="s">
+      <c r="A39" s="247" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="59"/>
@@ -12239,7 +12239,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="248"/>
-      <c r="B41" s="240" t="s">
+      <c r="B41" s="238" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -13277,7 +13277,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="248"/>
-      <c r="B42" s="240"/>
+      <c r="B42" s="238"/>
       <c r="C42" s="47" t="s">
         <v>94</v>
       </c>
@@ -14313,7 +14313,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="248"/>
-      <c r="B43" s="240"/>
+      <c r="B43" s="238"/>
       <c r="C43" s="47" t="s">
         <v>98</v>
       </c>
@@ -15349,7 +15349,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A44" s="248"/>
-      <c r="B44" s="240"/>
+      <c r="B44" s="238"/>
       <c r="C44" s="47" t="s">
         <v>102</v>
       </c>
@@ -16385,7 +16385,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="248"/>
-      <c r="B45" s="240"/>
+      <c r="B45" s="238"/>
       <c r="C45" s="47" t="s">
         <v>106</v>
       </c>
@@ -17421,7 +17421,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="248"/>
-      <c r="B46" s="240"/>
+      <c r="B46" s="238"/>
       <c r="C46" s="47" t="s">
         <v>110</v>
       </c>
@@ -18457,7 +18457,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="248"/>
-      <c r="B47" s="240"/>
+      <c r="B47" s="238"/>
       <c r="C47" s="47" t="s">
         <v>114</v>
       </c>
@@ -19493,7 +19493,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="248"/>
-      <c r="B48" s="240"/>
+      <c r="B48" s="238"/>
       <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
@@ -20529,7 +20529,7 @@
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="248"/>
-      <c r="B49" s="240"/>
+      <c r="B49" s="238"/>
       <c r="C49" s="47" t="s">
         <v>122</v>
       </c>
@@ -21565,7 +21565,7 @@
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="248"/>
-      <c r="B50" s="240"/>
+      <c r="B50" s="238"/>
       <c r="C50" s="47" t="s">
         <v>126</v>
       </c>
@@ -22601,7 +22601,7 @@
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="248"/>
-      <c r="B51" s="240"/>
+      <c r="B51" s="238"/>
       <c r="C51" s="47" t="s">
         <v>130</v>
       </c>
@@ -23637,7 +23637,7 @@
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="249"/>
-      <c r="B52" s="241"/>
+      <c r="B52" s="239"/>
       <c r="C52" s="51" t="s">
         <v>134</v>
       </c>
@@ -24672,7 +24672,7 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="250" t="s">
+      <c r="A53" s="244" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="77"/>
@@ -24684,7 +24684,7 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="251"/>
+      <c r="A54" s="245"/>
       <c r="B54" s="80" t="s">
         <v>138</v>
       </c>
@@ -24704,8 +24704,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="251"/>
-      <c r="B55" s="254" t="s">
+      <c r="A55" s="245"/>
+      <c r="B55" s="240" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="84" t="s">
@@ -24726,8 +24726,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="251"/>
-      <c r="B56" s="254"/>
+      <c r="A56" s="245"/>
+      <c r="B56" s="240"/>
       <c r="C56" s="80" t="s">
         <v>94</v>
       </c>
@@ -24746,8 +24746,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="251"/>
-      <c r="B57" s="254"/>
+      <c r="A57" s="245"/>
+      <c r="B57" s="240"/>
       <c r="C57" s="80" t="s">
         <v>98</v>
       </c>
@@ -24766,8 +24766,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A58" s="251"/>
-      <c r="B58" s="254"/>
+      <c r="A58" s="245"/>
+      <c r="B58" s="240"/>
       <c r="C58" s="80" t="s">
         <v>102</v>
       </c>
@@ -24786,8 +24786,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="251"/>
-      <c r="B59" s="254"/>
+      <c r="A59" s="245"/>
+      <c r="B59" s="240"/>
       <c r="C59" s="80" t="s">
         <v>106</v>
       </c>
@@ -24806,8 +24806,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="251"/>
-      <c r="B60" s="254"/>
+      <c r="A60" s="245"/>
+      <c r="B60" s="240"/>
       <c r="C60" s="80" t="s">
         <v>110</v>
       </c>
@@ -24826,8 +24826,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="251"/>
-      <c r="B61" s="254"/>
+      <c r="A61" s="245"/>
+      <c r="B61" s="240"/>
       <c r="C61" s="80" t="s">
         <v>114</v>
       </c>
@@ -24846,8 +24846,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A62" s="251"/>
-      <c r="B62" s="254"/>
+      <c r="A62" s="245"/>
+      <c r="B62" s="240"/>
       <c r="C62" s="80" t="s">
         <v>118</v>
       </c>
@@ -24866,8 +24866,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A63" s="251"/>
-      <c r="B63" s="254"/>
+      <c r="A63" s="245"/>
+      <c r="B63" s="240"/>
       <c r="C63" s="80" t="s">
         <v>122</v>
       </c>
@@ -24886,8 +24886,8 @@
       <c r="H63" s="83"/>
     </row>
     <row r="64" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A64" s="251"/>
-      <c r="B64" s="254"/>
+      <c r="A64" s="245"/>
+      <c r="B64" s="240"/>
       <c r="C64" s="80" t="s">
         <v>126</v>
       </c>
@@ -24906,8 +24906,8 @@
       <c r="H64" s="83"/>
     </row>
     <row r="65" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="251"/>
-      <c r="B65" s="254"/>
+      <c r="A65" s="245"/>
+      <c r="B65" s="240"/>
       <c r="C65" s="80" t="s">
         <v>130</v>
       </c>
@@ -24926,8 +24926,8 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="252"/>
-      <c r="B66" s="255"/>
+      <c r="A66" s="246"/>
+      <c r="B66" s="241"/>
       <c r="C66" s="85" t="s">
         <v>134</v>
       </c>
@@ -24946,7 +24946,7 @@
       <c r="H66" s="87"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="253" t="s">
+      <c r="A67" s="247" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="59"/>
@@ -28046,7 +28046,7 @@
       <c r="AMJ69" s="13"/>
     </row>
     <row r="70" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="250" t="s">
+      <c r="A70" s="244" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="29"/>
@@ -28058,7 +28058,7 @@
       <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="251"/>
+      <c r="A71" s="245"/>
       <c r="B71" s="69" t="s">
         <v>155</v>
       </c>
@@ -28076,8 +28076,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="251"/>
-      <c r="B72" s="256" t="s">
+      <c r="A72" s="245"/>
+      <c r="B72" s="242" t="s">
         <v>158</v>
       </c>
       <c r="C72" s="69" t="s">
@@ -28098,8 +28098,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="251"/>
-      <c r="B73" s="256"/>
+      <c r="A73" s="245"/>
+      <c r="B73" s="242"/>
       <c r="C73" s="69" t="s">
         <v>30</v>
       </c>
@@ -28118,8 +28118,8 @@
       <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="251"/>
-      <c r="B74" s="256"/>
+      <c r="A74" s="245"/>
+      <c r="B74" s="242"/>
       <c r="C74" s="69" t="s">
         <v>12</v>
       </c>
@@ -28138,8 +28138,8 @@
       <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="251"/>
-      <c r="B75" s="256"/>
+      <c r="A75" s="245"/>
+      <c r="B75" s="242"/>
       <c r="C75" s="69" t="s">
         <v>167</v>
       </c>
@@ -28158,8 +28158,8 @@
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="252"/>
-      <c r="B76" s="257"/>
+      <c r="A76" s="246"/>
+      <c r="B76" s="243"/>
       <c r="C76" s="73" t="s">
         <v>25</v>
       </c>
@@ -28178,7 +28178,7 @@
       <c r="H76" s="76"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="253" t="s">
+      <c r="A77" s="247" t="s">
         <v>172</v>
       </c>
       <c r="B77" s="31"/>
@@ -30241,7 +30241,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="248"/>
-      <c r="B79" s="240" t="s">
+      <c r="B79" s="238" t="s">
         <v>176</v>
       </c>
       <c r="C79" s="47" t="s">
@@ -31279,7 +31279,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="248"/>
-      <c r="B80" s="240"/>
+      <c r="B80" s="238"/>
       <c r="C80" s="47" t="s">
         <v>179</v>
       </c>
@@ -32315,7 +32315,7 @@
     </row>
     <row r="81" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="248"/>
-      <c r="B81" s="240"/>
+      <c r="B81" s="238"/>
       <c r="C81" s="47" t="s">
         <v>182</v>
       </c>
@@ -33351,7 +33351,7 @@
     </row>
     <row r="82" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="248"/>
-      <c r="B82" s="240"/>
+      <c r="B82" s="238"/>
       <c r="C82" s="47" t="s">
         <v>185</v>
       </c>
@@ -34387,7 +34387,7 @@
     </row>
     <row r="83" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="249"/>
-      <c r="B83" s="241"/>
+      <c r="B83" s="239"/>
       <c r="C83" s="51" t="s">
         <v>25</v>
       </c>
@@ -35496,6 +35496,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B41:B52"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A21:A33"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A52"/>
     <mergeCell ref="B79:B83"/>
     <mergeCell ref="B55:B66"/>
     <mergeCell ref="B72:B76"/>
@@ -35503,13 +35510,6 @@
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="A70:A76"/>
     <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B41:B52"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A21:A33"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A39:A52"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -35549,16 +35549,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35587,7 +35587,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="252" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -35599,7 +35599,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="243"/>
+      <c r="A4" s="253"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -35619,7 +35619,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="243"/>
+      <c r="A5" s="253"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -35639,7 +35639,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="243"/>
+      <c r="A6" s="253"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -35659,7 +35659,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="243"/>
+      <c r="A7" s="253"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -35679,7 +35679,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="243"/>
+      <c r="A8" s="253"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -35699,7 +35699,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="243"/>
+      <c r="A9" s="253"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -35719,7 +35719,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="243"/>
+      <c r="A10" s="253"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -35739,7 +35739,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="244"/>
+      <c r="A11" s="254"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -35849,16 +35849,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35887,7 +35887,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="252" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -35937,7 +35937,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="243"/>
+      <c r="A4" s="253"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -35955,7 +35955,7 @@
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="243"/>
+      <c r="A5" s="253"/>
       <c r="B5" s="105" t="s">
         <v>209</v>
       </c>
@@ -35971,7 +35971,7 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="243"/>
+      <c r="A6" s="253"/>
       <c r="B6" s="105" t="s">
         <v>212</v>
       </c>
@@ -35987,7 +35987,7 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="243"/>
+      <c r="A7" s="253"/>
       <c r="B7" s="105" t="s">
         <v>213</v>
       </c>
@@ -36003,7 +36003,7 @@
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="243"/>
+      <c r="A8" s="253"/>
       <c r="B8" s="105" t="s">
         <v>214</v>
       </c>
@@ -36019,7 +36019,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="243"/>
+      <c r="A9" s="253"/>
       <c r="B9" s="105" t="s">
         <v>216</v>
       </c>
@@ -36037,7 +36037,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="243"/>
+      <c r="A10" s="253"/>
       <c r="B10" s="105" t="s">
         <v>218</v>
       </c>
@@ -36066,7 +36066,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="243"/>
+      <c r="A11" s="253"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -36082,7 +36082,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="243"/>
+      <c r="A12" s="253"/>
       <c r="B12" s="105" t="s">
         <v>222</v>
       </c>
@@ -36100,19 +36100,19 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="243"/>
+      <c r="A13" s="253"/>
       <c r="B13" s="105" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C13" s="106"/>
       <c r="D13" s="105" t="s">
         <v>224</v>
       </c>
       <c r="E13" s="106" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F13" s="105" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G13" s="194" t="s">
         <v>12</v>
@@ -36120,19 +36120,19 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="243"/>
+      <c r="A14" s="253"/>
       <c r="B14" s="105" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E14" s="106" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F14" s="105" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G14" s="194" t="s">
         <v>12</v>
@@ -36140,19 +36140,19 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="243"/>
+      <c r="A15" s="253"/>
       <c r="B15" s="105" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E15" s="106" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F15" s="105" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G15" s="194" t="s">
         <v>12</v>
@@ -36160,7 +36160,7 @@
       <c r="H15" s="107"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="244"/>
+      <c r="A16" s="254"/>
       <c r="B16" s="108" t="s">
         <v>225</v>
       </c>
@@ -36176,7 +36176,7 @@
       <c r="H16" s="110"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="244" t="s">
         <v>154</v>
       </c>
       <c r="B17" s="111"/>
@@ -36189,7 +36189,7 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="251"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="113" t="s">
         <v>228</v>
       </c>
@@ -36205,7 +36205,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="251"/>
+      <c r="A19" s="245"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>1</v>
@@ -36221,7 +36221,7 @@
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="251"/>
+      <c r="A20" s="245"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
         <v>209</v>
@@ -36237,7 +36237,7 @@
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="251"/>
+      <c r="A21" s="245"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
         <v>498</v>
@@ -36253,7 +36253,7 @@
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="251"/>
+      <c r="A22" s="245"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
         <v>499</v>
@@ -36269,7 +36269,7 @@
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="251"/>
+      <c r="A23" s="245"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
         <v>500</v>
@@ -36285,7 +36285,7 @@
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="251"/>
+      <c r="A24" s="245"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
         <v>501</v>
@@ -36301,7 +36301,7 @@
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="251"/>
+      <c r="A25" s="245"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
         <v>502</v>
@@ -36317,7 +36317,7 @@
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="251"/>
+      <c r="A26" s="245"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
         <v>503</v>
@@ -36333,7 +36333,7 @@
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="251"/>
+      <c r="A27" s="245"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
         <v>504</v>
@@ -36349,7 +36349,7 @@
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="251"/>
+      <c r="A28" s="245"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
         <v>505</v>
@@ -36365,7 +36365,7 @@
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="251"/>
+      <c r="A29" s="245"/>
       <c r="B29" s="113"/>
       <c r="C29" s="114" t="s">
         <v>506</v>
@@ -36381,7 +36381,7 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="251"/>
+      <c r="A30" s="245"/>
       <c r="B30" s="113" t="s">
         <v>230</v>
       </c>
@@ -36397,7 +36397,7 @@
       <c r="H30" s="115"/>
     </row>
     <row r="31" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="251"/>
+      <c r="A31" s="245"/>
       <c r="B31" s="222"/>
       <c r="C31" s="114" t="s">
         <v>1</v>
@@ -36413,7 +36413,7 @@
       <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="251"/>
+      <c r="A32" s="245"/>
       <c r="B32" s="222"/>
       <c r="C32" s="114" t="s">
         <v>209</v>
@@ -36429,7 +36429,7 @@
       <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="251"/>
+      <c r="A33" s="245"/>
       <c r="B33" s="222"/>
       <c r="C33" s="114" t="s">
         <v>498</v>
@@ -36445,7 +36445,7 @@
       <c r="H33" s="225"/>
     </row>
     <row r="34" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="251"/>
+      <c r="A34" s="245"/>
       <c r="B34" s="222"/>
       <c r="C34" s="114" t="s">
         <v>499</v>
@@ -36461,7 +36461,7 @@
       <c r="H34" s="225"/>
     </row>
     <row r="35" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="251"/>
+      <c r="A35" s="245"/>
       <c r="B35" s="222"/>
       <c r="C35" s="114" t="s">
         <v>500</v>
@@ -36477,7 +36477,7 @@
       <c r="H35" s="225"/>
     </row>
     <row r="36" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="251"/>
+      <c r="A36" s="245"/>
       <c r="B36" s="222"/>
       <c r="C36" s="114" t="s">
         <v>501</v>
@@ -36493,7 +36493,7 @@
       <c r="H36" s="225"/>
     </row>
     <row r="37" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="251"/>
+      <c r="A37" s="245"/>
       <c r="B37" s="222"/>
       <c r="C37" s="114" t="s">
         <v>502</v>
@@ -36509,7 +36509,7 @@
       <c r="H37" s="225"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="251"/>
+      <c r="A38" s="245"/>
       <c r="B38" s="222"/>
       <c r="C38" s="114" t="s">
         <v>503</v>
@@ -36525,7 +36525,7 @@
       <c r="H38" s="225"/>
     </row>
     <row r="39" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="251"/>
+      <c r="A39" s="245"/>
       <c r="B39" s="222"/>
       <c r="C39" s="114" t="s">
         <v>504</v>
@@ -36541,7 +36541,7 @@
       <c r="H39" s="225"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="251"/>
+      <c r="A40" s="245"/>
       <c r="B40" s="222"/>
       <c r="C40" s="114" t="s">
         <v>505</v>
@@ -36557,7 +36557,7 @@
       <c r="H40" s="225"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="251"/>
+      <c r="A41" s="245"/>
       <c r="B41" s="222"/>
       <c r="C41" s="114" t="s">
         <v>506</v>
@@ -36573,7 +36573,7 @@
       <c r="H41" s="225"/>
     </row>
     <row r="42" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="252"/>
+      <c r="A42" s="246"/>
       <c r="B42" s="116" t="s">
         <v>232</v>
       </c>
@@ -36591,7 +36591,7 @@
       <c r="H42" s="118"/>
     </row>
     <row r="43" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="253" t="s">
+      <c r="A43" s="247" t="s">
         <v>233</v>
       </c>
       <c r="B43" s="119"/>
@@ -36678,7 +36678,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="250" t="s">
+      <c r="A45" s="244" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="111"/>
@@ -36691,7 +36691,7 @@
       <c r="AMJ45" s="5"/>
     </row>
     <row r="46" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="251"/>
+      <c r="A46" s="245"/>
       <c r="B46" s="113" t="s">
         <v>73</v>
       </c>
@@ -36709,7 +36709,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="251"/>
+      <c r="A47" s="245"/>
       <c r="B47" s="113" t="s">
         <v>76</v>
       </c>
@@ -36727,7 +36727,7 @@
       <c r="H47" s="115"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="252"/>
+      <c r="A48" s="246"/>
       <c r="B48" s="116" t="s">
         <v>79</v>
       </c>
@@ -36745,7 +36745,7 @@
       <c r="H48" s="118"/>
     </row>
     <row r="49" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="253" t="s">
+      <c r="A49" s="247" t="s">
         <v>240</v>
       </c>
       <c r="B49" s="121"/>
@@ -36958,7 +36958,7 @@
       <c r="H58" s="110"/>
     </row>
     <row r="59" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="250" t="s">
+      <c r="A59" s="244" t="s">
         <v>479</v>
       </c>
       <c r="B59" s="123"/>
@@ -36971,7 +36971,7 @@
       <c r="AMJ59" s="5"/>
     </row>
     <row r="60" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="252"/>
+      <c r="A60" s="246"/>
       <c r="B60" s="116" t="s">
         <v>5</v>
       </c>
@@ -37011,7 +37011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
@@ -37033,16 +37033,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>469</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -45552,7 +45552,7 @@
     <row r="21" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="261"/>
       <c r="B21" s="105" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="105" t="s">
@@ -45562,7 +45562,7 @@
         <v>461</v>
       </c>
       <c r="F21" s="105" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G21" s="194" t="s">
         <v>321</v>
@@ -45582,7 +45582,7 @@
         <v>463</v>
       </c>
       <c r="F22" s="105" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G22" s="194" t="s">
         <v>322</v>
@@ -45673,7 +45673,7 @@
         <v>456</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="G27" s="194" t="s">
         <v>43</v>
@@ -45881,16 +45881,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -45919,7 +45919,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="253" t="s">
+      <c r="A3" s="247" t="s">
         <v>483</v>
       </c>
       <c r="B3" s="18"/>
@@ -46269,16 +46269,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>471</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -46632,11 +46632,11 @@
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="105" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E15" s="136"/>
       <c r="F15" s="106" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G15" s="194"/>
       <c r="H15" s="145"/>
@@ -46657,11 +46657,11 @@
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="105" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E16" s="136"/>
       <c r="F16" s="106" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G16" s="194"/>
       <c r="H16" s="145"/>
@@ -46769,16 +46769,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
-        <v>567</v>
-      </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="A1" s="250" t="s">
+        <v>566</v>
+      </c>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:20" s="152" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -46808,7 +46808,7 @@
     </row>
     <row r="3" spans="1:20" s="152" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="230" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B3" s="227"/>
       <c r="C3" s="227"/>
@@ -46819,7 +46819,7 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="253" t="s">
+      <c r="A4" s="247" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="153"/>
@@ -46915,7 +46915,7 @@
       <c r="H8" s="160"/>
     </row>
     <row r="9" spans="1:20" s="155" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="250" t="s">
+      <c r="A9" s="244" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="161"/>
@@ -46927,7 +46927,7 @@
       <c r="H9" s="162"/>
     </row>
     <row r="10" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="251"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="163" t="s">
         <v>30</v>
       </c>
@@ -46945,7 +46945,7 @@
       <c r="H10" s="164"/>
     </row>
     <row r="11" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="251"/>
+      <c r="A11" s="245"/>
       <c r="B11" s="163" t="s">
         <v>366</v>
       </c>
@@ -46961,7 +46961,7 @@
       <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="251"/>
+      <c r="A12" s="245"/>
       <c r="B12" s="163"/>
       <c r="C12" s="163" t="s">
         <v>368</v>
@@ -46977,7 +46977,7 @@
       <c r="H12" s="164"/>
     </row>
     <row r="13" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="251"/>
+      <c r="A13" s="245"/>
       <c r="B13" s="163"/>
       <c r="C13" s="163" t="s">
         <v>369</v>
@@ -46993,7 +46993,7 @@
       <c r="H13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="251"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="163"/>
       <c r="C14" s="163" t="s">
         <v>370</v>
@@ -47009,7 +47009,7 @@
       <c r="H14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="251"/>
+      <c r="A15" s="245"/>
       <c r="B15" s="163"/>
       <c r="C15" s="163" t="s">
         <v>371</v>
@@ -47025,7 +47025,7 @@
       <c r="H15" s="164"/>
     </row>
     <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="251"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="163"/>
       <c r="C16" s="163" t="s">
         <v>373</v>
@@ -47041,7 +47041,7 @@
       <c r="H16" s="164"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="251"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="163"/>
       <c r="C17" s="163" t="s">
         <v>552</v>
@@ -47059,7 +47059,7 @@
       <c r="H17" s="164"/>
     </row>
     <row r="18" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="251"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="163" t="s">
         <v>375</v>
       </c>
@@ -47075,7 +47075,7 @@
       <c r="H18" s="164"/>
     </row>
     <row r="19" spans="1:8" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="252"/>
+      <c r="A19" s="246"/>
       <c r="B19" s="165"/>
       <c r="C19" s="165" t="s">
         <v>373</v>
@@ -47119,7 +47119,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -47138,7 +47138,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="269" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B1" s="269"/>
       <c r="C1" s="269"/>
@@ -47146,7 +47146,7 @@
       <c r="E1" s="269"/>
       <c r="F1" s="269"/>
       <c r="G1" s="269"/>
-      <c r="H1" s="239"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:20" s="232" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -47176,7 +47176,7 @@
     </row>
     <row r="3" spans="1:20" s="152" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="230" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B3" s="227"/>
       <c r="C3" s="227"/>
@@ -47187,7 +47187,7 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="236" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="253" t="s">
+      <c r="A4" s="247" t="s">
         <v>555</v>
       </c>
       <c r="B4" s="153"/>
@@ -47213,17 +47213,17 @@
     <row r="5" spans="1:20" s="151" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="248"/>
       <c r="B5" s="105" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C5" s="157"/>
       <c r="D5" s="157" t="s">
-        <v>556</v>
+        <v>580</v>
       </c>
       <c r="E5" s="157" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="F5" s="157" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G5" s="180" t="s">
         <v>12</v>
@@ -47234,16 +47234,16 @@
       <c r="A6" s="248"/>
       <c r="B6" s="157"/>
       <c r="C6" s="157" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D6" s="157" t="s">
         <v>207</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F6" s="157" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="G6" s="180" t="s">
         <v>12</v>
@@ -47314,16 +47314,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="250" t="s">
         <v>472</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="239"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -48368,7 +48368,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="253" t="s">
+      <c r="A3" s="247" t="s">
         <v>377</v>
       </c>
       <c r="B3" s="169"/>
@@ -57668,7 +57668,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="250" t="s">
+      <c r="A13" s="244" t="s">
         <v>392</v>
       </c>
       <c r="B13" s="172"/>
@@ -57681,7 +57681,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="251"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="69" t="s">
         <v>206</v>
       </c>
@@ -57697,7 +57697,7 @@
       <c r="H14" s="174"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="251"/>
+      <c r="A15" s="245"/>
       <c r="B15" s="69" t="s">
         <v>256</v>
       </c>
@@ -57713,7 +57713,7 @@
       <c r="H15" s="174"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="251"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="69" t="s">
         <v>212</v>
       </c>
@@ -57729,7 +57729,7 @@
       <c r="H16" s="174"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="251"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="69" t="s">
         <v>262</v>
       </c>
@@ -57745,7 +57745,7 @@
       <c r="H17" s="174"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="251"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="69" t="s">
         <v>209</v>
       </c>
@@ -57761,7 +57761,7 @@
       <c r="H18" s="174"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="251"/>
+      <c r="A19" s="245"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -57777,7 +57777,7 @@
       <c r="H19" s="174"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="251"/>
+      <c r="A20" s="245"/>
       <c r="B20" s="69" t="s">
         <v>398</v>
       </c>
@@ -57793,7 +57793,7 @@
       <c r="H20" s="174"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="251"/>
+      <c r="A21" s="245"/>
       <c r="B21" s="69" t="s">
         <v>310</v>
       </c>
@@ -57809,7 +57809,7 @@
       <c r="H21" s="174"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="251"/>
+      <c r="A22" s="245"/>
       <c r="B22" s="69" t="s">
         <v>401</v>
       </c>
@@ -57825,7 +57825,7 @@
       <c r="H22" s="174"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="251"/>
+      <c r="A23" s="245"/>
       <c r="B23" s="69" t="s">
         <v>403</v>
       </c>
@@ -57841,7 +57841,7 @@
       <c r="H23" s="174"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="252"/>
+      <c r="A24" s="246"/>
       <c r="B24" s="73" t="s">
         <v>405</v>
       </c>
@@ -57857,7 +57857,7 @@
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="253" t="s">
+      <c r="A25" s="247" t="s">
         <v>343</v>
       </c>
       <c r="B25" s="176"/>
@@ -58045,7 +58045,7 @@
       <c r="H36" s="178"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="250" t="s">
+      <c r="A37" s="244" t="s">
         <v>278</v>
       </c>
       <c r="B37" s="172"/>
@@ -58058,7 +58058,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="251"/>
+      <c r="A38" s="245"/>
       <c r="B38" s="69" t="s">
         <v>206</v>
       </c>
@@ -58074,7 +58074,7 @@
       <c r="H38" s="174"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="251"/>
+      <c r="A39" s="245"/>
       <c r="B39" s="69" t="s">
         <v>256</v>
       </c>
@@ -58090,7 +58090,7 @@
       <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="251"/>
+      <c r="A40" s="245"/>
       <c r="B40" s="69" t="s">
         <v>212</v>
       </c>
@@ -58106,7 +58106,7 @@
       <c r="H40" s="174"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="251"/>
+      <c r="A41" s="245"/>
       <c r="B41" s="69" t="s">
         <v>262</v>
       </c>
@@ -58122,7 +58122,7 @@
       <c r="H41" s="174"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="251"/>
+      <c r="A42" s="245"/>
       <c r="B42" s="69" t="s">
         <v>424</v>
       </c>
@@ -58138,7 +58138,7 @@
       <c r="H42" s="174"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="251"/>
+      <c r="A43" s="245"/>
       <c r="B43" s="69" t="s">
         <v>343</v>
       </c>
@@ -58154,7 +58154,7 @@
       <c r="H43" s="174"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="251"/>
+      <c r="A44" s="245"/>
       <c r="B44" s="69" t="s">
         <v>209</v>
       </c>
@@ -58170,7 +58170,7 @@
       <c r="H44" s="174"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="251"/>
+      <c r="A45" s="245"/>
       <c r="B45" s="69" t="s">
         <v>388</v>
       </c>
@@ -58186,7 +58186,7 @@
       <c r="H45" s="174"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="251"/>
+      <c r="A46" s="245"/>
       <c r="B46" s="69" t="s">
         <v>429</v>
       </c>
@@ -58202,7 +58202,7 @@
       <c r="H46" s="174"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="251"/>
+      <c r="A47" s="245"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -58218,7 +58218,7 @@
       <c r="H47" s="174"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="252"/>
+      <c r="A48" s="246"/>
       <c r="B48" s="73" t="s">
         <v>401</v>
       </c>

</xml_diff>

<commit_message>
feat(dma): add more heading links
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/digitbrain.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBD35E8-199E-8B48-A1C0-7CF8E93CBD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C892EE-F40C-5444-A5DC-5087BBFEEB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="584">
   <si>
     <t>Concept</t>
   </si>
@@ -1875,6 +1875,9 @@
   <si>
     <t>Nested below each Microservice, these key(s) are the String identifier(s) of the Data Source(s) of each Microservice. &lt;br&gt; The value for each key is the UUID of the Data Asset that corresponds to it.</t>
   </si>
+  <si>
+    <t>Data Assets Mapping</t>
+  </si>
 </sst>
 </file>
 
@@ -2088,7 +2091,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2421,13 +2424,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3329,60 +3345,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3407,6 +3383,46 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3455,6 +3471,38 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4368,16 +4416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4406,7 +4454,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4418,7 +4466,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -4438,7 +4486,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -4458,7 +4506,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -4478,7 +4526,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="47" t="s">
         <v>19</v>
       </c>
@@ -4498,7 +4546,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="47" t="s">
         <v>22</v>
       </c>
@@ -4518,7 +4566,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="47" t="s">
         <v>25</v>
       </c>
@@ -4538,7 +4586,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="47" t="s">
         <v>26</v>
       </c>
@@ -4558,7 +4606,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="51" t="s">
         <v>30</v>
       </c>
@@ -4578,7 +4626,7 @@
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="255" t="s">
+      <c r="A12" s="245" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="213"/>
@@ -4590,7 +4638,7 @@
       <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="256"/>
+      <c r="A13" s="246"/>
       <c r="B13" s="55" t="s">
         <v>35</v>
       </c>
@@ -4610,7 +4658,7 @@
       <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="256"/>
+      <c r="A14" s="246"/>
       <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
@@ -4630,7 +4678,7 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="256"/>
+      <c r="A15" s="246"/>
       <c r="B15" s="55" t="s">
         <v>440</v>
       </c>
@@ -5666,7 +5714,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="256"/>
+      <c r="A16" s="246"/>
       <c r="B16" s="55"/>
       <c r="C16" s="56" t="s">
         <v>540</v>
@@ -6702,7 +6750,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="256"/>
+      <c r="A17" s="246"/>
       <c r="B17" s="55"/>
       <c r="C17" s="56" t="s">
         <v>542</v>
@@ -7738,7 +7786,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="256"/>
+      <c r="A18" s="246"/>
       <c r="B18" s="55"/>
       <c r="C18" s="56" t="s">
         <v>541</v>
@@ -8774,7 +8822,7 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="256"/>
+      <c r="A19" s="246"/>
       <c r="B19" s="55" t="s">
         <v>437</v>
       </c>
@@ -9810,7 +9858,7 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="257"/>
+      <c r="A20" s="247"/>
       <c r="B20" s="217" t="s">
         <v>438</v>
       </c>
@@ -11098,7 +11146,7 @@
       <c r="H33" s="54"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="244" t="s">
+      <c r="A34" s="250" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="62"/>
@@ -11110,7 +11158,7 @@
       <c r="H34" s="64"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="245"/>
+      <c r="A35" s="251"/>
       <c r="B35" s="65" t="s">
         <v>73</v>
       </c>
@@ -11130,7 +11178,7 @@
       <c r="H35" s="68"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="245"/>
+      <c r="A36" s="251"/>
       <c r="B36" s="69" t="s">
         <v>76</v>
       </c>
@@ -11150,7 +11198,7 @@
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="245"/>
+      <c r="A37" s="251"/>
       <c r="B37" s="69" t="s">
         <v>79</v>
       </c>
@@ -11170,7 +11218,7 @@
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="246"/>
+      <c r="A38" s="252"/>
       <c r="B38" s="73" t="s">
         <v>82</v>
       </c>
@@ -11190,7 +11238,7 @@
       <c r="H38" s="76"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="247" t="s">
+      <c r="A39" s="253" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="59"/>
@@ -12239,7 +12287,7 @@
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="248"/>
-      <c r="B41" s="238" t="s">
+      <c r="B41" s="240" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -13277,7 +13325,7 @@
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="248"/>
-      <c r="B42" s="238"/>
+      <c r="B42" s="240"/>
       <c r="C42" s="47" t="s">
         <v>94</v>
       </c>
@@ -14313,7 +14361,7 @@
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="248"/>
-      <c r="B43" s="238"/>
+      <c r="B43" s="240"/>
       <c r="C43" s="47" t="s">
         <v>98</v>
       </c>
@@ -15349,7 +15397,7 @@
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A44" s="248"/>
-      <c r="B44" s="238"/>
+      <c r="B44" s="240"/>
       <c r="C44" s="47" t="s">
         <v>102</v>
       </c>
@@ -16385,7 +16433,7 @@
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="248"/>
-      <c r="B45" s="238"/>
+      <c r="B45" s="240"/>
       <c r="C45" s="47" t="s">
         <v>106</v>
       </c>
@@ -17421,7 +17469,7 @@
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="248"/>
-      <c r="B46" s="238"/>
+      <c r="B46" s="240"/>
       <c r="C46" s="47" t="s">
         <v>110</v>
       </c>
@@ -18457,7 +18505,7 @@
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="248"/>
-      <c r="B47" s="238"/>
+      <c r="B47" s="240"/>
       <c r="C47" s="47" t="s">
         <v>114</v>
       </c>
@@ -19493,7 +19541,7 @@
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="248"/>
-      <c r="B48" s="238"/>
+      <c r="B48" s="240"/>
       <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
@@ -20529,7 +20577,7 @@
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="248"/>
-      <c r="B49" s="238"/>
+      <c r="B49" s="240"/>
       <c r="C49" s="47" t="s">
         <v>122</v>
       </c>
@@ -21565,7 +21613,7 @@
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="248"/>
-      <c r="B50" s="238"/>
+      <c r="B50" s="240"/>
       <c r="C50" s="47" t="s">
         <v>126</v>
       </c>
@@ -22601,7 +22649,7 @@
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="248"/>
-      <c r="B51" s="238"/>
+      <c r="B51" s="240"/>
       <c r="C51" s="47" t="s">
         <v>130</v>
       </c>
@@ -23637,7 +23685,7 @@
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="249"/>
-      <c r="B52" s="239"/>
+      <c r="B52" s="241"/>
       <c r="C52" s="51" t="s">
         <v>134</v>
       </c>
@@ -24672,7 +24720,7 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="244" t="s">
+      <c r="A53" s="250" t="s">
         <v>137</v>
       </c>
       <c r="B53" s="77"/>
@@ -24684,7 +24732,7 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="245"/>
+      <c r="A54" s="251"/>
       <c r="B54" s="80" t="s">
         <v>138</v>
       </c>
@@ -24704,8 +24752,8 @@
       <c r="H54" s="83"/>
     </row>
     <row r="55" spans="1:1024" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="245"/>
-      <c r="B55" s="240" t="s">
+      <c r="A55" s="251"/>
+      <c r="B55" s="254" t="s">
         <v>90</v>
       </c>
       <c r="C55" s="84" t="s">
@@ -24726,8 +24774,8 @@
       <c r="H55" s="83"/>
     </row>
     <row r="56" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="245"/>
-      <c r="B56" s="240"/>
+      <c r="A56" s="251"/>
+      <c r="B56" s="254"/>
       <c r="C56" s="80" t="s">
         <v>94</v>
       </c>
@@ -24746,8 +24794,8 @@
       <c r="H56" s="83"/>
     </row>
     <row r="57" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="245"/>
-      <c r="B57" s="240"/>
+      <c r="A57" s="251"/>
+      <c r="B57" s="254"/>
       <c r="C57" s="80" t="s">
         <v>98</v>
       </c>
@@ -24766,8 +24814,8 @@
       <c r="H57" s="83"/>
     </row>
     <row r="58" spans="1:1024" ht="85" x14ac:dyDescent="0.2">
-      <c r="A58" s="245"/>
-      <c r="B58" s="240"/>
+      <c r="A58" s="251"/>
+      <c r="B58" s="254"/>
       <c r="C58" s="80" t="s">
         <v>102</v>
       </c>
@@ -24786,8 +24834,8 @@
       <c r="H58" s="83"/>
     </row>
     <row r="59" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="245"/>
-      <c r="B59" s="240"/>
+      <c r="A59" s="251"/>
+      <c r="B59" s="254"/>
       <c r="C59" s="80" t="s">
         <v>106</v>
       </c>
@@ -24806,8 +24854,8 @@
       <c r="H59" s="83"/>
     </row>
     <row r="60" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="245"/>
-      <c r="B60" s="240"/>
+      <c r="A60" s="251"/>
+      <c r="B60" s="254"/>
       <c r="C60" s="80" t="s">
         <v>110</v>
       </c>
@@ -24826,8 +24874,8 @@
       <c r="H60" s="83"/>
     </row>
     <row r="61" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="245"/>
-      <c r="B61" s="240"/>
+      <c r="A61" s="251"/>
+      <c r="B61" s="254"/>
       <c r="C61" s="80" t="s">
         <v>114</v>
       </c>
@@ -24846,8 +24894,8 @@
       <c r="H61" s="83"/>
     </row>
     <row r="62" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A62" s="245"/>
-      <c r="B62" s="240"/>
+      <c r="A62" s="251"/>
+      <c r="B62" s="254"/>
       <c r="C62" s="80" t="s">
         <v>118</v>
       </c>
@@ -24866,8 +24914,8 @@
       <c r="H62" s="83"/>
     </row>
     <row r="63" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A63" s="245"/>
-      <c r="B63" s="240"/>
+      <c r="A63" s="251"/>
+      <c r="B63" s="254"/>
       <c r="C63" s="80" t="s">
         <v>122</v>
       </c>
@@ -24886,8 +24934,8 @@
       <c r="H63" s="83"/>
     </row>
     <row r="64" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A64" s="245"/>
-      <c r="B64" s="240"/>
+      <c r="A64" s="251"/>
+      <c r="B64" s="254"/>
       <c r="C64" s="80" t="s">
         <v>126</v>
       </c>
@@ -24906,8 +24954,8 @@
       <c r="H64" s="83"/>
     </row>
     <row r="65" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="245"/>
-      <c r="B65" s="240"/>
+      <c r="A65" s="251"/>
+      <c r="B65" s="254"/>
       <c r="C65" s="80" t="s">
         <v>130</v>
       </c>
@@ -24926,8 +24974,8 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:1024" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="246"/>
-      <c r="B66" s="241"/>
+      <c r="A66" s="252"/>
+      <c r="B66" s="255"/>
       <c r="C66" s="85" t="s">
         <v>134</v>
       </c>
@@ -24946,7 +24994,7 @@
       <c r="H66" s="87"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="247" t="s">
+      <c r="A67" s="253" t="s">
         <v>145</v>
       </c>
       <c r="B67" s="59"/>
@@ -28046,7 +28094,7 @@
       <c r="AMJ69" s="13"/>
     </row>
     <row r="70" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="244" t="s">
+      <c r="A70" s="250" t="s">
         <v>154</v>
       </c>
       <c r="B70" s="29"/>
@@ -28058,7 +28106,7 @@
       <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="245"/>
+      <c r="A71" s="251"/>
       <c r="B71" s="69" t="s">
         <v>155</v>
       </c>
@@ -28076,8 +28124,8 @@
       <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="245"/>
-      <c r="B72" s="242" t="s">
+      <c r="A72" s="251"/>
+      <c r="B72" s="256" t="s">
         <v>158</v>
       </c>
       <c r="C72" s="69" t="s">
@@ -28098,8 +28146,8 @@
       <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="245"/>
-      <c r="B73" s="242"/>
+      <c r="A73" s="251"/>
+      <c r="B73" s="256"/>
       <c r="C73" s="69" t="s">
         <v>30</v>
       </c>
@@ -28118,8 +28166,8 @@
       <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="245"/>
-      <c r="B74" s="242"/>
+      <c r="A74" s="251"/>
+      <c r="B74" s="256"/>
       <c r="C74" s="69" t="s">
         <v>12</v>
       </c>
@@ -28138,8 +28186,8 @@
       <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="245"/>
-      <c r="B75" s="242"/>
+      <c r="A75" s="251"/>
+      <c r="B75" s="256"/>
       <c r="C75" s="69" t="s">
         <v>167</v>
       </c>
@@ -28158,8 +28206,8 @@
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:1024" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="246"/>
-      <c r="B76" s="243"/>
+      <c r="A76" s="252"/>
+      <c r="B76" s="257"/>
       <c r="C76" s="73" t="s">
         <v>25</v>
       </c>
@@ -28178,7 +28226,7 @@
       <c r="H76" s="76"/>
     </row>
     <row r="77" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="247" t="s">
+      <c r="A77" s="253" t="s">
         <v>172</v>
       </c>
       <c r="B77" s="31"/>
@@ -30241,7 +30289,7 @@
     </row>
     <row r="79" spans="1:1024" s="14" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="248"/>
-      <c r="B79" s="238" t="s">
+      <c r="B79" s="240" t="s">
         <v>176</v>
       </c>
       <c r="C79" s="47" t="s">
@@ -31279,7 +31327,7 @@
     </row>
     <row r="80" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="248"/>
-      <c r="B80" s="238"/>
+      <c r="B80" s="240"/>
       <c r="C80" s="47" t="s">
         <v>179</v>
       </c>
@@ -32315,7 +32363,7 @@
     </row>
     <row r="81" spans="1:1024" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="248"/>
-      <c r="B81" s="238"/>
+      <c r="B81" s="240"/>
       <c r="C81" s="47" t="s">
         <v>182</v>
       </c>
@@ -33351,7 +33399,7 @@
     </row>
     <row r="82" spans="1:1024" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="248"/>
-      <c r="B82" s="238"/>
+      <c r="B82" s="240"/>
       <c r="C82" s="47" t="s">
         <v>185</v>
       </c>
@@ -34387,7 +34435,7 @@
     </row>
     <row r="83" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="249"/>
-      <c r="B83" s="239"/>
+      <c r="B83" s="241"/>
       <c r="C83" s="51" t="s">
         <v>25</v>
       </c>
@@ -35496,6 +35544,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="14">
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B55:B66"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A77:A83"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B41:B52"/>
     <mergeCell ref="A3:A11"/>
@@ -35503,13 +35558,6 @@
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A52"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B55:B66"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A70:A76"/>
-    <mergeCell ref="A77:A83"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -35549,16 +35597,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35587,7 +35635,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -35599,7 +35647,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
@@ -35619,7 +35667,7 @@
       <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
@@ -35639,7 +35687,7 @@
       <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="47" t="s">
         <v>25</v>
       </c>
@@ -35659,7 +35707,7 @@
       <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="47" t="s">
         <v>26</v>
       </c>
@@ -35679,7 +35727,7 @@
       <c r="H7" s="50"/>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -35699,7 +35747,7 @@
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
@@ -35719,7 +35767,7 @@
       <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="47" t="s">
         <v>19</v>
       </c>
@@ -35739,7 +35787,7 @@
       <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="51" t="s">
         <v>22</v>
       </c>
@@ -35849,16 +35897,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="36" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -35887,7 +35935,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="242" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="37"/>
@@ -35937,7 +35985,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="253"/>
+      <c r="A4" s="243"/>
       <c r="B4" s="105" t="s">
         <v>206</v>
       </c>
@@ -35955,7 +36003,7 @@
       <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="253"/>
+      <c r="A5" s="243"/>
       <c r="B5" s="105" t="s">
         <v>209</v>
       </c>
@@ -35971,7 +36019,7 @@
       <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:1024" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="253"/>
+      <c r="A6" s="243"/>
       <c r="B6" s="105" t="s">
         <v>212</v>
       </c>
@@ -35987,7 +36035,7 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="253"/>
+      <c r="A7" s="243"/>
       <c r="B7" s="105" t="s">
         <v>213</v>
       </c>
@@ -36003,7 +36051,7 @@
       <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="253"/>
+      <c r="A8" s="243"/>
       <c r="B8" s="105" t="s">
         <v>214</v>
       </c>
@@ -36019,7 +36067,7 @@
       <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="253"/>
+      <c r="A9" s="243"/>
       <c r="B9" s="105" t="s">
         <v>216</v>
       </c>
@@ -36037,7 +36085,7 @@
       <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="253"/>
+      <c r="A10" s="243"/>
       <c r="B10" s="105" t="s">
         <v>218</v>
       </c>
@@ -36066,7 +36114,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="253"/>
+      <c r="A11" s="243"/>
       <c r="B11" s="105" t="s">
         <v>3</v>
       </c>
@@ -36082,7 +36130,7 @@
       <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="253"/>
+      <c r="A12" s="243"/>
       <c r="B12" s="105" t="s">
         <v>222</v>
       </c>
@@ -36100,7 +36148,7 @@
       <c r="H12" s="107"/>
     </row>
     <row r="13" spans="1:1024" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="253"/>
+      <c r="A13" s="243"/>
       <c r="B13" s="105" t="s">
         <v>559</v>
       </c>
@@ -36120,7 +36168,7 @@
       <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="253"/>
+      <c r="A14" s="243"/>
       <c r="B14" s="105" t="s">
         <v>557</v>
       </c>
@@ -36140,7 +36188,7 @@
       <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="253"/>
+      <c r="A15" s="243"/>
       <c r="B15" s="105" t="s">
         <v>558</v>
       </c>
@@ -36160,7 +36208,7 @@
       <c r="H15" s="107"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="254"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="108" t="s">
         <v>225</v>
       </c>
@@ -36176,7 +36224,7 @@
       <c r="H16" s="110"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="244" t="s">
+      <c r="A17" s="250" t="s">
         <v>154</v>
       </c>
       <c r="B17" s="111"/>
@@ -36189,7 +36237,7 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="113" t="s">
         <v>228</v>
       </c>
@@ -36205,7 +36253,7 @@
       <c r="H18" s="115"/>
     </row>
     <row r="19" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="245"/>
+      <c r="A19" s="251"/>
       <c r="B19" s="113"/>
       <c r="C19" s="114" t="s">
         <v>1</v>
@@ -36221,7 +36269,7 @@
       <c r="H19" s="115"/>
     </row>
     <row r="20" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="245"/>
+      <c r="A20" s="251"/>
       <c r="B20" s="113"/>
       <c r="C20" s="114" t="s">
         <v>209</v>
@@ -36237,7 +36285,7 @@
       <c r="H20" s="115"/>
     </row>
     <row r="21" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="245"/>
+      <c r="A21" s="251"/>
       <c r="B21" s="113"/>
       <c r="C21" s="114" t="s">
         <v>498</v>
@@ -36253,7 +36301,7 @@
       <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="245"/>
+      <c r="A22" s="251"/>
       <c r="B22" s="113"/>
       <c r="C22" s="114" t="s">
         <v>499</v>
@@ -36269,7 +36317,7 @@
       <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="245"/>
+      <c r="A23" s="251"/>
       <c r="B23" s="113"/>
       <c r="C23" s="114" t="s">
         <v>500</v>
@@ -36285,7 +36333,7 @@
       <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="245"/>
+      <c r="A24" s="251"/>
       <c r="B24" s="113"/>
       <c r="C24" s="114" t="s">
         <v>501</v>
@@ -36301,7 +36349,7 @@
       <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="245"/>
+      <c r="A25" s="251"/>
       <c r="B25" s="113"/>
       <c r="C25" s="114" t="s">
         <v>502</v>
@@ -36317,7 +36365,7 @@
       <c r="H25" s="115"/>
     </row>
     <row r="26" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="245"/>
+      <c r="A26" s="251"/>
       <c r="B26" s="113"/>
       <c r="C26" s="114" t="s">
         <v>503</v>
@@ -36333,7 +36381,7 @@
       <c r="H26" s="115"/>
     </row>
     <row r="27" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="245"/>
+      <c r="A27" s="251"/>
       <c r="B27" s="113"/>
       <c r="C27" s="114" t="s">
         <v>504</v>
@@ -36349,7 +36397,7 @@
       <c r="H27" s="115"/>
     </row>
     <row r="28" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="245"/>
+      <c r="A28" s="251"/>
       <c r="B28" s="113"/>
       <c r="C28" s="114" t="s">
         <v>505</v>
@@ -36365,7 +36413,7 @@
       <c r="H28" s="115"/>
     </row>
     <row r="29" spans="1:1024" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="245"/>
+      <c r="A29" s="251"/>
       <c r="B29" s="113"/>
       <c r="C29" s="114" t="s">
         <v>506</v>
@@ -36381,7 +36429,7 @@
       <c r="H29" s="115"/>
     </row>
     <row r="30" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="245"/>
+      <c r="A30" s="251"/>
       <c r="B30" s="113" t="s">
         <v>230</v>
       </c>
@@ -36397,7 +36445,7 @@
       <c r="H30" s="115"/>
     </row>
     <row r="31" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="245"/>
+      <c r="A31" s="251"/>
       <c r="B31" s="222"/>
       <c r="C31" s="114" t="s">
         <v>1</v>
@@ -36413,7 +36461,7 @@
       <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="245"/>
+      <c r="A32" s="251"/>
       <c r="B32" s="222"/>
       <c r="C32" s="114" t="s">
         <v>209</v>
@@ -36429,7 +36477,7 @@
       <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="245"/>
+      <c r="A33" s="251"/>
       <c r="B33" s="222"/>
       <c r="C33" s="114" t="s">
         <v>498</v>
@@ -36445,7 +36493,7 @@
       <c r="H33" s="225"/>
     </row>
     <row r="34" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="245"/>
+      <c r="A34" s="251"/>
       <c r="B34" s="222"/>
       <c r="C34" s="114" t="s">
         <v>499</v>
@@ -36461,7 +36509,7 @@
       <c r="H34" s="225"/>
     </row>
     <row r="35" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="245"/>
+      <c r="A35" s="251"/>
       <c r="B35" s="222"/>
       <c r="C35" s="114" t="s">
         <v>500</v>
@@ -36477,7 +36525,7 @@
       <c r="H35" s="225"/>
     </row>
     <row r="36" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="245"/>
+      <c r="A36" s="251"/>
       <c r="B36" s="222"/>
       <c r="C36" s="114" t="s">
         <v>501</v>
@@ -36493,7 +36541,7 @@
       <c r="H36" s="225"/>
     </row>
     <row r="37" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="245"/>
+      <c r="A37" s="251"/>
       <c r="B37" s="222"/>
       <c r="C37" s="114" t="s">
         <v>502</v>
@@ -36509,7 +36557,7 @@
       <c r="H37" s="225"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="245"/>
+      <c r="A38" s="251"/>
       <c r="B38" s="222"/>
       <c r="C38" s="114" t="s">
         <v>503</v>
@@ -36525,7 +36573,7 @@
       <c r="H38" s="225"/>
     </row>
     <row r="39" spans="1:1024" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="245"/>
+      <c r="A39" s="251"/>
       <c r="B39" s="222"/>
       <c r="C39" s="114" t="s">
         <v>504</v>
@@ -36541,7 +36589,7 @@
       <c r="H39" s="225"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="245"/>
+      <c r="A40" s="251"/>
       <c r="B40" s="222"/>
       <c r="C40" s="114" t="s">
         <v>505</v>
@@ -36557,7 +36605,7 @@
       <c r="H40" s="225"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="245"/>
+      <c r="A41" s="251"/>
       <c r="B41" s="222"/>
       <c r="C41" s="114" t="s">
         <v>506</v>
@@ -36573,7 +36621,7 @@
       <c r="H41" s="225"/>
     </row>
     <row r="42" spans="1:1024" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="246"/>
+      <c r="A42" s="252"/>
       <c r="B42" s="116" t="s">
         <v>232</v>
       </c>
@@ -36591,7 +36639,7 @@
       <c r="H42" s="118"/>
     </row>
     <row r="43" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="247" t="s">
+      <c r="A43" s="253" t="s">
         <v>233</v>
       </c>
       <c r="B43" s="119"/>
@@ -36678,7 +36726,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="244" t="s">
+      <c r="A45" s="250" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="111"/>
@@ -36691,7 +36739,7 @@
       <c r="AMJ45" s="5"/>
     </row>
     <row r="46" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="245"/>
+      <c r="A46" s="251"/>
       <c r="B46" s="113" t="s">
         <v>73</v>
       </c>
@@ -36709,7 +36757,7 @@
       <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="245"/>
+      <c r="A47" s="251"/>
       <c r="B47" s="113" t="s">
         <v>76</v>
       </c>
@@ -36727,7 +36775,7 @@
       <c r="H47" s="115"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="246"/>
+      <c r="A48" s="252"/>
       <c r="B48" s="116" t="s">
         <v>79</v>
       </c>
@@ -36745,7 +36793,7 @@
       <c r="H48" s="118"/>
     </row>
     <row r="49" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="247" t="s">
+      <c r="A49" s="253" t="s">
         <v>240</v>
       </c>
       <c r="B49" s="121"/>
@@ -36958,7 +37006,7 @@
       <c r="H58" s="110"/>
     </row>
     <row r="59" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="244" t="s">
+      <c r="A59" s="250" t="s">
         <v>479</v>
       </c>
       <c r="B59" s="123"/>
@@ -36971,7 +37019,7 @@
       <c r="AMJ59" s="5"/>
     </row>
     <row r="60" spans="1:1024" ht="90.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="246"/>
+      <c r="A60" s="252"/>
       <c r="B60" s="116" t="s">
         <v>5</v>
       </c>
@@ -37033,16 +37081,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>469</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -45881,16 +45929,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -45919,7 +45967,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="253" t="s">
         <v>483</v>
       </c>
       <c r="B3" s="18"/>
@@ -46245,14 +46293,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BJ19"/>
+  <dimension ref="A1:BJ23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -46269,16 +46317,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>471</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -46318,7 +46366,7 @@
       <c r="G3" s="207"/>
       <c r="H3" s="143"/>
     </row>
-    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="267"/>
       <c r="B4" s="106" t="s">
         <v>206</v>
@@ -46461,7 +46509,7 @@
       <c r="P8" s="144"/>
       <c r="Q8" s="144"/>
     </row>
-    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="267"/>
       <c r="B9" s="106" t="s">
         <v>268</v>
@@ -46571,7 +46619,7 @@
       <c r="P12" s="144"/>
       <c r="Q12" s="144"/>
     </row>
-    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="267"/>
       <c r="B13" s="106" t="s">
         <v>281</v>
@@ -46625,73 +46673,71 @@
       <c r="P14" s="144"/>
       <c r="Q14" s="144"/>
     </row>
-    <row r="15" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="267"/>
       <c r="B15" s="106" t="s">
-        <v>555</v>
+        <v>289</v>
       </c>
       <c r="C15" s="106"/>
-      <c r="D15" s="105" t="s">
-        <v>573</v>
-      </c>
-      <c r="E15" s="136"/>
+      <c r="D15" s="106" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>291</v>
+      </c>
       <c r="F15" s="106" t="s">
-        <v>556</v>
+        <v>292</v>
       </c>
       <c r="G15" s="194"/>
-      <c r="H15" s="145"/>
+      <c r="H15" s="137"/>
       <c r="I15" s="144"/>
-      <c r="J15" s="146"/>
-      <c r="K15" s="147"/>
+      <c r="J15" s="144"/>
+      <c r="K15" s="144"/>
       <c r="L15" s="144"/>
       <c r="M15" s="144"/>
-      <c r="N15" s="146"/>
-      <c r="O15" s="147"/>
+      <c r="N15" s="144"/>
+      <c r="O15" s="144"/>
       <c r="P15" s="144"/>
       <c r="Q15" s="144"/>
     </row>
-    <row r="16" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="267"/>
-      <c r="B16" s="106" t="s">
-        <v>288</v>
-      </c>
-      <c r="C16" s="106"/>
-      <c r="D16" s="105" t="s">
-        <v>567</v>
-      </c>
-      <c r="E16" s="136"/>
-      <c r="F16" s="106" t="s">
-        <v>569</v>
-      </c>
-      <c r="G16" s="194"/>
-      <c r="H16" s="145"/>
+    <row r="16" spans="1:17" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="268"/>
+      <c r="B16" s="109" t="s">
+        <v>293</v>
+      </c>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="109" t="s">
+        <v>294</v>
+      </c>
+      <c r="F16" s="109" t="s">
+        <v>295</v>
+      </c>
+      <c r="G16" s="195"/>
+      <c r="H16" s="139"/>
       <c r="I16" s="144"/>
-      <c r="J16" s="146"/>
-      <c r="K16" s="147"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
       <c r="L16" s="144"/>
       <c r="M16" s="144"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="147"/>
+      <c r="N16" s="144"/>
+      <c r="O16" s="144"/>
       <c r="P16" s="144"/>
       <c r="Q16" s="144"/>
     </row>
-    <row r="17" spans="1:17" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="267"/>
-      <c r="B17" s="106" t="s">
-        <v>289</v>
-      </c>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106" t="s">
-        <v>290</v>
-      </c>
-      <c r="E17" s="106" t="s">
-        <v>291</v>
-      </c>
-      <c r="F17" s="106" t="s">
-        <v>292</v>
-      </c>
-      <c r="G17" s="194"/>
-      <c r="H17" s="137"/>
+    <row r="17" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="266" t="s">
+        <v>583</v>
+      </c>
+      <c r="B17" s="272"/>
+      <c r="C17" s="272"/>
+      <c r="D17" s="272"/>
+      <c r="E17" s="272"/>
+      <c r="F17" s="272"/>
+      <c r="G17" s="273"/>
+      <c r="H17" s="274"/>
       <c r="I17" s="144"/>
       <c r="J17" s="144"/>
       <c r="K17" s="144"/>
@@ -46702,39 +46748,87 @@
       <c r="P17" s="144"/>
       <c r="Q17" s="144"/>
     </row>
-    <row r="18" spans="1:17" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="268"/>
+    <row r="18" spans="1:17" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="270"/>
       <c r="B18" s="109" t="s">
-        <v>293</v>
+        <v>555</v>
       </c>
       <c r="C18" s="109"/>
-      <c r="D18" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="109" t="s">
-        <v>294</v>
-      </c>
+      <c r="D18" s="108" t="s">
+        <v>573</v>
+      </c>
+      <c r="E18" s="138"/>
       <c r="F18" s="109" t="s">
-        <v>295</v>
+        <v>556</v>
       </c>
       <c r="G18" s="195"/>
-      <c r="H18" s="139"/>
+      <c r="H18" s="271"/>
       <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
-      <c r="K18" s="144"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="147"/>
       <c r="L18" s="144"/>
       <c r="M18" s="144"/>
-      <c r="N18" s="144"/>
-      <c r="O18" s="144"/>
+      <c r="N18" s="146"/>
+      <c r="O18" s="147"/>
       <c r="P18" s="144"/>
       <c r="Q18" s="144"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="266" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="272"/>
+      <c r="C19" s="272"/>
+      <c r="D19" s="275"/>
+      <c r="E19" s="276"/>
+      <c r="F19" s="272"/>
+      <c r="G19" s="273"/>
+      <c r="H19" s="277"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="146"/>
+      <c r="K19" s="147"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="144"/>
+      <c r="N19" s="146"/>
+      <c r="O19" s="147"/>
+      <c r="P19" s="144"/>
+      <c r="Q19" s="144"/>
+    </row>
+    <row r="20" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="270"/>
+      <c r="B20" s="109" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="108" t="s">
+        <v>567</v>
+      </c>
+      <c r="E20" s="138"/>
+      <c r="F20" s="109" t="s">
+        <v>569</v>
+      </c>
+      <c r="G20" s="195"/>
+      <c r="H20" s="271"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="146"/>
+      <c r="K20" s="147"/>
+      <c r="L20" s="144"/>
+      <c r="M20" s="144"/>
+      <c r="N20" s="146"/>
+      <c r="O20" s="147"/>
+      <c r="P20" s="144"/>
+      <c r="Q20" s="144"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A3:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -46769,16 +46863,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:20" s="152" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -46819,7 +46913,7 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="156" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="247" t="s">
+      <c r="A4" s="253" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="153"/>
@@ -46915,7 +47009,7 @@
       <c r="H8" s="160"/>
     </row>
     <row r="9" spans="1:20" s="155" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="244" t="s">
+      <c r="A9" s="250" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="161"/>
@@ -46927,7 +47021,7 @@
       <c r="H9" s="162"/>
     </row>
     <row r="10" spans="1:20" ht="18.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="245"/>
+      <c r="A10" s="251"/>
       <c r="B10" s="163" t="s">
         <v>30</v>
       </c>
@@ -46945,7 +47039,7 @@
       <c r="H10" s="164"/>
     </row>
     <row r="11" spans="1:20" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="245"/>
+      <c r="A11" s="251"/>
       <c r="B11" s="163" t="s">
         <v>366</v>
       </c>
@@ -46961,7 +47055,7 @@
       <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:20" ht="40.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="245"/>
+      <c r="A12" s="251"/>
       <c r="B12" s="163"/>
       <c r="C12" s="163" t="s">
         <v>368</v>
@@ -46977,7 +47071,7 @@
       <c r="H12" s="164"/>
     </row>
     <row r="13" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="245"/>
+      <c r="A13" s="251"/>
       <c r="B13" s="163"/>
       <c r="C13" s="163" t="s">
         <v>369</v>
@@ -46993,7 +47087,7 @@
       <c r="H13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+      <c r="A14" s="251"/>
       <c r="B14" s="163"/>
       <c r="C14" s="163" t="s">
         <v>370</v>
@@ -47009,7 +47103,7 @@
       <c r="H14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="245"/>
+      <c r="A15" s="251"/>
       <c r="B15" s="163"/>
       <c r="C15" s="163" t="s">
         <v>371</v>
@@ -47025,7 +47119,7 @@
       <c r="H15" s="164"/>
     </row>
     <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="245"/>
+      <c r="A16" s="251"/>
       <c r="B16" s="163"/>
       <c r="C16" s="163" t="s">
         <v>373</v>
@@ -47041,7 +47135,7 @@
       <c r="H16" s="164"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="245"/>
+      <c r="A17" s="251"/>
       <c r="B17" s="163"/>
       <c r="C17" s="163" t="s">
         <v>552</v>
@@ -47059,7 +47153,7 @@
       <c r="H17" s="164"/>
     </row>
     <row r="18" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="163" t="s">
         <v>375</v>
       </c>
@@ -47075,7 +47169,7 @@
       <c r="H18" s="164"/>
     </row>
     <row r="19" spans="1:8" ht="18.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="246"/>
+      <c r="A19" s="252"/>
       <c r="B19" s="165"/>
       <c r="C19" s="165" t="s">
         <v>373</v>
@@ -47146,7 +47240,7 @@
       <c r="E1" s="269"/>
       <c r="F1" s="269"/>
       <c r="G1" s="269"/>
-      <c r="H1" s="251"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:20" s="232" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -47187,7 +47281,7 @@
       <c r="H3" s="229"/>
     </row>
     <row r="4" spans="1:20" s="236" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="247" t="s">
+      <c r="A4" s="253" t="s">
         <v>555</v>
       </c>
       <c r="B4" s="153"/>
@@ -47314,16 +47408,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="238" t="s">
         <v>472</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:1024" s="42" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -48368,7 +48462,7 @@
       <c r="AMJ2" s="41"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="253" t="s">
         <v>377</v>
       </c>
       <c r="B3" s="169"/>
@@ -57668,7 +57762,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="244" t="s">
+      <c r="A13" s="250" t="s">
         <v>392</v>
       </c>
       <c r="B13" s="172"/>
@@ -57681,7 +57775,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="245"/>
+      <c r="A14" s="251"/>
       <c r="B14" s="69" t="s">
         <v>206</v>
       </c>
@@ -57697,7 +57791,7 @@
       <c r="H14" s="174"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="245"/>
+      <c r="A15" s="251"/>
       <c r="B15" s="69" t="s">
         <v>256</v>
       </c>
@@ -57713,7 +57807,7 @@
       <c r="H15" s="174"/>
     </row>
     <row r="16" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="245"/>
+      <c r="A16" s="251"/>
       <c r="B16" s="69" t="s">
         <v>212</v>
       </c>
@@ -57729,7 +57823,7 @@
       <c r="H16" s="174"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="245"/>
+      <c r="A17" s="251"/>
       <c r="B17" s="69" t="s">
         <v>262</v>
       </c>
@@ -57745,7 +57839,7 @@
       <c r="H17" s="174"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="245"/>
+      <c r="A18" s="251"/>
       <c r="B18" s="69" t="s">
         <v>209</v>
       </c>
@@ -57761,7 +57855,7 @@
       <c r="H18" s="174"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="245"/>
+      <c r="A19" s="251"/>
       <c r="B19" s="69" t="s">
         <v>5</v>
       </c>
@@ -57777,7 +57871,7 @@
       <c r="H19" s="174"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="245"/>
+      <c r="A20" s="251"/>
       <c r="B20" s="69" t="s">
         <v>398</v>
       </c>
@@ -57793,7 +57887,7 @@
       <c r="H20" s="174"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="245"/>
+      <c r="A21" s="251"/>
       <c r="B21" s="69" t="s">
         <v>310</v>
       </c>
@@ -57809,7 +57903,7 @@
       <c r="H21" s="174"/>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="245"/>
+      <c r="A22" s="251"/>
       <c r="B22" s="69" t="s">
         <v>401</v>
       </c>
@@ -57825,7 +57919,7 @@
       <c r="H22" s="174"/>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="245"/>
+      <c r="A23" s="251"/>
       <c r="B23" s="69" t="s">
         <v>403</v>
       </c>
@@ -57841,7 +57935,7 @@
       <c r="H23" s="174"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="246"/>
+      <c r="A24" s="252"/>
       <c r="B24" s="73" t="s">
         <v>405</v>
       </c>
@@ -57857,7 +57951,7 @@
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="247" t="s">
+      <c r="A25" s="253" t="s">
         <v>343</v>
       </c>
       <c r="B25" s="176"/>
@@ -58045,7 +58139,7 @@
       <c r="H36" s="178"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="244" t="s">
+      <c r="A37" s="250" t="s">
         <v>278</v>
       </c>
       <c r="B37" s="172"/>
@@ -58058,7 +58152,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="245"/>
+      <c r="A38" s="251"/>
       <c r="B38" s="69" t="s">
         <v>206</v>
       </c>
@@ -58074,7 +58168,7 @@
       <c r="H38" s="174"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="245"/>
+      <c r="A39" s="251"/>
       <c r="B39" s="69" t="s">
         <v>256</v>
       </c>
@@ -58090,7 +58184,7 @@
       <c r="H39" s="174"/>
     </row>
     <row r="40" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="245"/>
+      <c r="A40" s="251"/>
       <c r="B40" s="69" t="s">
         <v>212</v>
       </c>
@@ -58106,7 +58200,7 @@
       <c r="H40" s="174"/>
     </row>
     <row r="41" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="245"/>
+      <c r="A41" s="251"/>
       <c r="B41" s="69" t="s">
         <v>262</v>
       </c>
@@ -58122,7 +58216,7 @@
       <c r="H41" s="174"/>
     </row>
     <row r="42" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="245"/>
+      <c r="A42" s="251"/>
       <c r="B42" s="69" t="s">
         <v>424</v>
       </c>
@@ -58138,7 +58232,7 @@
       <c r="H42" s="174"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="245"/>
+      <c r="A43" s="251"/>
       <c r="B43" s="69" t="s">
         <v>343</v>
       </c>
@@ -58154,7 +58248,7 @@
       <c r="H43" s="174"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="245"/>
+      <c r="A44" s="251"/>
       <c r="B44" s="69" t="s">
         <v>209</v>
       </c>
@@ -58170,7 +58264,7 @@
       <c r="H44" s="174"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="245"/>
+      <c r="A45" s="251"/>
       <c r="B45" s="69" t="s">
         <v>388</v>
       </c>
@@ -58186,7 +58280,7 @@
       <c r="H45" s="174"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="245"/>
+      <c r="A46" s="251"/>
       <c r="B46" s="69" t="s">
         <v>429</v>
       </c>
@@ -58202,7 +58296,7 @@
       <c r="H46" s="174"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="245"/>
+      <c r="A47" s="251"/>
       <c r="B47" s="69" t="s">
         <v>5</v>
       </c>
@@ -58218,7 +58312,7 @@
       <c r="H47" s="174"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="246"/>
+      <c r="A48" s="252"/>
       <c r="B48" s="73" t="s">
         <v>401</v>
       </c>

</xml_diff>

<commit_message>
fix(dma): fix broken links
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\digitbrain.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76A7823-D61D-417B-B791-5C4F3338A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A3DCFA-7CF9-44EB-A599-5B78654F4D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="705" windowWidth="27675" windowHeight="14100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="575">
   <si>
     <t>Concept</t>
   </si>
@@ -1786,12 +1786,6 @@
     <t xml:space="preserve"> Deployment Substructure</t>
   </si>
   <si>
-    <t>[Deployment](deployment.md)</t>
-  </si>
-  <si>
-    <t>*This substructure is part of [DMA Tuple](dma_tuple.md)*</t>
-  </si>
-  <si>
     <t>Characteristics of the Deployment (i.e. Cloud or Edge infrastructure) for every Microservice associated to the DMA Tuple</t>
   </si>
   <si>
@@ -1804,9 +1798,6 @@
     <t>See above</t>
   </si>
   <si>
-    <t>[DataAssetsMapping](dataassetsmapping.md)</t>
-  </si>
-  <si>
     <t xml:space="preserve">*MICROSERVICE_ID* </t>
   </si>
   <si>
@@ -1853,13 +1844,19 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>[DataAssetsMapping](../dataassetsmapping.md)</t>
+  </si>
+  <si>
+    <t>[Deployment](../deployment.md)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1966,29 +1963,6 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2414,12 +2388,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3162,26 +3135,6 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -3225,10 +3178,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3239,122 +3188,6 @@
     </xf>
     <xf numFmtId="49" fontId="13" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3425,10 +3258,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -3443,10 +3272,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3469,19 +3294,7 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3529,6 +3342,98 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3537,17 +3442,115 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -4456,16 +4459,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>452</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -4494,7 +4497,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="256" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4506,7 +4509,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="229"/>
+      <c r="A4" s="257"/>
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -4526,7 +4529,7 @@
       <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="229"/>
+      <c r="A5" s="257"/>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
@@ -4546,7 +4549,7 @@
       <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="229"/>
+      <c r="A6" s="257"/>
       <c r="B6" s="43" t="s">
         <v>16</v>
       </c>
@@ -4566,7 +4569,7 @@
       <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="229"/>
+      <c r="A7" s="257"/>
       <c r="B7" s="43" t="s">
         <v>19</v>
       </c>
@@ -4586,7 +4589,7 @@
       <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="229"/>
+      <c r="A8" s="257"/>
       <c r="B8" s="43" t="s">
         <v>22</v>
       </c>
@@ -4606,7 +4609,7 @@
       <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="229"/>
+      <c r="A9" s="257"/>
       <c r="B9" s="43" t="s">
         <v>25</v>
       </c>
@@ -4626,7 +4629,7 @@
       <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="229"/>
+      <c r="A10" s="257"/>
       <c r="B10" s="43" t="s">
         <v>26</v>
       </c>
@@ -4646,7 +4649,7 @@
       <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="230"/>
+      <c r="A11" s="258"/>
       <c r="B11" s="47" t="s">
         <v>30</v>
       </c>
@@ -4666,7 +4669,7 @@
       <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="231" t="s">
+      <c r="A12" s="259" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="184"/>
@@ -4678,7 +4681,7 @@
       <c r="H12" s="187"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="232"/>
+      <c r="A13" s="260"/>
       <c r="B13" s="51" t="s">
         <v>35</v>
       </c>
@@ -4698,7 +4701,7 @@
       <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="232"/>
+      <c r="A14" s="260"/>
       <c r="B14" s="51" t="s">
         <v>38</v>
       </c>
@@ -4718,7 +4721,7 @@
       <c r="H14" s="54"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="232"/>
+      <c r="A15" s="260"/>
       <c r="B15" s="51" t="s">
         <v>426</v>
       </c>
@@ -5754,7 +5757,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="232"/>
+      <c r="A16" s="260"/>
       <c r="B16" s="51"/>
       <c r="C16" s="52" t="s">
         <v>526</v>
@@ -6790,7 +6793,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="232"/>
+      <c r="A17" s="260"/>
       <c r="B17" s="51"/>
       <c r="C17" s="52" t="s">
         <v>528</v>
@@ -7826,7 +7829,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="232"/>
+      <c r="A18" s="260"/>
       <c r="B18" s="51"/>
       <c r="C18" s="52" t="s">
         <v>527</v>
@@ -8862,7 +8865,7 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="232"/>
+      <c r="A19" s="260"/>
       <c r="B19" s="51" t="s">
         <v>423</v>
       </c>
@@ -9898,7 +9901,7 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="233"/>
+      <c r="A20" s="261"/>
       <c r="B20" s="188" t="s">
         <v>424</v>
       </c>
@@ -10934,7 +10937,7 @@
       <c r="AMJ20" s="4"/>
     </row>
     <row r="21" spans="1:1024" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="224" t="s">
+      <c r="A21" s="262" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="55"/>
@@ -10946,7 +10949,7 @@
       <c r="H21" s="57"/>
     </row>
     <row r="22" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="224"/>
+      <c r="A22" s="262"/>
       <c r="B22" s="43" t="s">
         <v>40</v>
       </c>
@@ -10966,7 +10969,7 @@
       <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="224"/>
+      <c r="A23" s="262"/>
       <c r="B23" s="43" t="s">
         <v>44</v>
       </c>
@@ -10986,7 +10989,7 @@
       <c r="H23" s="46"/>
     </row>
     <row r="24" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="262"/>
       <c r="B24" s="43" t="s">
         <v>46</v>
       </c>
@@ -11006,7 +11009,7 @@
       <c r="H24" s="46"/>
     </row>
     <row r="25" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="262"/>
       <c r="B25" s="43" t="s">
         <v>48</v>
       </c>
@@ -11026,7 +11029,7 @@
       <c r="H25" s="46"/>
     </row>
     <row r="26" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="224"/>
+      <c r="A26" s="262"/>
       <c r="B26" s="43" t="s">
         <v>50</v>
       </c>
@@ -11046,7 +11049,7 @@
       <c r="H26" s="46"/>
     </row>
     <row r="27" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="224"/>
+      <c r="A27" s="262"/>
       <c r="B27" s="43" t="s">
         <v>53</v>
       </c>
@@ -11066,7 +11069,7 @@
       <c r="H27" s="46"/>
     </row>
     <row r="28" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="224"/>
+      <c r="A28" s="262"/>
       <c r="B28" s="43" t="s">
         <v>57</v>
       </c>
@@ -11086,7 +11089,7 @@
       <c r="H28" s="46"/>
     </row>
     <row r="29" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="224"/>
+      <c r="A29" s="262"/>
       <c r="B29" s="43" t="s">
         <v>61</v>
       </c>
@@ -11106,7 +11109,7 @@
       <c r="H29" s="46"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="224"/>
+      <c r="A30" s="262"/>
       <c r="B30" s="43" t="s">
         <v>63</v>
       </c>
@@ -11126,7 +11129,7 @@
       <c r="H30" s="46"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="224"/>
+      <c r="A31" s="262"/>
       <c r="B31" s="43" t="s">
         <v>65</v>
       </c>
@@ -11146,7 +11149,7 @@
       <c r="H31" s="46"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="224"/>
+      <c r="A32" s="262"/>
       <c r="B32" s="43" t="s">
         <v>67</v>
       </c>
@@ -11166,7 +11169,7 @@
       <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="225"/>
+      <c r="A33" s="263"/>
       <c r="B33" s="47" t="s">
         <v>69</v>
       </c>
@@ -11186,7 +11189,7 @@
       <c r="H33" s="50"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="220" t="s">
+      <c r="A34" s="264" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="58"/>
@@ -11198,7 +11201,7 @@
       <c r="H34" s="60"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="221"/>
+      <c r="A35" s="265"/>
       <c r="B35" s="61" t="s">
         <v>73</v>
       </c>
@@ -11218,7 +11221,7 @@
       <c r="H35" s="64"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="221"/>
+      <c r="A36" s="265"/>
       <c r="B36" s="65" t="s">
         <v>76</v>
       </c>
@@ -11238,7 +11241,7 @@
       <c r="H36" s="68"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="221"/>
+      <c r="A37" s="265"/>
       <c r="B37" s="65" t="s">
         <v>79</v>
       </c>
@@ -11258,7 +11261,7 @@
       <c r="H37" s="68"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="222"/>
+      <c r="A38" s="266"/>
       <c r="B38" s="69" t="s">
         <v>82</v>
       </c>
@@ -11278,31 +11281,31 @@
       <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="223" t="s">
-        <v>570</v>
-      </c>
-      <c r="B39" s="247"/>
-      <c r="C39" s="247"/>
-      <c r="D39" s="247"/>
-      <c r="E39" s="248"/>
-      <c r="F39" s="247"/>
-      <c r="G39" s="249"/>
+      <c r="A39" s="267" t="s">
+        <v>567</v>
+      </c>
+      <c r="B39" s="212"/>
+      <c r="C39" s="212"/>
+      <c r="D39" s="212"/>
+      <c r="E39" s="213"/>
+      <c r="F39" s="212"/>
+      <c r="G39" s="214"/>
       <c r="H39" s="57"/>
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="224"/>
-      <c r="B40" s="209" t="s">
-        <v>571</v>
+      <c r="A40" s="262"/>
+      <c r="B40" s="204" t="s">
+        <v>568</v>
       </c>
       <c r="C40" s="44"/>
-      <c r="D40" s="209" t="s">
+      <c r="D40" s="204" t="s">
         <v>85</v>
       </c>
       <c r="E40" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="209" t="s">
-        <v>572</v>
+      <c r="F40" s="204" t="s">
+        <v>569</v>
       </c>
       <c r="G40" s="155" t="s">
         <v>43</v>
@@ -12326,20 +12329,20 @@
       <c r="AMJ40" s="4"/>
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="224"/>
-      <c r="B41" s="218" t="s">
+      <c r="A41" s="262"/>
+      <c r="B41" s="254" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="209" t="s">
-        <v>573</v>
-      </c>
-      <c r="D41" s="209" t="s">
+      <c r="C41" s="204" t="s">
+        <v>570</v>
+      </c>
+      <c r="D41" s="204" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="209" t="s">
+      <c r="F41" s="204" t="s">
         <v>89</v>
       </c>
       <c r="G41" s="155" t="s">
@@ -13364,18 +13367,18 @@
       <c r="AMJ41" s="4"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A42" s="224"/>
-      <c r="B42" s="218"/>
-      <c r="C42" s="209" t="s">
+      <c r="A42" s="262"/>
+      <c r="B42" s="254"/>
+      <c r="C42" s="204" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="209" t="s">
+      <c r="D42" s="204" t="s">
         <v>91</v>
       </c>
       <c r="E42" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="209" t="s">
+      <c r="F42" s="204" t="s">
         <v>93</v>
       </c>
       <c r="G42" s="155" t="s">
@@ -14400,18 +14403,18 @@
       <c r="AMJ42" s="4"/>
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="224"/>
-      <c r="B43" s="218"/>
-      <c r="C43" s="209" t="s">
+      <c r="A43" s="262"/>
+      <c r="B43" s="254"/>
+      <c r="C43" s="204" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="209" t="s">
+      <c r="D43" s="204" t="s">
         <v>95</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>574</v>
-      </c>
-      <c r="F43" s="209" t="s">
+        <v>571</v>
+      </c>
+      <c r="F43" s="204" t="s">
         <v>96</v>
       </c>
       <c r="G43" s="155" t="s">
@@ -15436,18 +15439,18 @@
       <c r="AMJ43" s="4"/>
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="224"/>
-      <c r="B44" s="218"/>
-      <c r="C44" s="209" t="s">
+      <c r="A44" s="262"/>
+      <c r="B44" s="254"/>
+      <c r="C44" s="204" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="209" t="s">
+      <c r="D44" s="204" t="s">
         <v>98</v>
       </c>
       <c r="E44" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="F44" s="209" t="s">
+      <c r="F44" s="204" t="s">
         <v>100</v>
       </c>
       <c r="G44" s="155" t="s">
@@ -16472,18 +16475,18 @@
       <c r="AMJ44" s="4"/>
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="224"/>
-      <c r="B45" s="218"/>
-      <c r="C45" s="209" t="s">
+      <c r="A45" s="262"/>
+      <c r="B45" s="254"/>
+      <c r="C45" s="204" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="209" t="s">
+      <c r="D45" s="204" t="s">
         <v>102</v>
       </c>
       <c r="E45" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F45" s="209" t="s">
+      <c r="F45" s="204" t="s">
         <v>104</v>
       </c>
       <c r="G45" s="155" t="s">
@@ -17508,18 +17511,18 @@
       <c r="AMJ45" s="4"/>
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="224"/>
-      <c r="B46" s="218"/>
-      <c r="C46" s="209" t="s">
+      <c r="A46" s="262"/>
+      <c r="B46" s="254"/>
+      <c r="C46" s="204" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="209" t="s">
+      <c r="D46" s="204" t="s">
         <v>106</v>
       </c>
       <c r="E46" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="209" t="s">
+      <c r="F46" s="204" t="s">
         <v>108</v>
       </c>
       <c r="G46" s="155" t="s">
@@ -18544,18 +18547,18 @@
       <c r="AMJ46" s="4"/>
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="224"/>
-      <c r="B47" s="218"/>
-      <c r="C47" s="209" t="s">
+      <c r="A47" s="262"/>
+      <c r="B47" s="254"/>
+      <c r="C47" s="204" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="209" t="s">
+      <c r="D47" s="204" t="s">
         <v>110</v>
       </c>
       <c r="E47" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="209" t="s">
+      <c r="F47" s="204" t="s">
         <v>112</v>
       </c>
       <c r="G47" s="155" t="s">
@@ -19580,18 +19583,18 @@
       <c r="AMJ47" s="4"/>
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="224"/>
-      <c r="B48" s="218"/>
-      <c r="C48" s="209" t="s">
+      <c r="A48" s="262"/>
+      <c r="B48" s="254"/>
+      <c r="C48" s="204" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="209" t="s">
+      <c r="D48" s="204" t="s">
         <v>114</v>
       </c>
       <c r="E48" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="F48" s="209" t="s">
+      <c r="F48" s="204" t="s">
         <v>116</v>
       </c>
       <c r="G48" s="155" t="s">
@@ -20616,18 +20619,18 @@
       <c r="AMJ48" s="4"/>
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="224"/>
-      <c r="B49" s="218"/>
-      <c r="C49" s="209" t="s">
+      <c r="A49" s="262"/>
+      <c r="B49" s="254"/>
+      <c r="C49" s="204" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="209" t="s">
+      <c r="D49" s="204" t="s">
         <v>118</v>
       </c>
       <c r="E49" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="F49" s="209" t="s">
+      <c r="F49" s="204" t="s">
         <v>120</v>
       </c>
       <c r="G49" s="155" t="s">
@@ -21652,18 +21655,18 @@
       <c r="AMJ49" s="4"/>
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="224"/>
-      <c r="B50" s="218"/>
-      <c r="C50" s="209" t="s">
+      <c r="A50" s="262"/>
+      <c r="B50" s="254"/>
+      <c r="C50" s="204" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="209" t="s">
+      <c r="D50" s="204" t="s">
         <v>122</v>
       </c>
       <c r="E50" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="F50" s="209" t="s">
+      <c r="F50" s="204" t="s">
         <v>124</v>
       </c>
       <c r="G50" s="155" t="s">
@@ -22688,18 +22691,18 @@
       <c r="AMJ50" s="4"/>
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="224"/>
-      <c r="B51" s="218"/>
-      <c r="C51" s="209" t="s">
+      <c r="A51" s="262"/>
+      <c r="B51" s="254"/>
+      <c r="C51" s="204" t="s">
         <v>125</v>
       </c>
-      <c r="D51" s="209" t="s">
+      <c r="D51" s="204" t="s">
         <v>126</v>
       </c>
       <c r="E51" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="F51" s="209" t="s">
+      <c r="F51" s="204" t="s">
         <v>128</v>
       </c>
       <c r="G51" s="155" t="s">
@@ -23724,18 +23727,18 @@
       <c r="AMJ51" s="4"/>
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="225"/>
-      <c r="B52" s="219"/>
-      <c r="C52" s="210" t="s">
+      <c r="A52" s="263"/>
+      <c r="B52" s="255"/>
+      <c r="C52" s="205" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="210" t="s">
+      <c r="D52" s="205" t="s">
         <v>130</v>
       </c>
       <c r="E52" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="F52" s="210" t="s">
+      <c r="F52" s="205" t="s">
         <v>429</v>
       </c>
       <c r="G52" s="156" t="s">
@@ -24760,280 +24763,280 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="231" t="s">
-        <v>575</v>
-      </c>
-      <c r="B53" s="250"/>
-      <c r="C53" s="250"/>
-      <c r="D53" s="250"/>
-      <c r="E53" s="251"/>
-      <c r="F53" s="250"/>
-      <c r="G53" s="252"/>
-      <c r="H53" s="253"/>
+      <c r="A53" s="259" t="s">
+        <v>572</v>
+      </c>
+      <c r="B53" s="215"/>
+      <c r="C53" s="215"/>
+      <c r="D53" s="215"/>
+      <c r="E53" s="216"/>
+      <c r="F53" s="215"/>
+      <c r="G53" s="217"/>
+      <c r="H53" s="218"/>
     </row>
     <row r="54" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="232"/>
-      <c r="B54" s="254" t="s">
+      <c r="A54" s="260"/>
+      <c r="B54" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="255"/>
-      <c r="D54" s="254" t="s">
+      <c r="C54" s="220"/>
+      <c r="D54" s="219" t="s">
         <v>133</v>
       </c>
-      <c r="E54" s="256" t="s">
+      <c r="E54" s="221" t="s">
         <v>134</v>
       </c>
-      <c r="F54" s="254" t="s">
+      <c r="F54" s="219" t="s">
         <v>135</v>
       </c>
-      <c r="G54" s="257" t="s">
+      <c r="G54" s="222" t="s">
         <v>43</v>
       </c>
-      <c r="H54" s="258"/>
+      <c r="H54" s="223"/>
     </row>
     <row r="55" spans="1:1024" ht="46.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="233"/>
-      <c r="B55" s="259" t="s">
+      <c r="A55" s="261"/>
+      <c r="B55" s="224" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="260"/>
-      <c r="D55" s="259" t="s">
+      <c r="C55" s="225"/>
+      <c r="D55" s="224" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="261" t="s">
+      <c r="E55" s="226" t="s">
         <v>138</v>
       </c>
-      <c r="F55" s="259" t="s">
+      <c r="F55" s="224" t="s">
         <v>139</v>
       </c>
-      <c r="G55" s="262" t="s">
+      <c r="G55" s="227" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="263"/>
+      <c r="H55" s="228"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="264" t="s">
+      <c r="A56" s="268" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="265"/>
-      <c r="C56" s="265"/>
-      <c r="D56" s="265"/>
-      <c r="E56" s="266"/>
-      <c r="F56" s="265"/>
-      <c r="G56" s="267"/>
-      <c r="H56" s="268"/>
+      <c r="B56" s="229"/>
+      <c r="C56" s="229"/>
+      <c r="D56" s="229"/>
+      <c r="E56" s="230"/>
+      <c r="F56" s="229"/>
+      <c r="G56" s="231"/>
+      <c r="H56" s="232"/>
     </row>
     <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="269"/>
-      <c r="B57" s="270" t="s">
+      <c r="B57" s="233" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="271"/>
-      <c r="D57" s="270" t="s">
+      <c r="C57" s="234"/>
+      <c r="D57" s="233" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="272"/>
-      <c r="F57" s="270" t="s">
+      <c r="E57" s="235"/>
+      <c r="F57" s="233" t="s">
         <v>143</v>
       </c>
-      <c r="G57" s="273" t="s">
+      <c r="G57" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="H57" s="274"/>
+      <c r="H57" s="237"/>
     </row>
     <row r="58" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="269"/>
-      <c r="B58" s="275" t="s">
+      <c r="B58" s="271" t="s">
         <v>144</v>
       </c>
-      <c r="C58" s="270" t="s">
+      <c r="C58" s="233" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="270" t="s">
+      <c r="D58" s="233" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="272" t="s">
+      <c r="E58" s="235" t="s">
         <v>146</v>
       </c>
-      <c r="F58" s="270" t="s">
+      <c r="F58" s="233" t="s">
         <v>147</v>
       </c>
-      <c r="G58" s="273" t="s">
+      <c r="G58" s="236" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="274"/>
+      <c r="H58" s="237"/>
     </row>
     <row r="59" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="269"/>
-      <c r="B59" s="275"/>
-      <c r="C59" s="270" t="s">
+      <c r="B59" s="271"/>
+      <c r="C59" s="233" t="s">
         <v>30</v>
       </c>
-      <c r="D59" s="270" t="s">
+      <c r="D59" s="233" t="s">
         <v>148</v>
       </c>
-      <c r="E59" s="272" t="s">
+      <c r="E59" s="235" t="s">
         <v>149</v>
       </c>
-      <c r="F59" s="270" t="s">
+      <c r="F59" s="233" t="s">
         <v>150</v>
       </c>
-      <c r="G59" s="273" t="s">
+      <c r="G59" s="236" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="274"/>
+      <c r="H59" s="237"/>
     </row>
     <row r="60" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="269"/>
-      <c r="B60" s="275"/>
-      <c r="C60" s="270" t="s">
+      <c r="B60" s="271"/>
+      <c r="C60" s="233" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="270" t="s">
+      <c r="D60" s="233" t="s">
         <v>151</v>
       </c>
-      <c r="E60" s="272" t="s">
+      <c r="E60" s="235" t="s">
         <v>55</v>
       </c>
-      <c r="F60" s="272" t="s">
+      <c r="F60" s="235" t="s">
         <v>152</v>
       </c>
-      <c r="G60" s="273" t="s">
+      <c r="G60" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="H60" s="274"/>
+      <c r="H60" s="237"/>
     </row>
     <row r="61" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="269"/>
-      <c r="B61" s="275"/>
-      <c r="C61" s="270" t="s">
+      <c r="B61" s="271"/>
+      <c r="C61" s="233" t="s">
         <v>153</v>
       </c>
-      <c r="D61" s="276" t="s">
+      <c r="D61" s="238" t="s">
         <v>154</v>
       </c>
-      <c r="E61" s="272" t="s">
+      <c r="E61" s="235" t="s">
         <v>70</v>
       </c>
-      <c r="F61" s="270" t="s">
+      <c r="F61" s="233" t="s">
         <v>155</v>
       </c>
-      <c r="G61" s="273" t="s">
+      <c r="G61" s="236" t="s">
         <v>43</v>
       </c>
-      <c r="H61" s="274"/>
+      <c r="H61" s="237"/>
     </row>
     <row r="62" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="277"/>
-      <c r="B62" s="278"/>
-      <c r="C62" s="279" t="s">
+      <c r="A62" s="270"/>
+      <c r="B62" s="272"/>
+      <c r="C62" s="239" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="279" t="s">
+      <c r="D62" s="239" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="280" t="s">
+      <c r="E62" s="240" t="s">
         <v>156</v>
       </c>
-      <c r="F62" s="279" t="s">
+      <c r="F62" s="239" t="s">
         <v>157</v>
       </c>
-      <c r="G62" s="281" t="s">
+      <c r="G62" s="241" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="282"/>
+      <c r="H62" s="242"/>
     </row>
     <row r="63" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="231" t="s">
+      <c r="A63" s="259" t="s">
         <v>158</v>
       </c>
-      <c r="B63" s="283"/>
-      <c r="C63" s="283"/>
-      <c r="D63" s="283"/>
-      <c r="E63" s="284"/>
-      <c r="F63" s="283"/>
-      <c r="G63" s="285"/>
-      <c r="H63" s="253"/>
+      <c r="B63" s="243"/>
+      <c r="C63" s="243"/>
+      <c r="D63" s="243"/>
+      <c r="E63" s="244"/>
+      <c r="F63" s="243"/>
+      <c r="G63" s="245"/>
+      <c r="H63" s="218"/>
     </row>
     <row r="64" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="232"/>
-      <c r="B64" s="286" t="s">
+      <c r="A64" s="260"/>
+      <c r="B64" s="246" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="287"/>
-      <c r="D64" s="286" t="s">
+      <c r="C64" s="247"/>
+      <c r="D64" s="246" t="s">
         <v>160</v>
       </c>
-      <c r="E64" s="288"/>
-      <c r="F64" s="286" t="s">
+      <c r="E64" s="248"/>
+      <c r="F64" s="246" t="s">
         <v>161</v>
       </c>
-      <c r="G64" s="257" t="s">
+      <c r="G64" s="222" t="s">
         <v>43</v>
       </c>
-      <c r="H64" s="289"/>
+      <c r="H64" s="249"/>
     </row>
     <row r="65" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="232"/>
-      <c r="B65" s="290" t="s">
+      <c r="A65" s="260"/>
+      <c r="B65" s="273" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="286" t="s">
+      <c r="C65" s="246" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="286" t="s">
+      <c r="D65" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="286" t="s">
+      <c r="E65" s="246" t="s">
         <v>163</v>
       </c>
-      <c r="F65" s="286" t="s">
+      <c r="F65" s="246" t="s">
         <v>164</v>
       </c>
-      <c r="G65" s="257" t="s">
+      <c r="G65" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="289"/>
+      <c r="H65" s="249"/>
     </row>
     <row r="66" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="232"/>
-      <c r="B66" s="290"/>
-      <c r="C66" s="286" t="s">
+      <c r="A66" s="260"/>
+      <c r="B66" s="273"/>
+      <c r="C66" s="246" t="s">
         <v>165</v>
       </c>
-      <c r="D66" s="286" t="s">
+      <c r="D66" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="E66" s="286" t="s">
+      <c r="E66" s="246" t="s">
         <v>166</v>
       </c>
-      <c r="F66" s="286" t="s">
+      <c r="F66" s="246" t="s">
         <v>167</v>
       </c>
-      <c r="G66" s="257" t="s">
+      <c r="G66" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="H66" s="289"/>
+      <c r="H66" s="249"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="232"/>
-      <c r="B67" s="290"/>
-      <c r="C67" s="286" t="s">
+      <c r="A67" s="260"/>
+      <c r="B67" s="273"/>
+      <c r="C67" s="246" t="s">
         <v>168</v>
       </c>
-      <c r="D67" s="286" t="s">
+      <c r="D67" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="286" t="s">
+      <c r="E67" s="246" t="s">
         <v>169</v>
       </c>
-      <c r="F67" s="286" t="s">
+      <c r="F67" s="246" t="s">
         <v>170</v>
       </c>
-      <c r="G67" s="257" t="s">
+      <c r="G67" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="289"/>
+      <c r="H67" s="249"/>
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
       <c r="K67" s="13"/>
@@ -26052,24 +26055,24 @@
       <c r="AMJ67" s="13"/>
     </row>
     <row r="68" spans="1:1024" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="232"/>
-      <c r="B68" s="290"/>
-      <c r="C68" s="286" t="s">
+      <c r="A68" s="260"/>
+      <c r="B68" s="273"/>
+      <c r="C68" s="246" t="s">
         <v>171</v>
       </c>
-      <c r="D68" s="286" t="s">
+      <c r="D68" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="286" t="s">
+      <c r="E68" s="246" t="s">
         <v>172</v>
       </c>
-      <c r="F68" s="286" t="s">
+      <c r="F68" s="246" t="s">
         <v>173</v>
       </c>
-      <c r="G68" s="257" t="s">
+      <c r="G68" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="289"/>
+      <c r="H68" s="249"/>
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
       <c r="K68" s="13"/>
@@ -27088,24 +27091,24 @@
       <c r="AMJ68" s="13"/>
     </row>
     <row r="69" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="233"/>
-      <c r="B69" s="291"/>
-      <c r="C69" s="292" t="s">
+      <c r="A69" s="261"/>
+      <c r="B69" s="274"/>
+      <c r="C69" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="292" t="s">
+      <c r="D69" s="250" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="292" t="s">
+      <c r="E69" s="250" t="s">
         <v>174</v>
       </c>
-      <c r="F69" s="292" t="s">
+      <c r="F69" s="250" t="s">
         <v>175</v>
       </c>
-      <c r="G69" s="262" t="s">
+      <c r="G69" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="293"/>
+      <c r="H69" s="251"/>
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
@@ -28126,6 +28129,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="12">
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="B65:B69"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B41:B52"/>
     <mergeCell ref="A3:A11"/>
@@ -28133,11 +28141,6 @@
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="A63:A69"/>
-    <mergeCell ref="B65:B69"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -28177,16 +28180,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:8" s="31" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -28215,7 +28218,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="256" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -28227,7 +28230,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="229"/>
+      <c r="A4" s="257"/>
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -28247,7 +28250,7 @@
       <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="229"/>
+      <c r="A5" s="257"/>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
@@ -28267,7 +28270,7 @@
       <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="229"/>
+      <c r="A6" s="257"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -28287,7 +28290,7 @@
       <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="229"/>
+      <c r="A7" s="257"/>
       <c r="B7" s="43" t="s">
         <v>26</v>
       </c>
@@ -28307,7 +28310,7 @@
       <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="229"/>
+      <c r="A8" s="257"/>
       <c r="B8" s="43" t="s">
         <v>30</v>
       </c>
@@ -28327,7 +28330,7 @@
       <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="229"/>
+      <c r="A9" s="257"/>
       <c r="B9" s="43" t="s">
         <v>16</v>
       </c>
@@ -28347,7 +28350,7 @@
       <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="229"/>
+      <c r="A10" s="257"/>
       <c r="B10" s="43" t="s">
         <v>19</v>
       </c>
@@ -28367,7 +28370,7 @@
       <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="230"/>
+      <c r="A11" s="258"/>
       <c r="B11" s="47" t="s">
         <v>22</v>
       </c>
@@ -28387,7 +28390,7 @@
       <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="234" t="s">
+      <c r="A12" s="275" t="s">
         <v>189</v>
       </c>
       <c r="B12" s="73"/>
@@ -28399,7 +28402,7 @@
       <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="235"/>
+      <c r="A13" s="276"/>
       <c r="B13" s="78" t="s">
         <v>190</v>
       </c>
@@ -28419,7 +28422,7 @@
       <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="235"/>
+      <c r="A14" s="276"/>
       <c r="B14" s="78" t="s">
         <v>418</v>
       </c>
@@ -28477,16 +28480,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:1024" s="32" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -28515,7 +28518,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="256" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="33"/>
@@ -28565,7 +28568,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="229"/>
+      <c r="A4" s="257"/>
       <c r="B4" s="80" t="s">
         <v>192</v>
       </c>
@@ -28583,7 +28586,7 @@
       <c r="H4" s="82"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="229"/>
+      <c r="A5" s="257"/>
       <c r="B5" s="80" t="s">
         <v>195</v>
       </c>
@@ -28599,7 +28602,7 @@
       <c r="H5" s="82"/>
     </row>
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="229"/>
+      <c r="A6" s="257"/>
       <c r="B6" s="80" t="s">
         <v>198</v>
       </c>
@@ -28615,7 +28618,7 @@
       <c r="H6" s="82"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="229"/>
+      <c r="A7" s="257"/>
       <c r="B7" s="80" t="s">
         <v>199</v>
       </c>
@@ -28631,7 +28634,7 @@
       <c r="H7" s="82"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="229"/>
+      <c r="A8" s="257"/>
       <c r="B8" s="80" t="s">
         <v>200</v>
       </c>
@@ -28647,7 +28650,7 @@
       <c r="H8" s="82"/>
     </row>
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="229"/>
+      <c r="A9" s="257"/>
       <c r="B9" s="80" t="s">
         <v>202</v>
       </c>
@@ -28665,7 +28668,7 @@
       <c r="H9" s="82"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="229"/>
+      <c r="A10" s="257"/>
       <c r="B10" s="80" t="s">
         <v>204</v>
       </c>
@@ -28694,7 +28697,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="229"/>
+      <c r="A11" s="257"/>
       <c r="B11" s="80" t="s">
         <v>3</v>
       </c>
@@ -28710,7 +28713,7 @@
       <c r="H11" s="82"/>
     </row>
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="229"/>
+      <c r="A12" s="257"/>
       <c r="B12" s="80" t="s">
         <v>208</v>
       </c>
@@ -28728,7 +28731,7 @@
       <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="229"/>
+      <c r="A13" s="257"/>
       <c r="B13" s="80" t="s">
         <v>545</v>
       </c>
@@ -28748,7 +28751,7 @@
       <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="229"/>
+      <c r="A14" s="257"/>
       <c r="B14" s="80" t="s">
         <v>543</v>
       </c>
@@ -28768,7 +28771,7 @@
       <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="229"/>
+      <c r="A15" s="257"/>
       <c r="B15" s="80" t="s">
         <v>544</v>
       </c>
@@ -28788,7 +28791,7 @@
       <c r="H15" s="82"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="230"/>
+      <c r="A16" s="258"/>
       <c r="B16" s="83" t="s">
         <v>211</v>
       </c>
@@ -28804,7 +28807,7 @@
       <c r="H16" s="85"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="220" t="s">
+      <c r="A17" s="264" t="s">
         <v>140</v>
       </c>
       <c r="B17" s="86"/>
@@ -28817,7 +28820,7 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="221"/>
+      <c r="A18" s="265"/>
       <c r="B18" s="88" t="s">
         <v>214</v>
       </c>
@@ -28833,7 +28836,7 @@
       <c r="H18" s="90"/>
     </row>
     <row r="19" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="221"/>
+      <c r="A19" s="265"/>
       <c r="B19" s="88"/>
       <c r="C19" s="89" t="s">
         <v>1</v>
@@ -28849,7 +28852,7 @@
       <c r="H19" s="90"/>
     </row>
     <row r="20" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="221"/>
+      <c r="A20" s="265"/>
       <c r="B20" s="88"/>
       <c r="C20" s="89" t="s">
         <v>195</v>
@@ -28865,7 +28868,7 @@
       <c r="H20" s="90"/>
     </row>
     <row r="21" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="221"/>
+      <c r="A21" s="265"/>
       <c r="B21" s="88"/>
       <c r="C21" s="89" t="s">
         <v>484</v>
@@ -28881,7 +28884,7 @@
       <c r="H21" s="90"/>
     </row>
     <row r="22" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="221"/>
+      <c r="A22" s="265"/>
       <c r="B22" s="88"/>
       <c r="C22" s="89" t="s">
         <v>485</v>
@@ -28897,7 +28900,7 @@
       <c r="H22" s="90"/>
     </row>
     <row r="23" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="221"/>
+      <c r="A23" s="265"/>
       <c r="B23" s="88"/>
       <c r="C23" s="89" t="s">
         <v>486</v>
@@ -28913,7 +28916,7 @@
       <c r="H23" s="90"/>
     </row>
     <row r="24" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="221"/>
+      <c r="A24" s="265"/>
       <c r="B24" s="88"/>
       <c r="C24" s="89" t="s">
         <v>487</v>
@@ -28929,7 +28932,7 @@
       <c r="H24" s="90"/>
     </row>
     <row r="25" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="221"/>
+      <c r="A25" s="265"/>
       <c r="B25" s="88"/>
       <c r="C25" s="89" t="s">
         <v>488</v>
@@ -28945,7 +28948,7 @@
       <c r="H25" s="90"/>
     </row>
     <row r="26" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="221"/>
+      <c r="A26" s="265"/>
       <c r="B26" s="88"/>
       <c r="C26" s="89" t="s">
         <v>489</v>
@@ -28961,7 +28964,7 @@
       <c r="H26" s="90"/>
     </row>
     <row r="27" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="221"/>
+      <c r="A27" s="265"/>
       <c r="B27" s="88"/>
       <c r="C27" s="89" t="s">
         <v>490</v>
@@ -28977,7 +28980,7 @@
       <c r="H27" s="90"/>
     </row>
     <row r="28" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="221"/>
+      <c r="A28" s="265"/>
       <c r="B28" s="88"/>
       <c r="C28" s="89" t="s">
         <v>491</v>
@@ -28993,7 +28996,7 @@
       <c r="H28" s="90"/>
     </row>
     <row r="29" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="221"/>
+      <c r="A29" s="265"/>
       <c r="B29" s="88"/>
       <c r="C29" s="89" t="s">
         <v>492</v>
@@ -29009,7 +29012,7 @@
       <c r="H29" s="90"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="221"/>
+      <c r="A30" s="265"/>
       <c r="B30" s="88" t="s">
         <v>216</v>
       </c>
@@ -29025,7 +29028,7 @@
       <c r="H30" s="90"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="221"/>
+      <c r="A31" s="265"/>
       <c r="B31" s="193"/>
       <c r="C31" s="89" t="s">
         <v>1</v>
@@ -29041,7 +29044,7 @@
       <c r="H31" s="196"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="221"/>
+      <c r="A32" s="265"/>
       <c r="B32" s="193"/>
       <c r="C32" s="89" t="s">
         <v>195</v>
@@ -29057,7 +29060,7 @@
       <c r="H32" s="196"/>
     </row>
     <row r="33" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="221"/>
+      <c r="A33" s="265"/>
       <c r="B33" s="193"/>
       <c r="C33" s="89" t="s">
         <v>484</v>
@@ -29073,7 +29076,7 @@
       <c r="H33" s="196"/>
     </row>
     <row r="34" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="221"/>
+      <c r="A34" s="265"/>
       <c r="B34" s="193"/>
       <c r="C34" s="89" t="s">
         <v>485</v>
@@ -29089,7 +29092,7 @@
       <c r="H34" s="196"/>
     </row>
     <row r="35" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="221"/>
+      <c r="A35" s="265"/>
       <c r="B35" s="193"/>
       <c r="C35" s="89" t="s">
         <v>486</v>
@@ -29105,7 +29108,7 @@
       <c r="H35" s="196"/>
     </row>
     <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="221"/>
+      <c r="A36" s="265"/>
       <c r="B36" s="193"/>
       <c r="C36" s="89" t="s">
         <v>487</v>
@@ -29121,7 +29124,7 @@
       <c r="H36" s="196"/>
     </row>
     <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="221"/>
+      <c r="A37" s="265"/>
       <c r="B37" s="193"/>
       <c r="C37" s="89" t="s">
         <v>488</v>
@@ -29137,7 +29140,7 @@
       <c r="H37" s="196"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="221"/>
+      <c r="A38" s="265"/>
       <c r="B38" s="193"/>
       <c r="C38" s="89" t="s">
         <v>489</v>
@@ -29153,7 +29156,7 @@
       <c r="H38" s="196"/>
     </row>
     <row r="39" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="221"/>
+      <c r="A39" s="265"/>
       <c r="B39" s="193"/>
       <c r="C39" s="89" t="s">
         <v>490</v>
@@ -29169,7 +29172,7 @@
       <c r="H39" s="196"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="221"/>
+      <c r="A40" s="265"/>
       <c r="B40" s="193"/>
       <c r="C40" s="89" t="s">
         <v>491</v>
@@ -29185,7 +29188,7 @@
       <c r="H40" s="196"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="221"/>
+      <c r="A41" s="265"/>
       <c r="B41" s="193"/>
       <c r="C41" s="89" t="s">
         <v>492</v>
@@ -29201,7 +29204,7 @@
       <c r="H41" s="196"/>
     </row>
     <row r="42" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="222"/>
+      <c r="A42" s="266"/>
       <c r="B42" s="91" t="s">
         <v>218</v>
       </c>
@@ -29219,7 +29222,7 @@
       <c r="H42" s="93"/>
     </row>
     <row r="43" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="223" t="s">
+      <c r="A43" s="267" t="s">
         <v>219</v>
       </c>
       <c r="B43" s="94"/>
@@ -29269,7 +29272,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="225"/>
+      <c r="A44" s="263"/>
       <c r="B44" s="83" t="s">
         <v>220</v>
       </c>
@@ -29306,7 +29309,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="220" t="s">
+      <c r="A45" s="264" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="86"/>
@@ -29319,7 +29322,7 @@
       <c r="AMJ45" s="5"/>
     </row>
     <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="221"/>
+      <c r="A46" s="265"/>
       <c r="B46" s="88" t="s">
         <v>73</v>
       </c>
@@ -29337,7 +29340,7 @@
       <c r="H46" s="90"/>
     </row>
     <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="221"/>
+      <c r="A47" s="265"/>
       <c r="B47" s="88" t="s">
         <v>76</v>
       </c>
@@ -29355,7 +29358,7 @@
       <c r="H47" s="90"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="222"/>
+      <c r="A48" s="266"/>
       <c r="B48" s="91" t="s">
         <v>79</v>
       </c>
@@ -29373,7 +29376,7 @@
       <c r="H48" s="93"/>
     </row>
     <row r="49" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="223" t="s">
+      <c r="A49" s="267" t="s">
         <v>226</v>
       </c>
       <c r="B49" s="96"/>
@@ -29404,7 +29407,7 @@
       <c r="AMJ49" s="5"/>
     </row>
     <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="224"/>
+      <c r="A50" s="262"/>
       <c r="B50" s="80" t="s">
         <v>227</v>
       </c>
@@ -29422,7 +29425,7 @@
       <c r="H50" s="82"/>
     </row>
     <row r="51" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="224"/>
+      <c r="A51" s="262"/>
       <c r="B51" s="80" t="s">
         <v>229</v>
       </c>
@@ -29440,7 +29443,7 @@
       <c r="H51" s="82"/>
     </row>
     <row r="52" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="224"/>
+      <c r="A52" s="262"/>
       <c r="B52" s="80" t="s">
         <v>46</v>
       </c>
@@ -29458,7 +29461,7 @@
       <c r="H52" s="82"/>
     </row>
     <row r="53" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="224"/>
+      <c r="A53" s="262"/>
       <c r="B53" s="80" t="s">
         <v>48</v>
       </c>
@@ -29476,7 +29479,7 @@
       <c r="H53" s="82"/>
     </row>
     <row r="54" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="224"/>
+      <c r="A54" s="262"/>
       <c r="B54" s="80" t="s">
         <v>61</v>
       </c>
@@ -29514,7 +29517,7 @@
       <c r="AMJ54" s="5"/>
     </row>
     <row r="55" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="224"/>
+      <c r="A55" s="262"/>
       <c r="B55" s="80" t="s">
         <v>63</v>
       </c>
@@ -29532,7 +29535,7 @@
       <c r="H55" s="82"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="224"/>
+      <c r="A56" s="262"/>
       <c r="B56" s="80" t="s">
         <v>65</v>
       </c>
@@ -29550,7 +29553,7 @@
       <c r="H56" s="82"/>
     </row>
     <row r="57" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="224"/>
+      <c r="A57" s="262"/>
       <c r="B57" s="80" t="s">
         <v>67</v>
       </c>
@@ -29568,7 +29571,7 @@
       <c r="H57" s="82"/>
     </row>
     <row r="58" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="225"/>
+      <c r="A58" s="263"/>
       <c r="B58" s="83" t="s">
         <v>69</v>
       </c>
@@ -29586,7 +29589,7 @@
       <c r="H58" s="85"/>
     </row>
     <row r="59" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="220" t="s">
+      <c r="A59" s="264" t="s">
         <v>465</v>
       </c>
       <c r="B59" s="98"/>
@@ -29599,7 +29602,7 @@
       <c r="AMJ59" s="5"/>
     </row>
     <row r="60" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="222"/>
+      <c r="A60" s="266"/>
       <c r="B60" s="91" t="s">
         <v>5</v>
       </c>
@@ -29661,16 +29664,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>455</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
@@ -30715,7 +30718,7 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="277" t="s">
         <v>466</v>
       </c>
       <c r="B3" s="96"/>
@@ -30740,7 +30743,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
+      <c r="A4" s="278"/>
       <c r="B4" s="80" t="s">
         <v>192</v>
       </c>
@@ -30760,7 +30763,7 @@
       <c r="H4" s="101"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
+      <c r="A5" s="278"/>
       <c r="B5" s="80" t="s">
         <v>283</v>
       </c>
@@ -30780,7 +30783,7 @@
       <c r="H5" s="101"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
+      <c r="A6" s="278"/>
       <c r="B6" s="80" t="s">
         <v>473</v>
       </c>
@@ -30800,7 +30803,7 @@
       <c r="H6" s="101"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="278"/>
       <c r="B7" s="80" t="s">
         <v>286</v>
       </c>
@@ -30820,7 +30823,7 @@
       <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="239" t="s">
+      <c r="A8" s="280" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="98"/>
@@ -30833,7 +30836,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="241"/>
+      <c r="A9" s="282"/>
       <c r="B9" s="88" t="s">
         <v>289</v>
       </c>
@@ -31869,7 +31872,7 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="241"/>
+      <c r="A10" s="282"/>
       <c r="B10" s="88" t="s">
         <v>474</v>
       </c>
@@ -32905,7 +32908,7 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="241"/>
+      <c r="A11" s="282"/>
       <c r="B11" s="88" t="s">
         <v>294</v>
       </c>
@@ -33941,7 +33944,7 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="241"/>
+      <c r="A12" s="282"/>
       <c r="B12" s="88" t="s">
         <v>475</v>
       </c>
@@ -34977,7 +34980,7 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="241"/>
+      <c r="A13" s="282"/>
       <c r="B13" s="88" t="s">
         <v>291</v>
       </c>
@@ -36013,7 +36016,7 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="236" t="s">
+      <c r="A14" s="277" t="s">
         <v>467</v>
       </c>
       <c r="B14" s="96"/>
@@ -36034,7 +36037,7 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="238"/>
+      <c r="A15" s="279"/>
       <c r="B15" s="83" t="s">
         <v>298</v>
       </c>
@@ -37070,7 +37073,7 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="1:1024" s="36" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="239" t="s">
+      <c r="A16" s="280" t="s">
         <v>301</v>
       </c>
       <c r="B16" s="86"/>
@@ -38098,7 +38101,7 @@
       <c r="AMJ16" s="35"/>
     </row>
     <row r="17" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="241"/>
+      <c r="A17" s="282"/>
       <c r="B17" s="88" t="s">
         <v>90</v>
       </c>
@@ -38118,7 +38121,7 @@
       <c r="H17" s="104"/>
     </row>
     <row r="18" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="241"/>
+      <c r="A18" s="282"/>
       <c r="B18" s="88" t="s">
         <v>94</v>
       </c>
@@ -38138,7 +38141,7 @@
       <c r="H18" s="104"/>
     </row>
     <row r="19" spans="1:1024" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="240"/>
+      <c r="A19" s="281"/>
       <c r="B19" s="91" t="s">
         <v>97</v>
       </c>
@@ -38158,7 +38161,7 @@
       <c r="H19" s="105"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="236" t="s">
+      <c r="A20" s="277" t="s">
         <v>306</v>
       </c>
       <c r="B20" s="96"/>
@@ -38178,9 +38181,9 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="237"/>
+      <c r="A21" s="278"/>
       <c r="B21" s="80" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C21" s="81"/>
       <c r="D21" s="80" t="s">
@@ -38190,7 +38193,7 @@
         <v>447</v>
       </c>
       <c r="F21" s="80" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="G21" s="165" t="s">
         <v>307</v>
@@ -38198,7 +38201,7 @@
       <c r="H21" s="101"/>
     </row>
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="237"/>
+      <c r="A22" s="278"/>
       <c r="B22" s="80" t="s">
         <v>516</v>
       </c>
@@ -38210,7 +38213,7 @@
         <v>449</v>
       </c>
       <c r="F22" s="80" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="G22" s="165" t="s">
         <v>308</v>
@@ -38218,7 +38221,7 @@
       <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="238"/>
+      <c r="A23" s="279"/>
       <c r="B23" s="83" t="s">
         <v>477</v>
       </c>
@@ -38238,7 +38241,7 @@
       <c r="H23" s="102"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="239" t="s">
+      <c r="A24" s="280" t="s">
         <v>468</v>
       </c>
       <c r="B24" s="107"/>
@@ -38251,7 +38254,7 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="240"/>
+      <c r="A25" s="281"/>
       <c r="B25" s="91" t="s">
         <v>311</v>
       </c>
@@ -38269,7 +38272,7 @@
       <c r="H25" s="105"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="236" t="s">
+      <c r="A26" s="277" t="s">
         <v>314</v>
       </c>
       <c r="B26" s="96"/>
@@ -38289,7 +38292,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="237"/>
+      <c r="A27" s="278"/>
       <c r="B27" s="80" t="s">
         <v>105</v>
       </c>
@@ -38301,7 +38304,7 @@
         <v>442</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="G27" s="165" t="s">
         <v>43</v>
@@ -38309,7 +38312,7 @@
       <c r="H27" s="101"/>
     </row>
     <row r="28" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="237"/>
+      <c r="A28" s="278"/>
       <c r="B28" s="80" t="s">
         <v>113</v>
       </c>
@@ -38329,7 +38332,7 @@
       <c r="H28" s="101"/>
     </row>
     <row r="29" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="237"/>
+      <c r="A29" s="278"/>
       <c r="B29" s="80" t="s">
         <v>117</v>
       </c>
@@ -38349,7 +38352,7 @@
       <c r="H29" s="101"/>
     </row>
     <row r="30" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="237"/>
+      <c r="A30" s="278"/>
       <c r="B30" s="80" t="s">
         <v>121</v>
       </c>
@@ -38369,7 +38372,7 @@
       <c r="H30" s="101"/>
     </row>
     <row r="31" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="238"/>
+      <c r="A31" s="279"/>
       <c r="B31" s="83" t="s">
         <v>125</v>
       </c>
@@ -38389,7 +38392,7 @@
       <c r="H31" s="102"/>
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="239" t="s">
+      <c r="A32" s="280" t="s">
         <v>319</v>
       </c>
       <c r="B32" s="98"/>
@@ -38402,7 +38405,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="241"/>
+      <c r="A33" s="282"/>
       <c r="B33" s="88" t="s">
         <v>129</v>
       </c>
@@ -38422,7 +38425,7 @@
       <c r="H33" s="104"/>
     </row>
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="241"/>
+      <c r="A34" s="282"/>
       <c r="B34" s="88" t="s">
         <v>517</v>
       </c>
@@ -38440,7 +38443,7 @@
       <c r="H34" s="197"/>
     </row>
     <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="240"/>
+      <c r="A35" s="281"/>
       <c r="B35" s="91" t="s">
         <v>320</v>
       </c>
@@ -38509,16 +38512,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -38547,7 +38550,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="223" t="s">
+      <c r="A3" s="267" t="s">
         <v>469</v>
       </c>
       <c r="B3" s="18"/>
@@ -38574,7 +38577,7 @@
       <c r="AMJ3" s="109"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="224"/>
+      <c r="A4" s="262"/>
       <c r="B4" s="81" t="s">
         <v>192</v>
       </c>
@@ -38594,7 +38597,7 @@
       <c r="H4" s="112"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="224"/>
+      <c r="A5" s="262"/>
       <c r="B5" s="81" t="s">
         <v>242</v>
       </c>
@@ -38614,7 +38617,7 @@
       <c r="H5" s="112"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="224"/>
+      <c r="A6" s="262"/>
       <c r="B6" s="81" t="s">
         <v>198</v>
       </c>
@@ -38632,7 +38635,7 @@
       <c r="H6" s="112"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
+      <c r="A7" s="262"/>
       <c r="B7" s="81" t="s">
         <v>248</v>
       </c>
@@ -38652,7 +38655,7 @@
       <c r="H7" s="112"/>
     </row>
     <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="224"/>
+      <c r="A8" s="262"/>
       <c r="B8" s="81" t="s">
         <v>251</v>
       </c>
@@ -38672,7 +38675,7 @@
       <c r="H8" s="112"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="224"/>
+      <c r="A9" s="262"/>
       <c r="B9" s="81" t="s">
         <v>254</v>
       </c>
@@ -38692,7 +38695,7 @@
       <c r="H9" s="112"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="224"/>
+      <c r="A10" s="262"/>
       <c r="B10" s="81" t="s">
         <v>195</v>
       </c>
@@ -38710,7 +38713,7 @@
       <c r="H10" s="112"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="224"/>
+      <c r="A11" s="262"/>
       <c r="B11" s="81" t="s">
         <v>261</v>
       </c>
@@ -38728,7 +38731,7 @@
       <c r="H11" s="112"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="262"/>
       <c r="B12" s="81" t="s">
         <v>329</v>
       </c>
@@ -38746,7 +38749,7 @@
       <c r="H12" s="112"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="262"/>
       <c r="B13" s="81" t="s">
         <v>267</v>
       </c>
@@ -38764,7 +38767,7 @@
       <c r="H13" s="112"/>
     </row>
     <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="224"/>
+      <c r="A14" s="262"/>
       <c r="B14" s="81" t="s">
         <v>333</v>
       </c>
@@ -38782,7 +38785,7 @@
       <c r="H14" s="112"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="224"/>
+      <c r="A15" s="262"/>
       <c r="B15" s="81" t="s">
         <v>336</v>
       </c>
@@ -38800,7 +38803,7 @@
       <c r="H15" s="112"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="262"/>
       <c r="B16" s="81" t="s">
         <v>339</v>
       </c>
@@ -38818,7 +38821,7 @@
       <c r="H16" s="112"/>
     </row>
     <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="262"/>
       <c r="B17" s="81" t="s">
         <v>343</v>
       </c>
@@ -38836,7 +38839,7 @@
       <c r="H17" s="112"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="263"/>
       <c r="B18" s="84" t="s">
         <v>279</v>
       </c>
@@ -38873,14 +38876,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BJ23"/>
+  <dimension ref="A1:BJ20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A16"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38897,16 +38900,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -38935,7 +38938,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="119" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="242" t="s">
+      <c r="A3" s="283" t="s">
         <v>469</v>
       </c>
       <c r="B3" s="117"/>
@@ -38947,7 +38950,7 @@
       <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="244"/>
+      <c r="A4" s="285"/>
       <c r="B4" s="81" t="s">
         <v>192</v>
       </c>
@@ -38976,7 +38979,7 @@
       <c r="Q4" s="119"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="244"/>
+      <c r="A5" s="285"/>
       <c r="B5" s="81" t="s">
         <v>242</v>
       </c>
@@ -39005,7 +39008,7 @@
       <c r="Q5" s="119"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="244"/>
+      <c r="A6" s="285"/>
       <c r="B6" s="81" t="s">
         <v>198</v>
       </c>
@@ -39032,7 +39035,7 @@
       <c r="Q6" s="119"/>
     </row>
     <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="244"/>
+      <c r="A7" s="285"/>
       <c r="B7" s="81" t="s">
         <v>248</v>
       </c>
@@ -39061,7 +39064,7 @@
       <c r="Q7" s="119"/>
     </row>
     <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="244"/>
+      <c r="A8" s="285"/>
       <c r="B8" s="81" t="s">
         <v>251</v>
       </c>
@@ -39090,7 +39093,7 @@
       <c r="Q8" s="119"/>
     </row>
     <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
+      <c r="A9" s="285"/>
       <c r="B9" s="81" t="s">
         <v>254</v>
       </c>
@@ -39119,7 +39122,7 @@
       <c r="Q9" s="119"/>
     </row>
     <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="244"/>
+      <c r="A10" s="285"/>
       <c r="B10" s="81" t="s">
         <v>195</v>
       </c>
@@ -39146,7 +39149,7 @@
       <c r="Q10" s="119"/>
     </row>
     <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="244"/>
+      <c r="A11" s="285"/>
       <c r="B11" s="81" t="s">
         <v>261</v>
       </c>
@@ -39173,7 +39176,7 @@
       <c r="Q11" s="119"/>
     </row>
     <row r="12" spans="1:17" s="126" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="244"/>
+      <c r="A12" s="285"/>
       <c r="B12" s="81" t="s">
         <v>264</v>
       </c>
@@ -39200,7 +39203,7 @@
       <c r="Q12" s="119"/>
     </row>
     <row r="13" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="244"/>
+      <c r="A13" s="285"/>
       <c r="B13" s="81" t="s">
         <v>267</v>
       </c>
@@ -39227,7 +39230,7 @@
       <c r="Q13" s="119"/>
     </row>
     <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="244"/>
+      <c r="A14" s="285"/>
       <c r="B14" s="81" t="s">
         <v>271</v>
       </c>
@@ -39254,7 +39257,7 @@
       <c r="Q14" s="119"/>
     </row>
     <row r="15" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="244"/>
+      <c r="A15" s="285"/>
       <c r="B15" s="81" t="s">
         <v>275</v>
       </c>
@@ -39281,7 +39284,7 @@
       <c r="Q15" s="119"/>
     </row>
     <row r="16" spans="1:17" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="245"/>
+      <c r="A16" s="286"/>
       <c r="B16" s="84" t="s">
         <v>279</v>
       </c>
@@ -39307,63 +39310,63 @@
       <c r="P16" s="119"/>
       <c r="Q16" s="119"/>
     </row>
-    <row r="17" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="242" t="s">
-        <v>569</v>
-      </c>
-      <c r="B17" s="212"/>
-      <c r="C17" s="212"/>
-      <c r="D17" s="212"/>
-      <c r="E17" s="212"/>
-      <c r="F17" s="212"/>
-      <c r="G17" s="213"/>
-      <c r="H17" s="214"/>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119"/>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="119"/>
-      <c r="N17" s="119"/>
-      <c r="O17" s="119"/>
-      <c r="P17" s="119"/>
-      <c r="Q17" s="119"/>
+    <row r="17" spans="1:17" s="293" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="288" t="s">
+        <v>566</v>
+      </c>
+      <c r="B17" s="289"/>
+      <c r="C17" s="289"/>
+      <c r="D17" s="289"/>
+      <c r="E17" s="289"/>
+      <c r="F17" s="289"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="291"/>
+      <c r="I17" s="292"/>
+      <c r="J17" s="292"/>
+      <c r="K17" s="292"/>
+      <c r="L17" s="292"/>
+      <c r="M17" s="292"/>
+      <c r="N17" s="292"/>
+      <c r="O17" s="292"/>
+      <c r="P17" s="292"/>
+      <c r="Q17" s="292"/>
     </row>
-    <row r="18" spans="1:17" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="243"/>
-      <c r="B18" s="84" t="s">
+    <row r="18" spans="1:17" s="293" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="294"/>
+      <c r="B18" s="295" t="s">
         <v>541</v>
       </c>
-      <c r="C18" s="84"/>
-      <c r="D18" s="83" t="s">
-        <v>559</v>
-      </c>
-      <c r="E18" s="113"/>
-      <c r="F18" s="84" t="s">
+      <c r="C18" s="295"/>
+      <c r="D18" s="296" t="s">
+        <v>573</v>
+      </c>
+      <c r="E18" s="297"/>
+      <c r="F18" s="295" t="s">
         <v>542</v>
       </c>
-      <c r="G18" s="166"/>
-      <c r="H18" s="211"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="121"/>
-      <c r="K18" s="122"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="121"/>
-      <c r="O18" s="122"/>
-      <c r="P18" s="119"/>
-      <c r="Q18" s="119"/>
+      <c r="G18" s="298"/>
+      <c r="H18" s="299"/>
+      <c r="I18" s="292"/>
+      <c r="J18" s="300"/>
+      <c r="K18" s="301"/>
+      <c r="L18" s="292"/>
+      <c r="M18" s="292"/>
+      <c r="N18" s="300"/>
+      <c r="O18" s="301"/>
+      <c r="P18" s="292"/>
+      <c r="Q18" s="292"/>
     </row>
     <row r="19" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="242" t="s">
+      <c r="A19" s="283" t="s">
         <v>274</v>
       </c>
-      <c r="B19" s="212"/>
-      <c r="C19" s="212"/>
-      <c r="D19" s="215"/>
-      <c r="E19" s="216"/>
-      <c r="F19" s="212"/>
-      <c r="G19" s="213"/>
-      <c r="H19" s="217"/>
+      <c r="B19" s="207"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="209"/>
+      <c r="E19" s="210"/>
+      <c r="F19" s="207"/>
+      <c r="G19" s="208"/>
+      <c r="H19" s="211"/>
       <c r="I19" s="119"/>
       <c r="J19" s="121"/>
       <c r="K19" s="122"/>
@@ -39375,20 +39378,20 @@
       <c r="Q19" s="119"/>
     </row>
     <row r="20" spans="1:17" ht="48" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="243"/>
+      <c r="A20" s="284"/>
       <c r="B20" s="84" t="s">
         <v>274</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="83" t="s">
-        <v>553</v>
+        <v>574</v>
       </c>
       <c r="E20" s="113"/>
       <c r="F20" s="84" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G20" s="166"/>
-      <c r="H20" s="211"/>
+      <c r="H20" s="206"/>
       <c r="I20" s="119"/>
       <c r="J20" s="121"/>
       <c r="K20" s="122"/>
@@ -39399,9 +39402,6 @@
       <c r="P20" s="119"/>
       <c r="Q20" s="119"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -39418,14 +39418,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -39443,18 +39443,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>552</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
-    <row r="2" spans="1:20" s="127" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="127" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
@@ -39480,64 +39480,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="127" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="201" t="s">
-        <v>554</v>
-      </c>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="200"/>
+    <row r="3" spans="1:20" s="131" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="267" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
     </row>
-    <row r="4" spans="1:20" s="131" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="223" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
-      <c r="K4" s="130"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="130"/>
-      <c r="O4" s="130"/>
-      <c r="P4" s="130"/>
-      <c r="Q4" s="130"/>
-      <c r="R4" s="130"/>
-      <c r="S4" s="130"/>
-      <c r="T4" s="130"/>
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="262"/>
+      <c r="B4" s="132" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="G4" s="155" t="s">
+        <v>463</v>
+      </c>
+      <c r="H4" s="133"/>
     </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224"/>
+    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="262"/>
       <c r="B5" s="132" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5" s="132"/>
       <c r="D5" s="132" t="s">
-        <v>193</v>
+        <v>9</v>
       </c>
       <c r="E5" s="132"/>
       <c r="F5" s="132" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G5" s="155" t="s">
-        <v>463</v>
+        <v>12</v>
       </c>
       <c r="H5" s="133"/>
     </row>
-    <row r="6" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="224"/>
+    <row r="6" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="262"/>
       <c r="B6" s="132" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="132"/>
       <c r="D6" s="132" t="s">
@@ -39545,235 +39551,214 @@
       </c>
       <c r="E6" s="132"/>
       <c r="F6" s="132" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G6" s="155" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="133"/>
     </row>
-    <row r="7" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
-      <c r="B7" s="132" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132" t="s">
-        <v>348</v>
-      </c>
-      <c r="G7" s="155" t="s">
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="263"/>
+      <c r="B7" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134" t="s">
+        <v>451</v>
+      </c>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134" t="s">
+        <v>349</v>
+      </c>
+      <c r="G7" s="156" t="s">
+        <v>463</v>
+      </c>
+      <c r="H7" s="135"/>
+    </row>
+    <row r="8" spans="1:20" s="130" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="264" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" s="136"/>
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="137"/>
+    </row>
+    <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="265"/>
+      <c r="B9" s="138" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138" t="s">
+        <v>350</v>
+      </c>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138" t="s">
+        <v>351</v>
+      </c>
+      <c r="G9" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="133"/>
+      <c r="H9" s="139"/>
     </row>
-    <row r="8" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="225"/>
-      <c r="B8" s="134" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134" t="s">
-        <v>451</v>
-      </c>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134" t="s">
-        <v>349</v>
-      </c>
-      <c r="G8" s="156" t="s">
-        <v>463</v>
-      </c>
-      <c r="H8" s="135"/>
-    </row>
-    <row r="9" spans="1:20" s="130" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="220" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" s="136"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="137"/>
-    </row>
-    <row r="10" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="221"/>
+    <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="265"/>
       <c r="B10" s="138" t="s">
-        <v>30</v>
+        <v>352</v>
       </c>
       <c r="C10" s="138"/>
       <c r="D10" s="138" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E10" s="138"/>
       <c r="F10" s="138" t="s">
-        <v>351</v>
-      </c>
-      <c r="G10" s="182" t="s">
-        <v>12</v>
-      </c>
+        <v>471</v>
+      </c>
+      <c r="G10" s="158"/>
       <c r="H10" s="139"/>
     </row>
-    <row r="11" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="221"/>
-      <c r="B11" s="138" t="s">
-        <v>352</v>
-      </c>
-      <c r="C11" s="138"/>
+    <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="265"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="138" t="s">
+        <v>354</v>
+      </c>
       <c r="D11" s="138" t="s">
-        <v>353</v>
+        <v>193</v>
       </c>
       <c r="E11" s="138"/>
       <c r="F11" s="138" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="G11" s="158"/>
       <c r="H11" s="139"/>
     </row>
-    <row r="12" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="221"/>
+    <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="265"/>
       <c r="B12" s="138"/>
       <c r="C12" s="138" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D12" s="138" t="s">
         <v>193</v>
       </c>
       <c r="E12" s="138"/>
       <c r="F12" s="138" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G12" s="158"/>
       <c r="H12" s="139"/>
     </row>
-    <row r="13" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="221"/>
+    <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="265"/>
       <c r="B13" s="138"/>
       <c r="C13" s="138" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D13" s="138" t="s">
         <v>193</v>
       </c>
       <c r="E13" s="138"/>
       <c r="F13" s="138" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="G13" s="158"/>
       <c r="H13" s="139"/>
     </row>
-    <row r="14" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="221"/>
+    <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="265"/>
       <c r="B14" s="138"/>
       <c r="C14" s="138" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D14" s="138" t="s">
-        <v>193</v>
+        <v>462</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="138" t="s">
-        <v>461</v>
+        <v>358</v>
       </c>
       <c r="G14" s="158"/>
       <c r="H14" s="139"/>
     </row>
-    <row r="15" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="221"/>
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="265"/>
       <c r="B15" s="138"/>
       <c r="C15" s="138" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D15" s="138" t="s">
-        <v>462</v>
+        <v>296</v>
       </c>
       <c r="E15" s="138"/>
       <c r="F15" s="138" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G15" s="158"/>
       <c r="H15" s="139"/>
     </row>
-    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="221"/>
+    <row r="16" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="265"/>
       <c r="B16" s="138"/>
       <c r="C16" s="138" t="s">
-        <v>359</v>
+        <v>538</v>
       </c>
       <c r="D16" s="138" t="s">
-        <v>296</v>
-      </c>
-      <c r="E16" s="138"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="138" t="s">
+        <v>540</v>
+      </c>
       <c r="F16" s="138" t="s">
-        <v>360</v>
+        <v>539</v>
       </c>
       <c r="G16" s="158"/>
       <c r="H16" s="139"/>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="221"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138" t="s">
-        <v>538</v>
-      </c>
+    <row r="17" spans="1:8" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="265"/>
+      <c r="B17" s="138" t="s">
+        <v>361</v>
+      </c>
+      <c r="C17" s="138"/>
       <c r="D17" s="138" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="138" t="s">
-        <v>540</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="E17" s="138"/>
       <c r="F17" s="138" t="s">
-        <v>539</v>
+        <v>472</v>
       </c>
       <c r="G17" s="158"/>
       <c r="H17" s="139"/>
     </row>
-    <row r="18" spans="1:8" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="221"/>
-      <c r="B18" s="138" t="s">
-        <v>361</v>
-      </c>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138" t="s">
-        <v>353</v>
-      </c>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138" t="s">
-        <v>472</v>
-      </c>
-      <c r="G18" s="158"/>
-      <c r="H18" s="139"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="222"/>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140" t="s">
+    <row r="18" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="266"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="140" t="s">
         <v>359</v>
       </c>
-      <c r="D19" s="140" t="s">
+      <c r="D18" s="140" t="s">
         <v>296</v>
       </c>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140" t="s">
+      <c r="E18" s="140"/>
+      <c r="F18" s="140" t="s">
         <v>362</v>
       </c>
-      <c r="G19" s="159"/>
-      <c r="H19" s="141"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="141"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A19"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A18"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A3" location="'DMA Tuple'!B16" display="*This substructure is part of [DMA Tuple](dma_tuple.md)*" xr:uid="{52E8B918-22AC-EA49-B23C-55BC94E32B06}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -39786,24 +39771,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E34272-1DAE-CB41-B732-6A741ADD2A30}">
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="142" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="142" customWidth="1"/>
-    <col min="3" max="4" width="20.7109375" style="204" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="204" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="204" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="205" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="199" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="199" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="199" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="200" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="110" customWidth="1"/>
     <col min="9" max="1023" width="10.42578125" style="110" hidden="1" customWidth="1"/>
     <col min="1024" max="1024" width="9.140625" style="110" hidden="1" customWidth="1"/>
@@ -39811,18 +39796,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="246" t="s">
-        <v>556</v>
-      </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="227"/>
+      <c r="A1" s="287" t="s">
+        <v>554</v>
+      </c>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="253"/>
     </row>
-    <row r="2" spans="1:20" s="203" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="198" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
@@ -39848,111 +39833,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="127" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="201" t="s">
-        <v>554</v>
-      </c>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="200"/>
+    <row r="3" spans="1:20" s="202" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="267" t="s">
+        <v>541</v>
+      </c>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="201"/>
+      <c r="J3" s="201"/>
+      <c r="K3" s="201"/>
+      <c r="L3" s="201"/>
+      <c r="M3" s="201"/>
+      <c r="N3" s="201"/>
+      <c r="O3" s="201"/>
+      <c r="P3" s="201"/>
+      <c r="Q3" s="201"/>
+      <c r="R3" s="201"/>
+      <c r="S3" s="201"/>
+      <c r="T3" s="201"/>
     </row>
-    <row r="4" spans="1:20" s="207" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="223" t="s">
-        <v>541</v>
-      </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="206"/>
-      <c r="J4" s="206"/>
-      <c r="K4" s="206"/>
-      <c r="L4" s="206"/>
-      <c r="M4" s="206"/>
-      <c r="N4" s="206"/>
-      <c r="O4" s="206"/>
-      <c r="P4" s="206"/>
-      <c r="Q4" s="206"/>
-      <c r="R4" s="206"/>
-      <c r="S4" s="206"/>
-      <c r="T4" s="206"/>
+    <row r="4" spans="1:20" s="126" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="262"/>
+      <c r="B4" s="80" t="s">
+        <v>557</v>
+      </c>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="132" t="s">
+        <v>564</v>
+      </c>
+      <c r="F4" s="132" t="s">
+        <v>555</v>
+      </c>
+      <c r="G4" s="155" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="133"/>
     </row>
-    <row r="5" spans="1:20" s="126" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224"/>
-      <c r="B5" s="80" t="s">
-        <v>560</v>
-      </c>
-      <c r="C5" s="132"/>
+    <row r="5" spans="1:20" s="126" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="262"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="132" t="s">
+        <v>558</v>
+      </c>
       <c r="D5" s="132" t="s">
-        <v>566</v>
+        <v>193</v>
       </c>
       <c r="E5" s="132" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="F5" s="132" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="G5" s="155" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="133"/>
     </row>
-    <row r="6" spans="1:20" s="126" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="224"/>
+    <row r="6" spans="1:20" s="126" customFormat="1" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="262"/>
       <c r="B6" s="132"/>
-      <c r="C6" s="132" t="s">
-        <v>561</v>
-      </c>
-      <c r="D6" s="132" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="132" t="s">
-        <v>558</v>
-      </c>
-      <c r="F6" s="132" t="s">
-        <v>568</v>
-      </c>
-      <c r="G6" s="155" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="155"/>
       <c r="H6" s="133"/>
     </row>
-    <row r="7" spans="1:20" s="126" customFormat="1" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="155"/>
-      <c r="H7" s="133"/>
-    </row>
-    <row r="8" spans="1:20" s="208" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="225"/>
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="156"/>
-      <c r="H8" s="135"/>
+    <row r="7" spans="1:20" s="203" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="263"/>
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="135"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A3:A7"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A3" location="'DMA Tuple'!B15" display="*This substructure is part of [DMA Tuple](dma_tuple.md)*" xr:uid="{B8007B79-FF0D-2248-83A7-B34D7B7972A9}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -39988,16 +39958,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="252" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:1024" s="38" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -41042,7 +41012,7 @@
       <c r="AMJ2" s="37"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="223" t="s">
+      <c r="A3" s="267" t="s">
         <v>363</v>
       </c>
       <c r="B3" s="144"/>
@@ -41054,7 +41024,7 @@
       <c r="H3" s="145"/>
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224"/>
+      <c r="A4" s="262"/>
       <c r="B4" s="43" t="s">
         <v>192</v>
       </c>
@@ -42086,7 +42056,7 @@
       <c r="AMJ4" s="23"/>
     </row>
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="224"/>
+      <c r="A5" s="262"/>
       <c r="B5" s="43" t="s">
         <v>242</v>
       </c>
@@ -43118,7 +43088,7 @@
       <c r="AMJ5" s="23"/>
     </row>
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="224"/>
+      <c r="A6" s="262"/>
       <c r="B6" s="43" t="s">
         <v>198</v>
       </c>
@@ -44150,7 +44120,7 @@
       <c r="AMJ6" s="23"/>
     </row>
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
+      <c r="A7" s="262"/>
       <c r="B7" s="43" t="s">
         <v>366</v>
       </c>
@@ -45182,7 +45152,7 @@
       <c r="AMJ7" s="23"/>
     </row>
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="224"/>
+      <c r="A8" s="262"/>
       <c r="B8" s="43" t="s">
         <v>368</v>
       </c>
@@ -46214,7 +46184,7 @@
       <c r="AMJ8" s="23"/>
     </row>
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="224"/>
+      <c r="A9" s="262"/>
       <c r="B9" s="43" t="s">
         <v>370</v>
       </c>
@@ -47246,7 +47216,7 @@
       <c r="AMJ9" s="23"/>
     </row>
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="224"/>
+      <c r="A10" s="262"/>
       <c r="B10" s="43" t="s">
         <v>372</v>
       </c>
@@ -48278,7 +48248,7 @@
       <c r="AMJ10" s="23"/>
     </row>
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="224"/>
+      <c r="A11" s="262"/>
       <c r="B11" s="43" t="s">
         <v>374</v>
       </c>
@@ -49310,7 +49280,7 @@
       <c r="AMJ11" s="23"/>
     </row>
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="225"/>
+      <c r="A12" s="263"/>
       <c r="B12" s="47" t="s">
         <v>376</v>
       </c>
@@ -50342,7 +50312,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="220" t="s">
+      <c r="A13" s="264" t="s">
         <v>378</v>
       </c>
       <c r="B13" s="147"/>
@@ -50355,7 +50325,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="221"/>
+      <c r="A14" s="265"/>
       <c r="B14" s="65" t="s">
         <v>192</v>
       </c>
@@ -50371,7 +50341,7 @@
       <c r="H14" s="149"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="221"/>
+      <c r="A15" s="265"/>
       <c r="B15" s="65" t="s">
         <v>242</v>
       </c>
@@ -50387,7 +50357,7 @@
       <c r="H15" s="149"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="221"/>
+      <c r="A16" s="265"/>
       <c r="B16" s="65" t="s">
         <v>198</v>
       </c>
@@ -50403,7 +50373,7 @@
       <c r="H16" s="149"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="221"/>
+      <c r="A17" s="265"/>
       <c r="B17" s="65" t="s">
         <v>248</v>
       </c>
@@ -50419,7 +50389,7 @@
       <c r="H17" s="149"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="221"/>
+      <c r="A18" s="265"/>
       <c r="B18" s="65" t="s">
         <v>195</v>
       </c>
@@ -50435,7 +50405,7 @@
       <c r="H18" s="149"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="221"/>
+      <c r="A19" s="265"/>
       <c r="B19" s="65" t="s">
         <v>5</v>
       </c>
@@ -50451,7 +50421,7 @@
       <c r="H19" s="149"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="221"/>
+      <c r="A20" s="265"/>
       <c r="B20" s="65" t="s">
         <v>384</v>
       </c>
@@ -50467,7 +50437,7 @@
       <c r="H20" s="149"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="221"/>
+      <c r="A21" s="265"/>
       <c r="B21" s="65" t="s">
         <v>296</v>
       </c>
@@ -50483,7 +50453,7 @@
       <c r="H21" s="149"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="221"/>
+      <c r="A22" s="265"/>
       <c r="B22" s="65" t="s">
         <v>387</v>
       </c>
@@ -50499,7 +50469,7 @@
       <c r="H22" s="149"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="221"/>
+      <c r="A23" s="265"/>
       <c r="B23" s="65" t="s">
         <v>389</v>
       </c>
@@ -50515,7 +50485,7 @@
       <c r="H23" s="149"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="222"/>
+      <c r="A24" s="266"/>
       <c r="B24" s="69" t="s">
         <v>391</v>
       </c>
@@ -50531,7 +50501,7 @@
       <c r="H24" s="150"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="223" t="s">
+      <c r="A25" s="267" t="s">
         <v>329</v>
       </c>
       <c r="B25" s="151"/>
@@ -50543,7 +50513,7 @@
       <c r="H25" s="152"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="224"/>
+      <c r="A26" s="262"/>
       <c r="B26" s="43" t="s">
         <v>192</v>
       </c>
@@ -50559,7 +50529,7 @@
       <c r="H26" s="146"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="224"/>
+      <c r="A27" s="262"/>
       <c r="B27" s="43" t="s">
         <v>242</v>
       </c>
@@ -50575,7 +50545,7 @@
       <c r="H27" s="146"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="224"/>
+      <c r="A28" s="262"/>
       <c r="B28" s="43" t="s">
         <v>198</v>
       </c>
@@ -50591,7 +50561,7 @@
       <c r="H28" s="146"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="224"/>
+      <c r="A29" s="262"/>
       <c r="B29" s="43" t="s">
         <v>248</v>
       </c>
@@ -50607,7 +50577,7 @@
       <c r="H29" s="146"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="224"/>
+      <c r="A30" s="262"/>
       <c r="B30" s="43" t="s">
         <v>396</v>
       </c>
@@ -50623,7 +50593,7 @@
       <c r="H30" s="146"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="224"/>
+      <c r="A31" s="262"/>
       <c r="B31" s="43" t="s">
         <v>195</v>
       </c>
@@ -50639,7 +50609,7 @@
       <c r="H31" s="146"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="224"/>
+      <c r="A32" s="262"/>
       <c r="B32" s="43" t="s">
         <v>374</v>
       </c>
@@ -50655,7 +50625,7 @@
       <c r="H32" s="146"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="224"/>
+      <c r="A33" s="262"/>
       <c r="B33" s="43" t="s">
         <v>400</v>
       </c>
@@ -50671,7 +50641,7 @@
       <c r="H33" s="146"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="224"/>
+      <c r="A34" s="262"/>
       <c r="B34" s="43" t="s">
         <v>5</v>
       </c>
@@ -50687,7 +50657,7 @@
       <c r="H34" s="146"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="224"/>
+      <c r="A35" s="262"/>
       <c r="B35" s="43" t="s">
         <v>403</v>
       </c>
@@ -50703,7 +50673,7 @@
       <c r="H35" s="146"/>
     </row>
     <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="225"/>
+      <c r="A36" s="263"/>
       <c r="B36" s="47" t="s">
         <v>405</v>
       </c>
@@ -50719,7 +50689,7 @@
       <c r="H36" s="153"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="220" t="s">
+      <c r="A37" s="264" t="s">
         <v>264</v>
       </c>
       <c r="B37" s="147"/>
@@ -50732,7 +50702,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="221"/>
+      <c r="A38" s="265"/>
       <c r="B38" s="65" t="s">
         <v>192</v>
       </c>
@@ -50748,7 +50718,7 @@
       <c r="H38" s="149"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="221"/>
+      <c r="A39" s="265"/>
       <c r="B39" s="65" t="s">
         <v>242</v>
       </c>
@@ -50764,7 +50734,7 @@
       <c r="H39" s="149"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="221"/>
+      <c r="A40" s="265"/>
       <c r="B40" s="65" t="s">
         <v>198</v>
       </c>
@@ -50780,7 +50750,7 @@
       <c r="H40" s="149"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="221"/>
+      <c r="A41" s="265"/>
       <c r="B41" s="65" t="s">
         <v>248</v>
       </c>
@@ -50796,7 +50766,7 @@
       <c r="H41" s="149"/>
     </row>
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="221"/>
+      <c r="A42" s="265"/>
       <c r="B42" s="65" t="s">
         <v>410</v>
       </c>
@@ -50812,7 +50782,7 @@
       <c r="H42" s="149"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="221"/>
+      <c r="A43" s="265"/>
       <c r="B43" s="65" t="s">
         <v>329</v>
       </c>
@@ -50828,7 +50798,7 @@
       <c r="H43" s="149"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="221"/>
+      <c r="A44" s="265"/>
       <c r="B44" s="65" t="s">
         <v>195</v>
       </c>
@@ -50844,7 +50814,7 @@
       <c r="H44" s="149"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="221"/>
+      <c r="A45" s="265"/>
       <c r="B45" s="65" t="s">
         <v>374</v>
       </c>
@@ -50860,7 +50830,7 @@
       <c r="H45" s="149"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="221"/>
+      <c r="A46" s="265"/>
       <c r="B46" s="65" t="s">
         <v>415</v>
       </c>
@@ -50876,7 +50846,7 @@
       <c r="H46" s="149"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="221"/>
+      <c r="A47" s="265"/>
       <c r="B47" s="65" t="s">
         <v>5</v>
       </c>
@@ -50892,7 +50862,7 @@
       <c r="H47" s="149"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="222"/>
+      <c r="A48" s="266"/>
       <c r="B48" s="69" t="s">
         <v>387</v>
       </c>

</xml_diff>

<commit_message>
fix: ensure condition is always specified
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jay\code\digitbrain.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A3DCFA-7CF9-44EB-A599-5B78654F4D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F4433-207D-4F15-8FA1-B12111D878D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="574">
   <si>
     <t>Concept</t>
   </si>
@@ -1732,9 +1732,6 @@
     <t>[s3-server]\n    access_key: 123abc</t>
   </si>
   <si>
-    <t>required</t>
-  </si>
-  <si>
     <t>/data/rclone.conf</t>
   </si>
   <si>
@@ -1753,9 +1750,6 @@
     <t>DataAssetsMapping</t>
   </si>
   <si>
-    <t>Mapping the available Data assets in this DMA Tuple to available Microservices. Required if Data assets are required. Not all microservices need a Data asset.</t>
-  </si>
-  <si>
     <t>PATH</t>
   </si>
   <si>
@@ -1850,6 +1844,9 @@
   </si>
   <si>
     <t>[Deployment](../deployment.md)</t>
+  </si>
+  <si>
+    <t>Mapping required Data assets to Microservices specified in the MA Pair. Not every Microservice needs a Data asset.</t>
   </si>
 </sst>
 </file>
@@ -3350,32 +3347,51 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="13" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3387,30 +3403,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3440,6 +3432,58 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3482,6 +3526,14 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3492,61 +3544,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4442,7 +4439,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39:A52"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4459,16 +4456,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>452</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -4497,7 +4494,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="256" t="s">
+      <c r="A3" s="278" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -4509,7 +4506,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="257"/>
+      <c r="A4" s="279"/>
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -4529,7 +4526,7 @@
       <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="257"/>
+      <c r="A5" s="279"/>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
@@ -4549,7 +4546,7 @@
       <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="257"/>
+      <c r="A6" s="279"/>
       <c r="B6" s="43" t="s">
         <v>16</v>
       </c>
@@ -4569,7 +4566,7 @@
       <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="257"/>
+      <c r="A7" s="279"/>
       <c r="B7" s="43" t="s">
         <v>19</v>
       </c>
@@ -4589,7 +4586,7 @@
       <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="257"/>
+      <c r="A8" s="279"/>
       <c r="B8" s="43" t="s">
         <v>22</v>
       </c>
@@ -4609,7 +4606,7 @@
       <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="257"/>
+      <c r="A9" s="279"/>
       <c r="B9" s="43" t="s">
         <v>25</v>
       </c>
@@ -4629,7 +4626,7 @@
       <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
+      <c r="A10" s="279"/>
       <c r="B10" s="43" t="s">
         <v>26</v>
       </c>
@@ -4649,7 +4646,7 @@
       <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:1024" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="258"/>
+      <c r="A11" s="280"/>
       <c r="B11" s="47" t="s">
         <v>30</v>
       </c>
@@ -4669,7 +4666,7 @@
       <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="259" t="s">
+      <c r="A12" s="264" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="184"/>
@@ -4681,7 +4678,7 @@
       <c r="H12" s="187"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="260"/>
+      <c r="A13" s="265"/>
       <c r="B13" s="51" t="s">
         <v>35</v>
       </c>
@@ -4701,7 +4698,7 @@
       <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="260"/>
+      <c r="A14" s="265"/>
       <c r="B14" s="51" t="s">
         <v>38</v>
       </c>
@@ -4721,7 +4718,7 @@
       <c r="H14" s="54"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="260"/>
+      <c r="A15" s="265"/>
       <c r="B15" s="51" t="s">
         <v>426</v>
       </c>
@@ -4730,7 +4727,7 @@
         <v>529</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F15" s="51" t="s">
         <v>427</v>
@@ -5757,7 +5754,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="260"/>
+      <c r="A16" s="265"/>
       <c r="B16" s="51"/>
       <c r="C16" s="52" t="s">
         <v>526</v>
@@ -5766,13 +5763,13 @@
         <v>9</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F16" s="51" t="s">
         <v>530</v>
       </c>
       <c r="G16" s="160" t="s">
-        <v>535</v>
+        <v>12</v>
       </c>
       <c r="H16" s="54"/>
       <c r="I16" s="4"/>
@@ -6793,7 +6790,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="260"/>
+      <c r="A17" s="265"/>
       <c r="B17" s="51"/>
       <c r="C17" s="52" t="s">
         <v>528</v>
@@ -6808,7 +6805,7 @@
         <v>531</v>
       </c>
       <c r="G17" s="160" t="s">
-        <v>535</v>
+        <v>12</v>
       </c>
       <c r="H17" s="54"/>
       <c r="I17" s="4"/>
@@ -7829,7 +7826,7 @@
       <c r="AMJ17" s="4"/>
     </row>
     <row r="18" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="260"/>
+      <c r="A18" s="265"/>
       <c r="B18" s="51"/>
       <c r="C18" s="52" t="s">
         <v>527</v>
@@ -8865,7 +8862,7 @@
       <c r="AMJ18" s="4"/>
     </row>
     <row r="19" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="260"/>
+      <c r="A19" s="265"/>
       <c r="B19" s="51" t="s">
         <v>423</v>
       </c>
@@ -9901,7 +9898,7 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="261"/>
+      <c r="A20" s="266"/>
       <c r="B20" s="188" t="s">
         <v>424</v>
       </c>
@@ -10937,7 +10934,7 @@
       <c r="AMJ20" s="4"/>
     </row>
     <row r="21" spans="1:1024" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="262" t="s">
+      <c r="A21" s="281" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="55"/>
@@ -10949,7 +10946,7 @@
       <c r="H21" s="57"/>
     </row>
     <row r="22" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="262"/>
+      <c r="A22" s="281"/>
       <c r="B22" s="43" t="s">
         <v>40</v>
       </c>
@@ -10969,7 +10966,7 @@
       <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="262"/>
+      <c r="A23" s="281"/>
       <c r="B23" s="43" t="s">
         <v>44</v>
       </c>
@@ -10989,7 +10986,7 @@
       <c r="H23" s="46"/>
     </row>
     <row r="24" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="262"/>
+      <c r="A24" s="281"/>
       <c r="B24" s="43" t="s">
         <v>46</v>
       </c>
@@ -11009,7 +11006,7 @@
       <c r="H24" s="46"/>
     </row>
     <row r="25" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="262"/>
+      <c r="A25" s="281"/>
       <c r="B25" s="43" t="s">
         <v>48</v>
       </c>
@@ -11029,7 +11026,7 @@
       <c r="H25" s="46"/>
     </row>
     <row r="26" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="262"/>
+      <c r="A26" s="281"/>
       <c r="B26" s="43" t="s">
         <v>50</v>
       </c>
@@ -11049,7 +11046,7 @@
       <c r="H26" s="46"/>
     </row>
     <row r="27" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="262"/>
+      <c r="A27" s="281"/>
       <c r="B27" s="43" t="s">
         <v>53</v>
       </c>
@@ -11069,7 +11066,7 @@
       <c r="H27" s="46"/>
     </row>
     <row r="28" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="262"/>
+      <c r="A28" s="281"/>
       <c r="B28" s="43" t="s">
         <v>57</v>
       </c>
@@ -11089,7 +11086,7 @@
       <c r="H28" s="46"/>
     </row>
     <row r="29" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="262"/>
+      <c r="A29" s="281"/>
       <c r="B29" s="43" t="s">
         <v>61</v>
       </c>
@@ -11109,7 +11106,7 @@
       <c r="H29" s="46"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="262"/>
+      <c r="A30" s="281"/>
       <c r="B30" s="43" t="s">
         <v>63</v>
       </c>
@@ -11129,7 +11126,7 @@
       <c r="H30" s="46"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="262"/>
+      <c r="A31" s="281"/>
       <c r="B31" s="43" t="s">
         <v>65</v>
       </c>
@@ -11149,7 +11146,7 @@
       <c r="H31" s="46"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="262"/>
+      <c r="A32" s="281"/>
       <c r="B32" s="43" t="s">
         <v>67</v>
       </c>
@@ -11169,7 +11166,7 @@
       <c r="H32" s="46"/>
     </row>
     <row r="33" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="263"/>
+      <c r="A33" s="282"/>
       <c r="B33" s="47" t="s">
         <v>69</v>
       </c>
@@ -11189,7 +11186,7 @@
       <c r="H33" s="50"/>
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="264" t="s">
+      <c r="A34" s="283" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="58"/>
@@ -11201,7 +11198,7 @@
       <c r="H34" s="60"/>
     </row>
     <row r="35" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="265"/>
+      <c r="A35" s="284"/>
       <c r="B35" s="61" t="s">
         <v>73</v>
       </c>
@@ -11221,7 +11218,7 @@
       <c r="H35" s="64"/>
     </row>
     <row r="36" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="265"/>
+      <c r="A36" s="284"/>
       <c r="B36" s="65" t="s">
         <v>76</v>
       </c>
@@ -11241,7 +11238,7 @@
       <c r="H36" s="68"/>
     </row>
     <row r="37" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="265"/>
+      <c r="A37" s="284"/>
       <c r="B37" s="65" t="s">
         <v>79</v>
       </c>
@@ -11261,7 +11258,7 @@
       <c r="H37" s="68"/>
     </row>
     <row r="38" spans="1:1024" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="266"/>
+      <c r="A38" s="285"/>
       <c r="B38" s="69" t="s">
         <v>82</v>
       </c>
@@ -11281,8 +11278,8 @@
       <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="267" t="s">
-        <v>567</v>
+      <c r="A39" s="286" t="s">
+        <v>565</v>
       </c>
       <c r="B39" s="212"/>
       <c r="C39" s="212"/>
@@ -11293,9 +11290,9 @@
       <c r="H39" s="57"/>
     </row>
     <row r="40" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="262"/>
+      <c r="A40" s="281"/>
       <c r="B40" s="204" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C40" s="44"/>
       <c r="D40" s="204" t="s">
@@ -11305,7 +11302,7 @@
         <v>86</v>
       </c>
       <c r="F40" s="204" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G40" s="155" t="s">
         <v>43</v>
@@ -12329,12 +12326,12 @@
       <c r="AMJ40" s="4"/>
     </row>
     <row r="41" spans="1:1024" s="10" customFormat="1" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="262"/>
-      <c r="B41" s="254" t="s">
+      <c r="A41" s="281"/>
+      <c r="B41" s="276" t="s">
         <v>87</v>
       </c>
       <c r="C41" s="204" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D41" s="204" t="s">
         <v>9</v>
@@ -13367,8 +13364,8 @@
       <c r="AMJ41" s="4"/>
     </row>
     <row r="42" spans="1:1024" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A42" s="262"/>
-      <c r="B42" s="254"/>
+      <c r="A42" s="281"/>
+      <c r="B42" s="276"/>
       <c r="C42" s="204" t="s">
         <v>90</v>
       </c>
@@ -14403,8 +14400,8 @@
       <c r="AMJ42" s="4"/>
     </row>
     <row r="43" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="262"/>
-      <c r="B43" s="254"/>
+      <c r="A43" s="281"/>
+      <c r="B43" s="276"/>
       <c r="C43" s="204" t="s">
         <v>94</v>
       </c>
@@ -14412,7 +14409,7 @@
         <v>95</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F43" s="204" t="s">
         <v>96</v>
@@ -15439,8 +15436,8 @@
       <c r="AMJ43" s="4"/>
     </row>
     <row r="44" spans="1:1024" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="262"/>
-      <c r="B44" s="254"/>
+      <c r="A44" s="281"/>
+      <c r="B44" s="276"/>
       <c r="C44" s="204" t="s">
         <v>97</v>
       </c>
@@ -16475,8 +16472,8 @@
       <c r="AMJ44" s="4"/>
     </row>
     <row r="45" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="262"/>
-      <c r="B45" s="254"/>
+      <c r="A45" s="281"/>
+      <c r="B45" s="276"/>
       <c r="C45" s="204" t="s">
         <v>101</v>
       </c>
@@ -17511,8 +17508,8 @@
       <c r="AMJ45" s="4"/>
     </row>
     <row r="46" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="262"/>
-      <c r="B46" s="254"/>
+      <c r="A46" s="281"/>
+      <c r="B46" s="276"/>
       <c r="C46" s="204" t="s">
         <v>105</v>
       </c>
@@ -18547,8 +18544,8 @@
       <c r="AMJ46" s="4"/>
     </row>
     <row r="47" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="262"/>
-      <c r="B47" s="254"/>
+      <c r="A47" s="281"/>
+      <c r="B47" s="276"/>
       <c r="C47" s="204" t="s">
         <v>109</v>
       </c>
@@ -19583,8 +19580,8 @@
       <c r="AMJ47" s="4"/>
     </row>
     <row r="48" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="262"/>
-      <c r="B48" s="254"/>
+      <c r="A48" s="281"/>
+      <c r="B48" s="276"/>
       <c r="C48" s="204" t="s">
         <v>113</v>
       </c>
@@ -20619,8 +20616,8 @@
       <c r="AMJ48" s="4"/>
     </row>
     <row r="49" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="262"/>
-      <c r="B49" s="254"/>
+      <c r="A49" s="281"/>
+      <c r="B49" s="276"/>
       <c r="C49" s="204" t="s">
         <v>117</v>
       </c>
@@ -21655,8 +21652,8 @@
       <c r="AMJ49" s="4"/>
     </row>
     <row r="50" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="262"/>
-      <c r="B50" s="254"/>
+      <c r="A50" s="281"/>
+      <c r="B50" s="276"/>
       <c r="C50" s="204" t="s">
         <v>121</v>
       </c>
@@ -22691,8 +22688,8 @@
       <c r="AMJ50" s="4"/>
     </row>
     <row r="51" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="262"/>
-      <c r="B51" s="254"/>
+      <c r="A51" s="281"/>
+      <c r="B51" s="276"/>
       <c r="C51" s="204" t="s">
         <v>125</v>
       </c>
@@ -23727,8 +23724,8 @@
       <c r="AMJ51" s="4"/>
     </row>
     <row r="52" spans="1:1024" s="16" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="263"/>
-      <c r="B52" s="255"/>
+      <c r="A52" s="282"/>
+      <c r="B52" s="277"/>
       <c r="C52" s="205" t="s">
         <v>129</v>
       </c>
@@ -24763,8 +24760,8 @@
       <c r="AMJ52" s="15"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="259" t="s">
-        <v>572</v>
+      <c r="A53" s="264" t="s">
+        <v>570</v>
       </c>
       <c r="B53" s="215"/>
       <c r="C53" s="215"/>
@@ -24775,7 +24772,7 @@
       <c r="H53" s="218"/>
     </row>
     <row r="54" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="260"/>
+      <c r="A54" s="265"/>
       <c r="B54" s="219" t="s">
         <v>132</v>
       </c>
@@ -24795,7 +24792,7 @@
       <c r="H54" s="223"/>
     </row>
     <row r="55" spans="1:1024" ht="46.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="261"/>
+      <c r="A55" s="266"/>
       <c r="B55" s="224" t="s">
         <v>136</v>
       </c>
@@ -24815,7 +24812,7 @@
       <c r="H55" s="228"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="268" t="s">
+      <c r="A56" s="267" t="s">
         <v>140</v>
       </c>
       <c r="B56" s="229"/>
@@ -24827,7 +24824,7 @@
       <c r="H56" s="232"/>
     </row>
     <row r="57" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="269"/>
+      <c r="A57" s="268"/>
       <c r="B57" s="233" t="s">
         <v>141</v>
       </c>
@@ -24845,8 +24842,8 @@
       <c r="H57" s="237"/>
     </row>
     <row r="58" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="269"/>
-      <c r="B58" s="271" t="s">
+      <c r="A58" s="268"/>
+      <c r="B58" s="270" t="s">
         <v>144</v>
       </c>
       <c r="C58" s="233" t="s">
@@ -24867,8 +24864,8 @@
       <c r="H58" s="237"/>
     </row>
     <row r="59" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="269"/>
-      <c r="B59" s="271"/>
+      <c r="A59" s="268"/>
+      <c r="B59" s="270"/>
       <c r="C59" s="233" t="s">
         <v>30</v>
       </c>
@@ -24887,8 +24884,8 @@
       <c r="H59" s="237"/>
     </row>
     <row r="60" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="269"/>
-      <c r="B60" s="271"/>
+      <c r="A60" s="268"/>
+      <c r="B60" s="270"/>
       <c r="C60" s="233" t="s">
         <v>12</v>
       </c>
@@ -24907,8 +24904,8 @@
       <c r="H60" s="237"/>
     </row>
     <row r="61" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="269"/>
-      <c r="B61" s="271"/>
+      <c r="A61" s="268"/>
+      <c r="B61" s="270"/>
       <c r="C61" s="233" t="s">
         <v>153</v>
       </c>
@@ -24927,8 +24924,8 @@
       <c r="H61" s="237"/>
     </row>
     <row r="62" spans="1:1024" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="270"/>
-      <c r="B62" s="272"/>
+      <c r="A62" s="269"/>
+      <c r="B62" s="271"/>
       <c r="C62" s="239" t="s">
         <v>25</v>
       </c>
@@ -24947,7 +24944,7 @@
       <c r="H62" s="242"/>
     </row>
     <row r="63" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="259" t="s">
+      <c r="A63" s="264" t="s">
         <v>158</v>
       </c>
       <c r="B63" s="243"/>
@@ -24959,7 +24956,7 @@
       <c r="H63" s="218"/>
     </row>
     <row r="64" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="260"/>
+      <c r="A64" s="265"/>
       <c r="B64" s="246" t="s">
         <v>159</v>
       </c>
@@ -24977,8 +24974,8 @@
       <c r="H64" s="249"/>
     </row>
     <row r="65" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="260"/>
-      <c r="B65" s="273" t="s">
+      <c r="A65" s="265"/>
+      <c r="B65" s="272" t="s">
         <v>162</v>
       </c>
       <c r="C65" s="246" t="s">
@@ -24999,8 +24996,8 @@
       <c r="H65" s="249"/>
     </row>
     <row r="66" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="260"/>
-      <c r="B66" s="273"/>
+      <c r="A66" s="265"/>
+      <c r="B66" s="272"/>
       <c r="C66" s="246" t="s">
         <v>165</v>
       </c>
@@ -25019,8 +25016,8 @@
       <c r="H66" s="249"/>
     </row>
     <row r="67" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="260"/>
-      <c r="B67" s="273"/>
+      <c r="A67" s="265"/>
+      <c r="B67" s="272"/>
       <c r="C67" s="246" t="s">
         <v>168</v>
       </c>
@@ -26055,8 +26052,8 @@
       <c r="AMJ67" s="13"/>
     </row>
     <row r="68" spans="1:1024" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="260"/>
-      <c r="B68" s="273"/>
+      <c r="A68" s="265"/>
+      <c r="B68" s="272"/>
       <c r="C68" s="246" t="s">
         <v>171</v>
       </c>
@@ -27091,8 +27088,8 @@
       <c r="AMJ68" s="13"/>
     </row>
     <row r="69" spans="1:1024" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="261"/>
-      <c r="B69" s="274"/>
+      <c r="A69" s="266"/>
+      <c r="B69" s="273"/>
       <c r="C69" s="250" t="s">
         <v>25</v>
       </c>
@@ -28129,11 +28126,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="12">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="A63:A69"/>
-    <mergeCell ref="B65:B69"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B41:B52"/>
     <mergeCell ref="A3:A11"/>
@@ -28141,6 +28133,11 @@
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="A63:A69"/>
+    <mergeCell ref="B65:B69"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -28162,7 +28159,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14:H14"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -28180,16 +28177,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:8" s="31" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -28218,7 +28215,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="256" t="s">
+      <c r="A3" s="278" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="27"/>
@@ -28230,7 +28227,7 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="257"/>
+      <c r="A4" s="279"/>
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -28250,7 +28247,7 @@
       <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="257"/>
+      <c r="A5" s="279"/>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
@@ -28270,7 +28267,7 @@
       <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="257"/>
+      <c r="A6" s="279"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -28290,7 +28287,7 @@
       <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="257"/>
+      <c r="A7" s="279"/>
       <c r="B7" s="43" t="s">
         <v>26</v>
       </c>
@@ -28310,7 +28307,7 @@
       <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="257"/>
+      <c r="A8" s="279"/>
       <c r="B8" s="43" t="s">
         <v>30</v>
       </c>
@@ -28330,7 +28327,7 @@
       <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="257"/>
+      <c r="A9" s="279"/>
       <c r="B9" s="43" t="s">
         <v>16</v>
       </c>
@@ -28350,7 +28347,7 @@
       <c r="H9" s="46"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
+      <c r="A10" s="279"/>
       <c r="B10" s="43" t="s">
         <v>19</v>
       </c>
@@ -28370,7 +28367,7 @@
       <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="258"/>
+      <c r="A11" s="280"/>
       <c r="B11" s="47" t="s">
         <v>22</v>
       </c>
@@ -28390,7 +28387,7 @@
       <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:8" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="275" t="s">
+      <c r="A12" s="287" t="s">
         <v>189</v>
       </c>
       <c r="B12" s="73"/>
@@ -28402,7 +28399,7 @@
       <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="276"/>
+      <c r="A13" s="288"/>
       <c r="B13" s="78" t="s">
         <v>190</v>
       </c>
@@ -28422,7 +28419,7 @@
       <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:8" ht="103.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="276"/>
+      <c r="A14" s="288"/>
       <c r="B14" s="78" t="s">
         <v>418</v>
       </c>
@@ -28463,7 +28460,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -28480,16 +28477,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:1024" s="32" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -28518,7 +28515,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="256" t="s">
+      <c r="A3" s="278" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="33"/>
@@ -28568,7 +28565,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="257"/>
+      <c r="A4" s="279"/>
       <c r="B4" s="80" t="s">
         <v>192</v>
       </c>
@@ -28586,7 +28583,7 @@
       <c r="H4" s="82"/>
     </row>
     <row r="5" spans="1:1024" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="257"/>
+      <c r="A5" s="279"/>
       <c r="B5" s="80" t="s">
         <v>195</v>
       </c>
@@ -28598,11 +28595,13 @@
       <c r="F5" s="80" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="165"/>
+      <c r="G5" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H5" s="82"/>
     </row>
     <row r="6" spans="1:1024" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="257"/>
+      <c r="A6" s="279"/>
       <c r="B6" s="80" t="s">
         <v>198</v>
       </c>
@@ -28614,11 +28613,13 @@
       <c r="F6" s="80" t="s">
         <v>479</v>
       </c>
-      <c r="G6" s="165"/>
+      <c r="G6" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H6" s="82"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="257"/>
+      <c r="A7" s="279"/>
       <c r="B7" s="80" t="s">
         <v>199</v>
       </c>
@@ -28630,11 +28631,13 @@
       <c r="F7" s="80" t="s">
         <v>480</v>
       </c>
-      <c r="G7" s="165"/>
+      <c r="G7" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="82"/>
     </row>
     <row r="8" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="257"/>
+      <c r="A8" s="279"/>
       <c r="B8" s="80" t="s">
         <v>200</v>
       </c>
@@ -28646,11 +28649,13 @@
       <c r="F8" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="G8" s="165"/>
+      <c r="G8" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="82"/>
     </row>
     <row r="9" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="257"/>
+      <c r="A9" s="279"/>
       <c r="B9" s="80" t="s">
         <v>202</v>
       </c>
@@ -28668,7 +28673,7 @@
       <c r="H9" s="82"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
+      <c r="A10" s="279"/>
       <c r="B10" s="80" t="s">
         <v>204</v>
       </c>
@@ -28680,7 +28685,9 @@
       <c r="F10" s="80" t="s">
         <v>206</v>
       </c>
-      <c r="G10" s="165"/>
+      <c r="G10" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="82"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -28697,7 +28704,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="257"/>
+      <c r="A11" s="279"/>
       <c r="B11" s="80" t="s">
         <v>3</v>
       </c>
@@ -28709,11 +28716,13 @@
       <c r="F11" s="80" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="165"/>
+      <c r="G11" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="82"/>
     </row>
     <row r="12" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="257"/>
+      <c r="A12" s="279"/>
       <c r="B12" s="80" t="s">
         <v>208</v>
       </c>
@@ -28731,19 +28740,19 @@
       <c r="H12" s="82"/>
     </row>
     <row r="13" spans="1:1024" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="257"/>
+      <c r="A13" s="279"/>
       <c r="B13" s="80" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C13" s="81"/>
       <c r="D13" s="80" t="s">
         <v>210</v>
       </c>
       <c r="E13" s="81" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F13" s="80" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G13" s="165" t="s">
         <v>12</v>
@@ -28751,19 +28760,19 @@
       <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="257"/>
+      <c r="A14" s="279"/>
       <c r="B14" s="80" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C14" s="81"/>
       <c r="D14" s="80" t="s">
         <v>196</v>
       </c>
       <c r="E14" s="81" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F14" s="80" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G14" s="165" t="s">
         <v>12</v>
@@ -28771,19 +28780,19 @@
       <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="257"/>
+      <c r="A15" s="279"/>
       <c r="B15" s="80" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C15" s="81"/>
       <c r="D15" s="80" t="s">
         <v>196</v>
       </c>
       <c r="E15" s="81" t="s">
+        <v>546</v>
+      </c>
+      <c r="F15" s="80" t="s">
         <v>548</v>
-      </c>
-      <c r="F15" s="80" t="s">
-        <v>550</v>
       </c>
       <c r="G15" s="165" t="s">
         <v>12</v>
@@ -28791,7 +28800,7 @@
       <c r="H15" s="82"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="258"/>
+      <c r="A16" s="280"/>
       <c r="B16" s="83" t="s">
         <v>211</v>
       </c>
@@ -28803,11 +28812,13 @@
       <c r="F16" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="G16" s="166"/>
+      <c r="G16" s="166" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="85"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="264" t="s">
+      <c r="A17" s="283" t="s">
         <v>140</v>
       </c>
       <c r="B17" s="86"/>
@@ -28820,7 +28831,7 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="265"/>
+      <c r="A18" s="284"/>
       <c r="B18" s="88" t="s">
         <v>214</v>
       </c>
@@ -28832,11 +28843,13 @@
       <c r="F18" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="G18" s="168"/>
+      <c r="G18" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="90"/>
     </row>
     <row r="19" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="265"/>
+      <c r="A19" s="284"/>
       <c r="B19" s="88"/>
       <c r="C19" s="89" t="s">
         <v>1</v>
@@ -28848,11 +28861,13 @@
       <c r="F19" s="88" t="s">
         <v>496</v>
       </c>
-      <c r="G19" s="168"/>
+      <c r="G19" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="90"/>
     </row>
     <row r="20" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="265"/>
+      <c r="A20" s="284"/>
       <c r="B20" s="88"/>
       <c r="C20" s="89" t="s">
         <v>195</v>
@@ -28864,11 +28879,13 @@
       <c r="F20" s="88" t="s">
         <v>497</v>
       </c>
-      <c r="G20" s="168"/>
+      <c r="G20" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="90"/>
     </row>
     <row r="21" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="265"/>
+      <c r="A21" s="284"/>
       <c r="B21" s="88"/>
       <c r="C21" s="89" t="s">
         <v>484</v>
@@ -28880,11 +28897,13 @@
       <c r="F21" s="88" t="s">
         <v>498</v>
       </c>
-      <c r="G21" s="168"/>
+      <c r="G21" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="90"/>
     </row>
     <row r="22" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="265"/>
+      <c r="A22" s="284"/>
       <c r="B22" s="88"/>
       <c r="C22" s="89" t="s">
         <v>485</v>
@@ -28896,11 +28915,13 @@
       <c r="F22" s="88" t="s">
         <v>499</v>
       </c>
-      <c r="G22" s="168"/>
+      <c r="G22" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="90"/>
     </row>
     <row r="23" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="265"/>
+      <c r="A23" s="284"/>
       <c r="B23" s="88"/>
       <c r="C23" s="89" t="s">
         <v>486</v>
@@ -28912,11 +28933,13 @@
       <c r="F23" s="88" t="s">
         <v>500</v>
       </c>
-      <c r="G23" s="168"/>
+      <c r="G23" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="90"/>
     </row>
     <row r="24" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="265"/>
+      <c r="A24" s="284"/>
       <c r="B24" s="88"/>
       <c r="C24" s="89" t="s">
         <v>487</v>
@@ -28928,11 +28951,13 @@
       <c r="F24" s="88" t="s">
         <v>501</v>
       </c>
-      <c r="G24" s="168"/>
+      <c r="G24" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="90"/>
     </row>
     <row r="25" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="265"/>
+      <c r="A25" s="284"/>
       <c r="B25" s="88"/>
       <c r="C25" s="89" t="s">
         <v>488</v>
@@ -28944,11 +28969,13 @@
       <c r="F25" s="88" t="s">
         <v>502</v>
       </c>
-      <c r="G25" s="168"/>
+      <c r="G25" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="90"/>
     </row>
     <row r="26" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="265"/>
+      <c r="A26" s="284"/>
       <c r="B26" s="88"/>
       <c r="C26" s="89" t="s">
         <v>489</v>
@@ -28960,11 +28987,13 @@
       <c r="F26" s="88" t="s">
         <v>503</v>
       </c>
-      <c r="G26" s="168"/>
+      <c r="G26" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H26" s="90"/>
     </row>
     <row r="27" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="265"/>
+      <c r="A27" s="284"/>
       <c r="B27" s="88"/>
       <c r="C27" s="89" t="s">
         <v>490</v>
@@ -28976,11 +29005,13 @@
       <c r="F27" s="88" t="s">
         <v>504</v>
       </c>
-      <c r="G27" s="168"/>
+      <c r="G27" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="90"/>
     </row>
     <row r="28" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="265"/>
+      <c r="A28" s="284"/>
       <c r="B28" s="88"/>
       <c r="C28" s="89" t="s">
         <v>491</v>
@@ -28992,11 +29023,13 @@
       <c r="F28" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="G28" s="168"/>
+      <c r="G28" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="90"/>
     </row>
     <row r="29" spans="1:1024" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="265"/>
+      <c r="A29" s="284"/>
       <c r="B29" s="88"/>
       <c r="C29" s="89" t="s">
         <v>492</v>
@@ -29008,11 +29041,13 @@
       <c r="F29" s="88" t="s">
         <v>506</v>
       </c>
-      <c r="G29" s="168"/>
+      <c r="G29" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="90"/>
     </row>
     <row r="30" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="265"/>
+      <c r="A30" s="284"/>
       <c r="B30" s="88" t="s">
         <v>216</v>
       </c>
@@ -29024,11 +29059,13 @@
       <c r="F30" s="88" t="s">
         <v>217</v>
       </c>
-      <c r="G30" s="168"/>
+      <c r="G30" s="168" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="90"/>
     </row>
     <row r="31" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="265"/>
+      <c r="A31" s="284"/>
       <c r="B31" s="193"/>
       <c r="C31" s="89" t="s">
         <v>1</v>
@@ -29040,11 +29077,13 @@
       <c r="F31" s="88" t="s">
         <v>507</v>
       </c>
-      <c r="G31" s="195"/>
+      <c r="G31" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="196"/>
     </row>
     <row r="32" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="265"/>
+      <c r="A32" s="284"/>
       <c r="B32" s="193"/>
       <c r="C32" s="89" t="s">
         <v>195</v>
@@ -29056,11 +29095,13 @@
       <c r="F32" s="88" t="s">
         <v>508</v>
       </c>
-      <c r="G32" s="195"/>
+      <c r="G32" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="196"/>
     </row>
     <row r="33" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="265"/>
+      <c r="A33" s="284"/>
       <c r="B33" s="193"/>
       <c r="C33" s="89" t="s">
         <v>484</v>
@@ -29072,11 +29113,13 @@
       <c r="F33" s="88" t="s">
         <v>509</v>
       </c>
-      <c r="G33" s="195"/>
+      <c r="G33" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="196"/>
     </row>
     <row r="34" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="265"/>
+      <c r="A34" s="284"/>
       <c r="B34" s="193"/>
       <c r="C34" s="89" t="s">
         <v>485</v>
@@ -29088,11 +29131,13 @@
       <c r="F34" s="88" t="s">
         <v>510</v>
       </c>
-      <c r="G34" s="195"/>
+      <c r="G34" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="196"/>
     </row>
     <row r="35" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="265"/>
+      <c r="A35" s="284"/>
       <c r="B35" s="193"/>
       <c r="C35" s="89" t="s">
         <v>486</v>
@@ -29104,11 +29149,13 @@
       <c r="F35" s="88" t="s">
         <v>511</v>
       </c>
-      <c r="G35" s="195"/>
+      <c r="G35" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" s="196"/>
     </row>
     <row r="36" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="265"/>
+      <c r="A36" s="284"/>
       <c r="B36" s="193"/>
       <c r="C36" s="89" t="s">
         <v>487</v>
@@ -29120,11 +29167,13 @@
       <c r="F36" s="88" t="s">
         <v>512</v>
       </c>
-      <c r="G36" s="195"/>
+      <c r="G36" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="196"/>
     </row>
     <row r="37" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="265"/>
+      <c r="A37" s="284"/>
       <c r="B37" s="193"/>
       <c r="C37" s="89" t="s">
         <v>488</v>
@@ -29136,11 +29185,13 @@
       <c r="F37" s="88" t="s">
         <v>502</v>
       </c>
-      <c r="G37" s="195"/>
+      <c r="G37" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H37" s="196"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="265"/>
+      <c r="A38" s="284"/>
       <c r="B38" s="193"/>
       <c r="C38" s="89" t="s">
         <v>489</v>
@@ -29152,11 +29203,13 @@
       <c r="F38" s="88" t="s">
         <v>503</v>
       </c>
-      <c r="G38" s="195"/>
+      <c r="G38" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H38" s="196"/>
     </row>
     <row r="39" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="265"/>
+      <c r="A39" s="284"/>
       <c r="B39" s="193"/>
       <c r="C39" s="89" t="s">
         <v>490</v>
@@ -29168,11 +29221,13 @@
       <c r="F39" s="88" t="s">
         <v>504</v>
       </c>
-      <c r="G39" s="195"/>
+      <c r="G39" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H39" s="196"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="265"/>
+      <c r="A40" s="284"/>
       <c r="B40" s="193"/>
       <c r="C40" s="89" t="s">
         <v>491</v>
@@ -29184,11 +29239,13 @@
       <c r="F40" s="88" t="s">
         <v>513</v>
       </c>
-      <c r="G40" s="195"/>
+      <c r="G40" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H40" s="196"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="265"/>
+      <c r="A41" s="284"/>
       <c r="B41" s="193"/>
       <c r="C41" s="89" t="s">
         <v>492</v>
@@ -29200,11 +29257,13 @@
       <c r="F41" s="88" t="s">
         <v>514</v>
       </c>
-      <c r="G41" s="195"/>
+      <c r="G41" s="195" t="s">
+        <v>43</v>
+      </c>
       <c r="H41" s="196"/>
     </row>
     <row r="42" spans="1:1024" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="266"/>
+      <c r="A42" s="285"/>
       <c r="B42" s="91" t="s">
         <v>218</v>
       </c>
@@ -29222,7 +29281,7 @@
       <c r="H42" s="93"/>
     </row>
     <row r="43" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="267" t="s">
+      <c r="A43" s="286" t="s">
         <v>219</v>
       </c>
       <c r="B43" s="94"/>
@@ -29272,7 +29331,7 @@
       <c r="AMJ43" s="5"/>
     </row>
     <row r="44" spans="1:1024" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="263"/>
+      <c r="A44" s="282"/>
       <c r="B44" s="83" t="s">
         <v>220</v>
       </c>
@@ -29284,7 +29343,7 @@
       <c r="F44" s="83" t="s">
         <v>222</v>
       </c>
-      <c r="G44" s="169" t="s">
+      <c r="G44" s="166" t="s">
         <v>43</v>
       </c>
       <c r="H44" s="85"/>
@@ -29309,7 +29368,7 @@
       <c r="AMJ44" s="5"/>
     </row>
     <row r="45" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="264" t="s">
+      <c r="A45" s="283" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="86"/>
@@ -29321,8 +29380,8 @@
       <c r="H45" s="87"/>
       <c r="AMJ45" s="5"/>
     </row>
-    <row r="46" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="265"/>
+    <row r="46" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="284"/>
       <c r="B46" s="88" t="s">
         <v>73</v>
       </c>
@@ -29334,13 +29393,13 @@
       <c r="F46" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="G46" s="169" t="s">
+      <c r="G46" s="168" t="s">
         <v>43</v>
       </c>
       <c r="H46" s="90"/>
     </row>
-    <row r="47" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="265"/>
+    <row r="47" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="284"/>
       <c r="B47" s="88" t="s">
         <v>76</v>
       </c>
@@ -29352,13 +29411,13 @@
       <c r="F47" s="88" t="s">
         <v>224</v>
       </c>
-      <c r="G47" s="169" t="s">
+      <c r="G47" s="168" t="s">
         <v>43</v>
       </c>
       <c r="H47" s="90"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="266"/>
+      <c r="A48" s="285"/>
       <c r="B48" s="91" t="s">
         <v>79</v>
       </c>
@@ -29376,7 +29435,7 @@
       <c r="H48" s="93"/>
     </row>
     <row r="49" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="267" t="s">
+      <c r="A49" s="286" t="s">
         <v>226</v>
       </c>
       <c r="B49" s="96"/>
@@ -29407,7 +29466,7 @@
       <c r="AMJ49" s="5"/>
     </row>
     <row r="50" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="262"/>
+      <c r="A50" s="281"/>
       <c r="B50" s="80" t="s">
         <v>227</v>
       </c>
@@ -29425,7 +29484,7 @@
       <c r="H50" s="82"/>
     </row>
     <row r="51" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="262"/>
+      <c r="A51" s="281"/>
       <c r="B51" s="80" t="s">
         <v>229</v>
       </c>
@@ -29443,7 +29502,7 @@
       <c r="H51" s="82"/>
     </row>
     <row r="52" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="262"/>
+      <c r="A52" s="281"/>
       <c r="B52" s="80" t="s">
         <v>46</v>
       </c>
@@ -29461,7 +29520,7 @@
       <c r="H52" s="82"/>
     </row>
     <row r="53" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="262"/>
+      <c r="A53" s="281"/>
       <c r="B53" s="80" t="s">
         <v>48</v>
       </c>
@@ -29479,7 +29538,7 @@
       <c r="H53" s="82"/>
     </row>
     <row r="54" spans="1:1024" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="262"/>
+      <c r="A54" s="281"/>
       <c r="B54" s="80" t="s">
         <v>61</v>
       </c>
@@ -29517,7 +29576,7 @@
       <c r="AMJ54" s="5"/>
     </row>
     <row r="55" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="262"/>
+      <c r="A55" s="281"/>
       <c r="B55" s="80" t="s">
         <v>63</v>
       </c>
@@ -29535,7 +29594,7 @@
       <c r="H55" s="82"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="262"/>
+      <c r="A56" s="281"/>
       <c r="B56" s="80" t="s">
         <v>65</v>
       </c>
@@ -29553,7 +29612,7 @@
       <c r="H56" s="82"/>
     </row>
     <row r="57" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="262"/>
+      <c r="A57" s="281"/>
       <c r="B57" s="80" t="s">
         <v>67</v>
       </c>
@@ -29571,7 +29630,7 @@
       <c r="H57" s="82"/>
     </row>
     <row r="58" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="263"/>
+      <c r="A58" s="282"/>
       <c r="B58" s="83" t="s">
         <v>69</v>
       </c>
@@ -29589,7 +29648,7 @@
       <c r="H58" s="85"/>
     </row>
     <row r="59" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="264" t="s">
+      <c r="A59" s="283" t="s">
         <v>465</v>
       </c>
       <c r="B59" s="98"/>
@@ -29602,7 +29661,7 @@
       <c r="AMJ59" s="5"/>
     </row>
     <row r="60" spans="1:1024" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="266"/>
+      <c r="A60" s="285"/>
       <c r="B60" s="91" t="s">
         <v>5</v>
       </c>
@@ -29614,11 +29673,13 @@
       <c r="F60" s="91" t="s">
         <v>238</v>
       </c>
-      <c r="G60" s="169"/>
+      <c r="G60" s="169" t="s">
+        <v>43</v>
+      </c>
       <c r="H60" s="93"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection insertRows="0" deleteRows="0"/>
   <mergeCells count="7">
     <mergeCell ref="A49:A58"/>
     <mergeCell ref="A59:A60"/>
@@ -29629,25 +29690,25 @@
     <mergeCell ref="A45:A48"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMJ37"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -29664,16 +29725,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>455</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:1024" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
@@ -30718,7 +30779,7 @@
       <c r="AMJ2" s="17"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="289" t="s">
         <v>466</v>
       </c>
       <c r="B3" s="96"/>
@@ -30743,7 +30804,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="278"/>
+      <c r="A4" s="290"/>
       <c r="B4" s="80" t="s">
         <v>192</v>
       </c>
@@ -30763,7 +30824,7 @@
       <c r="H4" s="101"/>
     </row>
     <row r="5" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="278"/>
+      <c r="A5" s="290"/>
       <c r="B5" s="80" t="s">
         <v>283</v>
       </c>
@@ -30783,7 +30844,7 @@
       <c r="H5" s="101"/>
     </row>
     <row r="6" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="278"/>
+      <c r="A6" s="290"/>
       <c r="B6" s="80" t="s">
         <v>473</v>
       </c>
@@ -30803,7 +30864,7 @@
       <c r="H6" s="101"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="278"/>
+      <c r="A7" s="290"/>
       <c r="B7" s="80" t="s">
         <v>286</v>
       </c>
@@ -30823,7 +30884,7 @@
       <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="280" t="s">
+      <c r="A8" s="292" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="98"/>
@@ -30836,7 +30897,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="282"/>
+      <c r="A9" s="294"/>
       <c r="B9" s="88" t="s">
         <v>289</v>
       </c>
@@ -31872,7 +31933,7 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="282"/>
+      <c r="A10" s="294"/>
       <c r="B10" s="88" t="s">
         <v>474</v>
       </c>
@@ -32908,7 +32969,7 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="282"/>
+      <c r="A11" s="294"/>
       <c r="B11" s="88" t="s">
         <v>294</v>
       </c>
@@ -33944,7 +34005,7 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="282"/>
+      <c r="A12" s="294"/>
       <c r="B12" s="88" t="s">
         <v>475</v>
       </c>
@@ -34980,7 +35041,7 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="282"/>
+      <c r="A13" s="294"/>
       <c r="B13" s="88" t="s">
         <v>291</v>
       </c>
@@ -36016,7 +36077,7 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="277" t="s">
+      <c r="A14" s="289" t="s">
         <v>467</v>
       </c>
       <c r="B14" s="96"/>
@@ -36037,7 +36098,7 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="16" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="279"/>
+      <c r="A15" s="291"/>
       <c r="B15" s="83" t="s">
         <v>298</v>
       </c>
@@ -37073,7 +37134,7 @@
       <c r="AMJ15" s="17"/>
     </row>
     <row r="16" spans="1:1024" s="36" customFormat="1" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="280" t="s">
+      <c r="A16" s="292" t="s">
         <v>301</v>
       </c>
       <c r="B16" s="86"/>
@@ -38101,7 +38162,7 @@
       <c r="AMJ16" s="35"/>
     </row>
     <row r="17" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="282"/>
+      <c r="A17" s="294"/>
       <c r="B17" s="88" t="s">
         <v>90</v>
       </c>
@@ -38121,7 +38182,7 @@
       <c r="H17" s="104"/>
     </row>
     <row r="18" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="282"/>
+      <c r="A18" s="294"/>
       <c r="B18" s="88" t="s">
         <v>94</v>
       </c>
@@ -38141,7 +38202,7 @@
       <c r="H18" s="104"/>
     </row>
     <row r="19" spans="1:1024" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="281"/>
+      <c r="A19" s="293"/>
       <c r="B19" s="91" t="s">
         <v>97</v>
       </c>
@@ -38161,7 +38222,7 @@
       <c r="H19" s="105"/>
     </row>
     <row r="20" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="277" t="s">
+      <c r="A20" s="289" t="s">
         <v>306</v>
       </c>
       <c r="B20" s="96"/>
@@ -38181,9 +38242,9 @@
       <c r="AMJ20" s="5"/>
     </row>
     <row r="21" spans="1:1024" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="278"/>
+      <c r="A21" s="290"/>
       <c r="B21" s="80" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C21" s="81"/>
       <c r="D21" s="80" t="s">
@@ -38193,7 +38254,7 @@
         <v>447</v>
       </c>
       <c r="F21" s="80" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G21" s="165" t="s">
         <v>307</v>
@@ -38201,7 +38262,7 @@
       <c r="H21" s="101"/>
     </row>
     <row r="22" spans="1:1024" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="278"/>
+      <c r="A22" s="290"/>
       <c r="B22" s="80" t="s">
         <v>516</v>
       </c>
@@ -38213,7 +38274,7 @@
         <v>449</v>
       </c>
       <c r="F22" s="80" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G22" s="165" t="s">
         <v>308</v>
@@ -38221,7 +38282,7 @@
       <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:1024" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="279"/>
+      <c r="A23" s="291"/>
       <c r="B23" s="83" t="s">
         <v>477</v>
       </c>
@@ -38241,7 +38302,7 @@
       <c r="H23" s="102"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="280" t="s">
+      <c r="A24" s="292" t="s">
         <v>468</v>
       </c>
       <c r="B24" s="107"/>
@@ -38254,7 +38315,7 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="281"/>
+      <c r="A25" s="293"/>
       <c r="B25" s="91" t="s">
         <v>311</v>
       </c>
@@ -38272,7 +38333,7 @@
       <c r="H25" s="105"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="277" t="s">
+      <c r="A26" s="289" t="s">
         <v>314</v>
       </c>
       <c r="B26" s="96"/>
@@ -38292,7 +38353,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="278"/>
+      <c r="A27" s="290"/>
       <c r="B27" s="80" t="s">
         <v>105</v>
       </c>
@@ -38304,7 +38365,7 @@
         <v>442</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="G27" s="165" t="s">
         <v>43</v>
@@ -38312,7 +38373,7 @@
       <c r="H27" s="101"/>
     </row>
     <row r="28" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="278"/>
+      <c r="A28" s="290"/>
       <c r="B28" s="80" t="s">
         <v>113</v>
       </c>
@@ -38332,7 +38393,7 @@
       <c r="H28" s="101"/>
     </row>
     <row r="29" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="278"/>
+      <c r="A29" s="290"/>
       <c r="B29" s="80" t="s">
         <v>117</v>
       </c>
@@ -38352,7 +38413,7 @@
       <c r="H29" s="101"/>
     </row>
     <row r="30" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="278"/>
+      <c r="A30" s="290"/>
       <c r="B30" s="80" t="s">
         <v>121</v>
       </c>
@@ -38372,7 +38433,7 @@
       <c r="H30" s="101"/>
     </row>
     <row r="31" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="279"/>
+      <c r="A31" s="291"/>
       <c r="B31" s="83" t="s">
         <v>125</v>
       </c>
@@ -38392,7 +38453,7 @@
       <c r="H31" s="102"/>
     </row>
     <row r="32" spans="1:1024" s="7" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="280" t="s">
+      <c r="A32" s="292" t="s">
         <v>319</v>
       </c>
       <c r="B32" s="98"/>
@@ -38405,7 +38466,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="282"/>
+      <c r="A33" s="294"/>
       <c r="B33" s="88" t="s">
         <v>129</v>
       </c>
@@ -38425,7 +38486,7 @@
       <c r="H33" s="104"/>
     </row>
     <row r="34" spans="1:8" ht="89.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="282"/>
+      <c r="A34" s="294"/>
       <c r="B34" s="88" t="s">
         <v>517</v>
       </c>
@@ -38443,7 +38504,7 @@
       <c r="H34" s="197"/>
     </row>
     <row r="35" spans="1:8" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="281"/>
+      <c r="A35" s="293"/>
       <c r="B35" s="91" t="s">
         <v>320</v>
       </c>
@@ -38460,8 +38521,6 @@
       </c>
       <c r="H35" s="105"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
   <mergeCells count="9">
@@ -38494,7 +38553,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38512,16 +38571,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -38550,7 +38609,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="267" t="s">
+      <c r="A3" s="286" t="s">
         <v>469</v>
       </c>
       <c r="B3" s="18"/>
@@ -38577,7 +38636,7 @@
       <c r="AMJ3" s="109"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="262"/>
+      <c r="A4" s="281"/>
       <c r="B4" s="81" t="s">
         <v>192</v>
       </c>
@@ -38597,7 +38656,7 @@
       <c r="H4" s="112"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="262"/>
+      <c r="A5" s="281"/>
       <c r="B5" s="81" t="s">
         <v>242</v>
       </c>
@@ -38617,7 +38676,7 @@
       <c r="H5" s="112"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="262"/>
+      <c r="A6" s="281"/>
       <c r="B6" s="81" t="s">
         <v>198</v>
       </c>
@@ -38635,7 +38694,7 @@
       <c r="H6" s="112"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="262"/>
+      <c r="A7" s="281"/>
       <c r="B7" s="81" t="s">
         <v>248</v>
       </c>
@@ -38655,7 +38714,7 @@
       <c r="H7" s="112"/>
     </row>
     <row r="8" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="262"/>
+      <c r="A8" s="281"/>
       <c r="B8" s="81" t="s">
         <v>251</v>
       </c>
@@ -38675,7 +38734,7 @@
       <c r="H8" s="112"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="262"/>
+      <c r="A9" s="281"/>
       <c r="B9" s="81" t="s">
         <v>254</v>
       </c>
@@ -38695,7 +38754,7 @@
       <c r="H9" s="112"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="262"/>
+      <c r="A10" s="281"/>
       <c r="B10" s="81" t="s">
         <v>195</v>
       </c>
@@ -38709,11 +38768,13 @@
       <c r="F10" s="111" t="s">
         <v>327</v>
       </c>
-      <c r="G10" s="165"/>
+      <c r="G10" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="112"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="262"/>
+      <c r="A11" s="281"/>
       <c r="B11" s="81" t="s">
         <v>261</v>
       </c>
@@ -38727,11 +38788,13 @@
       <c r="F11" s="111" t="s">
         <v>328</v>
       </c>
-      <c r="G11" s="165"/>
+      <c r="G11" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H11" s="112"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="262"/>
+      <c r="A12" s="281"/>
       <c r="B12" s="81" t="s">
         <v>329</v>
       </c>
@@ -38745,11 +38808,13 @@
       <c r="F12" s="111" t="s">
         <v>331</v>
       </c>
-      <c r="G12" s="165"/>
+      <c r="G12" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H12" s="112"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="262"/>
+      <c r="A13" s="281"/>
       <c r="B13" s="81" t="s">
         <v>267</v>
       </c>
@@ -38763,11 +38828,13 @@
       <c r="F13" s="111" t="s">
         <v>270</v>
       </c>
-      <c r="G13" s="165"/>
+      <c r="G13" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="112"/>
     </row>
     <row r="14" spans="1:1024" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="262"/>
+      <c r="A14" s="281"/>
       <c r="B14" s="81" t="s">
         <v>333</v>
       </c>
@@ -38781,11 +38848,13 @@
       <c r="F14" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="G14" s="165"/>
+      <c r="G14" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H14" s="112"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="262"/>
+      <c r="A15" s="281"/>
       <c r="B15" s="81" t="s">
         <v>336</v>
       </c>
@@ -38799,11 +38868,13 @@
       <c r="F15" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="G15" s="165"/>
+      <c r="G15" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H15" s="112"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="262"/>
+      <c r="A16" s="281"/>
       <c r="B16" s="81" t="s">
         <v>339</v>
       </c>
@@ -38817,11 +38888,13 @@
       <c r="F16" s="111" t="s">
         <v>342</v>
       </c>
-      <c r="G16" s="165"/>
+      <c r="G16" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="112"/>
     </row>
     <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="262"/>
+      <c r="A17" s="281"/>
       <c r="B17" s="81" t="s">
         <v>343</v>
       </c>
@@ -38835,11 +38908,13 @@
       <c r="F17" s="111" t="s">
         <v>344</v>
       </c>
-      <c r="G17" s="165"/>
+      <c r="G17" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="112"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="263"/>
+      <c r="A18" s="282"/>
       <c r="B18" s="84" t="s">
         <v>279</v>
       </c>
@@ -38853,7 +38928,9 @@
       <c r="F18" s="113" t="s">
         <v>281</v>
       </c>
-      <c r="G18" s="166"/>
+      <c r="G18" s="166" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="114"/>
     </row>
     <row r="20" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
@@ -38883,7 +38960,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38900,16 +38977,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
@@ -38938,7 +39015,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="119" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="283" t="s">
+      <c r="A3" s="295" t="s">
         <v>469</v>
       </c>
       <c r="B3" s="117"/>
@@ -38950,7 +39027,7 @@
       <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="285"/>
+      <c r="A4" s="299"/>
       <c r="B4" s="81" t="s">
         <v>192</v>
       </c>
@@ -38979,7 +39056,7 @@
       <c r="Q4" s="119"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="285"/>
+      <c r="A5" s="299"/>
       <c r="B5" s="81" t="s">
         <v>242</v>
       </c>
@@ -39008,7 +39085,7 @@
       <c r="Q5" s="119"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="285"/>
+      <c r="A6" s="299"/>
       <c r="B6" s="81" t="s">
         <v>198</v>
       </c>
@@ -39035,7 +39112,7 @@
       <c r="Q6" s="119"/>
     </row>
     <row r="7" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="285"/>
+      <c r="A7" s="299"/>
       <c r="B7" s="81" t="s">
         <v>248</v>
       </c>
@@ -39064,7 +39141,7 @@
       <c r="Q7" s="119"/>
     </row>
     <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="285"/>
+      <c r="A8" s="299"/>
       <c r="B8" s="81" t="s">
         <v>251</v>
       </c>
@@ -39093,7 +39170,7 @@
       <c r="Q8" s="119"/>
     </row>
     <row r="9" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="285"/>
+      <c r="A9" s="299"/>
       <c r="B9" s="81" t="s">
         <v>254</v>
       </c>
@@ -39122,7 +39199,7 @@
       <c r="Q9" s="119"/>
     </row>
     <row r="10" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="285"/>
+      <c r="A10" s="299"/>
       <c r="B10" s="81" t="s">
         <v>195</v>
       </c>
@@ -39136,7 +39213,9 @@
       <c r="F10" s="81" t="s">
         <v>260</v>
       </c>
-      <c r="G10" s="165"/>
+      <c r="G10" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="120"/>
       <c r="I10" s="119"/>
       <c r="J10" s="121"/>
@@ -39149,7 +39228,7 @@
       <c r="Q10" s="119"/>
     </row>
     <row r="11" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="285"/>
+      <c r="A11" s="299"/>
       <c r="B11" s="81" t="s">
         <v>261</v>
       </c>
@@ -39163,7 +39242,9 @@
       <c r="F11" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="G11" s="165"/>
+      <c r="G11" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H11" s="120"/>
       <c r="I11" s="119"/>
       <c r="J11" s="121"/>
@@ -39176,7 +39257,7 @@
       <c r="Q11" s="119"/>
     </row>
     <row r="12" spans="1:17" s="126" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="285"/>
+      <c r="A12" s="299"/>
       <c r="B12" s="81" t="s">
         <v>264</v>
       </c>
@@ -39190,7 +39271,9 @@
       <c r="F12" s="81" t="s">
         <v>266</v>
       </c>
-      <c r="G12" s="165"/>
+      <c r="G12" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H12" s="120"/>
       <c r="I12" s="119"/>
       <c r="J12" s="121"/>
@@ -39203,7 +39286,7 @@
       <c r="Q12" s="119"/>
     </row>
     <row r="13" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="285"/>
+      <c r="A13" s="299"/>
       <c r="B13" s="81" t="s">
         <v>267</v>
       </c>
@@ -39217,7 +39300,9 @@
       <c r="F13" s="81" t="s">
         <v>270</v>
       </c>
-      <c r="G13" s="165"/>
+      <c r="G13" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="120"/>
       <c r="I13" s="119"/>
       <c r="J13" s="121"/>
@@ -39230,7 +39315,7 @@
       <c r="Q13" s="119"/>
     </row>
     <row r="14" spans="1:17" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="285"/>
+      <c r="A14" s="299"/>
       <c r="B14" s="81" t="s">
         <v>271</v>
       </c>
@@ -39244,7 +39329,9 @@
       <c r="F14" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="G14" s="165"/>
+      <c r="G14" s="165" t="s">
+        <v>12</v>
+      </c>
       <c r="H14" s="120"/>
       <c r="I14" s="119"/>
       <c r="J14" s="121"/>
@@ -39257,7 +39344,7 @@
       <c r="Q14" s="119"/>
     </row>
     <row r="15" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="285"/>
+      <c r="A15" s="299"/>
       <c r="B15" s="81" t="s">
         <v>275</v>
       </c>
@@ -39271,7 +39358,9 @@
       <c r="F15" s="81" t="s">
         <v>278</v>
       </c>
-      <c r="G15" s="165"/>
+      <c r="G15" s="165" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="112"/>
       <c r="I15" s="119"/>
       <c r="J15" s="119"/>
@@ -39284,7 +39373,7 @@
       <c r="Q15" s="119"/>
     </row>
     <row r="16" spans="1:17" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="286"/>
+      <c r="A16" s="300"/>
       <c r="B16" s="84" t="s">
         <v>279</v>
       </c>
@@ -39298,7 +39387,9 @@
       <c r="F16" s="84" t="s">
         <v>281</v>
       </c>
-      <c r="G16" s="166"/>
+      <c r="G16" s="166" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="114"/>
       <c r="I16" s="119"/>
       <c r="J16" s="119"/>
@@ -39310,54 +39401,56 @@
       <c r="P16" s="119"/>
       <c r="Q16" s="119"/>
     </row>
-    <row r="17" spans="1:17" s="293" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="288" t="s">
-        <v>566</v>
-      </c>
-      <c r="B17" s="289"/>
-      <c r="C17" s="289"/>
-      <c r="D17" s="289"/>
-      <c r="E17" s="289"/>
-      <c r="F17" s="289"/>
-      <c r="G17" s="290"/>
-      <c r="H17" s="291"/>
-      <c r="I17" s="292"/>
-      <c r="J17" s="292"/>
-      <c r="K17" s="292"/>
-      <c r="L17" s="292"/>
-      <c r="M17" s="292"/>
-      <c r="N17" s="292"/>
-      <c r="O17" s="292"/>
-      <c r="P17" s="292"/>
-      <c r="Q17" s="292"/>
+    <row r="17" spans="1:17" s="256" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="297" t="s">
+        <v>564</v>
+      </c>
+      <c r="B17" s="252"/>
+      <c r="C17" s="252"/>
+      <c r="D17" s="252"/>
+      <c r="E17" s="252"/>
+      <c r="F17" s="252"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="254"/>
+      <c r="I17" s="255"/>
+      <c r="J17" s="255"/>
+      <c r="K17" s="255"/>
+      <c r="L17" s="255"/>
+      <c r="M17" s="255"/>
+      <c r="N17" s="255"/>
+      <c r="O17" s="255"/>
+      <c r="P17" s="255"/>
+      <c r="Q17" s="255"/>
     </row>
-    <row r="18" spans="1:17" s="293" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="294"/>
-      <c r="B18" s="295" t="s">
-        <v>541</v>
-      </c>
-      <c r="C18" s="295"/>
-      <c r="D18" s="296" t="s">
+    <row r="18" spans="1:17" s="256" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="298"/>
+      <c r="B18" s="257" t="s">
+        <v>540</v>
+      </c>
+      <c r="C18" s="257"/>
+      <c r="D18" s="258" t="s">
+        <v>571</v>
+      </c>
+      <c r="E18" s="259"/>
+      <c r="F18" s="257" t="s">
         <v>573</v>
       </c>
-      <c r="E18" s="297"/>
-      <c r="F18" s="295" t="s">
-        <v>542</v>
-      </c>
-      <c r="G18" s="298"/>
-      <c r="H18" s="299"/>
-      <c r="I18" s="292"/>
-      <c r="J18" s="300"/>
-      <c r="K18" s="301"/>
-      <c r="L18" s="292"/>
-      <c r="M18" s="292"/>
-      <c r="N18" s="300"/>
-      <c r="O18" s="301"/>
-      <c r="P18" s="292"/>
-      <c r="Q18" s="292"/>
+      <c r="G18" s="260" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="261"/>
+      <c r="I18" s="255"/>
+      <c r="J18" s="262"/>
+      <c r="K18" s="263"/>
+      <c r="L18" s="255"/>
+      <c r="M18" s="255"/>
+      <c r="N18" s="262"/>
+      <c r="O18" s="263"/>
+      <c r="P18" s="255"/>
+      <c r="Q18" s="255"/>
     </row>
     <row r="19" spans="1:17" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="283" t="s">
+      <c r="A19" s="295" t="s">
         <v>274</v>
       </c>
       <c r="B19" s="207"/>
@@ -39378,19 +39471,21 @@
       <c r="Q19" s="119"/>
     </row>
     <row r="20" spans="1:17" ht="48" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="284"/>
+      <c r="A20" s="296"/>
       <c r="B20" s="84" t="s">
         <v>274</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="83" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E20" s="113"/>
       <c r="F20" s="84" t="s">
-        <v>553</v>
-      </c>
-      <c r="G20" s="166"/>
+        <v>551</v>
+      </c>
+      <c r="G20" s="166" t="s">
+        <v>12</v>
+      </c>
       <c r="H20" s="206"/>
       <c r="I20" s="119"/>
       <c r="J20" s="121"/>
@@ -39425,7 +39520,7 @@
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -39443,16 +39538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
-        <v>552</v>
-      </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="A1" s="274" t="s">
+        <v>550</v>
+      </c>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:20" s="127" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -39481,7 +39576,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="131" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="267" t="s">
+      <c r="A3" s="286" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="128"/>
@@ -39505,7 +39600,7 @@
       <c r="T3" s="130"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="262"/>
+      <c r="A4" s="281"/>
       <c r="B4" s="132" t="s">
         <v>8</v>
       </c>
@@ -39523,7 +39618,7 @@
       <c r="H4" s="133"/>
     </row>
     <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="262"/>
+      <c r="A5" s="281"/>
       <c r="B5" s="132" t="s">
         <v>13</v>
       </c>
@@ -39541,7 +39636,7 @@
       <c r="H5" s="133"/>
     </row>
     <row r="6" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="262"/>
+      <c r="A6" s="281"/>
       <c r="B6" s="132" t="s">
         <v>16</v>
       </c>
@@ -39559,7 +39654,7 @@
       <c r="H6" s="133"/>
     </row>
     <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="263"/>
+      <c r="A7" s="282"/>
       <c r="B7" s="134" t="s">
         <v>19</v>
       </c>
@@ -39577,7 +39672,7 @@
       <c r="H7" s="135"/>
     </row>
     <row r="8" spans="1:20" s="130" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="264" t="s">
+      <c r="A8" s="283" t="s">
         <v>274</v>
       </c>
       <c r="B8" s="136"/>
@@ -39589,7 +39684,7 @@
       <c r="H8" s="137"/>
     </row>
     <row r="9" spans="1:20" ht="18.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="265"/>
+      <c r="A9" s="284"/>
       <c r="B9" s="138" t="s">
         <v>30</v>
       </c>
@@ -39607,7 +39702,7 @@
       <c r="H9" s="139"/>
     </row>
     <row r="10" spans="1:20" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="265"/>
+      <c r="A10" s="284"/>
       <c r="B10" s="138" t="s">
         <v>352</v>
       </c>
@@ -39623,7 +39718,7 @@
       <c r="H10" s="139"/>
     </row>
     <row r="11" spans="1:20" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="265"/>
+      <c r="A11" s="284"/>
       <c r="B11" s="138"/>
       <c r="C11" s="138" t="s">
         <v>354</v>
@@ -39635,11 +39730,13 @@
       <c r="F11" s="138" t="s">
         <v>459</v>
       </c>
-      <c r="G11" s="158"/>
+      <c r="G11" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="139"/>
     </row>
     <row r="12" spans="1:20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="265"/>
+      <c r="A12" s="284"/>
       <c r="B12" s="138"/>
       <c r="C12" s="138" t="s">
         <v>355</v>
@@ -39651,11 +39748,13 @@
       <c r="F12" s="138" t="s">
         <v>460</v>
       </c>
-      <c r="G12" s="158"/>
+      <c r="G12" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="139"/>
     </row>
     <row r="13" spans="1:20" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="265"/>
+      <c r="A13" s="284"/>
       <c r="B13" s="138"/>
       <c r="C13" s="138" t="s">
         <v>356</v>
@@ -39667,11 +39766,13 @@
       <c r="F13" s="138" t="s">
         <v>461</v>
       </c>
-      <c r="G13" s="158"/>
+      <c r="G13" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="139"/>
     </row>
     <row r="14" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="265"/>
+      <c r="A14" s="284"/>
       <c r="B14" s="138"/>
       <c r="C14" s="138" t="s">
         <v>357</v>
@@ -39683,11 +39784,13 @@
       <c r="F14" s="138" t="s">
         <v>358</v>
       </c>
-      <c r="G14" s="158"/>
+      <c r="G14" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="139"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="265"/>
+      <c r="A15" s="284"/>
       <c r="B15" s="138"/>
       <c r="C15" s="138" t="s">
         <v>359</v>
@@ -39699,29 +39802,33 @@
       <c r="F15" s="138" t="s">
         <v>360</v>
       </c>
-      <c r="G15" s="158"/>
+      <c r="G15" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="139"/>
     </row>
     <row r="16" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="265"/>
+      <c r="A16" s="284"/>
       <c r="B16" s="138"/>
       <c r="C16" s="138" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D16" s="138" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="138" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F16" s="138" t="s">
-        <v>539</v>
-      </c>
-      <c r="G16" s="158"/>
+        <v>538</v>
+      </c>
+      <c r="G16" s="158" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="139"/>
     </row>
     <row r="17" spans="1:8" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="265"/>
+      <c r="A17" s="284"/>
       <c r="B17" s="138" t="s">
         <v>361</v>
       </c>
@@ -39737,7 +39844,7 @@
       <c r="H17" s="139"/>
     </row>
     <row r="18" spans="1:8" ht="18.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="266"/>
+      <c r="A18" s="285"/>
       <c r="B18" s="140"/>
       <c r="C18" s="140" t="s">
         <v>359</v>
@@ -39749,11 +39856,13 @@
       <c r="F18" s="140" t="s">
         <v>362</v>
       </c>
-      <c r="G18" s="159"/>
+      <c r="G18" s="159" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="141"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection insertRows="0" deleteRows="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:A7"/>
@@ -39796,16 +39905,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="287" t="s">
-        <v>554</v>
-      </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
-      <c r="H1" s="253"/>
+      <c r="A1" s="301" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="301"/>
+      <c r="C1" s="301"/>
+      <c r="D1" s="301"/>
+      <c r="E1" s="301"/>
+      <c r="F1" s="301"/>
+      <c r="G1" s="301"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:20" s="198" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -39834,8 +39943,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="202" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="267" t="s">
-        <v>541</v>
+      <c r="A3" s="286" t="s">
+        <v>540</v>
       </c>
       <c r="B3" s="128"/>
       <c r="C3" s="128"/>
@@ -39858,19 +39967,19 @@
       <c r="T3" s="201"/>
     </row>
     <row r="4" spans="1:20" s="126" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="262"/>
+      <c r="A4" s="281"/>
       <c r="B4" s="80" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C4" s="132"/>
       <c r="D4" s="132" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E4" s="132" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F4" s="132" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G4" s="155" t="s">
         <v>12</v>
@@ -39878,19 +39987,19 @@
       <c r="H4" s="133"/>
     </row>
     <row r="5" spans="1:20" s="126" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="262"/>
+      <c r="A5" s="281"/>
       <c r="B5" s="132"/>
       <c r="C5" s="132" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D5" s="132" t="s">
         <v>193</v>
       </c>
       <c r="E5" s="132" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F5" s="132" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G5" s="155" t="s">
         <v>12</v>
@@ -39898,7 +40007,7 @@
       <c r="H5" s="133"/>
     </row>
     <row r="6" spans="1:20" s="126" customFormat="1" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="262"/>
+      <c r="A6" s="281"/>
       <c r="B6" s="132"/>
       <c r="C6" s="132"/>
       <c r="D6" s="132"/>
@@ -39908,7 +40017,7 @@
       <c r="H6" s="133"/>
     </row>
     <row r="7" spans="1:20" s="203" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="263"/>
+      <c r="A7" s="282"/>
       <c r="B7" s="134"/>
       <c r="C7" s="134"/>
       <c r="D7" s="134"/>
@@ -39941,7 +40050,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -39958,16 +40067,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="274" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="253"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:1024" s="38" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -41012,7 +41121,7 @@
       <c r="AMJ2" s="37"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="267" t="s">
+      <c r="A3" s="286" t="s">
         <v>363</v>
       </c>
       <c r="B3" s="144"/>
@@ -41024,7 +41133,7 @@
       <c r="H3" s="145"/>
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="262"/>
+      <c r="A4" s="281"/>
       <c r="B4" s="43" t="s">
         <v>192</v>
       </c>
@@ -41036,7 +41145,9 @@
       <c r="F4" s="132" t="s">
         <v>364</v>
       </c>
-      <c r="G4" s="43"/>
+      <c r="G4" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H4" s="133"/>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
@@ -42056,7 +42167,7 @@
       <c r="AMJ4" s="23"/>
     </row>
     <row r="5" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="262"/>
+      <c r="A5" s="281"/>
       <c r="B5" s="43" t="s">
         <v>242</v>
       </c>
@@ -42068,7 +42179,9 @@
       <c r="F5" s="132" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="43"/>
+      <c r="G5" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H5" s="133"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
@@ -43088,7 +43201,7 @@
       <c r="AMJ5" s="23"/>
     </row>
     <row r="6" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="262"/>
+      <c r="A6" s="281"/>
       <c r="B6" s="43" t="s">
         <v>198</v>
       </c>
@@ -43100,7 +43213,9 @@
       <c r="F6" s="132" t="s">
         <v>365</v>
       </c>
-      <c r="G6" s="43"/>
+      <c r="G6" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H6" s="146"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
@@ -44120,7 +44235,7 @@
       <c r="AMJ6" s="23"/>
     </row>
     <row r="7" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="262"/>
+      <c r="A7" s="281"/>
       <c r="B7" s="43" t="s">
         <v>366</v>
       </c>
@@ -44132,7 +44247,9 @@
       <c r="F7" s="132" t="s">
         <v>367</v>
       </c>
-      <c r="G7" s="43"/>
+      <c r="G7" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" s="133"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
@@ -45152,7 +45269,7 @@
       <c r="AMJ7" s="23"/>
     </row>
     <row r="8" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="262"/>
+      <c r="A8" s="281"/>
       <c r="B8" s="43" t="s">
         <v>368</v>
       </c>
@@ -45164,7 +45281,9 @@
       <c r="F8" s="132" t="s">
         <v>369</v>
       </c>
-      <c r="G8" s="43"/>
+      <c r="G8" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H8" s="133"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
@@ -46184,7 +46303,7 @@
       <c r="AMJ8" s="23"/>
     </row>
     <row r="9" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="262"/>
+      <c r="A9" s="281"/>
       <c r="B9" s="43" t="s">
         <v>370</v>
       </c>
@@ -46196,7 +46315,9 @@
       <c r="F9" s="132" t="s">
         <v>371</v>
       </c>
-      <c r="G9" s="43"/>
+      <c r="G9" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" s="133"/>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
@@ -47216,7 +47337,7 @@
       <c r="AMJ9" s="23"/>
     </row>
     <row r="10" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="262"/>
+      <c r="A10" s="281"/>
       <c r="B10" s="43" t="s">
         <v>372</v>
       </c>
@@ -47228,7 +47349,9 @@
       <c r="F10" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="G10" s="43"/>
+      <c r="G10" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="133"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -48248,7 +48371,7 @@
       <c r="AMJ10" s="23"/>
     </row>
     <row r="11" spans="1:1024" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="262"/>
+      <c r="A11" s="281"/>
       <c r="B11" s="43" t="s">
         <v>374</v>
       </c>
@@ -48260,7 +48383,9 @@
       <c r="F11" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="133"/>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
@@ -49280,7 +49405,7 @@
       <c r="AMJ11" s="23"/>
     </row>
     <row r="12" spans="1:1024" s="26" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="263"/>
+      <c r="A12" s="282"/>
       <c r="B12" s="47" t="s">
         <v>376</v>
       </c>
@@ -49292,7 +49417,9 @@
       <c r="F12" s="134" t="s">
         <v>377</v>
       </c>
-      <c r="G12" s="47"/>
+      <c r="G12" s="47" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="135"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
@@ -50312,7 +50439,7 @@
       <c r="AMJ12" s="25"/>
     </row>
     <row r="13" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="264" t="s">
+      <c r="A13" s="283" t="s">
         <v>378</v>
       </c>
       <c r="B13" s="147"/>
@@ -50325,7 +50452,7 @@
       <c r="AMJ13" s="21"/>
     </row>
     <row r="14" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="265"/>
+      <c r="A14" s="284"/>
       <c r="B14" s="65" t="s">
         <v>192</v>
       </c>
@@ -50337,11 +50464,13 @@
       <c r="F14" s="65" t="s">
         <v>379</v>
       </c>
-      <c r="G14" s="65"/>
+      <c r="G14" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H14" s="149"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="265"/>
+      <c r="A15" s="284"/>
       <c r="B15" s="65" t="s">
         <v>242</v>
       </c>
@@ -50353,11 +50482,13 @@
       <c r="F15" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="G15" s="65"/>
+      <c r="G15" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H15" s="149"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="265"/>
+      <c r="A16" s="284"/>
       <c r="B16" s="65" t="s">
         <v>198</v>
       </c>
@@ -50369,11 +50500,13 @@
       <c r="F16" s="65" t="s">
         <v>380</v>
       </c>
-      <c r="G16" s="65"/>
+      <c r="G16" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H16" s="149"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="265"/>
+      <c r="A17" s="284"/>
       <c r="B17" s="65" t="s">
         <v>248</v>
       </c>
@@ -50385,11 +50518,13 @@
       <c r="F17" s="65" t="s">
         <v>381</v>
       </c>
-      <c r="G17" s="65"/>
+      <c r="G17" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H17" s="149"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="265"/>
+      <c r="A18" s="284"/>
       <c r="B18" s="65" t="s">
         <v>195</v>
       </c>
@@ -50401,11 +50536,13 @@
       <c r="F18" s="65" t="s">
         <v>382</v>
       </c>
-      <c r="G18" s="65"/>
+      <c r="G18" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H18" s="149"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="265"/>
+      <c r="A19" s="284"/>
       <c r="B19" s="65" t="s">
         <v>5</v>
       </c>
@@ -50417,11 +50554,13 @@
       <c r="F19" s="65" t="s">
         <v>383</v>
       </c>
-      <c r="G19" s="65"/>
+      <c r="G19" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H19" s="149"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="265"/>
+      <c r="A20" s="284"/>
       <c r="B20" s="65" t="s">
         <v>384</v>
       </c>
@@ -50433,11 +50572,13 @@
       <c r="F20" s="65" t="s">
         <v>385</v>
       </c>
-      <c r="G20" s="65"/>
+      <c r="G20" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="149"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="265"/>
+      <c r="A21" s="284"/>
       <c r="B21" s="65" t="s">
         <v>296</v>
       </c>
@@ -50449,11 +50590,13 @@
       <c r="F21" s="65" t="s">
         <v>386</v>
       </c>
-      <c r="G21" s="65"/>
+      <c r="G21" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="149"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="265"/>
+      <c r="A22" s="284"/>
       <c r="B22" s="65" t="s">
         <v>387</v>
       </c>
@@ -50465,11 +50608,13 @@
       <c r="F22" s="65" t="s">
         <v>388</v>
       </c>
-      <c r="G22" s="65"/>
+      <c r="G22" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="149"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="265"/>
+      <c r="A23" s="284"/>
       <c r="B23" s="65" t="s">
         <v>389</v>
       </c>
@@ -50481,11 +50626,13 @@
       <c r="F23" s="65" t="s">
         <v>390</v>
       </c>
-      <c r="G23" s="65"/>
+      <c r="G23" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="149"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="266"/>
+      <c r="A24" s="285"/>
       <c r="B24" s="69" t="s">
         <v>391</v>
       </c>
@@ -50497,11 +50644,13 @@
       <c r="F24" s="69" t="s">
         <v>392</v>
       </c>
-      <c r="G24" s="69"/>
+      <c r="G24" s="69" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="150"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="267" t="s">
+      <c r="A25" s="286" t="s">
         <v>329</v>
       </c>
       <c r="B25" s="151"/>
@@ -50513,7 +50662,7 @@
       <c r="H25" s="152"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="262"/>
+      <c r="A26" s="281"/>
       <c r="B26" s="43" t="s">
         <v>192</v>
       </c>
@@ -50525,11 +50674,13 @@
       <c r="F26" s="43" t="s">
         <v>393</v>
       </c>
-      <c r="G26" s="43"/>
+      <c r="G26" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H26" s="146"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="262"/>
+      <c r="A27" s="281"/>
       <c r="B27" s="43" t="s">
         <v>242</v>
       </c>
@@ -50541,11 +50692,13 @@
       <c r="F27" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="G27" s="43"/>
+      <c r="G27" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H27" s="146"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="262"/>
+      <c r="A28" s="281"/>
       <c r="B28" s="43" t="s">
         <v>198</v>
       </c>
@@ -50557,11 +50710,13 @@
       <c r="F28" s="43" t="s">
         <v>394</v>
       </c>
-      <c r="G28" s="43"/>
+      <c r="G28" s="43" t="s">
+        <v>463</v>
+      </c>
       <c r="H28" s="146"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="262"/>
+      <c r="A29" s="281"/>
       <c r="B29" s="43" t="s">
         <v>248</v>
       </c>
@@ -50573,11 +50728,13 @@
       <c r="F29" s="43" t="s">
         <v>395</v>
       </c>
-      <c r="G29" s="43"/>
+      <c r="G29" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H29" s="146"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="262"/>
+      <c r="A30" s="281"/>
       <c r="B30" s="43" t="s">
         <v>396</v>
       </c>
@@ -50589,11 +50746,13 @@
       <c r="F30" s="43" t="s">
         <v>397</v>
       </c>
-      <c r="G30" s="43"/>
+      <c r="G30" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H30" s="146"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="262"/>
+      <c r="A31" s="281"/>
       <c r="B31" s="43" t="s">
         <v>195</v>
       </c>
@@ -50605,11 +50764,13 @@
       <c r="F31" s="43" t="s">
         <v>398</v>
       </c>
-      <c r="G31" s="43"/>
+      <c r="G31" s="43" t="s">
+        <v>12</v>
+      </c>
       <c r="H31" s="146"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="262"/>
+      <c r="A32" s="281"/>
       <c r="B32" s="43" t="s">
         <v>374</v>
       </c>
@@ -50621,11 +50782,13 @@
       <c r="F32" s="43" t="s">
         <v>399</v>
       </c>
-      <c r="G32" s="43"/>
+      <c r="G32" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="146"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="262"/>
+      <c r="A33" s="281"/>
       <c r="B33" s="43" t="s">
         <v>400</v>
       </c>
@@ -50637,11 +50800,13 @@
       <c r="F33" s="43" t="s">
         <v>401</v>
       </c>
-      <c r="G33" s="43"/>
+      <c r="G33" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="146"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="262"/>
+      <c r="A34" s="281"/>
       <c r="B34" s="43" t="s">
         <v>5</v>
       </c>
@@ -50653,11 +50818,13 @@
       <c r="F34" s="43" t="s">
         <v>402</v>
       </c>
-      <c r="G34" s="43"/>
+      <c r="G34" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="146"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="262"/>
+      <c r="A35" s="281"/>
       <c r="B35" s="43" t="s">
         <v>403</v>
       </c>
@@ -50669,11 +50836,13 @@
       <c r="F35" s="43" t="s">
         <v>404</v>
       </c>
-      <c r="G35" s="43"/>
+      <c r="G35" s="43" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" s="146"/>
     </row>
     <row r="36" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="263"/>
+      <c r="A36" s="282"/>
       <c r="B36" s="47" t="s">
         <v>405</v>
       </c>
@@ -50685,11 +50854,13 @@
       <c r="F36" s="47" t="s">
         <v>406</v>
       </c>
-      <c r="G36" s="47"/>
+      <c r="G36" s="47" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="153"/>
     </row>
     <row r="37" spans="1:1024" s="20" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="264" t="s">
+      <c r="A37" s="283" t="s">
         <v>264</v>
       </c>
       <c r="B37" s="147"/>
@@ -50702,7 +50873,7 @@
       <c r="AMJ37" s="21"/>
     </row>
     <row r="38" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="265"/>
+      <c r="A38" s="284"/>
       <c r="B38" s="65" t="s">
         <v>192</v>
       </c>
@@ -50714,11 +50885,13 @@
       <c r="F38" s="65" t="s">
         <v>407</v>
       </c>
-      <c r="G38" s="65"/>
+      <c r="G38" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H38" s="149"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="265"/>
+      <c r="A39" s="284"/>
       <c r="B39" s="65" t="s">
         <v>242</v>
       </c>
@@ -50730,11 +50903,13 @@
       <c r="F39" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="G39" s="65"/>
+      <c r="G39" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H39" s="149"/>
     </row>
     <row r="40" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="265"/>
+      <c r="A40" s="284"/>
       <c r="B40" s="65" t="s">
         <v>198</v>
       </c>
@@ -50746,11 +50921,13 @@
       <c r="F40" s="65" t="s">
         <v>408</v>
       </c>
-      <c r="G40" s="65"/>
+      <c r="G40" s="65" t="s">
+        <v>463</v>
+      </c>
       <c r="H40" s="149"/>
     </row>
     <row r="41" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="265"/>
+      <c r="A41" s="284"/>
       <c r="B41" s="65" t="s">
         <v>248</v>
       </c>
@@ -50762,11 +50939,13 @@
       <c r="F41" s="65" t="s">
         <v>409</v>
       </c>
-      <c r="G41" s="65"/>
+      <c r="G41" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H41" s="149"/>
     </row>
     <row r="42" spans="1:1024" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="265"/>
+      <c r="A42" s="284"/>
       <c r="B42" s="65" t="s">
         <v>410</v>
       </c>
@@ -50778,11 +50957,13 @@
       <c r="F42" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="G42" s="65"/>
+      <c r="G42" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H42" s="149"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="265"/>
+      <c r="A43" s="284"/>
       <c r="B43" s="65" t="s">
         <v>329</v>
       </c>
@@ -50794,11 +50975,13 @@
       <c r="F43" s="65" t="s">
         <v>412</v>
       </c>
-      <c r="G43" s="65"/>
+      <c r="G43" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H43" s="149"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="265"/>
+      <c r="A44" s="284"/>
       <c r="B44" s="65" t="s">
         <v>195</v>
       </c>
@@ -50810,11 +50993,13 @@
       <c r="F44" s="65" t="s">
         <v>413</v>
       </c>
-      <c r="G44" s="65"/>
+      <c r="G44" s="65" t="s">
+        <v>12</v>
+      </c>
       <c r="H44" s="149"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="265"/>
+      <c r="A45" s="284"/>
       <c r="B45" s="65" t="s">
         <v>374</v>
       </c>
@@ -50826,11 +51011,13 @@
       <c r="F45" s="65" t="s">
         <v>414</v>
       </c>
-      <c r="G45" s="65"/>
+      <c r="G45" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H45" s="149"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="265"/>
+      <c r="A46" s="284"/>
       <c r="B46" s="65" t="s">
         <v>415</v>
       </c>
@@ -50842,11 +51029,13 @@
       <c r="F46" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="G46" s="65"/>
+      <c r="G46" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H46" s="149"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="265"/>
+      <c r="A47" s="284"/>
       <c r="B47" s="65" t="s">
         <v>5</v>
       </c>
@@ -50858,11 +51047,13 @@
       <c r="F47" s="65" t="s">
         <v>416</v>
       </c>
-      <c r="G47" s="65"/>
+      <c r="G47" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H47" s="149"/>
     </row>
     <row r="48" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="266"/>
+      <c r="A48" s="285"/>
       <c r="B48" s="69" t="s">
         <v>387</v>
       </c>
@@ -50874,7 +51065,9 @@
       <c r="F48" s="69" t="s">
         <v>417</v>
       </c>
-      <c r="G48" s="69"/>
+      <c r="G48" s="69" t="s">
+        <v>43</v>
+      </c>
       <c r="H48" s="150"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor(model): clean-up inSlots and outSlots
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deslauj/CODE/digitbrain.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C970D60-4A5C-D147-A81A-73A21BFCA518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFEE549-50F2-0C42-B264-7702762A1C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="856" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservice" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="548">
   <si>
     <t>Concept</t>
   </si>
@@ -1734,6 +1734,12 @@
   </si>
   <si>
     <t>[Slots](../slots.md)</t>
+  </si>
+  <si>
+    <t>inSlots</t>
+  </si>
+  <si>
+    <t>outSlots</t>
   </si>
 </sst>
 </file>
@@ -3493,6 +3499,34 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3619,34 +3653,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -7942,8 +7948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
@@ -7964,16 +7970,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="28" t="s">
@@ -8002,7 +8008,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" ht="22.25" customHeight="1">
-      <c r="A3" s="297" t="s">
+      <c r="A3" s="304" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="26"/>
@@ -8014,7 +8020,7 @@
       <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:1024" ht="17">
-      <c r="A4" s="298"/>
+      <c r="A4" s="305"/>
       <c r="B4" s="42" t="s">
         <v>8</v>
       </c>
@@ -8034,7 +8040,7 @@
       <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:1024" ht="34">
-      <c r="A5" s="298"/>
+      <c r="A5" s="305"/>
       <c r="B5" s="42" t="s">
         <v>12</v>
       </c>
@@ -8054,7 +8060,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:1024" ht="17">
-      <c r="A6" s="298"/>
+      <c r="A6" s="305"/>
       <c r="B6" s="42" t="s">
         <v>14</v>
       </c>
@@ -8074,7 +8080,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:1024" ht="17">
-      <c r="A7" s="298"/>
+      <c r="A7" s="305"/>
       <c r="B7" s="42" t="s">
         <v>16</v>
       </c>
@@ -8094,7 +8100,7 @@
       <c r="H7" s="45"/>
     </row>
     <row r="8" spans="1:1024" ht="17">
-      <c r="A8" s="298"/>
+      <c r="A8" s="305"/>
       <c r="B8" s="42" t="s">
         <v>19</v>
       </c>
@@ -8114,7 +8120,7 @@
       <c r="H8" s="259"/>
     </row>
     <row r="9" spans="1:1024" ht="34">
-      <c r="A9" s="298"/>
+      <c r="A9" s="305"/>
       <c r="B9" s="42" t="s">
         <v>21</v>
       </c>
@@ -8134,7 +8140,7 @@
       <c r="H9" s="259"/>
     </row>
     <row r="10" spans="1:1024" ht="51">
-      <c r="A10" s="298"/>
+      <c r="A10" s="305"/>
       <c r="B10" s="42" t="s">
         <v>22</v>
       </c>
@@ -8154,7 +8160,7 @@
       <c r="H10" s="259"/>
     </row>
     <row r="11" spans="1:1024" ht="35" thickBot="1">
-      <c r="A11" s="299"/>
+      <c r="A11" s="306"/>
       <c r="B11" s="46" t="s">
         <v>24</v>
       </c>
@@ -8174,7 +8180,7 @@
       <c r="H11" s="254"/>
     </row>
     <row r="12" spans="1:1024" ht="18.75" customHeight="1">
-      <c r="A12" s="292" t="s">
+      <c r="A12" s="299" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="174"/>
@@ -8186,7 +8192,7 @@
       <c r="H12" s="177"/>
     </row>
     <row r="13" spans="1:1024" ht="51">
-      <c r="A13" s="288"/>
+      <c r="A13" s="295"/>
       <c r="B13" s="50" t="s">
         <v>27</v>
       </c>
@@ -8206,7 +8212,7 @@
       <c r="H13" s="278"/>
     </row>
     <row r="14" spans="1:1024" ht="270.75" customHeight="1">
-      <c r="A14" s="288"/>
+      <c r="A14" s="295"/>
       <c r="B14" s="50" t="s">
         <v>29</v>
       </c>
@@ -8214,7 +8220,7 @@
       <c r="D14" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="E14" s="321" t="s">
+      <c r="E14" s="289" t="s">
         <v>426</v>
       </c>
       <c r="F14" s="50" t="s">
@@ -8226,7 +8232,7 @@
       <c r="H14" s="83"/>
     </row>
     <row r="15" spans="1:1024" s="10" customFormat="1" ht="91.5" customHeight="1">
-      <c r="A15" s="288"/>
+      <c r="A15" s="295"/>
       <c r="B15" s="50" t="s">
         <v>321</v>
       </c>
@@ -8234,7 +8240,7 @@
       <c r="D15" s="50" t="s">
         <v>412</v>
       </c>
-      <c r="E15" s="321" t="s">
+      <c r="E15" s="289" t="s">
         <v>518</v>
       </c>
       <c r="F15" s="50" t="s">
@@ -9262,7 +9268,7 @@
       <c r="AMJ15" s="4"/>
     </row>
     <row r="16" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1">
-      <c r="A16" s="289"/>
+      <c r="A16" s="296"/>
       <c r="B16" s="211" t="s">
         <v>405</v>
       </c>
@@ -10298,7 +10304,7 @@
       <c r="AMJ16" s="4"/>
     </row>
     <row r="17" spans="1:1024" ht="21.5" customHeight="1">
-      <c r="A17" s="300" t="s">
+      <c r="A17" s="307" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="53"/>
@@ -10310,7 +10316,7 @@
       <c r="H17" s="55"/>
     </row>
     <row r="18" spans="1:1024" ht="34">
-      <c r="A18" s="300"/>
+      <c r="A18" s="307"/>
       <c r="B18" s="42" t="s">
         <v>31</v>
       </c>
@@ -10330,7 +10336,7 @@
       <c r="H18" s="45"/>
     </row>
     <row r="19" spans="1:1024" ht="17">
-      <c r="A19" s="300"/>
+      <c r="A19" s="307"/>
       <c r="B19" s="42" t="s">
         <v>35</v>
       </c>
@@ -10350,7 +10356,7 @@
       <c r="H19" s="45"/>
     </row>
     <row r="20" spans="1:1024" ht="34">
-      <c r="A20" s="300"/>
+      <c r="A20" s="307"/>
       <c r="B20" s="42" t="s">
         <v>38</v>
       </c>
@@ -10370,7 +10376,7 @@
       <c r="H20" s="259"/>
     </row>
     <row r="21" spans="1:1024" ht="34">
-      <c r="A21" s="300"/>
+      <c r="A21" s="307"/>
       <c r="B21" s="42" t="s">
         <v>40</v>
       </c>
@@ -10390,7 +10396,7 @@
       <c r="H21" s="279"/>
     </row>
     <row r="22" spans="1:1024" ht="68">
-      <c r="A22" s="300"/>
+      <c r="A22" s="307"/>
       <c r="B22" s="42" t="s">
         <v>44</v>
       </c>
@@ -10410,7 +10416,7 @@
       <c r="H22" s="259"/>
     </row>
     <row r="23" spans="1:1024" ht="17">
-      <c r="A23" s="300"/>
+      <c r="A23" s="307"/>
       <c r="B23" s="42" t="s">
         <v>46</v>
       </c>
@@ -10430,7 +10436,7 @@
       <c r="H23" s="45"/>
     </row>
     <row r="24" spans="1:1024" ht="17">
-      <c r="A24" s="300"/>
+      <c r="A24" s="307"/>
       <c r="B24" s="42" t="s">
         <v>49</v>
       </c>
@@ -10450,7 +10456,7 @@
       <c r="H24" s="45"/>
     </row>
     <row r="25" spans="1:1024" ht="18" thickBot="1">
-      <c r="A25" s="294"/>
+      <c r="A25" s="301"/>
       <c r="B25" s="46" t="s">
         <v>52</v>
       </c>
@@ -10470,7 +10476,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:1024" ht="18.75" customHeight="1">
-      <c r="A26" s="301" t="s">
+      <c r="A26" s="308" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="56"/>
@@ -10482,7 +10488,7 @@
       <c r="H26" s="58"/>
     </row>
     <row r="27" spans="1:1024" ht="17.25" customHeight="1">
-      <c r="A27" s="302"/>
+      <c r="A27" s="309"/>
       <c r="B27" s="59" t="s">
         <v>56</v>
       </c>
@@ -10502,7 +10508,7 @@
       <c r="H27" s="278"/>
     </row>
     <row r="28" spans="1:1024" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A28" s="303"/>
+      <c r="A28" s="310"/>
       <c r="B28" s="63" t="s">
         <v>57</v>
       </c>
@@ -10522,7 +10528,7 @@
       <c r="H28" s="278"/>
     </row>
     <row r="29" spans="1:1024" ht="18.75" customHeight="1">
-      <c r="A29" s="293" t="s">
+      <c r="A29" s="300" t="s">
         <v>398</v>
       </c>
       <c r="B29" s="233"/>
@@ -10534,7 +10540,7 @@
       <c r="H29" s="236"/>
     </row>
     <row r="30" spans="1:1024" s="10" customFormat="1" ht="183" customHeight="1" thickBot="1">
-      <c r="A30" s="294"/>
+      <c r="A30" s="301"/>
       <c r="B30" s="227" t="s">
         <v>399</v>
       </c>
@@ -10542,7 +10548,7 @@
       <c r="D30" s="227" t="s">
         <v>414</v>
       </c>
-      <c r="E30" s="322" t="s">
+      <c r="E30" s="290" t="s">
         <v>534</v>
       </c>
       <c r="F30" s="227" t="s">
@@ -11570,7 +11576,7 @@
       <c r="AMJ30" s="4"/>
     </row>
     <row r="31" spans="1:1024" ht="18.75" customHeight="1">
-      <c r="A31" s="288" t="s">
+      <c r="A31" s="295" t="s">
         <v>401</v>
       </c>
       <c r="B31" s="189"/>
@@ -11582,7 +11588,7 @@
       <c r="H31" s="232"/>
     </row>
     <row r="32" spans="1:1024" ht="17">
-      <c r="A32" s="288"/>
+      <c r="A32" s="295"/>
       <c r="B32" s="192" t="s">
         <v>71</v>
       </c>
@@ -11602,7 +11608,7 @@
       <c r="H32" s="83"/>
     </row>
     <row r="33" spans="1:8" ht="46.75" customHeight="1" thickBot="1">
-      <c r="A33" s="289"/>
+      <c r="A33" s="296"/>
       <c r="B33" s="196" t="s">
         <v>73</v>
       </c>
@@ -11622,7 +11628,7 @@
       <c r="H33" s="83"/>
     </row>
     <row r="34" spans="1:8" ht="16">
-      <c r="A34" s="290" t="s">
+      <c r="A34" s="297" t="s">
         <v>75</v>
       </c>
       <c r="B34" s="283"/>
@@ -11634,7 +11640,7 @@
       <c r="H34" s="286"/>
     </row>
     <row r="35" spans="1:8" ht="116.25" customHeight="1" thickBot="1">
-      <c r="A35" s="291"/>
+      <c r="A35" s="298"/>
       <c r="B35" s="241" t="s">
         <v>76</v>
       </c>
@@ -11642,7 +11648,7 @@
       <c r="D35" s="241" t="s">
         <v>417</v>
       </c>
-      <c r="E35" s="323" t="s">
+      <c r="E35" s="291" t="s">
         <v>532</v>
       </c>
       <c r="F35" s="241" t="s">
@@ -11654,7 +11660,7 @@
       <c r="H35" s="241"/>
     </row>
     <row r="36" spans="1:8" ht="16">
-      <c r="A36" s="292" t="s">
+      <c r="A36" s="299" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="245"/>
@@ -11666,7 +11672,7 @@
       <c r="H36" s="191"/>
     </row>
     <row r="37" spans="1:8" ht="162" customHeight="1" thickBot="1">
-      <c r="A37" s="289"/>
+      <c r="A37" s="296"/>
       <c r="B37" s="228" t="s">
         <v>89</v>
       </c>
@@ -11674,7 +11680,7 @@
       <c r="D37" s="228" t="s">
         <v>418</v>
       </c>
-      <c r="E37" s="324" t="s">
+      <c r="E37" s="292" t="s">
         <v>533</v>
       </c>
       <c r="F37" s="228" t="s">
@@ -11755,16 +11761,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -11793,7 +11799,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>409</v>
       </c>
       <c r="B3" s="119"/>
@@ -11817,7 +11823,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:1024" s="225" customFormat="1" ht="17">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="220" t="s">
         <v>374</v>
       </c>
@@ -12853,7 +12859,7 @@
       <c r="AMJ4" s="224"/>
     </row>
     <row r="5" spans="1:1024" s="225" customFormat="1" ht="17">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="220" t="s">
         <v>376</v>
       </c>
@@ -13889,7 +13895,7 @@
       <c r="AMJ5" s="224"/>
     </row>
     <row r="6" spans="1:1024" s="225" customFormat="1" ht="52" thickBot="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="269" t="s">
         <v>375</v>
       </c>
@@ -14989,16 +14995,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -15027,7 +15033,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>398</v>
       </c>
       <c r="B3" s="119"/>
@@ -15051,7 +15057,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:1024" s="117" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="226" t="s">
         <v>400</v>
       </c>
@@ -16087,7 +16093,7 @@
       <c r="AMJ4" s="229"/>
     </row>
     <row r="5" spans="1:1024" s="117" customFormat="1" ht="51">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="226" t="s">
         <v>60</v>
       </c>
@@ -17123,7 +17129,7 @@
       <c r="AMJ5" s="229"/>
     </row>
     <row r="6" spans="1:1024" s="117" customFormat="1" ht="34">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="226" t="s">
         <v>62</v>
       </c>
@@ -18159,7 +18165,7 @@
       <c r="AMJ6" s="229"/>
     </row>
     <row r="7" spans="1:1024" s="117" customFormat="1" ht="85">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="226" t="s">
         <v>64</v>
       </c>
@@ -19195,7 +19201,7 @@
       <c r="AMJ7" s="229"/>
     </row>
     <row r="8" spans="1:1024" s="117" customFormat="1" ht="34">
-      <c r="A8" s="300"/>
+      <c r="A8" s="307"/>
       <c r="B8" s="226" t="s">
         <v>66</v>
       </c>
@@ -20231,7 +20237,7 @@
       <c r="AMJ8" s="229"/>
     </row>
     <row r="9" spans="1:1024" s="117" customFormat="1" ht="17">
-      <c r="A9" s="300"/>
+      <c r="A9" s="307"/>
       <c r="B9" s="226" t="s">
         <v>68</v>
       </c>
@@ -21267,7 +21273,7 @@
       <c r="AMJ9" s="229"/>
     </row>
     <row r="10" spans="1:1024" s="117" customFormat="1" ht="68">
-      <c r="A10" s="300"/>
+      <c r="A10" s="307"/>
       <c r="B10" s="226" t="s">
         <v>70</v>
       </c>
@@ -22303,7 +22309,7 @@
       <c r="AMJ10" s="229"/>
     </row>
     <row r="11" spans="1:1024" s="183" customFormat="1" ht="86" thickBot="1">
-      <c r="A11" s="294"/>
+      <c r="A11" s="301"/>
       <c r="B11" s="266" t="s">
         <v>424</v>
       </c>
@@ -23423,16 +23429,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>416</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -23461,7 +23467,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="119"/>
@@ -23485,7 +23491,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:1024" customFormat="1" ht="34">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="237" t="s">
         <v>78</v>
       </c>
@@ -24521,7 +24527,7 @@
       <c r="AMJ4" s="1"/>
     </row>
     <row r="5" spans="1:1024" customFormat="1" ht="34">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="237" t="s">
         <v>24</v>
       </c>
@@ -25557,7 +25563,7 @@
       <c r="AMJ5" s="1"/>
     </row>
     <row r="6" spans="1:1024" customFormat="1" ht="17">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="237" t="s">
         <v>11</v>
       </c>
@@ -26593,7 +26599,7 @@
       <c r="AMJ6" s="1"/>
     </row>
     <row r="7" spans="1:1024" customFormat="1" ht="34">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="237" t="s">
         <v>84</v>
       </c>
@@ -27629,7 +27635,7 @@
       <c r="AMJ7" s="1"/>
     </row>
     <row r="8" spans="1:1024" customFormat="1" ht="52" thickBot="1">
-      <c r="A8" s="294"/>
+      <c r="A8" s="301"/>
       <c r="B8" s="241" t="s">
         <v>21</v>
       </c>
@@ -28740,16 +28746,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>419</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -28778,7 +28784,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="119"/>
@@ -28802,7 +28808,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:1024" customFormat="1" ht="34">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="226" t="s">
         <v>78</v>
       </c>
@@ -29838,7 +29844,7 @@
       <c r="AMJ4" s="1"/>
     </row>
     <row r="5" spans="1:1024" customFormat="1" ht="34">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="226" t="s">
         <v>92</v>
       </c>
@@ -30874,7 +30880,7 @@
       <c r="AMJ5" s="1"/>
     </row>
     <row r="6" spans="1:1024" s="14" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="226" t="s">
         <v>94</v>
       </c>
@@ -31910,7 +31916,7 @@
       <c r="AMJ6" s="13"/>
     </row>
     <row r="7" spans="1:1024" s="14" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="226" t="s">
         <v>96</v>
       </c>
@@ -32946,7 +32952,7 @@
       <c r="AMJ7" s="13"/>
     </row>
     <row r="8" spans="1:1024" s="14" customFormat="1" ht="52" thickBot="1">
-      <c r="A8" s="294"/>
+      <c r="A8" s="301"/>
       <c r="B8" s="227" t="s">
         <v>21</v>
       </c>
@@ -34054,16 +34060,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -34092,7 +34098,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>536</v>
       </c>
       <c r="B3" s="119"/>
@@ -34116,7 +34122,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="251" t="s">
         <v>1</v>
       </c>
@@ -35152,7 +35158,7 @@
       <c r="AMJ4" s="5"/>
     </row>
     <row r="5" spans="1:1024" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="251" t="s">
         <v>114</v>
       </c>
@@ -36188,7 +36194,7 @@
       <c r="AMJ5" s="5"/>
     </row>
     <row r="6" spans="1:1024" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="251" t="s">
         <v>358</v>
       </c>
@@ -37224,7 +37230,7 @@
       <c r="AMJ6" s="5"/>
     </row>
     <row r="7" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="251" t="s">
         <v>359</v>
       </c>
@@ -38260,7 +38266,7 @@
       <c r="AMJ7" s="5"/>
     </row>
     <row r="8" spans="1:1024" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A8" s="300"/>
+      <c r="A8" s="307"/>
       <c r="B8" s="251" t="s">
         <v>360</v>
       </c>
@@ -39294,7 +39300,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A9" s="300"/>
+      <c r="A9" s="307"/>
       <c r="B9" s="251"/>
       <c r="C9" s="251" t="s">
         <v>420</v>
@@ -40330,7 +40336,7 @@
       <c r="AMJ9" s="5"/>
     </row>
     <row r="10" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A10" s="300"/>
+      <c r="A10" s="307"/>
       <c r="B10" s="251"/>
       <c r="C10" s="251" t="s">
         <v>421</v>
@@ -41366,7 +41372,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A11" s="300"/>
+      <c r="A11" s="307"/>
       <c r="B11" s="251"/>
       <c r="C11" s="251" t="s">
         <v>422</v>
@@ -42402,7 +42408,7 @@
       <c r="AMJ11" s="5"/>
     </row>
     <row r="12" spans="1:1024" customFormat="1" ht="48" customHeight="1">
-      <c r="A12" s="300"/>
+      <c r="A12" s="307"/>
       <c r="B12" s="251"/>
       <c r="C12" s="251" t="s">
         <v>423</v>
@@ -43438,7 +43444,7 @@
       <c r="AMJ12" s="5"/>
     </row>
     <row r="13" spans="1:1024" customFormat="1" ht="17" customHeight="1">
-      <c r="A13" s="300"/>
+      <c r="A13" s="307"/>
       <c r="B13" s="251" t="s">
         <v>361</v>
       </c>
@@ -44474,7 +44480,7 @@
       <c r="AMJ13" s="5"/>
     </row>
     <row r="14" spans="1:1024" customFormat="1" ht="17" customHeight="1" thickBot="1">
-      <c r="A14" s="294"/>
+      <c r="A14" s="301"/>
       <c r="B14" s="255" t="s">
         <v>362</v>
       </c>
@@ -45602,16 +45608,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:8" s="30" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="28" t="s">
@@ -45640,7 +45646,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.75" customHeight="1">
-      <c r="A3" s="297" t="s">
+      <c r="A3" s="304" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="26"/>
@@ -45652,7 +45658,7 @@
       <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="17">
-      <c r="A4" s="298"/>
+      <c r="A4" s="305"/>
       <c r="B4" s="226" t="s">
         <v>8</v>
       </c>
@@ -45672,7 +45678,7 @@
       <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:8" ht="34">
-      <c r="A5" s="298"/>
+      <c r="A5" s="305"/>
       <c r="B5" s="226" t="s">
         <v>12</v>
       </c>
@@ -45692,7 +45698,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:8" ht="51">
-      <c r="A6" s="298"/>
+      <c r="A6" s="305"/>
       <c r="B6" s="226" t="s">
         <v>21</v>
       </c>
@@ -45712,7 +45718,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:8" ht="51">
-      <c r="A7" s="298"/>
+      <c r="A7" s="305"/>
       <c r="B7" s="226" t="s">
         <v>22</v>
       </c>
@@ -45732,7 +45738,7 @@
       <c r="H7" s="259"/>
     </row>
     <row r="8" spans="1:8" ht="34">
-      <c r="A8" s="298"/>
+      <c r="A8" s="305"/>
       <c r="B8" s="226" t="s">
         <v>24</v>
       </c>
@@ -45752,7 +45758,7 @@
       <c r="H8" s="254"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A9" s="298"/>
+      <c r="A9" s="305"/>
       <c r="B9" s="226" t="s">
         <v>14</v>
       </c>
@@ -45772,7 +45778,7 @@
       <c r="H9" s="259"/>
     </row>
     <row r="10" spans="1:8" ht="17">
-      <c r="A10" s="298"/>
+      <c r="A10" s="305"/>
       <c r="B10" s="226" t="s">
         <v>16</v>
       </c>
@@ -45792,7 +45798,7 @@
       <c r="H10" s="45"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="299"/>
+      <c r="A11" s="306"/>
       <c r="B11" s="227" t="s">
         <v>19</v>
       </c>
@@ -45812,7 +45818,7 @@
       <c r="H11" s="258"/>
     </row>
     <row r="12" spans="1:8" ht="17.75" customHeight="1">
-      <c r="A12" s="304" t="s">
+      <c r="A12" s="311" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="66"/>
@@ -45824,7 +45830,7 @@
       <c r="H12" s="70"/>
     </row>
     <row r="13" spans="1:8" ht="34">
-      <c r="A13" s="305"/>
+      <c r="A13" s="312"/>
       <c r="B13" s="71" t="s">
         <v>109</v>
       </c>
@@ -45844,7 +45850,7 @@
       <c r="H13" s="83"/>
     </row>
     <row r="14" spans="1:8" ht="103.75" customHeight="1" thickBot="1">
-      <c r="A14" s="306"/>
+      <c r="A14" s="313"/>
       <c r="B14" s="248" t="s">
         <v>318</v>
       </c>
@@ -45891,12 +45897,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E10" sqref="E10"/>
       <selection pane="topRight" activeCell="E10" sqref="E10"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -45913,16 +45919,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="31" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="28" t="s">
@@ -45951,7 +45957,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A3" s="297" t="s">
+      <c r="A3" s="304" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="32"/>
@@ -46001,7 +46007,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17">
-      <c r="A4" s="298"/>
+      <c r="A4" s="305"/>
       <c r="B4" s="73" t="s">
         <v>111</v>
       </c>
@@ -46021,7 +46027,7 @@
       <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:1024" ht="19.25" customHeight="1">
-      <c r="A5" s="298"/>
+      <c r="A5" s="305"/>
       <c r="B5" s="73" t="s">
         <v>114</v>
       </c>
@@ -46039,7 +46045,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:1024" ht="35" customHeight="1">
-      <c r="A6" s="298"/>
+      <c r="A6" s="305"/>
       <c r="B6" s="73" t="s">
         <v>117</v>
       </c>
@@ -46057,7 +46063,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:1024" ht="17">
-      <c r="A7" s="298"/>
+      <c r="A7" s="305"/>
       <c r="B7" s="73" t="s">
         <v>118</v>
       </c>
@@ -46075,7 +46081,7 @@
       <c r="H7" s="259"/>
     </row>
     <row r="8" spans="1:1024" ht="17">
-      <c r="A8" s="298"/>
+      <c r="A8" s="305"/>
       <c r="B8" s="73" t="s">
         <v>119</v>
       </c>
@@ -46093,7 +46099,7 @@
       <c r="H8" s="259"/>
     </row>
     <row r="9" spans="1:1024" ht="70" customHeight="1">
-      <c r="A9" s="298"/>
+      <c r="A9" s="305"/>
       <c r="B9" s="73" t="s">
         <v>121</v>
       </c>
@@ -46111,7 +46117,7 @@
       <c r="H9" s="254"/>
     </row>
     <row r="10" spans="1:1024" s="9" customFormat="1" ht="17">
-      <c r="A10" s="298"/>
+      <c r="A10" s="305"/>
       <c r="B10" s="73" t="s">
         <v>123</v>
       </c>
@@ -46142,7 +46148,7 @@
       <c r="AMJ10" s="5"/>
     </row>
     <row r="11" spans="1:1024" ht="70" customHeight="1">
-      <c r="A11" s="298"/>
+      <c r="A11" s="305"/>
       <c r="B11" s="73" t="s">
         <v>3</v>
       </c>
@@ -46160,7 +46166,7 @@
       <c r="H11" s="259"/>
     </row>
     <row r="12" spans="1:1024" ht="17" customHeight="1">
-      <c r="A12" s="298"/>
+      <c r="A12" s="305"/>
       <c r="B12" s="73" t="s">
         <v>127</v>
       </c>
@@ -46178,7 +46184,7 @@
       <c r="H12" s="75"/>
     </row>
     <row r="13" spans="1:1024" ht="51">
-      <c r="A13" s="298"/>
+      <c r="A13" s="305"/>
       <c r="B13" s="73" t="s">
         <v>385</v>
       </c>
@@ -46198,7 +46204,7 @@
       <c r="H13" s="259"/>
     </row>
     <row r="14" spans="1:1024" ht="34">
-      <c r="A14" s="298"/>
+      <c r="A14" s="305"/>
       <c r="B14" s="73" t="s">
         <v>383</v>
       </c>
@@ -46218,7 +46224,7 @@
       <c r="H14" s="259"/>
     </row>
     <row r="15" spans="1:1024" ht="34">
-      <c r="A15" s="298"/>
+      <c r="A15" s="305"/>
       <c r="B15" s="73" t="s">
         <v>384</v>
       </c>
@@ -46238,7 +46244,7 @@
       <c r="H15" s="259"/>
     </row>
     <row r="16" spans="1:1024" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A16" s="299"/>
+      <c r="A16" s="306"/>
       <c r="B16" s="76" t="s">
         <v>130</v>
       </c>
@@ -46256,7 +46262,7 @@
       <c r="H16" s="279"/>
     </row>
     <row r="17" spans="1:1024" s="7" customFormat="1" ht="19">
-      <c r="A17" s="301" t="s">
+      <c r="A17" s="308" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="79"/>
@@ -46269,15 +46275,15 @@
       <c r="AMJ17" s="5"/>
     </row>
     <row r="18" spans="1:1024" ht="185.25" customHeight="1">
-      <c r="A18" s="302"/>
+      <c r="A18" s="309"/>
       <c r="B18" s="81" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="C18" s="82"/>
       <c r="D18" s="81" t="s">
         <v>545</v>
       </c>
-      <c r="E18" s="320" t="s">
+      <c r="E18" s="288" t="s">
         <v>531</v>
       </c>
       <c r="F18" s="81" t="s">
@@ -46289,15 +46295,15 @@
       <c r="H18" s="62"/>
     </row>
     <row r="19" spans="1:1024" ht="183.75" customHeight="1">
-      <c r="A19" s="302"/>
+      <c r="A19" s="309"/>
       <c r="B19" s="81" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="C19" s="82"/>
       <c r="D19" s="81" t="s">
         <v>545</v>
       </c>
-      <c r="E19" s="320" t="s">
+      <c r="E19" s="288" t="s">
         <v>530</v>
       </c>
       <c r="F19" s="81" t="s">
@@ -46309,7 +46315,7 @@
       <c r="H19" s="59"/>
     </row>
     <row r="20" spans="1:1024" ht="41.5" customHeight="1" thickBot="1">
-      <c r="A20" s="303"/>
+      <c r="A20" s="310"/>
       <c r="B20" s="84" t="s">
         <v>133</v>
       </c>
@@ -46327,7 +46333,7 @@
       <c r="H20" s="282"/>
     </row>
     <row r="21" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A21" s="293" t="s">
+      <c r="A21" s="300" t="s">
         <v>134</v>
       </c>
       <c r="B21" s="87"/>
@@ -46377,7 +46383,7 @@
       <c r="AMJ21" s="5"/>
     </row>
     <row r="22" spans="1:1024" s="9" customFormat="1" ht="18" thickBot="1">
-      <c r="A22" s="294"/>
+      <c r="A22" s="301"/>
       <c r="B22" s="76" t="s">
         <v>135</v>
       </c>
@@ -46414,7 +46420,7 @@
       <c r="AMJ22" s="5"/>
     </row>
     <row r="23" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A23" s="301" t="s">
+      <c r="A23" s="308" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="79"/>
@@ -46427,7 +46433,7 @@
       <c r="AMJ23" s="5"/>
     </row>
     <row r="24" spans="1:1024" ht="17">
-      <c r="A24" s="302"/>
+      <c r="A24" s="309"/>
       <c r="B24" s="81" t="s">
         <v>56</v>
       </c>
@@ -46445,7 +46451,7 @@
       <c r="H24" s="278"/>
     </row>
     <row r="25" spans="1:1024" ht="17">
-      <c r="A25" s="302"/>
+      <c r="A25" s="309"/>
       <c r="B25" s="81" t="s">
         <v>57</v>
       </c>
@@ -46463,7 +46469,7 @@
       <c r="H25" s="278"/>
     </row>
     <row r="26" spans="1:1024" ht="18" thickBot="1">
-      <c r="A26" s="303"/>
+      <c r="A26" s="310"/>
       <c r="B26" s="84" t="s">
         <v>58</v>
       </c>
@@ -46481,7 +46487,7 @@
       <c r="H26" s="278"/>
     </row>
     <row r="27" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A27" s="293" t="s">
+      <c r="A27" s="300" t="s">
         <v>141</v>
       </c>
       <c r="B27" s="89"/>
@@ -46512,7 +46518,7 @@
       <c r="AMJ27" s="5"/>
     </row>
     <row r="28" spans="1:1024" ht="34">
-      <c r="A28" s="300"/>
+      <c r="A28" s="307"/>
       <c r="B28" s="73" t="s">
         <v>142</v>
       </c>
@@ -46530,7 +46536,7 @@
       <c r="H28" s="75"/>
     </row>
     <row r="29" spans="1:1024" ht="34">
-      <c r="A29" s="300"/>
+      <c r="A29" s="307"/>
       <c r="B29" s="73" t="s">
         <v>144</v>
       </c>
@@ -46548,7 +46554,7 @@
       <c r="H29" s="75"/>
     </row>
     <row r="30" spans="1:1024" ht="17">
-      <c r="A30" s="300"/>
+      <c r="A30" s="307"/>
       <c r="B30" s="73" t="s">
         <v>35</v>
       </c>
@@ -46566,7 +46572,7 @@
       <c r="H30" s="75"/>
     </row>
     <row r="31" spans="1:1024" ht="17">
-      <c r="A31" s="300"/>
+      <c r="A31" s="307"/>
       <c r="B31" s="73" t="s">
         <v>37</v>
       </c>
@@ -46584,7 +46590,7 @@
       <c r="H31" s="75"/>
     </row>
     <row r="32" spans="1:1024" s="9" customFormat="1" ht="17">
-      <c r="A32" s="300"/>
+      <c r="A32" s="307"/>
       <c r="B32" s="73" t="s">
         <v>46</v>
       </c>
@@ -46622,7 +46628,7 @@
       <c r="AMJ32" s="5"/>
     </row>
     <row r="33" spans="1:1024" ht="17">
-      <c r="A33" s="300"/>
+      <c r="A33" s="307"/>
       <c r="B33" s="73" t="s">
         <v>48</v>
       </c>
@@ -46640,7 +46646,7 @@
       <c r="H33" s="75"/>
     </row>
     <row r="34" spans="1:1024" ht="17">
-      <c r="A34" s="300"/>
+      <c r="A34" s="307"/>
       <c r="B34" s="73" t="s">
         <v>49</v>
       </c>
@@ -46658,7 +46664,7 @@
       <c r="H34" s="75"/>
     </row>
     <row r="35" spans="1:1024" ht="17">
-      <c r="A35" s="300"/>
+      <c r="A35" s="307"/>
       <c r="B35" s="73" t="s">
         <v>51</v>
       </c>
@@ -46676,7 +46682,7 @@
       <c r="H35" s="75"/>
     </row>
     <row r="36" spans="1:1024" ht="18" thickBot="1">
-      <c r="A36" s="294"/>
+      <c r="A36" s="301"/>
       <c r="B36" s="76" t="s">
         <v>52</v>
       </c>
@@ -46694,7 +46700,7 @@
       <c r="H36" s="78"/>
     </row>
     <row r="37" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A37" s="301" t="s">
+      <c r="A37" s="308" t="s">
         <v>341</v>
       </c>
       <c r="B37" s="91"/>
@@ -46707,7 +46713,7 @@
       <c r="AMJ37" s="5"/>
     </row>
     <row r="38" spans="1:1024" ht="90.5" customHeight="1" thickBot="1">
-      <c r="A38" s="303"/>
+      <c r="A38" s="310"/>
       <c r="B38" s="84" t="s">
         <v>5</v>
       </c>
@@ -46788,16 +46794,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="15" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="40" t="s">
@@ -47842,7 +47848,7 @@
       <c r="AMJ2" s="16"/>
     </row>
     <row r="3" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A3" s="311" t="s">
+      <c r="A3" s="318" t="s">
         <v>342</v>
       </c>
       <c r="B3" s="89"/>
@@ -47867,7 +47873,7 @@
       <c r="AMJ3" s="5"/>
     </row>
     <row r="4" spans="1:1024" ht="17.25" customHeight="1">
-      <c r="A4" s="307"/>
+      <c r="A4" s="314"/>
       <c r="B4" s="73" t="s">
         <v>111</v>
       </c>
@@ -47887,7 +47893,7 @@
       <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:1024" ht="17">
-      <c r="A5" s="307"/>
+      <c r="A5" s="314"/>
       <c r="B5" s="73" t="s">
         <v>196</v>
       </c>
@@ -47907,7 +47913,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:1024" ht="34">
-      <c r="A6" s="307"/>
+      <c r="A6" s="314"/>
       <c r="B6" s="73" t="s">
         <v>349</v>
       </c>
@@ -47927,7 +47933,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:1024" ht="18" thickBot="1">
-      <c r="A7" s="307"/>
+      <c r="A7" s="314"/>
       <c r="B7" s="73" t="s">
         <v>199</v>
       </c>
@@ -47947,7 +47953,7 @@
       <c r="H7" s="94"/>
     </row>
     <row r="8" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A8" s="301" t="s">
+      <c r="A8" s="308" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="91"/>
@@ -47960,7 +47966,7 @@
       <c r="AMJ8" s="5"/>
     </row>
     <row r="9" spans="1:1024" s="10" customFormat="1" ht="51">
-      <c r="A9" s="302"/>
+      <c r="A9" s="309"/>
       <c r="B9" s="81" t="s">
         <v>202</v>
       </c>
@@ -48996,7 +49002,7 @@
       <c r="AMJ9" s="8"/>
     </row>
     <row r="10" spans="1:1024" s="10" customFormat="1" ht="34">
-      <c r="A10" s="302"/>
+      <c r="A10" s="309"/>
       <c r="B10" s="81" t="s">
         <v>350</v>
       </c>
@@ -50032,7 +50038,7 @@
       <c r="AMJ10" s="8"/>
     </row>
     <row r="11" spans="1:1024" s="10" customFormat="1" ht="51">
-      <c r="A11" s="302"/>
+      <c r="A11" s="309"/>
       <c r="B11" s="81" t="s">
         <v>206</v>
       </c>
@@ -51068,7 +51074,7 @@
       <c r="AMJ11" s="8"/>
     </row>
     <row r="12" spans="1:1024" s="10" customFormat="1" ht="34">
-      <c r="A12" s="302"/>
+      <c r="A12" s="309"/>
       <c r="B12" s="81" t="s">
         <v>351</v>
       </c>
@@ -52104,7 +52110,7 @@
       <c r="AMJ12" s="8"/>
     </row>
     <row r="13" spans="1:1024" s="10" customFormat="1" ht="52" thickBot="1">
-      <c r="A13" s="303"/>
+      <c r="A13" s="310"/>
       <c r="B13" s="84" t="s">
         <v>204</v>
       </c>
@@ -53140,7 +53146,7 @@
       <c r="AMJ13" s="8"/>
     </row>
     <row r="14" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A14" s="307" t="s">
+      <c r="A14" s="314" t="s">
         <v>343</v>
       </c>
       <c r="B14" s="89"/>
@@ -53161,7 +53167,7 @@
       <c r="AMJ14" s="5"/>
     </row>
     <row r="15" spans="1:1024" s="15" customFormat="1" ht="35" thickBot="1">
-      <c r="A15" s="308"/>
+      <c r="A15" s="315"/>
       <c r="B15" s="76" t="s">
         <v>210</v>
       </c>
@@ -54197,7 +54203,7 @@
       <c r="AMJ15" s="16"/>
     </row>
     <row r="16" spans="1:1024" s="35" customFormat="1" ht="18.25" customHeight="1">
-      <c r="A16" s="309" t="s">
+      <c r="A16" s="316" t="s">
         <v>212</v>
       </c>
       <c r="B16" s="79"/>
@@ -55225,7 +55231,7 @@
       <c r="AMJ16" s="34"/>
     </row>
     <row r="17" spans="1:1024" ht="51">
-      <c r="A17" s="312"/>
+      <c r="A17" s="319"/>
       <c r="B17" s="81" t="s">
         <v>60</v>
       </c>
@@ -55245,7 +55251,7 @@
       <c r="H17" s="278"/>
     </row>
     <row r="18" spans="1:1024" ht="51">
-      <c r="A18" s="312"/>
+      <c r="A18" s="319"/>
       <c r="B18" s="81" t="s">
         <v>62</v>
       </c>
@@ -55265,7 +55271,7 @@
       <c r="H18" s="278"/>
     </row>
     <row r="19" spans="1:1024" ht="85">
-      <c r="A19" s="312"/>
+      <c r="A19" s="319"/>
       <c r="B19" s="81" t="s">
         <v>64</v>
       </c>
@@ -55285,7 +55291,7 @@
       <c r="H19" s="83"/>
     </row>
     <row r="20" spans="1:1024" ht="52" thickBot="1">
-      <c r="A20" s="310"/>
+      <c r="A20" s="317"/>
       <c r="B20" s="260" t="s">
         <v>394</v>
       </c>
@@ -55305,7 +55311,7 @@
       <c r="H20" s="86"/>
     </row>
     <row r="21" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A21" s="307" t="s">
+      <c r="A21" s="314" t="s">
         <v>217</v>
       </c>
       <c r="B21" s="89"/>
@@ -55325,7 +55331,7 @@
       <c r="AMJ21" s="5"/>
     </row>
     <row r="22" spans="1:1024" ht="146.75" customHeight="1">
-      <c r="A22" s="307"/>
+      <c r="A22" s="314"/>
       <c r="B22" s="73" t="s">
         <v>370</v>
       </c>
@@ -55345,7 +55351,7 @@
       <c r="H22" s="259"/>
     </row>
     <row r="23" spans="1:1024" ht="120" thickBot="1">
-      <c r="A23" s="308"/>
+      <c r="A23" s="315"/>
       <c r="B23" s="76" t="s">
         <v>352</v>
       </c>
@@ -55365,7 +55371,7 @@
       <c r="H23" s="258"/>
     </row>
     <row r="24" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A24" s="309" t="s">
+      <c r="A24" s="316" t="s">
         <v>344</v>
       </c>
       <c r="B24" s="98"/>
@@ -55378,7 +55384,7 @@
       <c r="AMJ24" s="5"/>
     </row>
     <row r="25" spans="1:1024" ht="18" thickBot="1">
-      <c r="A25" s="310"/>
+      <c r="A25" s="317"/>
       <c r="B25" s="84" t="s">
         <v>221</v>
       </c>
@@ -55396,7 +55402,7 @@
       <c r="H25" s="96"/>
     </row>
     <row r="26" spans="1:1024" s="6" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A26" s="311" t="s">
+      <c r="A26" s="318" t="s">
         <v>224</v>
       </c>
       <c r="B26" s="89"/>
@@ -55416,7 +55422,7 @@
       <c r="AMJ26" s="5"/>
     </row>
     <row r="27" spans="1:1024" ht="86" thickBot="1">
-      <c r="A27" s="307"/>
+      <c r="A27" s="314"/>
       <c r="B27" s="73" t="s">
         <v>424</v>
       </c>
@@ -55436,7 +55442,7 @@
       <c r="H27" s="254"/>
     </row>
     <row r="28" spans="1:1024" s="7" customFormat="1" ht="17.75" customHeight="1">
-      <c r="A28" s="309" t="s">
+      <c r="A28" s="316" t="s">
         <v>225</v>
       </c>
       <c r="B28" s="91"/>
@@ -55449,7 +55455,7 @@
       <c r="AMJ28" s="5"/>
     </row>
     <row r="29" spans="1:1024" ht="89.75" customHeight="1">
-      <c r="A29" s="312"/>
+      <c r="A29" s="319"/>
       <c r="B29" s="81" t="s">
         <v>70</v>
       </c>
@@ -55469,7 +55475,7 @@
       <c r="H29" s="278"/>
     </row>
     <row r="30" spans="1:1024" ht="89.75" customHeight="1" thickBot="1">
-      <c r="A30" s="310"/>
+      <c r="A30" s="317"/>
       <c r="B30" s="84" t="s">
         <v>371</v>
       </c>
@@ -55547,16 +55553,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="28" t="s">
@@ -55585,7 +55591,7 @@
       </c>
     </row>
     <row r="3" spans="1:1024" s="11" customFormat="1" ht="18.5" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>345</v>
       </c>
       <c r="B3" s="17"/>
@@ -55612,7 +55618,7 @@
       <c r="AMJ3" s="100"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="74" t="s">
         <v>111</v>
       </c>
@@ -55632,7 +55638,7 @@
       <c r="H4" s="103"/>
     </row>
     <row r="5" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="74" t="s">
         <v>156</v>
       </c>
@@ -55652,7 +55658,7 @@
       <c r="H5" s="103"/>
     </row>
     <row r="6" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="74" t="s">
         <v>117</v>
       </c>
@@ -55670,7 +55676,7 @@
       <c r="H6" s="103"/>
     </row>
     <row r="7" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="74" t="s">
         <v>162</v>
       </c>
@@ -55690,7 +55696,7 @@
       <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:1024" ht="34">
-      <c r="A8" s="300"/>
+      <c r="A8" s="307"/>
       <c r="B8" s="74" t="s">
         <v>165</v>
       </c>
@@ -55710,7 +55716,7 @@
       <c r="H8" s="103"/>
     </row>
     <row r="9" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A9" s="300"/>
+      <c r="A9" s="307"/>
       <c r="B9" s="74" t="s">
         <v>168</v>
       </c>
@@ -55730,7 +55736,7 @@
       <c r="H9" s="103"/>
     </row>
     <row r="10" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A10" s="300"/>
+      <c r="A10" s="307"/>
       <c r="B10" s="74" t="s">
         <v>114</v>
       </c>
@@ -55750,7 +55756,7 @@
       <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A11" s="300"/>
+      <c r="A11" s="307"/>
       <c r="B11" s="74" t="s">
         <v>175</v>
       </c>
@@ -55770,7 +55776,7 @@
       <c r="H11" s="103"/>
     </row>
     <row r="12" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A12" s="300"/>
+      <c r="A12" s="307"/>
       <c r="B12" s="74" t="s">
         <v>233</v>
       </c>
@@ -55790,7 +55796,7 @@
       <c r="H12" s="103"/>
     </row>
     <row r="13" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A13" s="300"/>
+      <c r="A13" s="307"/>
       <c r="B13" s="74" t="s">
         <v>181</v>
       </c>
@@ -55810,7 +55816,7 @@
       <c r="H13" s="103"/>
     </row>
     <row r="14" spans="1:1024" ht="85">
-      <c r="A14" s="300"/>
+      <c r="A14" s="307"/>
       <c r="B14" s="74" t="s">
         <v>237</v>
       </c>
@@ -55830,7 +55836,7 @@
       <c r="H14" s="103"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A15" s="300"/>
+      <c r="A15" s="307"/>
       <c r="B15" s="74" t="s">
         <v>239</v>
       </c>
@@ -55850,7 +55856,7 @@
       <c r="H15" s="103"/>
     </row>
     <row r="16" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A16" s="300"/>
+      <c r="A16" s="307"/>
       <c r="B16" s="74" t="s">
         <v>241</v>
       </c>
@@ -55870,7 +55876,7 @@
       <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="34">
-      <c r="A17" s="300"/>
+      <c r="A17" s="307"/>
       <c r="B17" s="74" t="s">
         <v>245</v>
       </c>
@@ -55890,7 +55896,7 @@
       <c r="H17" s="103"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A18" s="294"/>
+      <c r="A18" s="301"/>
       <c r="B18" s="77" t="s">
         <v>192</v>
       </c>
@@ -55953,16 +55959,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:17" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="28" t="s">
@@ -55991,7 +55997,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="110" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A3" s="313" t="s">
+      <c r="A3" s="320" t="s">
         <v>345</v>
       </c>
       <c r="B3" s="108"/>
@@ -56003,7 +56009,7 @@
       <c r="H3" s="109"/>
     </row>
     <row r="4" spans="1:17" ht="17" customHeight="1">
-      <c r="A4" s="317"/>
+      <c r="A4" s="324"/>
       <c r="B4" s="74" t="s">
         <v>111</v>
       </c>
@@ -56032,7 +56038,7 @@
       <c r="Q4" s="110"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" customHeight="1">
-      <c r="A5" s="317"/>
+      <c r="A5" s="324"/>
       <c r="B5" s="74" t="s">
         <v>156</v>
       </c>
@@ -56061,7 +56067,7 @@
       <c r="Q5" s="110"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1">
-      <c r="A6" s="317"/>
+      <c r="A6" s="324"/>
       <c r="B6" s="74" t="s">
         <v>117</v>
       </c>
@@ -56088,7 +56094,7 @@
       <c r="Q6" s="110"/>
     </row>
     <row r="7" spans="1:17" ht="34">
-      <c r="A7" s="317"/>
+      <c r="A7" s="324"/>
       <c r="B7" s="74" t="s">
         <v>162</v>
       </c>
@@ -56117,7 +56123,7 @@
       <c r="Q7" s="110"/>
     </row>
     <row r="8" spans="1:17" ht="34">
-      <c r="A8" s="317"/>
+      <c r="A8" s="324"/>
       <c r="B8" s="74" t="s">
         <v>165</v>
       </c>
@@ -56146,7 +56152,7 @@
       <c r="Q8" s="110"/>
     </row>
     <row r="9" spans="1:17" ht="17" customHeight="1">
-      <c r="A9" s="317"/>
+      <c r="A9" s="324"/>
       <c r="B9" s="74" t="s">
         <v>168</v>
       </c>
@@ -56175,7 +56181,7 @@
       <c r="Q9" s="110"/>
     </row>
     <row r="10" spans="1:17" ht="45.5" customHeight="1">
-      <c r="A10" s="317"/>
+      <c r="A10" s="324"/>
       <c r="B10" s="74" t="s">
         <v>114</v>
       </c>
@@ -56204,7 +56210,7 @@
       <c r="Q10" s="110"/>
     </row>
     <row r="11" spans="1:17" ht="36.5" customHeight="1">
-      <c r="A11" s="317"/>
+      <c r="A11" s="324"/>
       <c r="B11" s="74" t="s">
         <v>175</v>
       </c>
@@ -56233,7 +56239,7 @@
       <c r="Q11" s="110"/>
     </row>
     <row r="12" spans="1:17" s="117" customFormat="1" ht="34">
-      <c r="A12" s="317"/>
+      <c r="A12" s="324"/>
       <c r="B12" s="74" t="s">
         <v>178</v>
       </c>
@@ -56262,7 +56268,7 @@
       <c r="Q12" s="110"/>
     </row>
     <row r="13" spans="1:17" ht="17" customHeight="1">
-      <c r="A13" s="317"/>
+      <c r="A13" s="324"/>
       <c r="B13" s="74" t="s">
         <v>181</v>
       </c>
@@ -56291,7 +56297,7 @@
       <c r="Q13" s="110"/>
     </row>
     <row r="14" spans="1:17" ht="37.25" customHeight="1">
-      <c r="A14" s="317"/>
+      <c r="A14" s="324"/>
       <c r="B14" s="74" t="s">
         <v>185</v>
       </c>
@@ -56320,7 +56326,7 @@
       <c r="Q14" s="110"/>
     </row>
     <row r="15" spans="1:17" ht="21.5" customHeight="1">
-      <c r="A15" s="317"/>
+      <c r="A15" s="324"/>
       <c r="B15" s="74" t="s">
         <v>188</v>
       </c>
@@ -56349,7 +56355,7 @@
       <c r="Q15" s="110"/>
     </row>
     <row r="16" spans="1:17" ht="36.5" customHeight="1" thickBot="1">
-      <c r="A16" s="318"/>
+      <c r="A16" s="325"/>
       <c r="B16" s="77" t="s">
         <v>192</v>
       </c>
@@ -56378,7 +56384,7 @@
       <c r="Q16" s="110"/>
     </row>
     <row r="17" spans="1:17" s="205" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="315" t="s">
+      <c r="A17" s="322" t="s">
         <v>397</v>
       </c>
       <c r="B17" s="201"/>
@@ -56399,7 +56405,7 @@
       <c r="Q17" s="204"/>
     </row>
     <row r="18" spans="1:17" s="205" customFormat="1" ht="121.5" customHeight="1" thickBot="1">
-      <c r="A18" s="316"/>
+      <c r="A18" s="323"/>
       <c r="B18" s="206" t="s">
         <v>382</v>
       </c>
@@ -56407,7 +56413,7 @@
       <c r="D18" s="207" t="s">
         <v>402</v>
       </c>
-      <c r="E18" s="325" t="s">
+      <c r="E18" s="293" t="s">
         <v>490</v>
       </c>
       <c r="F18" s="206" t="s">
@@ -56428,7 +56434,7 @@
       <c r="Q18" s="204"/>
     </row>
     <row r="19" spans="1:17" ht="22" customHeight="1">
-      <c r="A19" s="313" t="s">
+      <c r="A19" s="320" t="s">
         <v>187</v>
       </c>
       <c r="B19" s="184"/>
@@ -56449,7 +56455,7 @@
       <c r="Q19" s="110"/>
     </row>
     <row r="20" spans="1:17" ht="368.25" customHeight="1" thickBot="1">
-      <c r="A20" s="314"/>
+      <c r="A20" s="321"/>
       <c r="B20" s="77" t="s">
         <v>187</v>
       </c>
@@ -56457,7 +56463,7 @@
       <c r="D20" s="76" t="s">
         <v>403</v>
       </c>
-      <c r="E20" s="326" t="s">
+      <c r="E20" s="294" t="s">
         <v>519</v>
       </c>
       <c r="F20" s="77" t="s">
@@ -56521,16 +56527,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:1024" s="37" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -57575,7 +57581,7 @@
       <c r="AMJ2" s="36"/>
     </row>
     <row r="3" spans="1:1024" ht="18.75" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>263</v>
       </c>
       <c r="B3" s="134"/>
@@ -57587,7 +57593,7 @@
       <c r="H3" s="135"/>
     </row>
     <row r="4" spans="1:1024" s="23" customFormat="1" ht="17">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="42" t="s">
         <v>111</v>
       </c>
@@ -58621,7 +58627,7 @@
       <c r="AMJ4" s="22"/>
     </row>
     <row r="5" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="42" t="s">
         <v>156</v>
       </c>
@@ -59655,7 +59661,7 @@
       <c r="AMJ5" s="22"/>
     </row>
     <row r="6" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="42" t="s">
         <v>117</v>
       </c>
@@ -60689,7 +60695,7 @@
       <c r="AMJ6" s="22"/>
     </row>
     <row r="7" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A7" s="300"/>
+      <c r="A7" s="307"/>
       <c r="B7" s="42" t="s">
         <v>266</v>
       </c>
@@ -61723,7 +61729,7 @@
       <c r="AMJ7" s="22"/>
     </row>
     <row r="8" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="300"/>
+      <c r="A8" s="307"/>
       <c r="B8" s="42" t="s">
         <v>268</v>
       </c>
@@ -62757,7 +62763,7 @@
       <c r="AMJ8" s="22"/>
     </row>
     <row r="9" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="300"/>
+      <c r="A9" s="307"/>
       <c r="B9" s="42" t="s">
         <v>270</v>
       </c>
@@ -63791,7 +63797,7 @@
       <c r="AMJ9" s="22"/>
     </row>
     <row r="10" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="300"/>
+      <c r="A10" s="307"/>
       <c r="B10" s="42" t="s">
         <v>272</v>
       </c>
@@ -64825,7 +64831,7 @@
       <c r="AMJ10" s="22"/>
     </row>
     <row r="11" spans="1:1024" s="23" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="300"/>
+      <c r="A11" s="307"/>
       <c r="B11" s="42" t="s">
         <v>274</v>
       </c>
@@ -65859,7 +65865,7 @@
       <c r="AMJ11" s="22"/>
     </row>
     <row r="12" spans="1:1024" s="25" customFormat="1" ht="18" thickBot="1">
-      <c r="A12" s="294"/>
+      <c r="A12" s="301"/>
       <c r="B12" s="46" t="s">
         <v>276</v>
       </c>
@@ -66893,7 +66899,7 @@
       <c r="AMJ12" s="24"/>
     </row>
     <row r="13" spans="1:1024" s="19" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A13" s="301" t="s">
+      <c r="A13" s="308" t="s">
         <v>278</v>
       </c>
       <c r="B13" s="137"/>
@@ -66906,7 +66912,7 @@
       <c r="AMJ13" s="20"/>
     </row>
     <row r="14" spans="1:1024" ht="17">
-      <c r="A14" s="302"/>
+      <c r="A14" s="309"/>
       <c r="B14" s="62" t="s">
         <v>111</v>
       </c>
@@ -66924,7 +66930,7 @@
       <c r="H14" s="139"/>
     </row>
     <row r="15" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A15" s="302"/>
+      <c r="A15" s="309"/>
       <c r="B15" s="62" t="s">
         <v>156</v>
       </c>
@@ -66942,7 +66948,7 @@
       <c r="H15" s="139"/>
     </row>
     <row r="16" spans="1:1024" ht="17">
-      <c r="A16" s="302"/>
+      <c r="A16" s="309"/>
       <c r="B16" s="62" t="s">
         <v>117</v>
       </c>
@@ -66960,7 +66966,7 @@
       <c r="H16" s="139"/>
     </row>
     <row r="17" spans="1:8" ht="17">
-      <c r="A17" s="302"/>
+      <c r="A17" s="309"/>
       <c r="B17" s="62" t="s">
         <v>162</v>
       </c>
@@ -66978,7 +66984,7 @@
       <c r="H17" s="139"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="302"/>
+      <c r="A18" s="309"/>
       <c r="B18" s="62" t="s">
         <v>114</v>
       </c>
@@ -66996,7 +67002,7 @@
       <c r="H18" s="139"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="302"/>
+      <c r="A19" s="309"/>
       <c r="B19" s="62" t="s">
         <v>5</v>
       </c>
@@ -67014,7 +67020,7 @@
       <c r="H19" s="139"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20" s="302"/>
+      <c r="A20" s="309"/>
       <c r="B20" s="62" t="s">
         <v>284</v>
       </c>
@@ -67032,7 +67038,7 @@
       <c r="H20" s="139"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21" s="302"/>
+      <c r="A21" s="309"/>
       <c r="B21" s="62" t="s">
         <v>208</v>
       </c>
@@ -67050,7 +67056,7 @@
       <c r="H21" s="139"/>
     </row>
     <row r="22" spans="1:8" ht="17">
-      <c r="A22" s="302"/>
+      <c r="A22" s="309"/>
       <c r="B22" s="62" t="s">
         <v>287</v>
       </c>
@@ -67068,7 +67074,7 @@
       <c r="H22" s="139"/>
     </row>
     <row r="23" spans="1:8" ht="17">
-      <c r="A23" s="302"/>
+      <c r="A23" s="309"/>
       <c r="B23" s="62" t="s">
         <v>289</v>
       </c>
@@ -67086,7 +67092,7 @@
       <c r="H23" s="139"/>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1">
-      <c r="A24" s="303"/>
+      <c r="A24" s="310"/>
       <c r="B24" s="63" t="s">
         <v>291</v>
       </c>
@@ -67104,7 +67110,7 @@
       <c r="H24" s="140"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A25" s="293" t="s">
+      <c r="A25" s="300" t="s">
         <v>233</v>
       </c>
       <c r="B25" s="141"/>
@@ -67116,7 +67122,7 @@
       <c r="H25" s="142"/>
     </row>
     <row r="26" spans="1:8" ht="17">
-      <c r="A26" s="300"/>
+      <c r="A26" s="307"/>
       <c r="B26" s="42" t="s">
         <v>111</v>
       </c>
@@ -67134,7 +67140,7 @@
       <c r="H26" s="136"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="300"/>
+      <c r="A27" s="307"/>
       <c r="B27" s="42" t="s">
         <v>156</v>
       </c>
@@ -67152,7 +67158,7 @@
       <c r="H27" s="136"/>
     </row>
     <row r="28" spans="1:8" ht="17">
-      <c r="A28" s="300"/>
+      <c r="A28" s="307"/>
       <c r="B28" s="42" t="s">
         <v>117</v>
       </c>
@@ -67170,7 +67176,7 @@
       <c r="H28" s="136"/>
     </row>
     <row r="29" spans="1:8" ht="17">
-      <c r="A29" s="300"/>
+      <c r="A29" s="307"/>
       <c r="B29" s="42" t="s">
         <v>162</v>
       </c>
@@ -67188,7 +67194,7 @@
       <c r="H29" s="136"/>
     </row>
     <row r="30" spans="1:8" ht="17">
-      <c r="A30" s="300"/>
+      <c r="A30" s="307"/>
       <c r="B30" s="42" t="s">
         <v>296</v>
       </c>
@@ -67206,7 +67212,7 @@
       <c r="H30" s="136"/>
     </row>
     <row r="31" spans="1:8" ht="17">
-      <c r="A31" s="300"/>
+      <c r="A31" s="307"/>
       <c r="B31" s="42" t="s">
         <v>114</v>
       </c>
@@ -67224,7 +67230,7 @@
       <c r="H31" s="136"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A32" s="300"/>
+      <c r="A32" s="307"/>
       <c r="B32" s="42" t="s">
         <v>274</v>
       </c>
@@ -67242,7 +67248,7 @@
       <c r="H32" s="136"/>
     </row>
     <row r="33" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A33" s="300"/>
+      <c r="A33" s="307"/>
       <c r="B33" s="42" t="s">
         <v>300</v>
       </c>
@@ -67260,7 +67266,7 @@
       <c r="H33" s="136"/>
     </row>
     <row r="34" spans="1:1024" ht="23.25" customHeight="1">
-      <c r="A34" s="300"/>
+      <c r="A34" s="307"/>
       <c r="B34" s="42" t="s">
         <v>5</v>
       </c>
@@ -67278,7 +67284,7 @@
       <c r="H34" s="136"/>
     </row>
     <row r="35" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A35" s="300"/>
+      <c r="A35" s="307"/>
       <c r="B35" s="42" t="s">
         <v>303</v>
       </c>
@@ -67296,7 +67302,7 @@
       <c r="H35" s="136"/>
     </row>
     <row r="36" spans="1:1024" ht="18" thickBot="1">
-      <c r="A36" s="294"/>
+      <c r="A36" s="301"/>
       <c r="B36" s="46" t="s">
         <v>305</v>
       </c>
@@ -67314,7 +67320,7 @@
       <c r="H36" s="143"/>
     </row>
     <row r="37" spans="1:1024" s="19" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A37" s="301" t="s">
+      <c r="A37" s="308" t="s">
         <v>178</v>
       </c>
       <c r="B37" s="137"/>
@@ -67327,7 +67333,7 @@
       <c r="AMJ37" s="20"/>
     </row>
     <row r="38" spans="1:1024" ht="17">
-      <c r="A38" s="302"/>
+      <c r="A38" s="309"/>
       <c r="B38" s="62" t="s">
         <v>111</v>
       </c>
@@ -67345,7 +67351,7 @@
       <c r="H38" s="139"/>
     </row>
     <row r="39" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A39" s="302"/>
+      <c r="A39" s="309"/>
       <c r="B39" s="62" t="s">
         <v>156</v>
       </c>
@@ -67363,7 +67369,7 @@
       <c r="H39" s="139"/>
     </row>
     <row r="40" spans="1:1024" ht="17">
-      <c r="A40" s="302"/>
+      <c r="A40" s="309"/>
       <c r="B40" s="62" t="s">
         <v>117</v>
       </c>
@@ -67381,7 +67387,7 @@
       <c r="H40" s="139"/>
     </row>
     <row r="41" spans="1:1024" ht="17">
-      <c r="A41" s="302"/>
+      <c r="A41" s="309"/>
       <c r="B41" s="62" t="s">
         <v>162</v>
       </c>
@@ -67399,7 +67405,7 @@
       <c r="H41" s="139"/>
     </row>
     <row r="42" spans="1:1024" ht="17">
-      <c r="A42" s="302"/>
+      <c r="A42" s="309"/>
       <c r="B42" s="62" t="s">
         <v>310</v>
       </c>
@@ -67417,7 +67423,7 @@
       <c r="H42" s="139"/>
     </row>
     <row r="43" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A43" s="302"/>
+      <c r="A43" s="309"/>
       <c r="B43" s="62" t="s">
         <v>233</v>
       </c>
@@ -67435,7 +67441,7 @@
       <c r="H43" s="139"/>
     </row>
     <row r="44" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A44" s="302"/>
+      <c r="A44" s="309"/>
       <c r="B44" s="62" t="s">
         <v>114</v>
       </c>
@@ -67453,7 +67459,7 @@
       <c r="H44" s="139"/>
     </row>
     <row r="45" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A45" s="302"/>
+      <c r="A45" s="309"/>
       <c r="B45" s="62" t="s">
         <v>274</v>
       </c>
@@ -67471,7 +67477,7 @@
       <c r="H45" s="139"/>
     </row>
     <row r="46" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A46" s="302"/>
+      <c r="A46" s="309"/>
       <c r="B46" s="62" t="s">
         <v>315</v>
       </c>
@@ -67489,7 +67495,7 @@
       <c r="H46" s="139"/>
     </row>
     <row r="47" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="A47" s="302"/>
+      <c r="A47" s="309"/>
       <c r="B47" s="62" t="s">
         <v>5</v>
       </c>
@@ -67507,7 +67513,7 @@
       <c r="H47" s="139"/>
     </row>
     <row r="48" spans="1:1024" ht="18" thickBot="1">
-      <c r="A48" s="303"/>
+      <c r="A48" s="310"/>
       <c r="B48" s="63" t="s">
         <v>287</v>
       </c>
@@ -67570,16 +67576,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="302" t="s">
         <v>389</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:20" s="118" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -67608,7 +67614,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="122" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="119"/>
@@ -67632,7 +67638,7 @@
       <c r="T3" s="121"/>
     </row>
     <row r="4" spans="1:20" ht="17">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="123" t="s">
         <v>8</v>
       </c>
@@ -67652,7 +67658,7 @@
       <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:20" ht="20" customHeight="1">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="123" t="s">
         <v>78</v>
       </c>
@@ -67672,7 +67678,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:20" ht="19.25" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="123" t="s">
         <v>523</v>
       </c>
@@ -67692,7 +67698,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:20" ht="18" thickBot="1">
-      <c r="A7" s="294"/>
+      <c r="A7" s="301"/>
       <c r="B7" s="125" t="s">
         <v>16</v>
       </c>
@@ -67712,7 +67718,7 @@
       <c r="H7" s="126"/>
     </row>
     <row r="8" spans="1:20" s="121" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A8" s="301" t="s">
+      <c r="A8" s="308" t="s">
         <v>187</v>
       </c>
       <c r="B8" s="127"/>
@@ -67724,7 +67730,7 @@
       <c r="H8" s="128"/>
     </row>
     <row r="9" spans="1:20" ht="53.25" customHeight="1">
-      <c r="A9" s="302"/>
+      <c r="A9" s="309"/>
       <c r="B9" s="129" t="s">
         <v>24</v>
       </c>
@@ -67744,7 +67750,7 @@
       <c r="H9" s="278"/>
     </row>
     <row r="10" spans="1:20" ht="34" customHeight="1">
-      <c r="A10" s="302"/>
+      <c r="A10" s="309"/>
       <c r="B10" s="129" t="s">
         <v>253</v>
       </c>
@@ -67760,7 +67766,7 @@
       <c r="H10" s="130"/>
     </row>
     <row r="11" spans="1:20" ht="40.75" customHeight="1">
-      <c r="A11" s="302"/>
+      <c r="A11" s="309"/>
       <c r="B11" s="129"/>
       <c r="C11" s="129" t="s">
         <v>254</v>
@@ -67780,7 +67786,7 @@
       <c r="H11" s="278"/>
     </row>
     <row r="12" spans="1:20" ht="35" customHeight="1">
-      <c r="A12" s="302"/>
+      <c r="A12" s="309"/>
       <c r="B12" s="129"/>
       <c r="C12" s="129" t="s">
         <v>255</v>
@@ -67800,7 +67806,7 @@
       <c r="H12" s="278"/>
     </row>
     <row r="13" spans="1:20" ht="37.25" customHeight="1">
-      <c r="A13" s="302"/>
+      <c r="A13" s="309"/>
       <c r="B13" s="129"/>
       <c r="C13" s="129" t="s">
         <v>256</v>
@@ -67820,7 +67826,7 @@
       <c r="H13" s="278"/>
     </row>
     <row r="14" spans="1:20" ht="34">
-      <c r="A14" s="302"/>
+      <c r="A14" s="309"/>
       <c r="B14" s="129"/>
       <c r="C14" s="129" t="s">
         <v>257</v>
@@ -67840,7 +67846,7 @@
       <c r="H14" s="278"/>
     </row>
     <row r="15" spans="1:20" ht="17">
-      <c r="A15" s="302"/>
+      <c r="A15" s="309"/>
       <c r="B15" s="129"/>
       <c r="C15" s="129" t="s">
         <v>259</v>
@@ -67860,7 +67866,7 @@
       <c r="H15" s="278"/>
     </row>
     <row r="16" spans="1:20" ht="34">
-      <c r="A16" s="302"/>
+      <c r="A16" s="309"/>
       <c r="B16" s="129"/>
       <c r="C16" s="129" t="s">
         <v>379</v>
@@ -67880,7 +67886,7 @@
       <c r="H16" s="278"/>
     </row>
     <row r="17" spans="1:8" ht="28.25" customHeight="1">
-      <c r="A17" s="302"/>
+      <c r="A17" s="309"/>
       <c r="B17" s="129" t="s">
         <v>261</v>
       </c>
@@ -67896,7 +67902,7 @@
       <c r="H17" s="130"/>
     </row>
     <row r="18" spans="1:8" ht="18.25" customHeight="1" thickBot="1">
-      <c r="A18" s="303"/>
+      <c r="A18" s="310"/>
       <c r="B18" s="131"/>
       <c r="C18" s="131" t="s">
         <v>259</v>
@@ -68001,16 +68007,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="47.75" customHeight="1">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="326" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="296"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="303"/>
     </row>
     <row r="2" spans="1:20" s="178" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="38" t="s">
@@ -68039,7 +68045,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" s="182" customFormat="1" ht="16.25" customHeight="1">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="300" t="s">
         <v>382</v>
       </c>
       <c r="B3" s="119"/>
@@ -68063,7 +68069,7 @@
       <c r="T3" s="181"/>
     </row>
     <row r="4" spans="1:20" s="117" customFormat="1" ht="99.75" customHeight="1">
-      <c r="A4" s="300"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="73" t="s">
         <v>392</v>
       </c>
@@ -68081,7 +68087,7 @@
       <c r="H4" s="124"/>
     </row>
     <row r="5" spans="1:20" s="117" customFormat="1" ht="84.75" customHeight="1">
-      <c r="A5" s="300"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="123"/>
       <c r="C5" s="123" t="s">
         <v>393</v>
@@ -68099,7 +68105,7 @@
       <c r="H5" s="259"/>
     </row>
     <row r="6" spans="1:20" s="117" customFormat="1" ht="19.25" customHeight="1">
-      <c r="A6" s="300"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="123"/>
       <c r="C6" s="123"/>
       <c r="D6" s="123"/>
@@ -68109,7 +68115,7 @@
       <c r="H6" s="259"/>
     </row>
     <row r="7" spans="1:20" s="183" customFormat="1" ht="17" thickBot="1">
-      <c r="A7" s="294"/>
+      <c r="A7" s="301"/>
       <c r="B7" s="125"/>
       <c r="C7" s="125"/>
       <c r="D7" s="125"/>

</xml_diff>